<commit_message>
added 5 other deepvein deposits
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="331">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -979,6 +979,42 @@
   </si>
   <si>
     <t>Salpetersäure</t>
+  </si>
+  <si>
+    <t>resource_name/iron_deepvein</t>
+  </si>
+  <si>
+    <t>resource_name/iron_vein</t>
+  </si>
+  <si>
+    <t>resource_name/carbon_deepvein</t>
+  </si>
+  <si>
+    <t>resource_name/carbon_vein</t>
+  </si>
+  <si>
+    <t>Carbonium-Ader</t>
+  </si>
+  <si>
+    <t>Ironium-Ader</t>
+  </si>
+  <si>
+    <t>Carbonium outcrop</t>
+  </si>
+  <si>
+    <t>Carbonium vein</t>
+  </si>
+  <si>
+    <t>Ironium vein</t>
+  </si>
+  <si>
+    <t>Ironium outcrop</t>
+  </si>
+  <si>
+    <t>Carbonium-Aufschluss</t>
+  </si>
+  <si>
+    <t>Ironium-Aufschluss</t>
   </si>
 </sst>
 </file>
@@ -1803,10 +1839,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K160"/>
+  <dimension ref="A1:K164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="F143" sqref="F143"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3002,183 +3039,227 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>276</v>
+        <v>321</v>
       </c>
       <c r="B145" t="s">
-        <v>277</v>
+        <v>326</v>
       </c>
       <c r="C145" t="s">
-        <v>277</v>
+        <v>323</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>292</v>
+        <v>322</v>
       </c>
       <c r="B146" t="s">
-        <v>307</v>
+        <v>325</v>
       </c>
       <c r="C146" t="s">
-        <v>311</v>
+        <v>329</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="B147" t="s">
-        <v>306</v>
+        <v>277</v>
       </c>
       <c r="C147" t="s">
-        <v>310</v>
+        <v>277</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="B148" t="s">
-        <v>279</v>
+        <v>307</v>
       </c>
       <c r="C148" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="B149" t="s">
-        <v>281</v>
+        <v>306</v>
       </c>
       <c r="C149" t="s">
-        <v>281</v>
+        <v>310</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B150" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C150" t="s">
-        <v>318</v>
+        <v>279</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>284</v>
+        <v>319</v>
       </c>
       <c r="B151" t="s">
-        <v>285</v>
+        <v>327</v>
       </c>
       <c r="C151" t="s">
-        <v>285</v>
+        <v>324</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>295</v>
+        <v>320</v>
       </c>
       <c r="B152" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="C152" t="s">
-        <v>309</v>
+        <v>330</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="B153" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="C153" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B154" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C154" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B155" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C155" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B156" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C156" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B157" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C157" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B158" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C158" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B159" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="C159" t="s">
-        <v>316</v>
+        <v>289</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
+        <v>294</v>
+      </c>
+      <c r="B160" t="s">
+        <v>301</v>
+      </c>
+      <c r="C160" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>298</v>
+      </c>
+      <c r="B161" t="s">
+        <v>304</v>
+      </c>
+      <c r="C161" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>290</v>
+      </c>
+      <c r="B162" t="s">
+        <v>291</v>
+      </c>
+      <c r="C162" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>293</v>
+      </c>
+      <c r="B163" t="s">
+        <v>302</v>
+      </c>
+      <c r="C163" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
         <v>297</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B164" t="s">
         <v>303</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C164" t="s">
         <v>317</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K1">
-    <sortState ref="A2:K160">
+    <sortState ref="A2:K164">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
reworked rare elment mines for deepveins
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="346">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -1015,6 +1015,51 @@
   </si>
   <si>
     <t>Ironium-Aufschluss</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/mining_drill</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/mining_drill</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/mining_drill_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/mining_drill_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/strip_mine_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/strip_mine_lvl_2</t>
+  </si>
+  <si>
+    <t>Strip Mine 2</t>
+  </si>
+  <si>
+    <t>Strip Mine 3</t>
+  </si>
+  <si>
+    <t>Mining Drill</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/mining_drill_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/mining_drill_lvl_3</t>
+  </si>
+  <si>
+    <t>Mines for underground resource veins</t>
+  </si>
+  <si>
+    <t>Mines for underground resource veins. More effective by dissolving metals</t>
+  </si>
+  <si>
+    <t>Fracking Drill 2</t>
+  </si>
+  <si>
+    <t>Fracking Drill 3</t>
   </si>
 </sst>
 </file>
@@ -1839,11 +1884,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K164"/>
+  <dimension ref="A1:K172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A155" sqref="A155"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2078,1188 +2123,1252 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>331</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>342</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>340</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>343</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>341</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>343</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B52" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B56" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B62" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B64" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>332</v>
       </c>
       <c r="B65" t="s">
-        <v>131</v>
+        <v>339</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>132</v>
+        <v>333</v>
       </c>
       <c r="B66" t="s">
-        <v>133</v>
+        <v>344</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>334</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>345</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B68" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B69" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B70" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B72" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B73" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>147</v>
+        <v>336</v>
       </c>
       <c r="B74" t="s">
-        <v>145</v>
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>148</v>
+        <v>335</v>
       </c>
       <c r="B75" t="s">
-        <v>149</v>
+        <v>338</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="B76" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="B77" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B78" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B79" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B80" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="B81" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B82" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="B83" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B84" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="B85" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="B86" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="B87" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="B88" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="B89" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="B90" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="B91" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="B92" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B93" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="B94" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="B95" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B96" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="B97" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="B98" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B99" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="B100" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="B101" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="B102" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="B103" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B104" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="B105" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="B106" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="B107" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="B108" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="B109" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="B110" t="s">
-        <v>165</v>
+        <v>203</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="B111" t="s">
-        <v>167</v>
+        <v>205</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="B112" t="s">
-        <v>169</v>
+        <v>207</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B113" t="s">
-        <v>171</v>
+        <v>209</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B114" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B115" t="s">
-        <v>175</v>
+        <v>213</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B116" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B117" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B118" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B119" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B120" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B121" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B122" t="s">
-        <v>231</v>
+        <v>173</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B123" t="s">
-        <v>233</v>
+        <v>175</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B124" t="s">
-        <v>235</v>
+        <v>177</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B125" t="s">
-        <v>237</v>
+        <v>179</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B126" t="s">
-        <v>239</v>
+        <v>181</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="B127" t="s">
-        <v>241</v>
+        <v>183</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
+        <v>228</v>
+      </c>
+      <c r="B128" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>229</v>
+      </c>
+      <c r="B129" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>230</v>
+      </c>
+      <c r="B130" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>232</v>
+      </c>
+      <c r="B131" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>234</v>
+      </c>
+      <c r="B132" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>236</v>
+      </c>
+      <c r="B133" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>238</v>
+      </c>
+      <c r="B134" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>240</v>
+      </c>
+      <c r="B135" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>242</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B136" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
         <v>244</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B137" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>246</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B138" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>248</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B139" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>250</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B140" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
         <v>252</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B141" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>254</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B142" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>256</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B143" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
         <v>258</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B144" t="s">
         <v>259</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
-        <v>260</v>
-      </c>
-      <c r="B137" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
-        <v>262</v>
-      </c>
-      <c r="B138" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
-        <v>264</v>
-      </c>
-      <c r="B139" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
-        <v>266</v>
-      </c>
-      <c r="B140" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
-        <v>268</v>
-      </c>
-      <c r="B141" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
-        <v>270</v>
-      </c>
-      <c r="B142" t="s">
-        <v>271</v>
-      </c>
-      <c r="C142" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
-        <v>272</v>
-      </c>
-      <c r="B143" t="s">
-        <v>273</v>
-      </c>
-      <c r="C143" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
-        <v>274</v>
-      </c>
-      <c r="B144" t="s">
-        <v>275</v>
-      </c>
-      <c r="C144" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>321</v>
+        <v>260</v>
       </c>
       <c r="B145" t="s">
-        <v>326</v>
-      </c>
-      <c r="C145" t="s">
-        <v>323</v>
+        <v>261</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>322</v>
+        <v>262</v>
       </c>
       <c r="B146" t="s">
-        <v>325</v>
-      </c>
-      <c r="C146" t="s">
-        <v>329</v>
+        <v>263</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="B147" t="s">
-        <v>277</v>
-      </c>
-      <c r="C147" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
       <c r="B148" t="s">
-        <v>307</v>
-      </c>
-      <c r="C148" t="s">
-        <v>311</v>
+        <v>267</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
       <c r="B149" t="s">
-        <v>306</v>
-      </c>
-      <c r="C149" t="s">
-        <v>310</v>
+        <v>269</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B150" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C150" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>319</v>
+        <v>272</v>
       </c>
       <c r="B151" t="s">
-        <v>327</v>
+        <v>273</v>
       </c>
       <c r="C151" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>320</v>
+        <v>274</v>
       </c>
       <c r="B152" t="s">
-        <v>328</v>
+        <v>275</v>
       </c>
       <c r="C152" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>280</v>
+        <v>321</v>
       </c>
       <c r="B153" t="s">
-        <v>281</v>
+        <v>326</v>
       </c>
       <c r="C153" t="s">
-        <v>281</v>
+        <v>323</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>282</v>
+        <v>322</v>
       </c>
       <c r="B154" t="s">
-        <v>283</v>
+        <v>325</v>
       </c>
       <c r="C154" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B155" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C155" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B156" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C156" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B157" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C157" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B158" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C158" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>288</v>
+        <v>319</v>
       </c>
       <c r="B159" t="s">
-        <v>289</v>
+        <v>327</v>
       </c>
       <c r="C159" t="s">
-        <v>289</v>
+        <v>324</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>294</v>
+        <v>320</v>
       </c>
       <c r="B160" t="s">
-        <v>301</v>
+        <v>328</v>
       </c>
       <c r="C160" t="s">
-        <v>314</v>
+        <v>330</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="B161" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
       <c r="C161" t="s">
-        <v>315</v>
+        <v>281</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B162" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="C162" t="s">
-        <v>291</v>
+        <v>318</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B163" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="C163" t="s">
-        <v>316</v>
+        <v>285</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
+        <v>295</v>
+      </c>
+      <c r="B164" t="s">
+        <v>300</v>
+      </c>
+      <c r="C164" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>299</v>
+      </c>
+      <c r="B165" t="s">
+        <v>305</v>
+      </c>
+      <c r="C165" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>286</v>
+      </c>
+      <c r="B166" t="s">
+        <v>287</v>
+      </c>
+      <c r="C166" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>288</v>
+      </c>
+      <c r="B167" t="s">
+        <v>289</v>
+      </c>
+      <c r="C167" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>294</v>
+      </c>
+      <c r="B168" t="s">
+        <v>301</v>
+      </c>
+      <c r="C168" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>298</v>
+      </c>
+      <c r="B169" t="s">
+        <v>304</v>
+      </c>
+      <c r="C169" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>290</v>
+      </c>
+      <c r="B170" t="s">
+        <v>291</v>
+      </c>
+      <c r="C170" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>293</v>
+      </c>
+      <c r="B171" t="s">
+        <v>302</v>
+      </c>
+      <c r="C171" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
         <v>297</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B172" t="s">
         <v>303</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C172" t="s">
         <v>317</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K1">
-    <sortState ref="A2:K164">
+    <sortState ref="A2:K172">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
added fluorine trap building
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="12400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="rebalance_localizations" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="366">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -1077,10 +1077,49 @@
     <t>gui/hud/building_name/fluorine_trap</t>
   </si>
   <si>
-    <t>Captures trace elements from atmosphere</t>
-  </si>
-  <si>
     <t>Atmospheric Fluorine Trap</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/solvent_condenser</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/solvent_condenser</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/fluorine_trap_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/fluorine_trap_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/solvent_condenser_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/solvent_condenser_lvl_3</t>
+  </si>
+  <si>
+    <t>Captures fluorine compounds from atmosphere</t>
+  </si>
+  <si>
+    <t>Solvent Condenser</t>
+  </si>
+  <si>
+    <t>Condenses hyrdo-fluorines into solvent liquid</t>
+  </si>
+  <si>
+    <t>Atmosphärische Fluorfalle</t>
+  </si>
+  <si>
+    <t>Extrahiert Fluorverbindungen aus der Atmophäre</t>
+  </si>
+  <si>
+    <t>Solvens</t>
+  </si>
+  <si>
+    <t>Verdichtet Fluorwasserstoffe zur Solvens-Flüssigkeit</t>
+  </si>
+  <si>
+    <t>Solvensverdichter</t>
   </si>
 </sst>
 </file>
@@ -1905,20 +1944,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K175"/>
+  <dimension ref="A1:K181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.1796875" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1950,7 +1989,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1958,7 +1997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1966,7 +2005,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1974,7 +2013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1982,7 +2021,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1990,7 +2029,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1998,7 +2037,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2006,7 +2045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2014,7 +2053,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -2022,7 +2061,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2030,7 +2069,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2038,7 +2077,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2046,7 +2085,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2054,7 +2093,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2062,7 +2101,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2070,7 +2109,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2078,7 +2117,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2086,7 +2125,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -2094,7 +2133,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2102,7 +2141,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2110,7 +2149,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -2118,15 +2157,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>349</v>
       </c>
       <c r="B23" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>358</v>
+      </c>
+      <c r="C23" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -2134,7 +2176,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -2142,7 +2184,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2150,7 +2192,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>331</v>
       </c>
@@ -2158,7 +2200,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>340</v>
       </c>
@@ -2166,7 +2208,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>341</v>
       </c>
@@ -2174,7 +2216,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -2182,7 +2224,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -2190,7 +2232,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -2198,7 +2240,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -2206,7 +2248,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -2214,7 +2256,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -2222,1201 +2264,1270 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>352</v>
+      </c>
+      <c r="B36" t="s">
+        <v>360</v>
+      </c>
+      <c r="C36" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>66</v>
-      </c>
-      <c r="B36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>68</v>
       </c>
       <c r="B37" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>70</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>72</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>74</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>76</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>78</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>80</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>82</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>84</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>86</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>88</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>90</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>92</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>94</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>96</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>98</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>100</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>102</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>104</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>106</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>108</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>110</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>112</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>114</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>116</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>118</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>120</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>350</v>
       </c>
-      <c r="B65" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+      <c r="B66" t="s">
+        <v>351</v>
+      </c>
+      <c r="C66" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>354</v>
+      </c>
+      <c r="B67" t="s">
+        <v>351</v>
+      </c>
+      <c r="C67" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>355</v>
+      </c>
+      <c r="B68" t="s">
+        <v>351</v>
+      </c>
+      <c r="C68" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>122</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B69" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>332</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B70" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>333</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B71" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>334</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B72" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>124</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B73" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>126</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B74" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>128</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B75" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>130</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B76" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>353</v>
+      </c>
+      <c r="B77" t="s">
+        <v>359</v>
+      </c>
+      <c r="C77" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>356</v>
+      </c>
+      <c r="B78" t="s">
+        <v>359</v>
+      </c>
+      <c r="C78" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>357</v>
+      </c>
+      <c r="B79" t="s">
+        <v>359</v>
+      </c>
+      <c r="C79" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>132</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B80" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>134</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B81" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>336</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B82" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>335</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B83" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>136</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B84" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>138</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B85" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>140</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B86" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>142</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B87" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>144</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B88" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>146</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B89" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>147</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B90" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>148</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B91" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>150</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B92" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>152</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B93" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>154</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B94" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>156</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B95" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>158</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B96" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>160</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B97" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>162</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B98" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>164</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B99" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>166</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B100" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>168</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B101" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>170</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B102" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>172</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B103" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>174</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B104" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>176</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B105" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>178</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B106" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>180</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B107" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>182</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B108" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>184</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B109" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>186</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B110" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>188</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B111" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>190</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B112" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>192</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B113" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>194</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B114" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>196</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B115" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>198</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B116" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>200</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B117" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>202</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B118" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>204</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B119" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>206</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B120" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>208</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B121" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>210</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B122" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>212</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B123" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>214</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B124" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>216</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B125" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>218</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B126" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>219</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B127" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>220</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B128" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>221</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B129" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>222</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B130" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>223</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B131" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>224</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B132" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>225</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B133" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>226</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B134" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>227</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B135" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>228</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B136" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>229</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B137" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>230</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B138" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>232</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B139" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>234</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B140" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>236</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B141" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>238</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B142" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>240</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B143" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>242</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B144" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>244</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B145" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>246</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B146" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>248</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B147" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>250</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B148" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>252</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B149" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>254</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B150" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>256</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B151" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>258</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B152" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>260</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B153" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A148" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>262</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B154" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>264</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B155" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" t="s">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>266</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B156" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A151" t="s">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>268</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B157" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A152" t="s">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>270</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B158" t="s">
         <v>271</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C158" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" t="s">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>272</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B159" t="s">
         <v>273</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C159" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" t="s">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>274</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B160" t="s">
         <v>275</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C160" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A155" t="s">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>321</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B161" t="s">
         <v>326</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C161" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A156" t="s">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>322</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B162" t="s">
         <v>325</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C162" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A157" t="s">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>276</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B163" t="s">
         <v>277</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C163" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A158" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>292</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B164" t="s">
         <v>307</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C164" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A159" t="s">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>296</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B165" t="s">
         <v>306</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C165" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A160" t="s">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>278</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B166" t="s">
         <v>279</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C166" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A161" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>346</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B167" t="s">
         <v>347</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C167" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A162" t="s">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>319</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B168" t="s">
         <v>327</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C168" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A163" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>320</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B169" t="s">
         <v>328</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C169" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A164" t="s">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>280</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B170" t="s">
         <v>281</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C170" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A165" t="s">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>282</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B171" t="s">
         <v>283</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C171" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A166" t="s">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>284</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B172" t="s">
         <v>285</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C172" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A167" t="s">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>295</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B173" t="s">
         <v>300</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C173" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A168" t="s">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>299</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B174" t="s">
         <v>305</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C174" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A169" t="s">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>286</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B175" t="s">
         <v>287</v>
       </c>
-      <c r="C169" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A170" t="s">
+      <c r="C175" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>288</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B176" t="s">
         <v>289</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C176" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>294</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B177" t="s">
         <v>301</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C177" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A172" t="s">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>298</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B178" t="s">
         <v>304</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C178" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A173" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>290</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B179" t="s">
         <v>291</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C179" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A174" t="s">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>293</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B180" t="s">
         <v>302</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C180" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A175" t="s">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>297</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B181" t="s">
         <v>303</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C181" t="s">
         <v>317</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K1">
-    <sortState ref="A2:K175">
+    <sortState ref="A2:K181">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
added liquid and ammonium deepveins
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="12405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28790" windowHeight="12410"/>
   </bookViews>
   <sheets>
     <sheet name="rebalance_localizations" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="389">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -1120,6 +1120,75 @@
   </si>
   <si>
     <t>Solvensverdichter</t>
+  </si>
+  <si>
+    <t>resource_name/mud_deepvein</t>
+  </si>
+  <si>
+    <t>resource_name/water_deepvein</t>
+  </si>
+  <si>
+    <t>resource_name/sludge_deepvein</t>
+  </si>
+  <si>
+    <t>resource_name/magma_deepvein</t>
+  </si>
+  <si>
+    <t>resource_name/morphium_deepvein</t>
+  </si>
+  <si>
+    <t>resource_name/ammonium_deepvein</t>
+  </si>
+  <si>
+    <t>Ammonium-Ader</t>
+  </si>
+  <si>
+    <t>Ammonium deep vein</t>
+  </si>
+  <si>
+    <t>Sludge well</t>
+  </si>
+  <si>
+    <t>Magma well</t>
+  </si>
+  <si>
+    <t>Morphium well</t>
+  </si>
+  <si>
+    <t>Water well</t>
+  </si>
+  <si>
+    <t>Mud well</t>
+  </si>
+  <si>
+    <t>Magmakammer</t>
+  </si>
+  <si>
+    <t>Morphiumquelle</t>
+  </si>
+  <si>
+    <t>Pumpjack</t>
+  </si>
+  <si>
+    <t>Pumpjack able to pump liquids from deep wells</t>
+  </si>
+  <si>
+    <t>Tiefpumpe</t>
+  </si>
+  <si>
+    <t>Tiefpumpe zur Förderung von unterirdischen Quellen</t>
+  </si>
+  <si>
+    <t>Grundwasserquelle</t>
+  </si>
+  <si>
+    <t>schlammige Gunrdwasserquelle</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/liquid_pumpjack</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/liquid_pumpjack</t>
   </si>
 </sst>
 </file>
@@ -1944,20 +2013,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K181"/>
+  <dimension ref="A1:K189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="54.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="54.1796875" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1989,7 +2058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1997,7 +2066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2005,7 +2074,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2013,7 +2082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2021,7 +2090,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2029,7 +2098,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2037,7 +2106,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2045,7 +2114,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2053,7 +2122,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -2061,7 +2130,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2069,7 +2138,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2077,7 +2146,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2085,7 +2154,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2093,7 +2162,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2101,7 +2170,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2109,7 +2178,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2117,7 +2186,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2125,7 +2194,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -2133,7 +2202,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2141,7 +2210,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2149,7 +2218,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -2157,7 +2226,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>349</v>
       </c>
@@ -2168,7 +2237,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -2176,7 +2245,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -2184,7 +2253,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2192,335 +2261,335 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>387</v>
+      </c>
+      <c r="B27" t="s">
+        <v>382</v>
+      </c>
+      <c r="C27" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>331</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>340</v>
-      </c>
-      <c r="B28" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>341</v>
       </c>
       <c r="B29" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>341</v>
+      </c>
+      <c r="B30" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>58</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>60</v>
       </c>
       <c r="B31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>62</v>
-      </c>
-      <c r="B33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>64</v>
       </c>
       <c r="B34" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>352</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>360</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>66</v>
-      </c>
-      <c r="B37" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>68</v>
       </c>
       <c r="B38" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>70</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>72</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>74</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>76</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>78</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>80</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>82</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>84</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>86</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>88</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>90</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>92</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>94</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>96</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>98</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>100</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>102</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>104</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>106</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>108</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>110</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>112</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>114</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>116</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>118</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>120</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>350</v>
-      </c>
-      <c r="B66" t="s">
-        <v>351</v>
-      </c>
-      <c r="C66" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>354</v>
       </c>
       <c r="B67" t="s">
         <v>351</v>
@@ -2529,9 +2598,9 @@
         <v>361</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B68" t="s">
         <v>351</v>
@@ -2540,95 +2609,95 @@
         <v>361</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>355</v>
+      </c>
+      <c r="B69" t="s">
+        <v>351</v>
+      </c>
+      <c r="C69" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>122</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>388</v>
+      </c>
+      <c r="B71" t="s">
+        <v>381</v>
+      </c>
+      <c r="C71" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>332</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B72" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>333</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B73" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>334</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B74" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>124</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B75" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>126</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B76" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>128</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B77" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>130</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B78" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>353</v>
-      </c>
-      <c r="B77" t="s">
-        <v>359</v>
-      </c>
-      <c r="C77" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>356</v>
-      </c>
-      <c r="B78" t="s">
-        <v>359</v>
-      </c>
-      <c r="C78" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>357</v>
       </c>
       <c r="B79" t="s">
         <v>359</v>
@@ -2637,897 +2706,982 @@
         <v>365</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>356</v>
+      </c>
+      <c r="B80" t="s">
+        <v>359</v>
+      </c>
+      <c r="C80" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>357</v>
+      </c>
+      <c r="B81" t="s">
+        <v>359</v>
+      </c>
+      <c r="C81" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>132</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B82" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>134</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B83" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>336</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B84" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>335</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B85" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>136</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B86" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>138</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B87" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>140</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B88" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>142</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B89" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>144</v>
-      </c>
-      <c r="B88" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>146</v>
-      </c>
-      <c r="B89" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>147</v>
       </c>
       <c r="B90" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
+        <v>146</v>
+      </c>
+      <c r="B91" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>147</v>
+      </c>
+      <c r="B92" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>148</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B93" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>150</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B94" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
         <v>152</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B95" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>154</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B96" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>156</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B97" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>158</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B98" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>160</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B99" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>162</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B100" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>164</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B101" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>166</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B102" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>168</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B103" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>170</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B104" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>172</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B105" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>174</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B106" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>176</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B107" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>178</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B108" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>180</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B109" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>182</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B110" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>184</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B111" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>186</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B112" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
         <v>188</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B113" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
         <v>190</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B114" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
         <v>192</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B115" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
         <v>194</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B116" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>196</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B117" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>198</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B118" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>200</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B119" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
         <v>202</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B120" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
         <v>204</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B121" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
         <v>206</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B122" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>208</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B123" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
         <v>210</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B124" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
         <v>212</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B125" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
         <v>214</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B126" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
         <v>216</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B127" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
         <v>218</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B128" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>219</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B129" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
         <v>220</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B130" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
         <v>221</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B131" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
         <v>222</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B132" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
         <v>223</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B133" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
         <v>224</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B134" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>225</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B135" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>226</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B136" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
         <v>227</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B137" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>228</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B138" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>229</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B139" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>230</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B140" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
         <v>232</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B141" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>234</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B142" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>236</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B143" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
         <v>238</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B144" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
         <v>240</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B145" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
         <v>242</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B146" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
         <v>244</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B147" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
         <v>246</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B148" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
         <v>248</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B149" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
         <v>250</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B150" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
         <v>252</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B151" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
         <v>254</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B152" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
         <v>256</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B153" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
         <v>258</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B154" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
         <v>260</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B155" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
         <v>262</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B156" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
         <v>264</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B157" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
         <v>266</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B158" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
         <v>268</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B159" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
         <v>270</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B160" t="s">
         <v>271</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C160" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>371</v>
+      </c>
+      <c r="B161" t="s">
+        <v>373</v>
+      </c>
+      <c r="C161" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
         <v>272</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B162" t="s">
         <v>273</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C162" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
         <v>274</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B163" t="s">
         <v>275</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C163" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
         <v>321</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B164" t="s">
         <v>326</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C164" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
         <v>322</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B165" t="s">
         <v>325</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C165" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
         <v>276</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B166" t="s">
         <v>277</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C166" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
         <v>292</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B167" t="s">
         <v>307</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C167" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
         <v>296</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B168" t="s">
         <v>306</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C168" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
         <v>278</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B169" t="s">
         <v>279</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C169" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
         <v>346</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B170" t="s">
         <v>347</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C170" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
         <v>319</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B171" t="s">
         <v>327</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C171" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
         <v>320</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B172" t="s">
         <v>328</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C172" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>369</v>
+      </c>
+      <c r="B173" t="s">
+        <v>375</v>
+      </c>
+      <c r="C173" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
         <v>280</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B174" t="s">
         <v>281</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C174" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>370</v>
+      </c>
+      <c r="B175" t="s">
+        <v>376</v>
+      </c>
+      <c r="C175" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>366</v>
+      </c>
+      <c r="B176" t="s">
+        <v>378</v>
+      </c>
+      <c r="C176" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
         <v>282</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B177" t="s">
         <v>283</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C177" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
         <v>284</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B178" t="s">
         <v>285</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C178" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
         <v>295</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B179" t="s">
         <v>300</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C179" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
         <v>299</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B180" t="s">
         <v>305</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C180" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>368</v>
+      </c>
+      <c r="B181" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
         <v>286</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B182" t="s">
         <v>287</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C182" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
         <v>288</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B183" t="s">
         <v>289</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C183" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
         <v>294</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B184" t="s">
         <v>301</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C184" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
         <v>298</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B185" t="s">
         <v>304</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C185" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
         <v>290</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B186" t="s">
         <v>291</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C186" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
         <v>293</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B187" t="s">
         <v>302</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C187" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
         <v>297</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B188" t="s">
         <v>303</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C188" t="s">
         <v>317</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>367</v>
+      </c>
+      <c r="B189" t="s">
+        <v>377</v>
+      </c>
+      <c r="C189" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K1">
-    <sortState ref="A2:K181">
+    <sortState ref="A2:K189">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
added a water placed energy connector
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WinData\EpicGames\Riftbreaker\TheRiftbreaker\mods\rebalance\gui\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\TheRiftbreaker\mods\rebalance\gui\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28790" windowHeight="12410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="rebalance_localizations" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="393">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -1189,6 +1189,18 @@
   </si>
   <si>
     <t>gui/hud/building_name/liquid_pumpjack</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/energy_connector_water</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/energy_connector_water</t>
+  </si>
+  <si>
+    <t>Energy Connector Water</t>
+  </si>
+  <si>
+    <t>Energy connector on platform that can be placed on liquids pools</t>
   </si>
 </sst>
 </file>
@@ -1694,48 +1706,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2013,20 +2025,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K189"/>
+  <dimension ref="A1:K191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.1796875" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2058,7 +2070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2066,7 +2078,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2074,7 +2086,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2082,7 +2094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2090,7 +2102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2098,7 +2110,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2106,7 +2118,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2114,7 +2126,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2122,7 +2134,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -2130,7 +2142,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2138,7 +2150,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2146,7 +2158,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2154,7 +2166,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2162,7 +2174,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2170,7 +2182,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2178,7 +2190,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2186,7 +2198,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2194,7 +2206,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -2202,7 +2214,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2210,7 +2222,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2218,7 +2230,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -2226,392 +2238,386 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>390</v>
+      </c>
+      <c r="B23" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>349</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>358</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>52</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>54</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>56</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>387</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>382</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>331</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>340</v>
-      </c>
-      <c r="B29" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>341</v>
       </c>
       <c r="B30" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>341</v>
+      </c>
+      <c r="B31" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>58</v>
-      </c>
-      <c r="B31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>60</v>
       </c>
       <c r="B32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>62</v>
-      </c>
-      <c r="B34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>64</v>
       </c>
       <c r="B35" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>352</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>360</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>66</v>
-      </c>
-      <c r="B38" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>68</v>
       </c>
       <c r="B39" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>70</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>72</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>74</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>76</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>78</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>80</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>82</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>84</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>86</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>88</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>90</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>92</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>94</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>96</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>98</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>100</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>102</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>104</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>106</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>108</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>110</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>112</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>114</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>116</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>118</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>120</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>389</v>
+      </c>
+      <c r="B68" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>350</v>
-      </c>
-      <c r="B67" t="s">
-        <v>351</v>
-      </c>
-      <c r="C67" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>354</v>
-      </c>
-      <c r="B68" t="s">
-        <v>351</v>
-      </c>
-      <c r="C68" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>355</v>
       </c>
       <c r="B69" t="s">
         <v>351</v>
@@ -2620,106 +2626,106 @@
         <v>361</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>354</v>
+      </c>
+      <c r="B70" t="s">
+        <v>351</v>
+      </c>
+      <c r="C70" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>355</v>
+      </c>
+      <c r="B71" t="s">
+        <v>351</v>
+      </c>
+      <c r="C71" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>122</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B72" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>388</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B73" t="s">
         <v>381</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C73" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>332</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B74" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>333</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B75" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>334</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B76" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>124</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B77" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>126</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B78" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>128</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B79" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>130</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B80" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>353</v>
-      </c>
-      <c r="B79" t="s">
-        <v>359</v>
-      </c>
-      <c r="C79" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>356</v>
-      </c>
-      <c r="B80" t="s">
-        <v>359</v>
-      </c>
-      <c r="C80" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>357</v>
       </c>
       <c r="B81" t="s">
         <v>359</v>
@@ -2728,960 +2734,982 @@
         <v>365</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>356</v>
+      </c>
+      <c r="B82" t="s">
+        <v>359</v>
+      </c>
+      <c r="C82" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>357</v>
+      </c>
+      <c r="B83" t="s">
+        <v>359</v>
+      </c>
+      <c r="C83" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>132</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B84" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>134</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B85" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>336</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B86" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>335</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B87" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>136</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B88" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>138</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B89" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>140</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B90" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>142</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B91" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>144</v>
-      </c>
-      <c r="B90" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>146</v>
-      </c>
-      <c r="B91" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>147</v>
       </c>
       <c r="B92" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>146</v>
+      </c>
+      <c r="B93" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>147</v>
+      </c>
+      <c r="B94" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>148</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B95" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>150</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B96" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>152</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B97" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>154</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B98" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>156</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B99" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>158</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B100" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>160</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B101" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>162</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B102" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>164</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B103" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>166</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B104" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>168</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B105" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>170</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B106" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>172</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B107" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>174</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B108" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>176</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B109" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>178</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B110" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>180</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B111" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>182</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B112" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>184</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B113" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>186</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B114" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>188</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B115" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>190</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B116" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>192</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B117" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>194</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B118" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>196</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B119" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>198</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B120" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>200</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B121" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>202</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B122" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>204</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B123" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>206</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B124" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>208</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B125" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>210</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B126" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>212</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B127" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>214</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B128" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>216</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B129" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>218</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B130" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>219</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B131" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>220</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B132" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>221</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B133" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>222</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B134" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>223</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B135" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>224</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B136" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>225</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B137" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>226</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B138" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>227</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B139" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>228</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B140" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>229</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B141" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>230</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B142" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>232</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B143" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>234</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B144" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>236</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B145" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>238</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B146" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>240</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B147" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>242</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B148" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>244</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B149" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A148" t="s">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>246</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B150" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>248</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B151" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" t="s">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>250</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B152" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A151" t="s">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>252</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B153" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A152" t="s">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>254</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B154" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>256</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B155" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" t="s">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>258</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B156" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A155" t="s">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>260</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B157" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A156" t="s">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>262</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B158" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A157" t="s">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>264</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B159" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A158" t="s">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>266</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B160" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A159" t="s">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>268</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B161" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A160" t="s">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>270</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B162" t="s">
         <v>271</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C162" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A161" t="s">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>371</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B163" t="s">
         <v>373</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C163" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A162" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>272</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B164" t="s">
         <v>273</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C164" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A163" t="s">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>274</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B165" t="s">
         <v>275</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C165" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A164" t="s">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>321</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B166" t="s">
         <v>326</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C166" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A165" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>322</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B167" t="s">
         <v>325</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C167" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A166" t="s">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>276</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B168" t="s">
         <v>277</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C168" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A167" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>292</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B169" t="s">
         <v>307</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C169" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A168" t="s">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>296</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B170" t="s">
         <v>306</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C170" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A169" t="s">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>278</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B171" t="s">
         <v>279</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C171" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A170" t="s">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>346</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B172" t="s">
         <v>347</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C172" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>319</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B173" t="s">
         <v>327</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C173" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A172" t="s">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>320</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B174" t="s">
         <v>328</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C174" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A173" t="s">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>369</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B175" t="s">
         <v>375</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C175" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A174" t="s">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>280</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B176" t="s">
         <v>281</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C176" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A175" t="s">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>370</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B177" t="s">
         <v>376</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C177" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A176" t="s">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>366</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B178" t="s">
         <v>378</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C178" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A177" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>282</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B179" t="s">
         <v>283</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C179" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A178" t="s">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>284</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B180" t="s">
         <v>285</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C180" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A179" t="s">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>295</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B181" t="s">
         <v>300</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C181" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A180" t="s">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>299</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B182" t="s">
         <v>305</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C182" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A181" t="s">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>368</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B183" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A182" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>286</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B184" t="s">
         <v>287</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C184" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A183" t="s">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>288</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B185" t="s">
         <v>289</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C185" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A184" t="s">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>294</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B186" t="s">
         <v>301</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C186" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A185" t="s">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>298</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B187" t="s">
         <v>304</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C187" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A186" t="s">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>290</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B188" t="s">
         <v>291</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C188" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A187" t="s">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>293</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B189" t="s">
         <v>302</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C189" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A188" t="s">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>297</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B190" t="s">
         <v>303</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C190" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A189" t="s">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>367</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B191" t="s">
         <v>377</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C191" t="s">
         <v>385</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K1">
-    <sortState ref="A2:K189">
+    <sortState ref="A2:K191">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
renaming solvent to reagent
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -5,24 +5,25 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\TheRiftbreaker\mods\rebalance\gui\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WinData\EpicGames\Riftbreaker\TheRiftbreaker\mods\rebalance\gui\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="12405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28790" windowHeight="12410"/>
   </bookViews>
   <sheets>
     <sheet name="rebalance_localizations" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$197</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="406">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -1083,27 +1084,15 @@
     <t>gui/hud/building_description/solvent_condenser</t>
   </si>
   <si>
-    <t>gui/hud/building_name/solvent_condenser</t>
-  </si>
-  <si>
     <t>gui/hud/building_name/fluorine_trap_lvl_2</t>
   </si>
   <si>
     <t>gui/hud/building_name/fluorine_trap_lvl_3</t>
   </si>
   <si>
-    <t>gui/hud/building_name/solvent_condenser_lvl_2</t>
-  </si>
-  <si>
-    <t>gui/hud/building_name/solvent_condenser_lvl_3</t>
-  </si>
-  <si>
     <t>Captures fluorine compounds from atmosphere</t>
   </si>
   <si>
-    <t>Solvent Condenser</t>
-  </si>
-  <si>
     <t>Condenses hyrdo-fluorines into solvent liquid</t>
   </si>
   <si>
@@ -1119,9 +1108,6 @@
     <t>Verdichtet Fluorwasserstoffe zur Solvens-Flüssigkeit</t>
   </si>
   <si>
-    <t>Solvensverdichter</t>
-  </si>
-  <si>
     <t>resource_name/mud_deepvein</t>
   </si>
   <si>
@@ -1201,6 +1187,60 @@
   </si>
   <si>
     <t>Energy connector on platform that can be placed on liquids pools</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/reagent_condenser</t>
+  </si>
+  <si>
+    <t>Condenses hyrdo-fluorines into reagent liquid</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/reagent_refinery</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/reagent_refinery_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/reagent_refinery_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/reagent_condenser</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/reagent_condenser_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/reagent_condenser_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/reagent_refinery</t>
+  </si>
+  <si>
+    <t>resource_name/reagent</t>
+  </si>
+  <si>
+    <t>Verdichtet Fluorwasserstoffe zur Reagenzlösung</t>
+  </si>
+  <si>
+    <t>produces reagent for chemical processing</t>
+  </si>
+  <si>
+    <t>Reagent Condenser</t>
+  </si>
+  <si>
+    <t>Reagent Refinery</t>
+  </si>
+  <si>
+    <t>Reagent</t>
+  </si>
+  <si>
+    <t>Reagenzlösung</t>
+  </si>
+  <si>
+    <t>Reagenz-Kondensator</t>
+  </si>
+  <si>
+    <t>Reagenz Raffinerie</t>
   </si>
 </sst>
 </file>
@@ -1706,48 +1746,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2025,20 +2065,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K191"/>
+  <dimension ref="A1:K197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C190" sqref="C190"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="54.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="54.1796875" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2070,7 +2110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2078,7 +2118,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2086,7 +2126,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2094,7 +2134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2102,7 +2142,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2110,7 +2150,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2118,7 +2158,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2126,7 +2166,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2134,7 +2174,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -2142,7 +2182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2150,7 +2190,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2158,7 +2198,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2166,7 +2206,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2174,7 +2214,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2182,7 +2222,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2190,7 +2230,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2198,7 +2238,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2206,7 +2246,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -2214,7 +2254,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2222,7 +2262,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2230,7 +2270,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -2238,26 +2278,26 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="B23" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>349</v>
       </c>
       <c r="B24" t="s">
+        <v>355</v>
+      </c>
+      <c r="C24" t="s">
         <v>358</v>
       </c>
-      <c r="C24" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -2265,7 +2305,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -2273,7 +2313,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -2281,18 +2321,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B28" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C28" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>331</v>
       </c>
@@ -2300,7 +2340,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>340</v>
       </c>
@@ -2308,7 +2348,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>341</v>
       </c>
@@ -2316,7 +2356,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -2324,7 +2364,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -2332,7 +2372,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2340,7 +2380,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>62</v>
       </c>
@@ -2348,7 +2388,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>64</v>
       </c>
@@ -2356,7 +2396,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -2364,1355 +2404,1517 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>388</v>
+      </c>
+      <c r="B38" t="s">
+        <v>389</v>
+      </c>
+      <c r="C38" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>390</v>
+      </c>
+      <c r="B39" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>391</v>
+      </c>
+      <c r="B40" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>392</v>
+      </c>
+      <c r="B41" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>352</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B42" t="s">
+        <v>356</v>
+      </c>
+      <c r="C42" t="s">
         <v>360</v>
       </c>
-      <c r="C38" t="s">
+    </row>
+    <row r="43" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>94</v>
+      </c>
+      <c r="B58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>102</v>
+      </c>
+      <c r="B62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>106</v>
+      </c>
+      <c r="B64" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>108</v>
+      </c>
+      <c r="B65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>116</v>
+      </c>
+      <c r="B69" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>118</v>
+      </c>
+      <c r="B70" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>384</v>
+      </c>
+      <c r="B72" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>350</v>
+      </c>
+      <c r="B73" t="s">
+        <v>351</v>
+      </c>
+      <c r="C73" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>353</v>
+      </c>
+      <c r="B74" t="s">
+        <v>351</v>
+      </c>
+      <c r="C74" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>354</v>
+      </c>
+      <c r="B75" t="s">
+        <v>351</v>
+      </c>
+      <c r="C75" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>383</v>
+      </c>
+      <c r="B77" t="s">
+        <v>376</v>
+      </c>
+      <c r="C77" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>332</v>
+      </c>
+      <c r="B78" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>333</v>
+      </c>
+      <c r="B79" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>334</v>
+      </c>
+      <c r="B80" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>124</v>
+      </c>
+      <c r="B81" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>126</v>
+      </c>
+      <c r="B82" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>128</v>
+      </c>
+      <c r="B83" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>130</v>
+      </c>
+      <c r="B84" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>393</v>
+      </c>
+      <c r="B85" t="s">
+        <v>400</v>
+      </c>
+      <c r="C85" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>394</v>
+      </c>
+      <c r="B86" t="s">
+        <v>400</v>
+      </c>
+      <c r="C86" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>395</v>
+      </c>
+      <c r="B87" t="s">
+        <v>400</v>
+      </c>
+      <c r="C87" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>396</v>
+      </c>
+      <c r="B88" t="s">
+        <v>401</v>
+      </c>
+      <c r="C88" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>132</v>
+      </c>
+      <c r="B89" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>134</v>
+      </c>
+      <c r="B90" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>336</v>
+      </c>
+      <c r="B91" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>335</v>
+      </c>
+      <c r="B92" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>136</v>
+      </c>
+      <c r="B93" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>138</v>
+      </c>
+      <c r="B94" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>140</v>
+      </c>
+      <c r="B95" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B96" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>144</v>
+      </c>
+      <c r="B97" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>146</v>
+      </c>
+      <c r="B98" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>147</v>
+      </c>
+      <c r="B99" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>148</v>
+      </c>
+      <c r="B100" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>150</v>
+      </c>
+      <c r="B101" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>152</v>
+      </c>
+      <c r="B102" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>154</v>
+      </c>
+      <c r="B103" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>156</v>
+      </c>
+      <c r="B104" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>158</v>
+      </c>
+      <c r="B105" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>160</v>
+      </c>
+      <c r="B106" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>162</v>
+      </c>
+      <c r="B107" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>164</v>
+      </c>
+      <c r="B108" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>166</v>
+      </c>
+      <c r="B109" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>168</v>
+      </c>
+      <c r="B110" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>170</v>
+      </c>
+      <c r="B111" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>172</v>
+      </c>
+      <c r="B112" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>174</v>
+      </c>
+      <c r="B113" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>176</v>
+      </c>
+      <c r="B114" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>178</v>
+      </c>
+      <c r="B115" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>180</v>
+      </c>
+      <c r="B116" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>182</v>
+      </c>
+      <c r="B117" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>184</v>
+      </c>
+      <c r="B118" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>186</v>
+      </c>
+      <c r="B119" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>188</v>
+      </c>
+      <c r="B120" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>190</v>
+      </c>
+      <c r="B121" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>192</v>
+      </c>
+      <c r="B122" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>194</v>
+      </c>
+      <c r="B123" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>196</v>
+      </c>
+      <c r="B124" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>198</v>
+      </c>
+      <c r="B125" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>200</v>
+      </c>
+      <c r="B126" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>202</v>
+      </c>
+      <c r="B127" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>204</v>
+      </c>
+      <c r="B128" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>206</v>
+      </c>
+      <c r="B129" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>208</v>
+      </c>
+      <c r="B130" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>210</v>
+      </c>
+      <c r="B131" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>212</v>
+      </c>
+      <c r="B132" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>214</v>
+      </c>
+      <c r="B133" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>216</v>
+      </c>
+      <c r="B134" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>218</v>
+      </c>
+      <c r="B135" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>219</v>
+      </c>
+      <c r="B136" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>220</v>
+      </c>
+      <c r="B137" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>221</v>
+      </c>
+      <c r="B138" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>222</v>
+      </c>
+      <c r="B139" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>223</v>
+      </c>
+      <c r="B140" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>224</v>
+      </c>
+      <c r="B141" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>225</v>
+      </c>
+      <c r="B142" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>226</v>
+      </c>
+      <c r="B143" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>227</v>
+      </c>
+      <c r="B144" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>228</v>
+      </c>
+      <c r="B145" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>229</v>
+      </c>
+      <c r="B146" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>230</v>
+      </c>
+      <c r="B147" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>232</v>
+      </c>
+      <c r="B148" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>234</v>
+      </c>
+      <c r="B149" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>236</v>
+      </c>
+      <c r="B150" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>238</v>
+      </c>
+      <c r="B151" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>240</v>
+      </c>
+      <c r="B152" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>242</v>
+      </c>
+      <c r="B153" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>244</v>
+      </c>
+      <c r="B154" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>246</v>
+      </c>
+      <c r="B155" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>248</v>
+      </c>
+      <c r="B156" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>250</v>
+      </c>
+      <c r="B157" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>252</v>
+      </c>
+      <c r="B158" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>254</v>
+      </c>
+      <c r="B159" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>256</v>
+      </c>
+      <c r="B160" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>258</v>
+      </c>
+      <c r="B161" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>260</v>
+      </c>
+      <c r="B162" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>262</v>
+      </c>
+      <c r="B163" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>264</v>
+      </c>
+      <c r="B164" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>266</v>
+      </c>
+      <c r="B165" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>268</v>
+      </c>
+      <c r="B166" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>270</v>
+      </c>
+      <c r="B167" t="s">
+        <v>271</v>
+      </c>
+      <c r="C167" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>366</v>
+      </c>
+      <c r="B168" t="s">
+        <v>368</v>
+      </c>
+      <c r="C168" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>272</v>
+      </c>
+      <c r="B169" t="s">
+        <v>273</v>
+      </c>
+      <c r="C169" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>274</v>
+      </c>
+      <c r="B170" t="s">
+        <v>275</v>
+      </c>
+      <c r="C170" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>321</v>
+      </c>
+      <c r="B171" t="s">
+        <v>326</v>
+      </c>
+      <c r="C171" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>322</v>
+      </c>
+      <c r="B172" t="s">
+        <v>325</v>
+      </c>
+      <c r="C172" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>276</v>
+      </c>
+      <c r="B173" t="s">
+        <v>277</v>
+      </c>
+      <c r="C173" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>292</v>
+      </c>
+      <c r="B174" t="s">
+        <v>307</v>
+      </c>
+      <c r="C174" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>296</v>
+      </c>
+      <c r="B175" t="s">
+        <v>306</v>
+      </c>
+      <c r="C175" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>278</v>
+      </c>
+      <c r="B176" t="s">
+        <v>279</v>
+      </c>
+      <c r="C176" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>346</v>
+      </c>
+      <c r="B177" t="s">
+        <v>347</v>
+      </c>
+      <c r="C177" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>319</v>
+      </c>
+      <c r="B178" t="s">
+        <v>327</v>
+      </c>
+      <c r="C178" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>320</v>
+      </c>
+      <c r="B179" t="s">
+        <v>328</v>
+      </c>
+      <c r="C179" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>72</v>
-      </c>
-      <c r="B43" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B46" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>82</v>
-      </c>
-      <c r="B48" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>84</v>
-      </c>
-      <c r="B49" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>86</v>
-      </c>
-      <c r="B50" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>92</v>
-      </c>
-      <c r="B53" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>94</v>
-      </c>
-      <c r="B54" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>96</v>
-      </c>
-      <c r="B55" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>98</v>
-      </c>
-      <c r="B56" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>100</v>
-      </c>
-      <c r="B57" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>102</v>
-      </c>
-      <c r="B58" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>104</v>
-      </c>
-      <c r="B59" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>106</v>
-      </c>
-      <c r="B60" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>108</v>
-      </c>
-      <c r="B61" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>110</v>
-      </c>
-      <c r="B62" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>112</v>
-      </c>
-      <c r="B63" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>114</v>
-      </c>
-      <c r="B64" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>116</v>
-      </c>
-      <c r="B65" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>118</v>
-      </c>
-      <c r="B66" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>120</v>
-      </c>
-      <c r="B67" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>389</v>
-      </c>
-      <c r="B68" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>350</v>
-      </c>
-      <c r="B69" t="s">
-        <v>351</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="B180" t="s">
+        <v>370</v>
+      </c>
+      <c r="C180" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>280</v>
+      </c>
+      <c r="B181" t="s">
+        <v>281</v>
+      </c>
+      <c r="C181" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>365</v>
+      </c>
+      <c r="B182" t="s">
+        <v>371</v>
+      </c>
+      <c r="C182" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>354</v>
-      </c>
-      <c r="B70" t="s">
-        <v>351</v>
-      </c>
-      <c r="C70" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>355</v>
-      </c>
-      <c r="B71" t="s">
-        <v>351</v>
-      </c>
-      <c r="C71" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>122</v>
-      </c>
-      <c r="B72" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>388</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="B183" t="s">
+        <v>373</v>
+      </c>
+      <c r="C183" t="s">
         <v>381</v>
       </c>
-      <c r="C73" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>332</v>
-      </c>
-      <c r="B74" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>333</v>
-      </c>
-      <c r="B75" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>334</v>
-      </c>
-      <c r="B76" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>124</v>
-      </c>
-      <c r="B77" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>126</v>
-      </c>
-      <c r="B78" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>128</v>
-      </c>
-      <c r="B79" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>130</v>
-      </c>
-      <c r="B80" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>353</v>
-      </c>
-      <c r="B81" t="s">
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>282</v>
+      </c>
+      <c r="B184" t="s">
+        <v>283</v>
+      </c>
+      <c r="C184" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>284</v>
+      </c>
+      <c r="B185" t="s">
+        <v>285</v>
+      </c>
+      <c r="C185" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>295</v>
+      </c>
+      <c r="B186" t="s">
+        <v>300</v>
+      </c>
+      <c r="C186" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>299</v>
+      </c>
+      <c r="B187" t="s">
+        <v>305</v>
+      </c>
+      <c r="C187" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>397</v>
+      </c>
+      <c r="B188" t="s">
+        <v>402</v>
+      </c>
+      <c r="C188" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>363</v>
+      </c>
+      <c r="B189" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>286</v>
+      </c>
+      <c r="B190" t="s">
+        <v>287</v>
+      </c>
+      <c r="C190" t="s">
         <v>359</v>
       </c>
-      <c r="C81" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>356</v>
-      </c>
-      <c r="B82" t="s">
-        <v>359</v>
-      </c>
-      <c r="C82" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>357</v>
-      </c>
-      <c r="B83" t="s">
-        <v>359</v>
-      </c>
-      <c r="C83" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>132</v>
-      </c>
-      <c r="B84" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>134</v>
-      </c>
-      <c r="B85" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>336</v>
-      </c>
-      <c r="B86" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>335</v>
-      </c>
-      <c r="B87" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>136</v>
-      </c>
-      <c r="B88" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>138</v>
-      </c>
-      <c r="B89" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>140</v>
-      </c>
-      <c r="B90" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>142</v>
-      </c>
-      <c r="B91" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>144</v>
-      </c>
-      <c r="B92" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>146</v>
-      </c>
-      <c r="B93" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>147</v>
-      </c>
-      <c r="B94" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>148</v>
-      </c>
-      <c r="B95" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>150</v>
-      </c>
-      <c r="B96" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>152</v>
-      </c>
-      <c r="B97" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>154</v>
-      </c>
-      <c r="B98" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>156</v>
-      </c>
-      <c r="B99" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>158</v>
-      </c>
-      <c r="B100" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>160</v>
-      </c>
-      <c r="B101" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>162</v>
-      </c>
-      <c r="B102" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>164</v>
-      </c>
-      <c r="B103" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>166</v>
-      </c>
-      <c r="B104" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>168</v>
-      </c>
-      <c r="B105" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>170</v>
-      </c>
-      <c r="B106" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>172</v>
-      </c>
-      <c r="B107" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>174</v>
-      </c>
-      <c r="B108" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>176</v>
-      </c>
-      <c r="B109" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>178</v>
-      </c>
-      <c r="B110" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>180</v>
-      </c>
-      <c r="B111" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>182</v>
-      </c>
-      <c r="B112" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>184</v>
-      </c>
-      <c r="B113" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>186</v>
-      </c>
-      <c r="B114" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>188</v>
-      </c>
-      <c r="B115" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>190</v>
-      </c>
-      <c r="B116" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>192</v>
-      </c>
-      <c r="B117" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>194</v>
-      </c>
-      <c r="B118" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>196</v>
-      </c>
-      <c r="B119" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>198</v>
-      </c>
-      <c r="B120" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>200</v>
-      </c>
-      <c r="B121" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>202</v>
-      </c>
-      <c r="B122" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>204</v>
-      </c>
-      <c r="B123" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>206</v>
-      </c>
-      <c r="B124" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>208</v>
-      </c>
-      <c r="B125" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>210</v>
-      </c>
-      <c r="B126" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>212</v>
-      </c>
-      <c r="B127" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>214</v>
-      </c>
-      <c r="B128" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>216</v>
-      </c>
-      <c r="B129" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>218</v>
-      </c>
-      <c r="B130" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>219</v>
-      </c>
-      <c r="B131" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>220</v>
-      </c>
-      <c r="B132" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>221</v>
-      </c>
-      <c r="B133" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>222</v>
-      </c>
-      <c r="B134" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>223</v>
-      </c>
-      <c r="B135" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>224</v>
-      </c>
-      <c r="B136" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>225</v>
-      </c>
-      <c r="B137" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>226</v>
-      </c>
-      <c r="B138" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>227</v>
-      </c>
-      <c r="B139" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>228</v>
-      </c>
-      <c r="B140" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>229</v>
-      </c>
-      <c r="B141" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>230</v>
-      </c>
-      <c r="B142" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>232</v>
-      </c>
-      <c r="B143" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>234</v>
-      </c>
-      <c r="B144" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>236</v>
-      </c>
-      <c r="B145" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>238</v>
-      </c>
-      <c r="B146" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>240</v>
-      </c>
-      <c r="B147" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>242</v>
-      </c>
-      <c r="B148" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>244</v>
-      </c>
-      <c r="B149" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>246</v>
-      </c>
-      <c r="B150" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>248</v>
-      </c>
-      <c r="B151" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>250</v>
-      </c>
-      <c r="B152" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>252</v>
-      </c>
-      <c r="B153" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>254</v>
-      </c>
-      <c r="B154" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>256</v>
-      </c>
-      <c r="B155" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>258</v>
-      </c>
-      <c r="B156" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>260</v>
-      </c>
-      <c r="B157" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>262</v>
-      </c>
-      <c r="B158" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>264</v>
-      </c>
-      <c r="B159" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>266</v>
-      </c>
-      <c r="B160" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>268</v>
-      </c>
-      <c r="B161" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>270</v>
-      </c>
-      <c r="B162" t="s">
-        <v>271</v>
-      </c>
-      <c r="C162" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>371</v>
-      </c>
-      <c r="B163" t="s">
-        <v>373</v>
-      </c>
-      <c r="C163" t="s">
+    </row>
+    <row r="191" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>288</v>
+      </c>
+      <c r="B191" t="s">
+        <v>289</v>
+      </c>
+      <c r="C191" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>294</v>
+      </c>
+      <c r="B192" t="s">
+        <v>301</v>
+      </c>
+      <c r="C192" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>298</v>
+      </c>
+      <c r="B193" t="s">
+        <v>304</v>
+      </c>
+      <c r="C193" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>290</v>
+      </c>
+      <c r="B194" t="s">
+        <v>291</v>
+      </c>
+      <c r="C194" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>293</v>
+      </c>
+      <c r="B195" t="s">
+        <v>302</v>
+      </c>
+      <c r="C195" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>297</v>
+      </c>
+      <c r="B196" t="s">
+        <v>303</v>
+      </c>
+      <c r="C196" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>362</v>
+      </c>
+      <c r="B197" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>272</v>
-      </c>
-      <c r="B164" t="s">
-        <v>273</v>
-      </c>
-      <c r="C164" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>274</v>
-      </c>
-      <c r="B165" t="s">
-        <v>275</v>
-      </c>
-      <c r="C165" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>321</v>
-      </c>
-      <c r="B166" t="s">
-        <v>326</v>
-      </c>
-      <c r="C166" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>322</v>
-      </c>
-      <c r="B167" t="s">
-        <v>325</v>
-      </c>
-      <c r="C167" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>276</v>
-      </c>
-      <c r="B168" t="s">
-        <v>277</v>
-      </c>
-      <c r="C168" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>292</v>
-      </c>
-      <c r="B169" t="s">
-        <v>307</v>
-      </c>
-      <c r="C169" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>296</v>
-      </c>
-      <c r="B170" t="s">
-        <v>306</v>
-      </c>
-      <c r="C170" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>278</v>
-      </c>
-      <c r="B171" t="s">
-        <v>279</v>
-      </c>
-      <c r="C171" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>346</v>
-      </c>
-      <c r="B172" t="s">
-        <v>347</v>
-      </c>
-      <c r="C172" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>319</v>
-      </c>
-      <c r="B173" t="s">
-        <v>327</v>
-      </c>
-      <c r="C173" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>320</v>
-      </c>
-      <c r="B174" t="s">
-        <v>328</v>
-      </c>
-      <c r="C174" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>369</v>
-      </c>
-      <c r="B175" t="s">
-        <v>375</v>
-      </c>
-      <c r="C175" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>280</v>
-      </c>
-      <c r="B176" t="s">
-        <v>281</v>
-      </c>
-      <c r="C176" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>370</v>
-      </c>
-      <c r="B177" t="s">
-        <v>376</v>
-      </c>
-      <c r="C177" t="s">
+      <c r="C197" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>366</v>
-      </c>
-      <c r="B178" t="s">
-        <v>378</v>
-      </c>
-      <c r="C178" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>282</v>
-      </c>
-      <c r="B179" t="s">
-        <v>283</v>
-      </c>
-      <c r="C179" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>284</v>
-      </c>
-      <c r="B180" t="s">
-        <v>285</v>
-      </c>
-      <c r="C180" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>295</v>
-      </c>
-      <c r="B181" t="s">
-        <v>300</v>
-      </c>
-      <c r="C181" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>299</v>
-      </c>
-      <c r="B182" t="s">
-        <v>305</v>
-      </c>
-      <c r="C182" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>368</v>
-      </c>
-      <c r="B183" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>286</v>
-      </c>
-      <c r="B184" t="s">
-        <v>287</v>
-      </c>
-      <c r="C184" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>288</v>
-      </c>
-      <c r="B185" t="s">
-        <v>289</v>
-      </c>
-      <c r="C185" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>294</v>
-      </c>
-      <c r="B186" t="s">
-        <v>301</v>
-      </c>
-      <c r="C186" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>298</v>
-      </c>
-      <c r="B187" t="s">
-        <v>304</v>
-      </c>
-      <c r="C187" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>290</v>
-      </c>
-      <c r="B188" t="s">
-        <v>291</v>
-      </c>
-      <c r="C188" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>293</v>
-      </c>
-      <c r="B189" t="s">
-        <v>302</v>
-      </c>
-      <c r="C189" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>297</v>
-      </c>
-      <c r="B190" t="s">
-        <v>303</v>
-      </c>
-      <c r="C190" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>367</v>
-      </c>
-      <c r="B191" t="s">
-        <v>377</v>
-      </c>
-      <c r="C191" t="s">
-        <v>385</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:K1">
-    <sortState ref="A2:K191">
-      <sortCondition ref="A1"/>
+  <autoFilter ref="A1:K197">
+    <sortState ref="A2:K197">
+      <sortCondition ref="A1:A197"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B3" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B4" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B5" t="s">
+        <v>400</v>
+      </c>
+      <c r="C5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>394</v>
+      </c>
+      <c r="B6" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B7" t="s">
+        <v>400</v>
+      </c>
+      <c r="C7" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B8" t="s">
+        <v>401</v>
+      </c>
+      <c r="C8" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>397</v>
+      </c>
+      <c r="B9" t="s">
+        <v>402</v>
+      </c>
+      <c r="C9" t="s">
+        <v>403</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added new content to tech tree
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28790" windowHeight="12410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="rebalance_localizations" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="452">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -1241,6 +1241,144 @@
   </si>
   <si>
     <t>Reagenz Raffinerie</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/nitrogen_chemistry</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/nitrogen_chemistry</t>
+  </si>
+  <si>
+    <t>Nitrogen Chemistry</t>
+  </si>
+  <si>
+    <t>Nitrogen Chemistry 2</t>
+  </si>
+  <si>
+    <t>Nitrogen Chemistry 3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/nitrogen_chemistry_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/nitrogen_chemistry_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/nitrogen_chemistry_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/nitrogen_chemistry_lvl_3</t>
+  </si>
+  <si>
+    <t>Optimized processing tech handling nitrogen compounds</t>
+  </si>
+  <si>
+    <t>Basic processing tech for handling nitrogen compounds, including ammonium</t>
+  </si>
+  <si>
+    <t>Improved processing tech handling nitrogen compounds</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/reactive_substances</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/reactive_substances</t>
+  </si>
+  <si>
+    <t>Reactive Substances</t>
+  </si>
+  <si>
+    <t>Research into extraction and production of reactive substances from the local enviorment</t>
+  </si>
+  <si>
+    <t>Advanced extraction and production methods for reactive substances from the local enviorment</t>
+  </si>
+  <si>
+    <t>Reactive Substances 2</t>
+  </si>
+  <si>
+    <t>Reactive Substances 3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/reactive_substances_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/reactive_substances_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/reactive_substances_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/reactive_substances_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/well_contruction</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/well_contruction</t>
+  </si>
+  <si>
+    <t>Well Construction</t>
+  </si>
+  <si>
+    <t>Construction of wells for liquid extraction</t>
+  </si>
+  <si>
+    <t>Well Construction 2</t>
+  </si>
+  <si>
+    <t>Well Construction 3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/well_contruction_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/well_contruction_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/well_contruction_lvl_3</t>
+  </si>
+  <si>
+    <t>Advanced well extraction methods, particularly fracking</t>
+  </si>
+  <si>
+    <t>Optimized well extraction by fracking</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/rare_element_mining_lvl1</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/rare_element_mining_lvl1</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/rare_element_mining_lvl2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/rare_element_mining_lvl2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/rare_element_mining_lvl3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/rare_element_mining_lvl3</t>
+  </si>
+  <si>
+    <t>Deep Ore Mining</t>
+  </si>
+  <si>
+    <t>Deep Ore Mining 2</t>
+  </si>
+  <si>
+    <t>Deep Ore Mining 3</t>
+  </si>
+  <si>
+    <t>Mining equipment for underground ore vein extraction</t>
+  </si>
+  <si>
+    <t>Advanced deep ore extraction methods utilizing reactive chemical to dissolve ores</t>
+  </si>
+  <si>
+    <t>Optimized deep ore extraction methods utilizing reactive chemical to dissolve ores</t>
   </si>
 </sst>
 </file>
@@ -2065,20 +2203,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K197"/>
+  <dimension ref="A1:K221"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H223" sqref="H223"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.1796875" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2110,7 +2248,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2118,7 +2256,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2126,7 +2264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2134,7 +2272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2142,7 +2280,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2150,7 +2288,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2158,7 +2296,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2166,7 +2304,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2174,7 +2312,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -2182,7 +2320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2190,7 +2328,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2198,7 +2336,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2206,7 +2344,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2214,7 +2352,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2222,7 +2360,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2230,7 +2368,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2238,7 +2376,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2246,7 +2384,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -2254,7 +2392,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -2262,7 +2400,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2270,7 +2408,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -2278,7 +2416,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>385</v>
       </c>
@@ -2286,7 +2424,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>349</v>
       </c>
@@ -2297,7 +2435,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -2305,7 +2443,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -2313,7 +2451,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -2321,7 +2459,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>382</v>
       </c>
@@ -2332,7 +2470,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>331</v>
       </c>
@@ -2340,7 +2478,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>340</v>
       </c>
@@ -2348,7 +2486,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>341</v>
       </c>
@@ -2356,7 +2494,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -2364,7 +2502,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -2372,7 +2510,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2380,7 +2518,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>62</v>
       </c>
@@ -2388,7 +2526,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>64</v>
       </c>
@@ -2396,7 +2534,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -2404,7 +2542,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>388</v>
       </c>
@@ -2415,7 +2553,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>390</v>
       </c>
@@ -2423,7 +2561,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>391</v>
       </c>
@@ -2431,7 +2569,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>392</v>
       </c>
@@ -2439,7 +2577,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>352</v>
       </c>
@@ -2450,7 +2588,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>66</v>
       </c>
@@ -2458,7 +2596,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -2466,7 +2604,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -2474,7 +2612,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -2482,7 +2620,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -2490,7 +2628,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>74</v>
       </c>
@@ -2498,7 +2636,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -2506,7 +2644,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>78</v>
       </c>
@@ -2514,7 +2652,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>80</v>
       </c>
@@ -2522,7 +2660,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>82</v>
       </c>
@@ -2530,7 +2668,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>84</v>
       </c>
@@ -2538,7 +2676,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -2546,7 +2684,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>88</v>
       </c>
@@ -2554,7 +2692,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>90</v>
       </c>
@@ -2562,7 +2700,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -2570,7 +2708,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>94</v>
       </c>
@@ -2578,7 +2716,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>96</v>
       </c>
@@ -2586,7 +2724,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>98</v>
       </c>
@@ -2594,7 +2732,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>100</v>
       </c>
@@ -2602,7 +2740,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>102</v>
       </c>
@@ -2610,7 +2748,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>104</v>
       </c>
@@ -2618,7 +2756,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>106</v>
       </c>
@@ -2626,7 +2764,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>108</v>
       </c>
@@ -2634,7 +2772,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>110</v>
       </c>
@@ -2642,7 +2780,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>112</v>
       </c>
@@ -2650,7 +2788,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>114</v>
       </c>
@@ -2658,7 +2796,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>116</v>
       </c>
@@ -2666,7 +2804,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>118</v>
       </c>
@@ -2674,7 +2812,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>120</v>
       </c>
@@ -2682,7 +2820,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>384</v>
       </c>
@@ -2690,7 +2828,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>350</v>
       </c>
@@ -2701,7 +2839,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>353</v>
       </c>
@@ -2712,7 +2850,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>354</v>
       </c>
@@ -2723,7 +2861,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>122</v>
       </c>
@@ -2731,7 +2869,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>383</v>
       </c>
@@ -2742,7 +2880,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>332</v>
       </c>
@@ -2750,7 +2888,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>333</v>
       </c>
@@ -2758,7 +2896,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>334</v>
       </c>
@@ -2766,7 +2904,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>124</v>
       </c>
@@ -2774,7 +2912,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>126</v>
       </c>
@@ -2782,7 +2920,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>128</v>
       </c>
@@ -2790,7 +2928,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>130</v>
       </c>
@@ -2798,7 +2936,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>393</v>
       </c>
@@ -2809,7 +2947,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>394</v>
       </c>
@@ -2820,7 +2958,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>395</v>
       </c>
@@ -2831,7 +2969,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>396</v>
       </c>
@@ -2842,7 +2980,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>132</v>
       </c>
@@ -2850,7 +2988,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>134</v>
       </c>
@@ -2858,7 +2996,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>336</v>
       </c>
@@ -2866,7 +3004,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>335</v>
       </c>
@@ -2874,7 +3012,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>136</v>
       </c>
@@ -2882,7 +3020,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>138</v>
       </c>
@@ -2890,7 +3028,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>140</v>
       </c>
@@ -2898,7 +3036,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>142</v>
       </c>
@@ -2906,7 +3044,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>144</v>
       </c>
@@ -2914,7 +3052,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>146</v>
       </c>
@@ -2922,7 +3060,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>147</v>
       </c>
@@ -2930,7 +3068,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>148</v>
       </c>
@@ -2938,7 +3076,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>150</v>
       </c>
@@ -2946,7 +3084,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>152</v>
       </c>
@@ -2954,7 +3092,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>154</v>
       </c>
@@ -2962,7 +3100,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>156</v>
       </c>
@@ -2970,7 +3108,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>158</v>
       </c>
@@ -2978,7 +3116,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>160</v>
       </c>
@@ -2986,7 +3124,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>162</v>
       </c>
@@ -2994,7 +3132,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>164</v>
       </c>
@@ -3002,7 +3140,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>166</v>
       </c>
@@ -3010,7 +3148,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>168</v>
       </c>
@@ -3018,7 +3156,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>170</v>
       </c>
@@ -3026,7 +3164,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>172</v>
       </c>
@@ -3034,7 +3172,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>174</v>
       </c>
@@ -3042,7 +3180,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>176</v>
       </c>
@@ -3050,7 +3188,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>178</v>
       </c>
@@ -3058,7 +3196,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>180</v>
       </c>
@@ -3066,7 +3204,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>182</v>
       </c>
@@ -3074,7 +3212,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>184</v>
       </c>
@@ -3082,7 +3220,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>186</v>
       </c>
@@ -3090,723 +3228,915 @@
         <v>187</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>407</v>
+      </c>
+      <c r="B120" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>412</v>
+      </c>
+      <c r="B121" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>413</v>
+      </c>
+      <c r="B122" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>441</v>
+      </c>
+      <c r="B123" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>443</v>
+      </c>
+      <c r="B124" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>445</v>
+      </c>
+      <c r="B125" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>418</v>
+      </c>
+      <c r="B126" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>425</v>
+      </c>
+      <c r="B127" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>427</v>
+      </c>
+      <c r="B128" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>188</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B129" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+    <row r="130" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>190</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B130" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
+    <row r="131" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>429</v>
+      </c>
+      <c r="B131" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>437</v>
+      </c>
+      <c r="B132" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>437</v>
+      </c>
+      <c r="B133" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>192</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B134" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
+    <row r="135" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>194</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B135" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+    <row r="136" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>196</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B136" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+    <row r="137" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>198</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B137" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+    <row r="138" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>200</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B138" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
+    <row r="139" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>202</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B139" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
+    <row r="140" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>204</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B140" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+    <row r="141" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>206</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B141" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+    <row r="142" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>208</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B142" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+    <row r="143" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>210</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B143" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+    <row r="144" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>212</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B144" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+    <row r="145" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>214</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B145" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+    <row r="146" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>216</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B146" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+    <row r="147" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>218</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B147" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+    <row r="148" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>219</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B148" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
+    <row r="149" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>220</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B149" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
+    <row r="150" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>221</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B150" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
+    <row r="151" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>222</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B151" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
+    <row r="152" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>223</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B152" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
+    <row r="153" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>224</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B153" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
+    <row r="154" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>225</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B154" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
+    <row r="155" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>226</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B155" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
+    <row r="156" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>227</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B156" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
+    <row r="157" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>228</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B157" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
+    <row r="158" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>229</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B158" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
+    <row r="159" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>406</v>
+      </c>
+      <c r="B159" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>411</v>
+      </c>
+      <c r="B160" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>414</v>
+      </c>
+      <c r="B161" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>440</v>
+      </c>
+      <c r="B162" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>442</v>
+      </c>
+      <c r="B163" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>444</v>
+      </c>
+      <c r="B164" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>419</v>
+      </c>
+      <c r="B165" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>426</v>
+      </c>
+      <c r="B166" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>428</v>
+      </c>
+      <c r="B167" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>230</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B168" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148" t="s">
+    <row r="169" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>232</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B169" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
+    <row r="170" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>430</v>
+      </c>
+      <c r="B170" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>435</v>
+      </c>
+      <c r="B171" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>436</v>
+      </c>
+      <c r="B172" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>234</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B173" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" t="s">
+    <row r="174" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>236</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B174" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151" t="s">
+    <row r="175" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>238</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B175" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A152" t="s">
+    <row r="176" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>240</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B176" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A153" t="s">
+    <row r="177" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>242</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B177" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A154" t="s">
+    <row r="178" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>244</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B178" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155" t="s">
+    <row r="179" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>246</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B179" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A156" t="s">
+    <row r="180" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>248</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B180" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A157" t="s">
+    <row r="181" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>250</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B181" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A158" t="s">
+    <row r="182" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>252</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B182" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A159" t="s">
+    <row r="183" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>254</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B183" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>256</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B184" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" t="s">
+    <row r="185" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>258</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B185" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" t="s">
+    <row r="186" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>260</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B186" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A163" t="s">
+    <row r="187" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>262</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B187" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" t="s">
+    <row r="188" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>264</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B188" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165" t="s">
+    <row r="189" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>266</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B189" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A166" t="s">
+    <row r="190" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>268</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B190" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A167" t="s">
+    <row r="191" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>270</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B191" t="s">
         <v>271</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C191" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A168" t="s">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>366</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B192" t="s">
         <v>368</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C192" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A169" t="s">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>272</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B193" t="s">
         <v>273</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C193" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A170" t="s">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>274</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B194" t="s">
         <v>275</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C194" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
         <v>321</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B195" t="s">
         <v>326</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C195" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A172" t="s">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
         <v>322</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B196" t="s">
         <v>325</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C196" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A173" t="s">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
         <v>276</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B197" t="s">
         <v>277</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C197" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A174" t="s">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
         <v>292</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B198" t="s">
         <v>307</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C198" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A175" t="s">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
         <v>296</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B199" t="s">
         <v>306</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C199" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A176" t="s">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>278</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B200" t="s">
         <v>279</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C200" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A177" t="s">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>346</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B201" t="s">
         <v>347</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C201" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A178" t="s">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>319</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B202" t="s">
         <v>327</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C202" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A179" t="s">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
         <v>320</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B203" t="s">
         <v>328</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C203" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A180" t="s">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
         <v>364</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B204" t="s">
         <v>370</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C204" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A181" t="s">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
         <v>280</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B205" t="s">
         <v>281</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C205" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A182" t="s">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>365</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B206" t="s">
         <v>371</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C206" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A183" t="s">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>361</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B207" t="s">
         <v>373</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C207" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A184" t="s">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
         <v>282</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B208" t="s">
         <v>283</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C208" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A185" t="s">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>284</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B209" t="s">
         <v>285</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C209" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186" t="s">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
         <v>295</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B210" t="s">
         <v>300</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C210" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A187" t="s">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
         <v>299</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B211" t="s">
         <v>305</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C211" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A188" t="s">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>397</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B212" t="s">
         <v>402</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C212" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189" t="s">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
         <v>363</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B213" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A190" t="s">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
         <v>286</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B214" t="s">
         <v>287</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C214" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A191" t="s">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>288</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B215" t="s">
         <v>289</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C215" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A192" t="s">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
         <v>294</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B216" t="s">
         <v>301</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C216" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A193" t="s">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>298</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B217" t="s">
         <v>304</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C217" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A194" t="s">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>290</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B218" t="s">
         <v>291</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C218" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A195" t="s">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>293</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B219" t="s">
         <v>302</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C219" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A196" t="s">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
         <v>297</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B220" t="s">
         <v>303</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C220" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A197" t="s">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
         <v>362</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B221" t="s">
         <v>372</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C221" t="s">
         <v>380</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K197">
-    <sortState ref="A2:K197">
+    <sortState ref="A2:K221">
       <sortCondition ref="A1:A197"/>
     </sortState>
   </autoFilter>
@@ -3822,9 +4152,9 @@
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>388</v>
       </c>
@@ -3835,7 +4165,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>390</v>
       </c>
@@ -3843,7 +4173,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>391</v>
       </c>
@@ -3851,7 +4181,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>392</v>
       </c>
@@ -3859,7 +4189,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>393</v>
       </c>
@@ -3870,7 +4200,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>394</v>
       </c>
@@ -3881,7 +4211,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>395</v>
       </c>
@@ -3892,7 +4222,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>396</v>
       </c>
@@ -3903,7 +4233,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>397</v>
       </c>

</xml_diff>

<commit_message>
added basic ammunition factories
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="460">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -1379,6 +1379,30 @@
   </si>
   <si>
     <t>Optimized deep ore extraction methods utilizing reactive chemical to dissolve ores</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/ammo_factory_explosive_liquid</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/ammo_factory_lowcaliber_highcaliber</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/ammo_factory_explosive_liquid</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/ammo_factory_lowcaliber_highcaliber</t>
+  </si>
+  <si>
+    <t>Explosives and liquid ammo factory</t>
+  </si>
+  <si>
+    <t>Low and High Caliber ammo factory</t>
+  </si>
+  <si>
+    <t>Produces basic explosives and liquid ammunitions</t>
+  </si>
+  <si>
+    <t>Produces basic low and ligh caliber ammunitions</t>
   </si>
 </sst>
 </file>
@@ -2203,11 +2227,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K221"/>
+  <dimension ref="A1:K225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H223" sqref="H223"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,237 +2306,237 @@
     </row>
     <row r="6" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>454</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>455</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>459</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>385</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>387</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>349</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>355</v>
-      </c>
-      <c r="C24" t="s">
-        <v>358</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>385</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>387</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>349</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>355</v>
+      </c>
+      <c r="C26" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>382</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>377</v>
-      </c>
-      <c r="C28" t="s">
-        <v>379</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>331</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>342</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>340</v>
+        <v>382</v>
       </c>
       <c r="B30" t="s">
-        <v>343</v>
+        <v>377</v>
+      </c>
+      <c r="C30" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B31" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>340</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>343</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>341</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>343</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
         <v>59</v>
@@ -2520,23 +2544,23 @@
     </row>
     <row r="35" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
         <v>63</v>
@@ -2544,34 +2568,34 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>388</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>389</v>
-      </c>
-      <c r="C38" t="s">
-        <v>398</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>390</v>
+        <v>65</v>
       </c>
       <c r="B39" t="s">
-        <v>399</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B40" t="s">
-        <v>399</v>
+        <v>389</v>
+      </c>
+      <c r="C40" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B41" t="s">
         <v>399</v>
@@ -2579,34 +2603,34 @@
     </row>
     <row r="42" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>352</v>
+        <v>391</v>
       </c>
       <c r="B42" t="s">
-        <v>356</v>
-      </c>
-      <c r="C42" t="s">
-        <v>360</v>
+        <v>399</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>392</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>399</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>352</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>356</v>
+      </c>
+      <c r="C44" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B45" t="s">
         <v>67</v>
@@ -2614,1529 +2638,1561 @@
     </row>
     <row r="46" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B46" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B54" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B55" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B56" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>92</v>
+        <v>452</v>
       </c>
       <c r="B57" t="s">
-        <v>93</v>
+        <v>456</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B59" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B60" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B61" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B62" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>106</v>
+        <v>453</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>457</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B65" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B67" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B68" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B70" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B71" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>384</v>
+        <v>114</v>
       </c>
       <c r="B72" t="s">
-        <v>386</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>350</v>
+        <v>116</v>
       </c>
       <c r="B73" t="s">
-        <v>351</v>
-      </c>
-      <c r="C73" t="s">
-        <v>357</v>
+        <v>117</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>353</v>
+        <v>118</v>
       </c>
       <c r="B74" t="s">
-        <v>351</v>
-      </c>
-      <c r="C74" t="s">
-        <v>357</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>354</v>
+        <v>120</v>
       </c>
       <c r="B75" t="s">
-        <v>351</v>
-      </c>
-      <c r="C75" t="s">
-        <v>357</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>122</v>
+        <v>384</v>
       </c>
       <c r="B76" t="s">
-        <v>123</v>
+        <v>386</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>383</v>
+        <v>350</v>
       </c>
       <c r="B77" t="s">
-        <v>376</v>
+        <v>351</v>
       </c>
       <c r="C77" t="s">
-        <v>378</v>
+        <v>357</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>332</v>
+        <v>353</v>
       </c>
       <c r="B78" t="s">
-        <v>339</v>
+        <v>351</v>
+      </c>
+      <c r="C78" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>333</v>
+        <v>354</v>
       </c>
       <c r="B79" t="s">
-        <v>344</v>
+        <v>351</v>
+      </c>
+      <c r="C79" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>334</v>
+        <v>122</v>
       </c>
       <c r="B80" t="s">
-        <v>345</v>
+        <v>123</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>124</v>
+        <v>383</v>
       </c>
       <c r="B81" t="s">
-        <v>125</v>
+        <v>376</v>
+      </c>
+      <c r="C81" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>126</v>
+        <v>332</v>
       </c>
       <c r="B82" t="s">
-        <v>127</v>
+        <v>339</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>128</v>
+        <v>333</v>
       </c>
       <c r="B83" t="s">
-        <v>129</v>
+        <v>344</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>130</v>
+        <v>334</v>
       </c>
       <c r="B84" t="s">
-        <v>131</v>
+        <v>345</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>393</v>
+        <v>124</v>
       </c>
       <c r="B85" t="s">
-        <v>400</v>
-      </c>
-      <c r="C85" t="s">
-        <v>404</v>
+        <v>125</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>394</v>
+        <v>126</v>
       </c>
       <c r="B86" t="s">
-        <v>400</v>
-      </c>
-      <c r="C86" t="s">
-        <v>404</v>
+        <v>127</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>395</v>
+        <v>128</v>
       </c>
       <c r="B87" t="s">
-        <v>400</v>
-      </c>
-      <c r="C87" t="s">
-        <v>404</v>
+        <v>129</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>396</v>
+        <v>130</v>
       </c>
       <c r="B88" t="s">
-        <v>401</v>
-      </c>
-      <c r="C88" t="s">
-        <v>405</v>
+        <v>131</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>132</v>
+        <v>393</v>
       </c>
       <c r="B89" t="s">
-        <v>133</v>
+        <v>400</v>
+      </c>
+      <c r="C89" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>134</v>
+        <v>394</v>
       </c>
       <c r="B90" t="s">
-        <v>135</v>
+        <v>400</v>
+      </c>
+      <c r="C90" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>336</v>
+        <v>395</v>
       </c>
       <c r="B91" t="s">
-        <v>337</v>
+        <v>400</v>
+      </c>
+      <c r="C91" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>335</v>
+        <v>396</v>
       </c>
       <c r="B92" t="s">
-        <v>338</v>
+        <v>401</v>
+      </c>
+      <c r="C92" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B93" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B94" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>140</v>
+        <v>336</v>
       </c>
       <c r="B95" t="s">
-        <v>141</v>
+        <v>337</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>142</v>
+        <v>335</v>
       </c>
       <c r="B96" t="s">
-        <v>143</v>
+        <v>338</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B97" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B98" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B99" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B100" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B101" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B102" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B103" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B104" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B105" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B106" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B107" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B108" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B109" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B110" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B111" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B112" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B113" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B114" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B115" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B116" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B117" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B118" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B119" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>407</v>
+        <v>180</v>
       </c>
       <c r="B120" t="s">
-        <v>416</v>
+        <v>181</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>412</v>
+        <v>182</v>
       </c>
       <c r="B121" t="s">
-        <v>417</v>
+        <v>183</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>413</v>
+        <v>184</v>
       </c>
       <c r="B122" t="s">
-        <v>415</v>
+        <v>185</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>441</v>
+        <v>186</v>
       </c>
       <c r="B123" t="s">
-        <v>449</v>
+        <v>187</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>443</v>
+        <v>407</v>
       </c>
       <c r="B124" t="s">
-        <v>450</v>
+        <v>416</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>445</v>
+        <v>412</v>
       </c>
       <c r="B125" t="s">
-        <v>451</v>
+        <v>417</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B126" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>425</v>
+        <v>441</v>
       </c>
       <c r="B127" t="s">
-        <v>422</v>
+        <v>449</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>427</v>
+        <v>443</v>
       </c>
       <c r="B128" t="s">
-        <v>422</v>
+        <v>450</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>188</v>
+        <v>445</v>
       </c>
       <c r="B129" t="s">
-        <v>189</v>
+        <v>451</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>190</v>
+        <v>418</v>
       </c>
       <c r="B130" t="s">
-        <v>191</v>
+        <v>421</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B131" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="B132" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>437</v>
+        <v>188</v>
       </c>
       <c r="B133" t="s">
-        <v>439</v>
+        <v>189</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B134" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>194</v>
+        <v>429</v>
       </c>
       <c r="B135" t="s">
-        <v>195</v>
+        <v>432</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>196</v>
+        <v>437</v>
       </c>
       <c r="B136" t="s">
-        <v>197</v>
+        <v>438</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>198</v>
+        <v>437</v>
       </c>
       <c r="B137" t="s">
-        <v>199</v>
+        <v>439</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B138" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B139" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B140" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B141" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B142" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B143" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B144" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B145" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B146" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B147" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B148" t="s">
-        <v>167</v>
+        <v>213</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B149" t="s">
-        <v>169</v>
+        <v>215</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B150" t="s">
-        <v>171</v>
+        <v>217</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B151" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B152" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B153" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B154" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B155" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B156" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B157" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B158" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>406</v>
+        <v>226</v>
       </c>
       <c r="B159" t="s">
-        <v>408</v>
+        <v>181</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>411</v>
+        <v>227</v>
       </c>
       <c r="B160" t="s">
-        <v>409</v>
+        <v>183</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>414</v>
+        <v>228</v>
       </c>
       <c r="B161" t="s">
-        <v>410</v>
+        <v>185</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>440</v>
+        <v>229</v>
       </c>
       <c r="B162" t="s">
-        <v>446</v>
+        <v>187</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>442</v>
+        <v>406</v>
       </c>
       <c r="B163" t="s">
-        <v>447</v>
+        <v>408</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>444</v>
+        <v>411</v>
       </c>
       <c r="B164" t="s">
-        <v>448</v>
+        <v>409</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B165" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>426</v>
+        <v>440</v>
       </c>
       <c r="B166" t="s">
-        <v>423</v>
+        <v>446</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>428</v>
+        <v>442</v>
       </c>
       <c r="B167" t="s">
-        <v>424</v>
+        <v>447</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>230</v>
+        <v>444</v>
       </c>
       <c r="B168" t="s">
-        <v>231</v>
+        <v>448</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>232</v>
+        <v>419</v>
       </c>
       <c r="B169" t="s">
-        <v>233</v>
+        <v>420</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B170" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="B171" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>436</v>
+        <v>230</v>
       </c>
       <c r="B172" t="s">
-        <v>434</v>
+        <v>231</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B173" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>236</v>
+        <v>430</v>
       </c>
       <c r="B174" t="s">
-        <v>237</v>
+        <v>431</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>238</v>
+        <v>435</v>
       </c>
       <c r="B175" t="s">
-        <v>239</v>
+        <v>433</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>436</v>
+      </c>
+      <c r="B176" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>234</v>
+      </c>
+      <c r="B177" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>236</v>
+      </c>
+      <c r="B178" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>238</v>
+      </c>
+      <c r="B179" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>240</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B180" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+    <row r="181" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>242</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B181" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="182" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>244</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B182" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="183" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>246</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B183" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>248</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B184" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+    <row r="185" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>250</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B185" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+    <row r="186" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>252</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B186" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+    <row r="187" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>254</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B187" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+    <row r="188" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>256</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B188" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+    <row r="189" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>258</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B189" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+    <row r="190" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>260</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B190" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+    <row r="191" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>262</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B191" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>264</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B192" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>266</v>
-      </c>
-      <c r="B189" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>268</v>
-      </c>
-      <c r="B190" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>270</v>
-      </c>
-      <c r="B191" t="s">
-        <v>271</v>
-      </c>
-      <c r="C191" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>366</v>
-      </c>
-      <c r="B192" t="s">
-        <v>368</v>
-      </c>
-      <c r="C192" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B193" t="s">
-        <v>273</v>
-      </c>
-      <c r="C193" t="s">
-        <v>312</v>
+        <v>267</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B194" t="s">
-        <v>275</v>
-      </c>
-      <c r="C194" t="s">
-        <v>308</v>
+        <v>269</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="B195" t="s">
-        <v>326</v>
+        <v>271</v>
       </c>
       <c r="C195" t="s">
-        <v>323</v>
+        <v>271</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>322</v>
+        <v>366</v>
       </c>
       <c r="B196" t="s">
-        <v>325</v>
+        <v>368</v>
       </c>
       <c r="C196" t="s">
-        <v>329</v>
+        <v>367</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B197" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C197" t="s">
-        <v>277</v>
+        <v>312</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="B198" t="s">
-        <v>307</v>
+        <v>275</v>
       </c>
       <c r="C198" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>296</v>
+        <v>321</v>
       </c>
       <c r="B199" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="C199" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>278</v>
+        <v>322</v>
       </c>
       <c r="B200" t="s">
-        <v>279</v>
+        <v>325</v>
       </c>
       <c r="C200" t="s">
-        <v>279</v>
+        <v>329</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>346</v>
+        <v>276</v>
       </c>
       <c r="B201" t="s">
-        <v>347</v>
+        <v>277</v>
       </c>
       <c r="C201" t="s">
-        <v>348</v>
+        <v>277</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="B202" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="C202" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="B203" t="s">
-        <v>328</v>
+        <v>306</v>
       </c>
       <c r="C203" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>364</v>
+        <v>278</v>
       </c>
       <c r="B204" t="s">
-        <v>370</v>
+        <v>279</v>
       </c>
       <c r="C204" t="s">
-        <v>374</v>
+        <v>279</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>280</v>
+        <v>346</v>
       </c>
       <c r="B205" t="s">
-        <v>281</v>
+        <v>347</v>
       </c>
       <c r="C205" t="s">
-        <v>281</v>
+        <v>348</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>365</v>
+        <v>319</v>
       </c>
       <c r="B206" t="s">
-        <v>371</v>
+        <v>327</v>
       </c>
       <c r="C206" t="s">
-        <v>375</v>
+        <v>324</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>361</v>
+        <v>320</v>
       </c>
       <c r="B207" t="s">
-        <v>373</v>
+        <v>328</v>
       </c>
       <c r="C207" t="s">
-        <v>381</v>
+        <v>330</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>282</v>
+        <v>364</v>
       </c>
       <c r="B208" t="s">
-        <v>283</v>
+        <v>370</v>
       </c>
       <c r="C208" t="s">
-        <v>318</v>
+        <v>374</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B209" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C209" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>295</v>
+        <v>365</v>
       </c>
       <c r="B210" t="s">
-        <v>300</v>
+        <v>371</v>
       </c>
       <c r="C210" t="s">
-        <v>309</v>
+        <v>375</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>299</v>
+        <v>361</v>
       </c>
       <c r="B211" t="s">
-        <v>305</v>
+        <v>373</v>
       </c>
       <c r="C211" t="s">
-        <v>313</v>
+        <v>381</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>397</v>
+        <v>282</v>
       </c>
       <c r="B212" t="s">
-        <v>402</v>
+        <v>283</v>
       </c>
       <c r="C212" t="s">
-        <v>403</v>
+        <v>318</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>363</v>
+        <v>284</v>
       </c>
       <c r="B213" t="s">
-        <v>369</v>
+        <v>285</v>
+      </c>
+      <c r="C213" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="B214" t="s">
-        <v>287</v>
+        <v>300</v>
       </c>
       <c r="C214" t="s">
-        <v>359</v>
+        <v>309</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="B215" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
       <c r="C215" t="s">
-        <v>289</v>
+        <v>313</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>294</v>
+        <v>397</v>
       </c>
       <c r="B216" t="s">
-        <v>301</v>
+        <v>402</v>
       </c>
       <c r="C216" t="s">
-        <v>314</v>
+        <v>403</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>298</v>
+        <v>363</v>
       </c>
       <c r="B217" t="s">
-        <v>304</v>
-      </c>
-      <c r="C217" t="s">
-        <v>315</v>
+        <v>369</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B218" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C218" t="s">
-        <v>291</v>
+        <v>359</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B219" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="C219" t="s">
-        <v>316</v>
+        <v>289</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B220" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C220" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
+        <v>298</v>
+      </c>
+      <c r="B221" t="s">
+        <v>304</v>
+      </c>
+      <c r="C221" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>290</v>
+      </c>
+      <c r="B222" t="s">
+        <v>291</v>
+      </c>
+      <c r="C222" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>293</v>
+      </c>
+      <c r="B223" t="s">
+        <v>302</v>
+      </c>
+      <c r="C223" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>297</v>
+      </c>
+      <c r="B224" t="s">
+        <v>303</v>
+      </c>
+      <c r="C224" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>362</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B225" t="s">
         <v>372</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C225" t="s">
         <v>380</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K197">
-    <sortState ref="A2:K221">
+    <sortState ref="A2:K225">
       <sortCondition ref="A1:A197"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
reworked 90mm cannon towers
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="12405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28790" windowHeight="12410"/>
   </bookViews>
   <sheets>
     <sheet name="rebalance_localizations" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="476">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -1403,6 +1403,54 @@
   </si>
   <si>
     <t>Produces basic low and ligh caliber ammunitions</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_cannon_cooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_cannon_acid</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_cannon_cryo</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_cannon_cooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_cannon_acid</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_cannon_cryo</t>
+  </si>
+  <si>
+    <t>Fires high caliber rounds dealing significant damage per shot. Cooling enables higher fire rate</t>
+  </si>
+  <si>
+    <t>90mm Gun Tower, Cooled</t>
+  </si>
+  <si>
+    <t>90mm Gun Tower, Acidic Rounds</t>
+  </si>
+  <si>
+    <t>90mm Gun Tower, Cryo Rounds</t>
+  </si>
+  <si>
+    <t>90mm Gun Tower, Incidiary Rounds</t>
+  </si>
+  <si>
+    <t>Fires high caliber rounds dealing significant damage per shot. Acid coatied rounds deal damage over time</t>
+  </si>
+  <si>
+    <t>Fires high caliber rounds dealing significant damage per shot. Cryo infused rounds slow targets</t>
+  </si>
+  <si>
+    <t>Fires high caliber rounds dealing significant damage per shot. Plasma charged rounds deal fire damage</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_cannon_incindiary</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_cannon_incindiary</t>
   </si>
 </sst>
 </file>
@@ -2227,20 +2275,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K225"/>
+  <dimension ref="A1:K233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="54.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="54.1796875" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2272,7 +2320,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2280,7 +2328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2288,7 +2336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2296,7 +2344,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2304,7 +2352,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>454</v>
       </c>
@@ -2312,7 +2360,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2320,7 +2368,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2328,7 +2376,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2336,7 +2384,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2344,7 +2392,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2352,7 +2400,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2360,7 +2408,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>455</v>
       </c>
@@ -2368,7 +2416,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2376,7 +2424,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2384,7 +2432,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2392,7 +2440,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2400,7 +2448,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -2408,7 +2456,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -2416,7 +2464,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -2424,7 +2472,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -2432,7 +2480,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -2440,7 +2488,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2448,7 +2496,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -2456,7 +2504,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>385</v>
       </c>
@@ -2464,7 +2512,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>349</v>
       </c>
@@ -2475,7 +2523,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -2483,7 +2531,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -2491,7 +2539,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -2499,7 +2547,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>382</v>
       </c>
@@ -2510,7 +2558,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>331</v>
       </c>
@@ -2518,7 +2566,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>340</v>
       </c>
@@ -2526,7 +2574,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>341</v>
       </c>
@@ -2534,7 +2582,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -2542,7 +2590,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -2550,7 +2598,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -2558,7 +2606,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -2566,7 +2614,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>64</v>
       </c>
@@ -2574,7 +2622,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -2582,7 +2630,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>388</v>
       </c>
@@ -2593,7 +2641,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>390</v>
       </c>
@@ -2601,7 +2649,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>391</v>
       </c>
@@ -2609,7 +2657,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>392</v>
       </c>
@@ -2617,7 +2665,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>352</v>
       </c>
@@ -2628,7 +2676,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>66</v>
       </c>
@@ -2636,7 +2684,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -2644,7 +2692,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>69</v>
       </c>
@@ -2652,7 +2700,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -2660,7 +2708,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>72</v>
       </c>
@@ -2668,7 +2716,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -2676,7 +2724,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -2684,1515 +2732,1579 @@
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>461</v>
+      </c>
+      <c r="B52" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>460</v>
+      </c>
+      <c r="B53" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>462</v>
+      </c>
+      <c r="B54" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>474</v>
+      </c>
+      <c r="B55" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>78</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B56" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="57" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>80</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B57" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="58" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>82</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B58" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="59" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>84</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B59" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="60" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>86</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B60" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="61" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>452</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B61" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="62" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>88</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B62" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="63" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>90</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B63" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="64" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>92</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B64" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="65" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>94</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B65" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="66" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>96</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B66" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="67" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>98</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B67" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="68" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>453</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B68" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="69" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>100</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B69" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="70" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>102</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B70" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="71" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>104</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B71" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="72" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>106</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B72" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="73" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>108</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B73" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="74" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>110</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B74" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="75" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>112</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B75" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="76" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>114</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B76" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="77" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>116</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B77" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="78" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>118</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B78" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="79" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>120</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B79" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="80" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>384</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B80" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>350</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B81" t="s">
         <v>351</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C81" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>353</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B82" t="s">
         <v>351</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C82" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>354</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B83" t="s">
         <v>351</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C83" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>122</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B84" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="85" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>383</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B85" t="s">
         <v>376</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C85" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="86" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>332</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B86" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="87" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>333</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B87" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="88" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>334</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B88" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="89" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>124</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B89" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="90" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>126</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B90" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="91" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>128</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B91" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="92" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>130</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B92" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="93" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>393</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B93" t="s">
         <v>400</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C93" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="94" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>394</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B94" t="s">
         <v>400</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C94" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="95" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
         <v>395</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B95" t="s">
         <v>400</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C95" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="96" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>396</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B96" t="s">
         <v>401</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C96" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="97" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>132</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B97" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="98" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>134</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B98" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="99" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>336</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B99" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="100" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>335</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B100" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="101" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>136</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B101" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>464</v>
+      </c>
+      <c r="B102" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>463</v>
+      </c>
+      <c r="B103" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>465</v>
+      </c>
+      <c r="B104" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>475</v>
+      </c>
+      <c r="B105" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>138</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B106" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="107" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>140</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B107" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="108" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>142</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B108" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="109" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>144</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B109" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="110" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>146</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B110" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="111" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>147</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B111" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="112" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>148</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B112" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="113" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
         <v>150</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B113" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="114" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
         <v>152</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B114" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="115" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
         <v>154</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B115" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="116" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
         <v>156</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B116" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="117" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>158</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B117" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="118" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>160</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B118" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="119" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>162</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B119" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="120" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
         <v>164</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B120" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="121" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
         <v>166</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B121" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="122" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
         <v>168</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B122" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="123" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>170</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B123" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="124" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
         <v>172</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B124" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="125" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
         <v>174</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B125" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="126" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
         <v>176</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B126" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="127" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
         <v>178</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B127" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    <row r="128" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
         <v>180</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B128" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+    <row r="129" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>182</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B129" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+    <row r="130" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
         <v>184</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B130" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+    <row r="131" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
         <v>186</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B131" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="132" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
         <v>407</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B132" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+    <row r="133" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
         <v>412</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B133" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="134" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
         <v>413</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B134" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+    <row r="135" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>441</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B135" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+    <row r="136" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>443</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B136" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="137" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
         <v>445</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B137" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+    <row r="138" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>418</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B138" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="139" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>425</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B139" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+    <row r="140" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>427</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B140" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+    <row r="141" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
         <v>188</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B141" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+    <row r="142" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>190</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B142" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="143" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>429</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B143" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="144" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
         <v>437</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B144" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    <row r="145" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
         <v>437</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B145" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    <row r="146" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
         <v>192</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B146" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="147" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
         <v>194</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B147" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="148" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
         <v>196</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B148" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="149" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
         <v>198</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B149" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="150" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
         <v>200</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B150" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="151" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
         <v>202</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B151" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="152" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
         <v>204</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B152" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="153" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
         <v>206</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B153" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="154" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
         <v>208</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B154" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="155" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
         <v>210</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B155" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="156" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
         <v>212</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B156" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="157" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
         <v>214</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B157" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="158" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
         <v>216</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B158" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="159" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
         <v>218</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B159" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+    <row r="160" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
         <v>219</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B160" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="161" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
         <v>220</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B161" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="162" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
         <v>221</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B162" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="163" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
         <v>222</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B163" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="164" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
         <v>223</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B164" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="165" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
         <v>224</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B165" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="166" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
         <v>225</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B166" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+    <row r="167" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
         <v>226</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B167" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+    <row r="168" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
         <v>227</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B168" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+    <row r="169" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
         <v>228</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B169" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="170" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
         <v>229</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B170" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+    <row r="171" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
         <v>406</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B171" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+    <row r="172" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
         <v>411</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B172" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+    <row r="173" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
         <v>414</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B173" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+    <row r="174" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
         <v>440</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B174" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+    <row r="175" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
         <v>442</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B175" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+    <row r="176" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
         <v>444</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B176" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+    <row r="177" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
         <v>419</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B177" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+    <row r="178" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
         <v>426</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B178" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+    <row r="179" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
         <v>428</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B179" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+    <row r="180" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
         <v>230</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B180" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+    <row r="181" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
         <v>232</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B181" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+    <row r="182" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
         <v>430</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B182" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+    <row r="183" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
         <v>435</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B183" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
         <v>436</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B184" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+    <row r="185" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
         <v>234</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B185" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="186" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
         <v>236</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B186" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+    <row r="187" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
         <v>238</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B187" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+    <row r="188" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
         <v>240</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B188" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+    <row r="189" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
         <v>242</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B189" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+    <row r="190" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
         <v>244</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B190" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+    <row r="191" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
         <v>246</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B191" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
         <v>248</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B192" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
         <v>250</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B193" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
         <v>252</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B194" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
         <v>254</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B195" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
         <v>256</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B196" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
         <v>258</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B197" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
         <v>260</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B198" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
         <v>262</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B199" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
         <v>264</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B200" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
         <v>266</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B201" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
         <v>268</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B202" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
         <v>270</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B203" t="s">
         <v>271</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C203" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
         <v>366</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B204" t="s">
         <v>368</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C204" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
         <v>272</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B205" t="s">
         <v>273</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C205" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
         <v>274</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B206" t="s">
         <v>275</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C206" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
         <v>321</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B207" t="s">
         <v>326</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C207" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
         <v>322</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B208" t="s">
         <v>325</v>
       </c>
-      <c r="C200" t="s">
+      <c r="C208" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
         <v>276</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B209" t="s">
         <v>277</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C209" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
         <v>292</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B210" t="s">
         <v>307</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C210" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
         <v>296</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B211" t="s">
         <v>306</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C211" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
         <v>278</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B212" t="s">
         <v>279</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C212" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
         <v>346</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B213" t="s">
         <v>347</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C213" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
         <v>319</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B214" t="s">
         <v>327</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C214" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
         <v>320</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B215" t="s">
         <v>328</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C215" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
         <v>364</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B216" t="s">
         <v>370</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C216" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
         <v>280</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B217" t="s">
         <v>281</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C217" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
         <v>365</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B218" t="s">
         <v>371</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C218" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
         <v>361</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B219" t="s">
         <v>373</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C219" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
         <v>282</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B220" t="s">
         <v>283</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C220" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
         <v>284</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B221" t="s">
         <v>285</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C221" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
         <v>295</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B222" t="s">
         <v>300</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C222" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
         <v>299</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B223" t="s">
         <v>305</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C223" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
         <v>397</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B224" t="s">
         <v>402</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C224" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
         <v>363</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B225" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
         <v>286</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B226" t="s">
         <v>287</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C226" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
         <v>288</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B227" t="s">
         <v>289</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C227" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
         <v>294</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B228" t="s">
         <v>301</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C228" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
         <v>298</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B229" t="s">
         <v>304</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C229" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
         <v>290</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B230" t="s">
         <v>291</v>
       </c>
-      <c r="C222" t="s">
+      <c r="C230" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
         <v>293</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B231" t="s">
         <v>302</v>
       </c>
-      <c r="C223" t="s">
+      <c r="C231" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
         <v>297</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B232" t="s">
         <v>303</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C232" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
         <v>362</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B233" t="s">
         <v>372</v>
       </c>
-      <c r="C225" t="s">
+      <c r="C233" t="s">
         <v>380</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K197">
-    <sortState ref="A2:K225">
+    <sortState ref="A2:K235">
       <sortCondition ref="A1:A197"/>
     </sortState>
   </autoFilter>
@@ -4208,9 +4320,9 @@
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>388</v>
       </c>
@@ -4221,7 +4333,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>390</v>
       </c>
@@ -4229,7 +4341,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>391</v>
       </c>
@@ -4237,7 +4349,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>392</v>
       </c>
@@ -4245,7 +4357,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>393</v>
       </c>
@@ -4256,7 +4368,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>394</v>
       </c>
@@ -4267,7 +4379,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>395</v>
       </c>
@@ -4278,7 +4390,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>396</v>
       </c>
@@ -4289,7 +4401,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>397</v>
       </c>

</xml_diff>

<commit_message>
localization strings, mostly defense
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -5,25 +5,25 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WinData\EpicGames\Riftbreaker\TheRiftbreaker\mods\rebalance\gui\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\TheRiftbreaker\mods\rebalance\gui\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28790" windowHeight="12410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="rebalance_localizations" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$197</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$191</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="568">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -1423,9 +1423,6 @@
     <t>gui/hud/building_name/tower_cannon_cryo</t>
   </si>
   <si>
-    <t>Fires high caliber rounds dealing significant damage per shot. Cooling enables higher fire rate</t>
-  </si>
-  <si>
     <t>90mm Gun Tower, Cooled</t>
   </si>
   <si>
@@ -1438,19 +1435,298 @@
     <t>90mm Gun Tower, Incidiary Rounds</t>
   </si>
   <si>
-    <t>Fires high caliber rounds dealing significant damage per shot. Acid coatied rounds deal damage over time</t>
-  </si>
-  <si>
-    <t>Fires high caliber rounds dealing significant damage per shot. Cryo infused rounds slow targets</t>
-  </si>
-  <si>
-    <t>Fires high caliber rounds dealing significant damage per shot. Plasma charged rounds deal fire damage</t>
-  </si>
-  <si>
     <t>gui/hud/building_description/tower_cannon_incindiary</t>
   </si>
   <si>
     <t>gui/hud/building_name/tower_cannon_incindiary</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/fire_control_station</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/fire_control_station</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_artillery_acid</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_artillery_napalm</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_minigun_supercooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_minigun_cooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_minigun_frag</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_minigun_platform</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_laser_cooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_laser_supercooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_artillery_propelled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_artillery_superpropelled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_rockets_propelled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_rockets_superpropelled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_plasma_base</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_plasma_charged</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_plasma_supercharged</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_railgun_cooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_railgun_supercooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_railgun_large</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_artillery_acid</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_artillery_napalm</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_minigun_cooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_minigun_supercooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_minigun_frag</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_minigun_platform</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_laser_cooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_laser_supercooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_artillery_propelled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_artillery_superpropelled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_rockets_propelled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_rockets_superpropelled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_plasma_base</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_plasma_charged</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_plasma_supercharged</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_railgun_cooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_railgun_supercooled</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/tower_railgun_large</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/biomass_morphed_press</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/biomass_plant_press</t>
+  </si>
+  <si>
+    <t>resource_name/biomass_morphed</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/biomass_morphed_press</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/biomass_plant_press</t>
+  </si>
+  <si>
+    <t>Fire Control Station</t>
+  </si>
+  <si>
+    <t>Minigun Tower, Cooled</t>
+  </si>
+  <si>
+    <t>Minigun Tower, Supercooled</t>
+  </si>
+  <si>
+    <t>Large Minigun Tower, Frag Rounds</t>
+  </si>
+  <si>
+    <t>Minigun Tower, Enviormental Cooling</t>
+  </si>
+  <si>
+    <t>Laser Tower, Cooled</t>
+  </si>
+  <si>
+    <t>Laser Tower, Supercooled</t>
+  </si>
+  <si>
+    <t>Artillery Tower, Propelled</t>
+  </si>
+  <si>
+    <t>Artillery Tower, Superpropelled</t>
+  </si>
+  <si>
+    <t>Artillery Tower, Napalm Shells</t>
+  </si>
+  <si>
+    <t>Artillery Tower, Acid Shells</t>
+  </si>
+  <si>
+    <t>Rocket Tower, Propelled</t>
+  </si>
+  <si>
+    <t>Rocket Tower, Superpropelled</t>
+  </si>
+  <si>
+    <t>Plasma Tower, Charged</t>
+  </si>
+  <si>
+    <t>Plasma Tower, Supercharged</t>
+  </si>
+  <si>
+    <t>Plasma Tower</t>
+  </si>
+  <si>
+    <t>Railgun Tower, Cooled</t>
+  </si>
+  <si>
+    <t>Railgun Tower, Supercooled</t>
+  </si>
+  <si>
+    <t>Large Railgun Tower</t>
+  </si>
+  <si>
+    <t>Morphed Biomass Press</t>
+  </si>
+  <si>
+    <t>Biomass Press</t>
+  </si>
+  <si>
+    <t>Morphed Biomass</t>
+  </si>
+  <si>
+    <t>Powers up/down defense buildings depending on if enemies are in vicinity or not</t>
+  </si>
+  <si>
+    <t>Artillery using piped resources to prepare rounds with acid payload</t>
+  </si>
+  <si>
+    <t>Artillery using piped resources to prepare rounds with napalm payload</t>
+  </si>
+  <si>
+    <t>Minigun cooled by piped supercoolant to maximize rate of fire</t>
+  </si>
+  <si>
+    <t>Minigun cooled by piped coolant to increase rate of fire</t>
+  </si>
+  <si>
+    <t>Large Minigun using cooling for optimal firepower and fragmentation rounds that hit multiple enemies per shot</t>
+  </si>
+  <si>
+    <t>Minigun on a Platform for defending flooded areas, liquid cooled via enviorment</t>
+  </si>
+  <si>
+    <t>Laser cooled by piped coolant to increase rate of fire</t>
+  </si>
+  <si>
+    <t>Laser cooled by piped supercoolant to maximize rate of fire</t>
+  </si>
+  <si>
+    <t>Artillery using extra propellant to increase firing rage</t>
+  </si>
+  <si>
+    <t>Artillery using extra reagent propellant to maximize firing rage</t>
+  </si>
+  <si>
+    <t>Rocket launcher using extra propellant to increase firing rage</t>
+  </si>
+  <si>
+    <t>Rocket launcher using extra reagent propellant to maximize firing rage</t>
+  </si>
+  <si>
+    <t>Plasma cannon uses energy to shoot plasma bolts that incindiate anything they come in contact with</t>
+  </si>
+  <si>
+    <t>Plasma cannon uses using pipes resources to additionally charge the bolts to increase damage</t>
+  </si>
+  <si>
+    <t>Plasma cannon uses using pipes resources to super-charge bolts to maximize damage</t>
+  </si>
+  <si>
+    <t>Railgun using piped coolant for stable operation</t>
+  </si>
+  <si>
+    <t>Railgun using piped supercoolant for miximizing rate of fire</t>
+  </si>
+  <si>
+    <t>Large Railgun using cooling for optimal firepower</t>
+  </si>
+  <si>
+    <t>Fires high caliber rounds dealing significant damage per shot cooled by piped coolant to increase rate of fire</t>
+  </si>
+  <si>
+    <t>Fires high caliber rounds dealing significant damage per shot using piped resources to prepare cryo infused rounds that slow targets</t>
+  </si>
+  <si>
+    <t>Fires high caliber rounds dealing significant damage per shot using piped resources to prepare plasma charged rounds deal fire damage</t>
+  </si>
+  <si>
+    <t>Fires high caliber rounds dealing significant damage per shot using piped resources to prepare acid coatied rounds deal damage over time</t>
+  </si>
+  <si>
+    <t>Extracts sludge from plant biomass</t>
+  </si>
+  <si>
+    <t>Extracts morphium from morphed biomass</t>
+  </si>
+  <si>
+    <t>gui/menu/inventory/stat_name/damage_over_time_length</t>
+  </si>
+  <si>
+    <t>Damage duration</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/biomass_morphed_processing</t>
+  </si>
+  <si>
+    <t>Allows Riftbreakers to collect and utilized morphed biomass from plants and creatues in the metallic biome and utilize it to produce morphium.</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/biomass_morpherd_processing</t>
+  </si>
+  <si>
+    <t>Morphed Biomass Handling</t>
   </si>
 </sst>
 </file>
@@ -1956,48 +2232,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2275,20 +2551,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K233"/>
+  <dimension ref="A1:K279"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.1796875" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2320,7 +2596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2328,7 +2604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2336,7 +2612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2344,7 +2620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2352,7 +2628,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>454</v>
       </c>
@@ -2360,7 +2636,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2368,7 +2644,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2376,7 +2652,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2384,7 +2660,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2392,7 +2668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2400,7 +2676,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2408,7 +2684,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>455</v>
       </c>
@@ -2416,7 +2692,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2424,7 +2700,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2432,7 +2708,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2440,7 +2716,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2448,7 +2724,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -2456,7 +2732,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -2464,7 +2740,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -2472,7 +2748,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -2480,7 +2756,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -2488,7 +2764,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2496,1816 +2772,2184 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>513</v>
+      </c>
+      <c r="B24" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>514</v>
+      </c>
+      <c r="B25" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>50</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+    <row r="27" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>385</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+    <row r="28" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>472</v>
+      </c>
+      <c r="B28" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>349</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>355</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    <row r="30" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>52</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="31" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>54</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="32" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>56</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="33" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>382</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" t="s">
         <v>377</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C33" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="34" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>331</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="35" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>340</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B35" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="36" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>341</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B36" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="37" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>58</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B37" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="38" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>60</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="39" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>61</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B39" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>62</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B40" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>64</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>65</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>388</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>389</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C43" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="44" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>390</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="45" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>391</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B45" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="46" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>392</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B46" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="47" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>352</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B47" t="s">
         <v>356</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C47" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="48" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>66</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B48" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="49" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>68</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B49" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="50" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>69</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B50" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="51" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>70</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="52" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>72</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B52" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    <row r="53" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>74</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B53" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    <row r="54" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>492</v>
+      </c>
+      <c r="B54" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>493</v>
+      </c>
+      <c r="B55" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>500</v>
+      </c>
+      <c r="B56" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>501</v>
+      </c>
+      <c r="B57" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>76</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B58" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="59" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>461</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B59" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>460</v>
+      </c>
+      <c r="B60" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>462</v>
+      </c>
+      <c r="B61" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>470</v>
+      </c>
+      <c r="B62" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>498</v>
+      </c>
+      <c r="B63" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>499</v>
+      </c>
+      <c r="B64" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>494</v>
+      </c>
+      <c r="B65" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>496</v>
+      </c>
+      <c r="B66" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>497</v>
+      </c>
+      <c r="B67" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>495</v>
+      </c>
+      <c r="B68" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>504</v>
+      </c>
+      <c r="B69" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>505</v>
+      </c>
+      <c r="B70" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>506</v>
+      </c>
+      <c r="B71" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>507</v>
+      </c>
+      <c r="B72" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>509</v>
+      </c>
+      <c r="B73" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>508</v>
+      </c>
+      <c r="B74" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>502</v>
+      </c>
+      <c r="B75" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>503</v>
+      </c>
+      <c r="B76" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>452</v>
+      </c>
+      <c r="B82" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>90</v>
+      </c>
+      <c r="B84" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>96</v>
+      </c>
+      <c r="B87" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>98</v>
+      </c>
+      <c r="B88" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>453</v>
+      </c>
+      <c r="B89" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>100</v>
+      </c>
+      <c r="B90" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>104</v>
+      </c>
+      <c r="B92" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>108</v>
+      </c>
+      <c r="B94" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>110</v>
+      </c>
+      <c r="B95" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>112</v>
+      </c>
+      <c r="B96" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>114</v>
+      </c>
+      <c r="B97" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>116</v>
+      </c>
+      <c r="B98" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>118</v>
+      </c>
+      <c r="B99" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>510</v>
+      </c>
+      <c r="B100" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>511</v>
+      </c>
+      <c r="B101" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>120</v>
+      </c>
+      <c r="B102" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>384</v>
+      </c>
+      <c r="B103" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>473</v>
+      </c>
+      <c r="B104" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>350</v>
+      </c>
+      <c r="B105" t="s">
+        <v>351</v>
+      </c>
+      <c r="C105" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>353</v>
+      </c>
+      <c r="B106" t="s">
+        <v>351</v>
+      </c>
+      <c r="C106" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>354</v>
+      </c>
+      <c r="B107" t="s">
+        <v>351</v>
+      </c>
+      <c r="C107" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>122</v>
+      </c>
+      <c r="B108" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>383</v>
+      </c>
+      <c r="B109" t="s">
+        <v>376</v>
+      </c>
+      <c r="C109" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>332</v>
+      </c>
+      <c r="B110" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>333</v>
+      </c>
+      <c r="B111" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>334</v>
+      </c>
+      <c r="B112" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>124</v>
+      </c>
+      <c r="B113" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>126</v>
+      </c>
+      <c r="B114" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>128</v>
+      </c>
+      <c r="B115" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>130</v>
+      </c>
+      <c r="B116" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>393</v>
+      </c>
+      <c r="B117" t="s">
+        <v>400</v>
+      </c>
+      <c r="C117" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>394</v>
+      </c>
+      <c r="B118" t="s">
+        <v>400</v>
+      </c>
+      <c r="C118" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>395</v>
+      </c>
+      <c r="B119" t="s">
+        <v>400</v>
+      </c>
+      <c r="C119" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>396</v>
+      </c>
+      <c r="B120" t="s">
+        <v>401</v>
+      </c>
+      <c r="C120" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>132</v>
+      </c>
+      <c r="B121" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>134</v>
+      </c>
+      <c r="B122" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>336</v>
+      </c>
+      <c r="B123" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>335</v>
+      </c>
+      <c r="B124" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>474</v>
+      </c>
+      <c r="B125" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>475</v>
+      </c>
+      <c r="B126" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>482</v>
+      </c>
+      <c r="B127" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>483</v>
+      </c>
+      <c r="B128" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>136</v>
+      </c>
+      <c r="B129" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>464</v>
+      </c>
+      <c r="B130" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>463</v>
+      </c>
+      <c r="B131" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>465</v>
+      </c>
+      <c r="B132" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>460</v>
-      </c>
-      <c r="B53" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>462</v>
-      </c>
-      <c r="B54" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>474</v>
-      </c>
-      <c r="B55" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>78</v>
-      </c>
-      <c r="B56" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>80</v>
-      </c>
-      <c r="B57" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>82</v>
-      </c>
-      <c r="B58" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>84</v>
-      </c>
-      <c r="B59" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>86</v>
-      </c>
-      <c r="B60" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>452</v>
-      </c>
-      <c r="B61" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>88</v>
-      </c>
-      <c r="B62" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>90</v>
-      </c>
-      <c r="B63" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>92</v>
-      </c>
-      <c r="B64" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>94</v>
-      </c>
-      <c r="B65" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>96</v>
-      </c>
-      <c r="B66" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>98</v>
-      </c>
-      <c r="B67" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>453</v>
-      </c>
-      <c r="B68" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>100</v>
-      </c>
-      <c r="B69" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>102</v>
-      </c>
-      <c r="B70" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>104</v>
-      </c>
-      <c r="B71" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>106</v>
-      </c>
-      <c r="B72" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>108</v>
-      </c>
-      <c r="B73" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>110</v>
-      </c>
-      <c r="B74" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>112</v>
-      </c>
-      <c r="B75" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>114</v>
-      </c>
-      <c r="B76" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>116</v>
-      </c>
-      <c r="B77" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>118</v>
-      </c>
-      <c r="B78" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>120</v>
-      </c>
-      <c r="B79" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>384</v>
-      </c>
-      <c r="B80" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>350</v>
-      </c>
-      <c r="B81" t="s">
-        <v>351</v>
-      </c>
-      <c r="C81" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>353</v>
-      </c>
-      <c r="B82" t="s">
-        <v>351</v>
-      </c>
-      <c r="C82" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>354</v>
-      </c>
-      <c r="B83" t="s">
-        <v>351</v>
-      </c>
-      <c r="C83" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>122</v>
-      </c>
-      <c r="B84" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>383</v>
-      </c>
-      <c r="B85" t="s">
-        <v>376</v>
-      </c>
-      <c r="C85" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>332</v>
-      </c>
-      <c r="B86" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>333</v>
-      </c>
-      <c r="B87" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>334</v>
-      </c>
-      <c r="B88" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>124</v>
-      </c>
-      <c r="B89" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>126</v>
-      </c>
-      <c r="B90" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>128</v>
-      </c>
-      <c r="B91" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>130</v>
-      </c>
-      <c r="B92" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>393</v>
-      </c>
-      <c r="B93" t="s">
-        <v>400</v>
-      </c>
-      <c r="C93" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>394</v>
-      </c>
-      <c r="B94" t="s">
-        <v>400</v>
-      </c>
-      <c r="C94" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
-        <v>395</v>
-      </c>
-      <c r="B95" t="s">
-        <v>400</v>
-      </c>
-      <c r="C95" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>396</v>
-      </c>
-      <c r="B96" t="s">
-        <v>401</v>
-      </c>
-      <c r="C96" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>132</v>
-      </c>
-      <c r="B97" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
-        <v>134</v>
-      </c>
-      <c r="B98" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
-        <v>336</v>
-      </c>
-      <c r="B99" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
-        <v>335</v>
-      </c>
-      <c r="B100" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>136</v>
-      </c>
-      <c r="B101" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
-        <v>464</v>
-      </c>
-      <c r="B102" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
-        <v>463</v>
-      </c>
-      <c r="B103" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
-        <v>465</v>
-      </c>
-      <c r="B104" t="s">
+      <c r="B133" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
-        <v>475</v>
-      </c>
-      <c r="B105" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+    <row r="134" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>480</v>
+      </c>
+      <c r="B134" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>481</v>
+      </c>
+      <c r="B135" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>477</v>
+      </c>
+      <c r="B136" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>478</v>
+      </c>
+      <c r="B137" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>479</v>
+      </c>
+      <c r="B138" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>476</v>
+      </c>
+      <c r="B139" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>486</v>
+      </c>
+      <c r="B140" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>487</v>
+      </c>
+      <c r="B141" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>488</v>
+      </c>
+      <c r="B142" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>489</v>
+      </c>
+      <c r="B143" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>491</v>
+      </c>
+      <c r="B144" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>490</v>
+      </c>
+      <c r="B145" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>484</v>
+      </c>
+      <c r="B146" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>485</v>
+      </c>
+      <c r="B147" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>138</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B148" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+    <row r="149" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>562</v>
+      </c>
+      <c r="B149" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>140</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B150" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+    <row r="151" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>142</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B151" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+    <row r="152" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>144</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B152" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+    <row r="153" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>146</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B153" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+    <row r="154" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>147</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B154" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
+    <row r="155" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>148</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B155" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
+    <row r="156" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>150</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B156" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
+    <row r="157" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>564</v>
+      </c>
+      <c r="B157" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>152</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B158" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
+    <row r="159" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>154</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B159" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
+    <row r="160" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>156</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B160" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
+    <row r="161" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>158</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B161" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
+    <row r="162" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>160</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B162" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
+    <row r="163" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>162</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B163" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
+    <row r="164" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>164</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B164" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+    <row r="165" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>166</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B165" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
+    <row r="166" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>168</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B166" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
+    <row r="167" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>170</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B167" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+    <row r="168" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>172</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B168" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+    <row r="169" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>174</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B169" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+    <row r="170" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>176</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B170" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
+    <row r="171" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>178</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B171" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
+    <row r="172" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>180</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B172" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+    <row r="173" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>182</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B173" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+    <row r="174" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>184</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B174" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+    <row r="175" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>186</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B175" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+    <row r="176" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>407</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B176" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+    <row r="177" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>412</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B177" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>413</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B178" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+    <row r="179" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>441</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B179" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+    <row r="180" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>443</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B180" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
+    <row r="181" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>445</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B181" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
+    <row r="182" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>418</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B182" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
+    <row r="183" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>425</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B183" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
+    <row r="184" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>427</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B184" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
+    <row r="185" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>188</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B185" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>190</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B186" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>429</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B187" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>437</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B188" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>437</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B189" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>192</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B190" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>194</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B191" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148" t="s">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>196</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B192" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>198</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B193" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" t="s">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>200</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B194" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151" t="s">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
         <v>202</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B195" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A152" t="s">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
         <v>204</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B196" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A153" t="s">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>566</v>
+      </c>
+      <c r="B197" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
         <v>206</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B198" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A154" t="s">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
         <v>208</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B199" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155" t="s">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>210</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B200" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A156" t="s">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>212</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B201" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A157" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>214</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B202" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A158" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
         <v>216</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B203" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A159" t="s">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
         <v>218</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B204" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160" t="s">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
         <v>219</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B205" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" t="s">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>220</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B206" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" t="s">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>221</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B207" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A163" t="s">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
         <v>222</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B208" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" t="s">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>223</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B209" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165" t="s">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
         <v>224</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B210" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A166" t="s">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
         <v>225</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B211" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A167" t="s">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>226</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B212" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A168" t="s">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
         <v>227</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B213" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A169" t="s">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
         <v>228</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B214" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A170" t="s">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>229</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B215" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
         <v>406</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B216" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A172" t="s">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>411</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B217" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A173" t="s">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>414</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B218" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A174" t="s">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>440</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B219" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A175" t="s">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
         <v>442</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B220" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A176" t="s">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
         <v>444</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B221" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A177" t="s">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>419</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B222" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A178" t="s">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>426</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B223" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A179" t="s">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>428</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B224" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A180" t="s">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>230</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B225" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A181" t="s">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>232</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B226" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A182" t="s">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
         <v>430</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B227" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A183" t="s">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
         <v>435</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B228" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A184" t="s">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
         <v>436</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B229" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A185" t="s">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
         <v>234</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B230" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186" t="s">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
         <v>236</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B231" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A187" t="s">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
         <v>238</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B232" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A188" t="s">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
         <v>240</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B233" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189" t="s">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
         <v>242</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B234" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A190" t="s">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
         <v>244</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B235" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A191" t="s">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
         <v>246</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B236" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A192" t="s">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
         <v>248</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B237" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A193" t="s">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
         <v>250</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B238" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A194" t="s">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
         <v>252</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B239" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A195" t="s">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
         <v>254</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B240" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A196" t="s">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
         <v>256</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B241" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A197" t="s">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
         <v>258</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B242" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A198" t="s">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
         <v>260</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B243" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A199" t="s">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
         <v>262</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B244" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A200" t="s">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
         <v>264</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B245" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A201" t="s">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
         <v>266</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B246" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A202" t="s">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
         <v>268</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B247" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A203" t="s">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
         <v>270</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B248" t="s">
         <v>271</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C248" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A204" t="s">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
         <v>366</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B249" t="s">
         <v>368</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C249" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A205" t="s">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
         <v>272</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B250" t="s">
         <v>273</v>
       </c>
-      <c r="C205" t="s">
+      <c r="C250" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A206" t="s">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>512</v>
+      </c>
+      <c r="B251" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
         <v>274</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B252" t="s">
         <v>275</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C252" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A207" t="s">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
         <v>321</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B253" t="s">
         <v>326</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C253" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A208" t="s">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
         <v>322</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B254" t="s">
         <v>325</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C254" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A209" t="s">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
         <v>276</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B255" t="s">
         <v>277</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C255" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A210" t="s">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
         <v>292</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B256" t="s">
         <v>307</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C256" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A211" t="s">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
         <v>296</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B257" t="s">
         <v>306</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C257" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A212" t="s">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
         <v>278</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B258" t="s">
         <v>279</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C258" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A213" t="s">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
         <v>346</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B259" t="s">
         <v>347</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C259" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A214" t="s">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
         <v>319</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B260" t="s">
         <v>327</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C260" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A215" t="s">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
         <v>320</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B261" t="s">
         <v>328</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C261" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A216" t="s">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
         <v>364</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B262" t="s">
         <v>370</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C262" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A217" t="s">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
         <v>280</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B263" t="s">
         <v>281</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C263" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A218" t="s">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
         <v>365</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B264" t="s">
         <v>371</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C264" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A219" t="s">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
         <v>361</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B265" t="s">
         <v>373</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C265" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A220" t="s">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
         <v>282</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B266" t="s">
         <v>283</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C266" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A221" t="s">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
         <v>284</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B267" t="s">
         <v>285</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C267" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A222" t="s">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
         <v>295</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B268" t="s">
         <v>300</v>
       </c>
-      <c r="C222" t="s">
+      <c r="C268" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A223" t="s">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
         <v>299</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B269" t="s">
         <v>305</v>
       </c>
-      <c r="C223" t="s">
+      <c r="C269" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A224" t="s">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
         <v>397</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B270" t="s">
         <v>402</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C270" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A225" t="s">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
         <v>363</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B271" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A226" t="s">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
         <v>286</v>
       </c>
-      <c r="B226" t="s">
+      <c r="B272" t="s">
         <v>287</v>
       </c>
-      <c r="C226" t="s">
+      <c r="C272" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A227" t="s">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
         <v>288</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B273" t="s">
         <v>289</v>
       </c>
-      <c r="C227" t="s">
+      <c r="C273" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A228" t="s">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
         <v>294</v>
       </c>
-      <c r="B228" t="s">
+      <c r="B274" t="s">
         <v>301</v>
       </c>
-      <c r="C228" t="s">
+      <c r="C274" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A229" t="s">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
         <v>298</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B275" t="s">
         <v>304</v>
       </c>
-      <c r="C229" t="s">
+      <c r="C275" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A230" t="s">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
         <v>290</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B276" t="s">
         <v>291</v>
       </c>
-      <c r="C230" t="s">
+      <c r="C276" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A231" t="s">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
         <v>293</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B277" t="s">
         <v>302</v>
       </c>
-      <c r="C231" t="s">
+      <c r="C277" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A232" t="s">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
         <v>297</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B278" t="s">
         <v>303</v>
       </c>
-      <c r="C232" t="s">
+      <c r="C278" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A233" t="s">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
         <v>362</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B279" t="s">
         <v>372</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C279" t="s">
         <v>380</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K197">
-    <sortState ref="A2:K235">
-      <sortCondition ref="A1:A197"/>
+  <autoFilter ref="A1:K191">
+    <sortState ref="A2:K279">
+      <sortCondition ref="A1:A191"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4320,9 +4964,9 @@
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>388</v>
       </c>
@@ -4333,7 +4977,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>390</v>
       </c>
@@ -4341,7 +4985,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>391</v>
       </c>
@@ -4349,7 +4993,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>392</v>
       </c>
@@ -4357,7 +5001,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>393</v>
       </c>
@@ -4368,7 +5012,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>394</v>
       </c>
@@ -4379,7 +5023,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>395</v>
       </c>
@@ -4390,7 +5034,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>396</v>
       </c>
@@ -4401,7 +5045,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>397</v>
       </c>

</xml_diff>

<commit_message>
added basic low caliber tower
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="590">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -1781,6 +1781,18 @@
   </si>
   <si>
     <t>Fires 20mm caliber rounds dealing low damage per shot using at a decent rate of fire</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/towers_lowcaliber</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/towers_lowcaliber</t>
+  </si>
+  <si>
+    <t>Low Caliber Towers</t>
+  </si>
+  <si>
+    <t>Provides basic defense towers utilizing low caliber ammunition.</t>
   </si>
 </sst>
 </file>
@@ -2605,11 +2617,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K288"/>
+  <dimension ref="A1:K290"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4240,18 +4252,18 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>429</v>
+        <v>587</v>
       </c>
       <c r="B196" t="s">
-        <v>432</v>
+        <v>589</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="B197" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -4259,822 +4271,838 @@
         <v>437</v>
       </c>
       <c r="B198" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>192</v>
+        <v>437</v>
       </c>
       <c r="B199" t="s">
-        <v>193</v>
+        <v>439</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B200" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B201" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B202" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B203" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B204" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B205" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>566</v>
+        <v>204</v>
       </c>
       <c r="B206" t="s">
-        <v>567</v>
+        <v>205</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>206</v>
+        <v>566</v>
       </c>
       <c r="B207" t="s">
-        <v>207</v>
+        <v>567</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B210" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B211" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B212" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B213" t="s">
-        <v>165</v>
+        <v>217</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B214" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B215" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B216" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B217" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B218" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B219" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B220" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B221" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B222" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B223" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B224" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>406</v>
+        <v>229</v>
       </c>
       <c r="B225" t="s">
-        <v>408</v>
+        <v>187</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="B226" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B227" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>440</v>
+        <v>414</v>
       </c>
       <c r="B228" t="s">
-        <v>446</v>
+        <v>410</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B229" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B230" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>419</v>
+        <v>444</v>
       </c>
       <c r="B231" t="s">
-        <v>420</v>
+        <v>448</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="B232" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B233" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>230</v>
+        <v>428</v>
       </c>
       <c r="B234" t="s">
-        <v>231</v>
+        <v>424</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B235" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>430</v>
+        <v>232</v>
       </c>
       <c r="B236" t="s">
-        <v>431</v>
+        <v>233</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>435</v>
+        <v>586</v>
       </c>
       <c r="B237" t="s">
-        <v>433</v>
+        <v>588</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="B238" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>234</v>
+        <v>435</v>
       </c>
       <c r="B239" t="s">
-        <v>235</v>
+        <v>433</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>236</v>
+        <v>436</v>
       </c>
       <c r="B240" t="s">
-        <v>237</v>
+        <v>434</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B241" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B242" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B243" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B244" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B245" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B246" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B247" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B248" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B249" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B250" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B251" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B252" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B253" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B254" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B255" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B256" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B257" t="s">
-        <v>271</v>
-      </c>
-      <c r="C257" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>366</v>
+        <v>268</v>
       </c>
       <c r="B258" t="s">
-        <v>368</v>
-      </c>
-      <c r="C258" t="s">
-        <v>367</v>
+        <v>269</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B259" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C259" t="s">
-        <v>312</v>
+        <v>271</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>512</v>
+        <v>366</v>
       </c>
       <c r="B260" t="s">
-        <v>536</v>
+        <v>368</v>
+      </c>
+      <c r="C260" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B261" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C261" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>321</v>
+        <v>512</v>
       </c>
       <c r="B262" t="s">
-        <v>326</v>
-      </c>
-      <c r="C262" t="s">
-        <v>323</v>
+        <v>536</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>322</v>
+        <v>274</v>
       </c>
       <c r="B263" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="C263" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>276</v>
+        <v>321</v>
       </c>
       <c r="B264" t="s">
-        <v>277</v>
+        <v>326</v>
       </c>
       <c r="C264" t="s">
-        <v>277</v>
+        <v>323</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>292</v>
+        <v>322</v>
       </c>
       <c r="B265" t="s">
-        <v>307</v>
+        <v>325</v>
       </c>
       <c r="C265" t="s">
-        <v>311</v>
+        <v>329</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="B266" t="s">
-        <v>306</v>
+        <v>277</v>
       </c>
       <c r="C266" t="s">
-        <v>310</v>
+        <v>277</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="B267" t="s">
-        <v>279</v>
+        <v>307</v>
       </c>
       <c r="C267" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>346</v>
+        <v>296</v>
       </c>
       <c r="B268" t="s">
-        <v>347</v>
+        <v>306</v>
       </c>
       <c r="C268" t="s">
-        <v>348</v>
+        <v>310</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>319</v>
+        <v>278</v>
       </c>
       <c r="B269" t="s">
-        <v>327</v>
+        <v>279</v>
       </c>
       <c r="C269" t="s">
-        <v>324</v>
+        <v>279</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>320</v>
+        <v>346</v>
       </c>
       <c r="B270" t="s">
-        <v>328</v>
+        <v>347</v>
       </c>
       <c r="C270" t="s">
-        <v>330</v>
+        <v>348</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>364</v>
+        <v>319</v>
       </c>
       <c r="B271" t="s">
-        <v>370</v>
+        <v>327</v>
       </c>
       <c r="C271" t="s">
-        <v>374</v>
+        <v>324</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>280</v>
+        <v>320</v>
       </c>
       <c r="B272" t="s">
-        <v>281</v>
+        <v>328</v>
       </c>
       <c r="C272" t="s">
-        <v>281</v>
+        <v>330</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B273" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C273" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>361</v>
+        <v>280</v>
       </c>
       <c r="B274" t="s">
-        <v>373</v>
+        <v>281</v>
       </c>
       <c r="C274" t="s">
-        <v>381</v>
+        <v>281</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>282</v>
+        <v>365</v>
       </c>
       <c r="B275" t="s">
-        <v>283</v>
+        <v>371</v>
       </c>
       <c r="C275" t="s">
-        <v>318</v>
+        <v>375</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>284</v>
+        <v>361</v>
       </c>
       <c r="B276" t="s">
-        <v>285</v>
+        <v>373</v>
       </c>
       <c r="C276" t="s">
-        <v>285</v>
+        <v>381</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="B277" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="C277" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="B278" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="C278" t="s">
-        <v>313</v>
+        <v>285</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>397</v>
+        <v>295</v>
       </c>
       <c r="B279" t="s">
-        <v>402</v>
+        <v>300</v>
       </c>
       <c r="C279" t="s">
-        <v>403</v>
+        <v>309</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>363</v>
+        <v>299</v>
       </c>
       <c r="B280" t="s">
-        <v>369</v>
+        <v>305</v>
+      </c>
+      <c r="C280" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>286</v>
+        <v>397</v>
       </c>
       <c r="B281" t="s">
-        <v>287</v>
+        <v>402</v>
       </c>
       <c r="C281" t="s">
-        <v>359</v>
+        <v>403</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>288</v>
+        <v>363</v>
       </c>
       <c r="B282" t="s">
-        <v>289</v>
-      </c>
-      <c r="C282" t="s">
-        <v>289</v>
+        <v>369</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B283" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="C283" t="s">
-        <v>314</v>
+        <v>359</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="B284" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="C284" t="s">
-        <v>315</v>
+        <v>289</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B285" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="C285" t="s">
-        <v>291</v>
+        <v>314</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="B286" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C286" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B287" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="C287" t="s">
-        <v>317</v>
+        <v>291</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
+        <v>293</v>
+      </c>
+      <c r="B288" t="s">
+        <v>302</v>
+      </c>
+      <c r="C288" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>297</v>
+      </c>
+      <c r="B289" t="s">
+        <v>303</v>
+      </c>
+      <c r="C289" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
         <v>362</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B290" t="s">
         <v>372</v>
       </c>
-      <c r="C288" t="s">
+      <c r="C290" t="s">
         <v>380</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K193">
-    <sortState ref="A2:K288">
+    <sortState ref="A2:K290">
       <sortCondition ref="A1:A193"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
localization strings for petroleum
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="641">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -1895,6 +1895,57 @@
   </si>
   <si>
     <t>Advanced well extraction methods - particularly fracking</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/petroleum_refinery</t>
+  </si>
+  <si>
+    <t>Refines petroleum into reagent and carbonium</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/petroleum_refinery_lvl_2</t>
+  </si>
+  <si>
+    <t>Refines petroleum into reagent and flammable gas</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/petroleum_refinery</t>
+  </si>
+  <si>
+    <t>Petroleum Refinery</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/petroleum_processing</t>
+  </si>
+  <si>
+    <t>Provides methods for petroleum processing into reagent chemicals</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/petroleum_processing_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/petroleum_processing</t>
+  </si>
+  <si>
+    <t>Petrochemistry</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/petroleum_processing_lvl_2</t>
+  </si>
+  <si>
+    <t>Advanced Petrochemistry</t>
+  </si>
+  <si>
+    <t>resource_name/petroleum</t>
+  </si>
+  <si>
+    <t>Petroleum</t>
+  </si>
+  <si>
+    <t>resource_name/petroleum_deepvein</t>
+  </si>
+  <si>
+    <t>Petroleum well</t>
   </si>
 </sst>
 </file>
@@ -2719,11 +2770,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K312"/>
+  <dimension ref="A1:K321"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H186" sqref="H186"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3108,34 +3159,34 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>386</v>
+        <v>624</v>
       </c>
       <c r="B44" t="s">
-        <v>387</v>
-      </c>
-      <c r="C44" t="s">
-        <v>396</v>
+        <v>625</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>388</v>
+        <v>626</v>
       </c>
       <c r="B45" t="s">
-        <v>397</v>
+        <v>627</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B46" t="s">
-        <v>397</v>
+        <v>387</v>
+      </c>
+      <c r="C46" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B47" t="s">
         <v>397</v>
@@ -3143,536 +3194,530 @@
     </row>
     <row r="48" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>389</v>
+      </c>
+      <c r="B48" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>390</v>
+      </c>
+      <c r="B49" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>350</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>354</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="51" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>65</v>
-      </c>
-      <c r="B49" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>67</v>
-      </c>
-      <c r="B50" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>68</v>
       </c>
       <c r="B51" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>69</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="55" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>71</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B55" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="56" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>73</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="57" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>484</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+    <row r="58" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>485</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+    <row r="59" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>492</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+    <row r="60" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>493</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+    <row r="61" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>75</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B61" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    <row r="62" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>457</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B62" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    <row r="63" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>456</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B63" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+    <row r="64" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>458</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B64" t="s">
         <v>532</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>462</v>
-      </c>
-      <c r="B63" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>556</v>
-      </c>
-      <c r="B64" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>490</v>
+        <v>462</v>
       </c>
       <c r="B65" t="s">
-        <v>519</v>
+        <v>533</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>491</v>
+        <v>556</v>
       </c>
       <c r="B66" t="s">
-        <v>520</v>
+        <v>557</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="B67" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="B68" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B69" t="s">
-        <v>613</v>
+        <v>517</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B70" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="B71" t="s">
-        <v>525</v>
+        <v>613</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="B72" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B73" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B74" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B75" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B76" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="B77" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="B78" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>547</v>
+        <v>494</v>
       </c>
       <c r="B79" t="s">
-        <v>551</v>
+        <v>523</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>548</v>
+        <v>495</v>
       </c>
       <c r="B80" t="s">
-        <v>614</v>
+        <v>524</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B81" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>77</v>
+        <v>548</v>
       </c>
       <c r="B82" t="s">
-        <v>78</v>
+        <v>614</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>546</v>
       </c>
       <c r="B83" t="s">
-        <v>80</v>
+        <v>552</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B84" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B85" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B86" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>448</v>
+        <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>452</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B88" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>448</v>
       </c>
       <c r="B89" t="s">
-        <v>90</v>
+        <v>452</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>595</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>593</v>
+        <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>594</v>
+        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>93</v>
+        <v>595</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>593</v>
       </c>
       <c r="B93" t="s">
-        <v>95</v>
+        <v>594</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>449</v>
+        <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>453</v>
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>449</v>
+      </c>
+      <c r="B97" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>98</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B98" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+    <row r="99" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>100</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B99" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    <row r="100" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>102</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B100" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+    <row r="101" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>104</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B101" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+    <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>106</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B102" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
+    <row r="103" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>108</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B103" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
+    <row r="104" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>110</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B104" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
+    <row r="105" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>112</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B105" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
+    <row r="106" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>114</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B106" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+    <row r="107" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>116</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B107" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+    <row r="108" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>502</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B108" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+    <row r="109" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>503</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B109" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+    <row r="110" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>118</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B110" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+    <row r="111" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>382</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B111" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+    <row r="112" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>465</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B112" t="s">
         <v>507</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
-        <v>348</v>
-      </c>
-      <c r="B111" t="s">
-        <v>349</v>
-      </c>
-      <c r="C111" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
-        <v>351</v>
-      </c>
-      <c r="B112" t="s">
-        <v>349</v>
-      </c>
-      <c r="C112" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B113" t="s">
         <v>349</v>
@@ -3683,1698 +3728,1776 @@
     </row>
     <row r="114" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>120</v>
+        <v>351</v>
       </c>
       <c r="B114" t="s">
-        <v>121</v>
+        <v>349</v>
+      </c>
+      <c r="C114" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>381</v>
+        <v>352</v>
       </c>
       <c r="B115" t="s">
-        <v>374</v>
+        <v>349</v>
       </c>
       <c r="C115" t="s">
-        <v>376</v>
+        <v>355</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>330</v>
+        <v>120</v>
       </c>
       <c r="B116" t="s">
-        <v>337</v>
+        <v>121</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>331</v>
+        <v>381</v>
       </c>
       <c r="B117" t="s">
-        <v>342</v>
+        <v>374</v>
+      </c>
+      <c r="C117" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B118" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>122</v>
+        <v>331</v>
       </c>
       <c r="B119" t="s">
-        <v>123</v>
+        <v>342</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>124</v>
+        <v>332</v>
       </c>
       <c r="B120" t="s">
-        <v>125</v>
+        <v>343</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>391</v>
+        <v>126</v>
       </c>
       <c r="B123" t="s">
-        <v>398</v>
-      </c>
-      <c r="C123" t="s">
-        <v>402</v>
+        <v>127</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>392</v>
+        <v>128</v>
       </c>
       <c r="B124" t="s">
-        <v>398</v>
-      </c>
-      <c r="C124" t="s">
-        <v>402</v>
+        <v>129</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>393</v>
+        <v>628</v>
       </c>
       <c r="B125" t="s">
-        <v>398</v>
-      </c>
-      <c r="C125" t="s">
-        <v>402</v>
+        <v>629</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B126" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C126" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>130</v>
+        <v>392</v>
       </c>
       <c r="B127" t="s">
-        <v>131</v>
+        <v>398</v>
+      </c>
+      <c r="C127" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
+        <v>393</v>
+      </c>
+      <c r="B128" t="s">
+        <v>398</v>
+      </c>
+      <c r="C128" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>394</v>
+      </c>
+      <c r="B129" t="s">
+        <v>399</v>
+      </c>
+      <c r="C129" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>130</v>
+      </c>
+      <c r="B130" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
         <v>132</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B131" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+    <row r="132" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
         <v>334</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B132" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+    <row r="133" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
         <v>333</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B133" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+    <row r="134" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
         <v>466</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B134" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+    <row r="135" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>467</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B135" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+    <row r="136" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>474</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B136" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+    <row r="137" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
         <v>475</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B137" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+    <row r="138" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>134</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B138" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+    <row r="139" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>460</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B139" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
+    <row r="140" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>459</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B140" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
+    <row r="141" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
         <v>461</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B141" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
+    <row r="142" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>463</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B142" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
+    <row r="143" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>553</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B143" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
+    <row r="144" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
         <v>472</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B144" t="s">
         <v>616</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
-        <v>473</v>
-      </c>
-      <c r="B142" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
-        <v>469</v>
-      </c>
-      <c r="B143" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
-        <v>470</v>
-      </c>
-      <c r="B144" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B145" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B146" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="B147" t="s">
-        <v>508</v>
+        <v>619</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B148" t="s">
-        <v>605</v>
+        <v>620</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="B149" t="s">
-        <v>606</v>
+        <v>621</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B150" t="s">
-        <v>607</v>
+        <v>508</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B151" t="s">
-        <v>509</v>
+        <v>605</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B152" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="B153" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="B154" t="s">
-        <v>609</v>
+        <v>509</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>543</v>
+        <v>482</v>
       </c>
       <c r="B155" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>545</v>
+        <v>476</v>
       </c>
       <c r="B156" t="s">
-        <v>555</v>
+        <v>608</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>544</v>
+        <v>477</v>
       </c>
       <c r="B157" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>136</v>
+        <v>543</v>
       </c>
       <c r="B158" t="s">
-        <v>137</v>
+        <v>611</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B159" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
       <c r="B160" t="s">
-        <v>538</v>
+        <v>610</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>572</v>
+        <v>136</v>
       </c>
       <c r="B161" t="s">
-        <v>582</v>
+        <v>137</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>573</v>
+        <v>549</v>
       </c>
       <c r="B162" t="s">
-        <v>585</v>
+        <v>550</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>574</v>
+        <v>537</v>
       </c>
       <c r="B163" t="s">
-        <v>588</v>
+        <v>538</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B164" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B165" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B166" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B167" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B168" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B169" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B170" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>138</v>
+        <v>579</v>
       </c>
       <c r="B171" t="s">
-        <v>139</v>
+        <v>591</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>140</v>
+        <v>580</v>
       </c>
       <c r="B172" t="s">
-        <v>141</v>
+        <v>584</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>142</v>
+        <v>581</v>
       </c>
       <c r="B173" t="s">
-        <v>143</v>
+        <v>587</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B174" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B175" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B176" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B177" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>539</v>
+        <v>145</v>
       </c>
       <c r="B178" t="s">
-        <v>540</v>
+        <v>143</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B179" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B180" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>154</v>
+        <v>539</v>
       </c>
       <c r="B181" t="s">
-        <v>155</v>
+        <v>540</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B182" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B183" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B184" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B185" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B186" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B187" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B188" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B189" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B190" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B191" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B192" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B193" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B194" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B195" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B196" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>405</v>
+        <v>180</v>
       </c>
       <c r="B197" t="s">
-        <v>622</v>
+        <v>181</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>410</v>
+        <v>182</v>
       </c>
       <c r="B198" t="s">
-        <v>414</v>
+        <v>183</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>411</v>
+        <v>184</v>
       </c>
       <c r="B199" t="s">
-        <v>413</v>
+        <v>185</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>437</v>
+        <v>405</v>
       </c>
       <c r="B200" t="s">
-        <v>445</v>
+        <v>622</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>439</v>
+        <v>410</v>
       </c>
       <c r="B201" t="s">
-        <v>446</v>
+        <v>414</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>441</v>
+        <v>411</v>
       </c>
       <c r="B202" t="s">
-        <v>447</v>
+        <v>413</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>415</v>
+        <v>630</v>
       </c>
       <c r="B203" t="s">
-        <v>418</v>
+        <v>631</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>422</v>
+        <v>632</v>
       </c>
       <c r="B204" t="s">
-        <v>419</v>
+        <v>631</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>424</v>
+        <v>437</v>
       </c>
       <c r="B205" t="s">
-        <v>419</v>
+        <v>445</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>186</v>
+        <v>439</v>
       </c>
       <c r="B206" t="s">
-        <v>187</v>
+        <v>446</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>188</v>
+        <v>441</v>
       </c>
       <c r="B207" t="s">
-        <v>189</v>
+        <v>447</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>559</v>
+        <v>415</v>
       </c>
       <c r="B208" t="s">
-        <v>561</v>
+        <v>418</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B209" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="B210" t="s">
-        <v>623</v>
+        <v>419</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>434</v>
+        <v>186</v>
       </c>
       <c r="B211" t="s">
-        <v>435</v>
+        <v>187</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>562</v>
+        <v>188</v>
       </c>
       <c r="B212" t="s">
-        <v>582</v>
+        <v>189</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B213" t="s">
-        <v>585</v>
+        <v>561</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>564</v>
+        <v>426</v>
       </c>
       <c r="B214" t="s">
-        <v>588</v>
+        <v>429</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>565</v>
+        <v>434</v>
       </c>
       <c r="B215" t="s">
-        <v>590</v>
+        <v>623</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>566</v>
+        <v>434</v>
       </c>
       <c r="B216" t="s">
-        <v>583</v>
+        <v>435</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="B217" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="B218" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="B219" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="B220" t="s">
-        <v>584</v>
+        <v>590</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="B221" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>190</v>
+        <v>567</v>
       </c>
       <c r="B222" t="s">
-        <v>191</v>
+        <v>586</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>192</v>
+        <v>568</v>
       </c>
       <c r="B223" t="s">
-        <v>193</v>
+        <v>589</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>194</v>
+        <v>569</v>
       </c>
       <c r="B224" t="s">
-        <v>195</v>
+        <v>591</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>196</v>
+        <v>570</v>
       </c>
       <c r="B225" t="s">
-        <v>197</v>
+        <v>584</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>198</v>
+        <v>571</v>
       </c>
       <c r="B226" t="s">
-        <v>199</v>
+        <v>587</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B227" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B228" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>541</v>
+        <v>194</v>
       </c>
       <c r="B229" t="s">
-        <v>542</v>
+        <v>195</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B230" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B231" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B232" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B233" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>212</v>
+        <v>541</v>
       </c>
       <c r="B234" t="s">
-        <v>213</v>
+        <v>542</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B235" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B236" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B237" t="s">
-        <v>165</v>
+        <v>209</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B238" t="s">
-        <v>167</v>
+        <v>211</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B239" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B240" t="s">
-        <v>171</v>
+        <v>215</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B241" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B242" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B243" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B244" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B245" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B246" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B247" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>404</v>
+        <v>223</v>
       </c>
       <c r="B248" t="s">
-        <v>406</v>
+        <v>177</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>409</v>
+        <v>224</v>
       </c>
       <c r="B249" t="s">
-        <v>407</v>
+        <v>179</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>412</v>
+        <v>225</v>
       </c>
       <c r="B250" t="s">
-        <v>408</v>
+        <v>181</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>436</v>
+        <v>226</v>
       </c>
       <c r="B251" t="s">
-        <v>442</v>
+        <v>183</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>438</v>
+        <v>227</v>
       </c>
       <c r="B252" t="s">
-        <v>443</v>
+        <v>185</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>440</v>
+        <v>404</v>
       </c>
       <c r="B253" t="s">
-        <v>444</v>
+        <v>406</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="B254" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="B255" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>425</v>
+        <v>633</v>
       </c>
       <c r="B256" t="s">
-        <v>421</v>
+        <v>634</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>228</v>
+        <v>635</v>
       </c>
       <c r="B257" t="s">
-        <v>229</v>
+        <v>636</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>230</v>
+        <v>436</v>
       </c>
       <c r="B258" t="s">
-        <v>231</v>
+        <v>442</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>558</v>
+        <v>438</v>
       </c>
       <c r="B259" t="s">
-        <v>560</v>
+        <v>443</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>427</v>
+        <v>440</v>
       </c>
       <c r="B260" t="s">
-        <v>428</v>
+        <v>444</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="B261" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="B262" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>232</v>
+        <v>425</v>
       </c>
       <c r="B263" t="s">
-        <v>233</v>
+        <v>421</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B264" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B265" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>238</v>
+        <v>558</v>
       </c>
       <c r="B266" t="s">
-        <v>239</v>
+        <v>560</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>240</v>
+        <v>427</v>
       </c>
       <c r="B267" t="s">
-        <v>241</v>
+        <v>428</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>242</v>
+        <v>432</v>
       </c>
       <c r="B268" t="s">
-        <v>243</v>
+        <v>430</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>244</v>
+        <v>433</v>
       </c>
       <c r="B269" t="s">
-        <v>245</v>
+        <v>431</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B270" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B271" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B272" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="B273" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B274" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="B275" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B276" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="B277" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="B278" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="B279" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="B280" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="B281" t="s">
-        <v>269</v>
-      </c>
-      <c r="C281" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>364</v>
+        <v>256</v>
       </c>
       <c r="B282" t="s">
-        <v>366</v>
-      </c>
-      <c r="C282" t="s">
-        <v>365</v>
+        <v>257</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="B283" t="s">
-        <v>271</v>
-      </c>
-      <c r="C283" t="s">
-        <v>310</v>
+        <v>259</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>504</v>
+        <v>260</v>
       </c>
       <c r="B284" t="s">
-        <v>512</v>
+        <v>261</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="B285" t="s">
-        <v>273</v>
-      </c>
-      <c r="C285" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>319</v>
+        <v>264</v>
       </c>
       <c r="B286" t="s">
-        <v>324</v>
-      </c>
-      <c r="C286" t="s">
-        <v>321</v>
+        <v>265</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>320</v>
+        <v>266</v>
       </c>
       <c r="B287" t="s">
-        <v>323</v>
-      </c>
-      <c r="C287" t="s">
-        <v>327</v>
+        <v>267</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B288" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C288" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>290</v>
+        <v>364</v>
       </c>
       <c r="B289" t="s">
-        <v>305</v>
+        <v>366</v>
       </c>
       <c r="C289" t="s">
-        <v>309</v>
+        <v>365</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="B290" t="s">
-        <v>304</v>
+        <v>271</v>
       </c>
       <c r="C290" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>276</v>
+        <v>504</v>
       </c>
       <c r="B291" t="s">
-        <v>277</v>
-      </c>
-      <c r="C291" t="s">
-        <v>277</v>
+        <v>512</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>344</v>
+        <v>272</v>
       </c>
       <c r="B292" t="s">
-        <v>345</v>
+        <v>273</v>
       </c>
       <c r="C292" t="s">
-        <v>346</v>
+        <v>306</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B293" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C293" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B294" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C294" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>362</v>
+        <v>274</v>
       </c>
       <c r="B295" t="s">
-        <v>368</v>
+        <v>275</v>
       </c>
       <c r="C295" t="s">
-        <v>372</v>
+        <v>275</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="B296" t="s">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="C296" t="s">
-        <v>279</v>
+        <v>309</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>363</v>
+        <v>294</v>
       </c>
       <c r="B297" t="s">
-        <v>369</v>
+        <v>304</v>
       </c>
       <c r="C297" t="s">
-        <v>373</v>
+        <v>308</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>359</v>
+        <v>276</v>
       </c>
       <c r="B298" t="s">
-        <v>371</v>
+        <v>277</v>
       </c>
       <c r="C298" t="s">
-        <v>379</v>
+        <v>277</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>280</v>
+        <v>344</v>
       </c>
       <c r="B299" t="s">
-        <v>281</v>
+        <v>345</v>
       </c>
       <c r="C299" t="s">
-        <v>316</v>
+        <v>346</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>282</v>
+        <v>317</v>
       </c>
       <c r="B300" t="s">
-        <v>283</v>
+        <v>325</v>
       </c>
       <c r="C300" t="s">
-        <v>283</v>
+        <v>322</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>293</v>
+        <v>318</v>
       </c>
       <c r="B301" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="C301" t="s">
-        <v>307</v>
+        <v>328</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>297</v>
+        <v>362</v>
       </c>
       <c r="B302" t="s">
-        <v>303</v>
+        <v>368</v>
       </c>
       <c r="C302" t="s">
-        <v>311</v>
+        <v>372</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>395</v>
+        <v>278</v>
       </c>
       <c r="B303" t="s">
-        <v>400</v>
+        <v>279</v>
       </c>
       <c r="C303" t="s">
-        <v>401</v>
+        <v>279</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B304" t="s">
-        <v>367</v>
+        <v>369</v>
+      </c>
+      <c r="C304" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>284</v>
+        <v>359</v>
       </c>
       <c r="B305" t="s">
-        <v>285</v>
+        <v>371</v>
       </c>
       <c r="C305" t="s">
-        <v>357</v>
+        <v>379</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="B306" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C306" t="s">
-        <v>287</v>
+        <v>316</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="B307" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
       <c r="C307" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B308" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C308" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="B309" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="C309" t="s">
-        <v>289</v>
+        <v>311</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>291</v>
+        <v>637</v>
       </c>
       <c r="B310" t="s">
-        <v>300</v>
-      </c>
-      <c r="C310" t="s">
-        <v>314</v>
+        <v>638</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>295</v>
+        <v>639</v>
       </c>
       <c r="B311" t="s">
-        <v>301</v>
-      </c>
-      <c r="C311" t="s">
-        <v>315</v>
+        <v>640</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
+        <v>395</v>
+      </c>
+      <c r="B312" t="s">
+        <v>400</v>
+      </c>
+      <c r="C312" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A313" t="s">
+        <v>361</v>
+      </c>
+      <c r="B313" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A314" t="s">
+        <v>284</v>
+      </c>
+      <c r="B314" t="s">
+        <v>285</v>
+      </c>
+      <c r="C314" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A315" t="s">
+        <v>286</v>
+      </c>
+      <c r="B315" t="s">
+        <v>287</v>
+      </c>
+      <c r="C315" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
+        <v>292</v>
+      </c>
+      <c r="B316" t="s">
+        <v>299</v>
+      </c>
+      <c r="C316" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
+        <v>296</v>
+      </c>
+      <c r="B317" t="s">
+        <v>302</v>
+      </c>
+      <c r="C317" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A318" t="s">
+        <v>288</v>
+      </c>
+      <c r="B318" t="s">
+        <v>289</v>
+      </c>
+      <c r="C318" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A319" t="s">
+        <v>291</v>
+      </c>
+      <c r="B319" t="s">
+        <v>300</v>
+      </c>
+      <c r="C319" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A320" t="s">
+        <v>295</v>
+      </c>
+      <c r="B320" t="s">
+        <v>301</v>
+      </c>
+      <c r="C320" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A321" t="s">
         <v>360</v>
       </c>
-      <c r="B312" t="s">
+      <c r="B321" t="s">
         <v>370</v>
       </c>
-      <c r="C312" t="s">
+      <c r="C321" t="s">
         <v>378</v>
       </c>
     </row>

</xml_diff>

<commit_message>
consolidated tech tree with update
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28790" windowHeight="12410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="rebalance_localizations" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$347</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$357</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="732">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -2174,6 +2174,51 @@
   </si>
   <si>
     <t>Optimized production of coolans on ammonium hydrocarbon basis</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/ammo_low_caliber_lvl4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/ammo_liquid_lvl4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/ammo_high_caliber_lvl4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/ammo_explosive_lvl4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/ammo_energy_cell_lvl4</t>
+  </si>
+  <si>
+    <t>High-Tech Energy Cell Production</t>
+  </si>
+  <si>
+    <t>High-Tech Explosives Production</t>
+  </si>
+  <si>
+    <t>High-Tech High Caliber Production</t>
+  </si>
+  <si>
+    <t>High-Tech Liquid Ammunitions Production</t>
+  </si>
+  <si>
+    <t>High-Tech Low Caliber Production</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/ammo_energy_cell_lvl4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/ammo_explosive_lvl4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/ammo_high_caliber_lvl4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/ammo_liquid_lvl4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/ammo_low_caliber_lvl4</t>
   </si>
 </sst>
 </file>
@@ -2998,20 +3043,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K359"/>
+  <dimension ref="A1:K369"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G172" sqref="G172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.1796875" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3043,7 +3088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3051,7 +3096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3059,7 +3104,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3067,7 +3112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -3075,7 +3120,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>448</v>
       </c>
@@ -3083,7 +3128,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3091,7 +3136,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -3099,7 +3144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -3107,7 +3152,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>590</v>
       </c>
@@ -3115,7 +3160,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -3123,7 +3168,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3131,7 +3176,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -3139,7 +3184,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>449</v>
       </c>
@@ -3147,7 +3192,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -3155,7 +3200,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3163,7 +3208,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -3171,7 +3216,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3179,7 +3224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -3187,7 +3232,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -3195,7 +3240,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -3203,7 +3248,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -3211,7 +3256,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -3219,7 +3264,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -3227,7 +3272,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>503</v>
       </c>
@@ -3235,7 +3280,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>651</v>
       </c>
@@ -3243,7 +3288,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>504</v>
       </c>
@@ -3251,7 +3296,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -3259,7 +3304,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>381</v>
       </c>
@@ -3267,7 +3312,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>462</v>
       </c>
@@ -3275,7 +3320,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>345</v>
       </c>
@@ -3286,7 +3331,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>671</v>
       </c>
@@ -3294,7 +3339,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -3302,7 +3347,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -3310,7 +3355,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -3318,7 +3363,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>378</v>
       </c>
@@ -3329,7 +3374,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>327</v>
       </c>
@@ -3337,7 +3382,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>336</v>
       </c>
@@ -3345,7 +3390,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>337</v>
       </c>
@@ -3353,7 +3398,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -3361,7 +3406,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -3369,7 +3414,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>60</v>
       </c>
@@ -3377,7 +3422,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>61</v>
       </c>
@@ -3385,7 +3430,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -3393,7 +3438,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>64</v>
       </c>
@@ -3401,7 +3446,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>622</v>
       </c>
@@ -3409,7 +3454,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>624</v>
       </c>
@@ -3417,7 +3462,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>659</v>
       </c>
@@ -3425,7 +3470,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>667</v>
       </c>
@@ -3433,7 +3478,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>668</v>
       </c>
@@ -3441,7 +3486,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>384</v>
       </c>
@@ -3452,7 +3497,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>386</v>
       </c>
@@ -3460,7 +3505,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>387</v>
       </c>
@@ -3468,7 +3513,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>388</v>
       </c>
@@ -3476,2567 +3521,2647 @@
         <v>395</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>689</v>
+      </c>
+      <c r="B55" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>690</v>
+      </c>
+      <c r="B56" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>686</v>
+      </c>
+      <c r="B57" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>348</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B58" t="s">
         <v>352</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C58" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+    <row r="59" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>65</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B59" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+    <row r="60" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>67</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B60" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+    <row r="61" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>68</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B61" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
+    <row r="62" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>69</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B62" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    <row r="63" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>714</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B63" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    <row r="64" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>713</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B64" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+    <row r="65" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>712</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B65" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    <row r="66" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>71</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B66" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    <row r="67" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>73</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B67" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+    <row r="68" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>482</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B68" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+    <row r="69" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>483</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B69" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+    <row r="70" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>490</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B70" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+    <row r="71" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>491</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B71" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+    <row r="72" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>75</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B72" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+    <row r="73" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>455</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B73" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+    <row r="74" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>454</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B74" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+    <row r="75" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>456</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B75" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+    <row r="76" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>460</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B76" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="77" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>554</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B77" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+    <row r="78" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>488</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B78" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+    <row r="79" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>489</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B79" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+    <row r="80" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>484</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B80" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+    <row r="81" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>486</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B81" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+    <row r="82" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>487</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B82" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+    <row r="83" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>485</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B83" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>494</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B84" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>495</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B85" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>496</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B86" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>497</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B87" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="88" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>499</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B88" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+    <row r="89" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>498</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B89" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="90" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>492</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B90" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+    <row r="91" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>493</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B91" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+    <row r="92" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>545</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B92" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+    <row r="93" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>546</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B93" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    <row r="94" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>544</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B94" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+    <row r="95" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>77</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B95" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+    <row r="96" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>79</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B96" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+    <row r="97" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>81</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B97" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+    <row r="98" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>83</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B98" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+    <row r="99" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>85</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B99" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+    <row r="100" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>446</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B100" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    <row r="101" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>87</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B101" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+    <row r="102" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>89</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B102" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+    <row r="103" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>91</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B103" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
+    <row r="104" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>591</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B104" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
+    <row r="105" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>92</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B105" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
+    <row r="106" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>94</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B106" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
+    <row r="107" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>96</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B107" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+    <row r="108" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>447</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B108" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+    <row r="109" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>98</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B109" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+    <row r="110" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>100</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B110" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+    <row r="111" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>102</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B111" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+    <row r="112" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>104</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B112" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+    <row r="113" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>106</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B113" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+    <row r="114" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>108</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B114" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
+    <row r="115" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>110</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B115" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
+    <row r="116" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>112</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B116" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
+    <row r="117" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>114</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B117" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
+    <row r="118" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>116</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B118" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
+    <row r="119" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>500</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B119" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
+    <row r="120" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>646</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B120" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
+    <row r="121" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>501</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B121" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
+    <row r="122" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>118</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B122" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
+    <row r="123" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>380</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B123" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+    <row r="124" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>463</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B124" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
+    <row r="125" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>346</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B125" t="s">
         <v>347</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C125" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
+    <row r="126" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>349</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B126" t="s">
         <v>347</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C126" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+    <row r="127" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>350</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B127" t="s">
         <v>347</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C127" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+    <row r="128" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>657</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B128" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+    <row r="129" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>120</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B129" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
+    <row r="130" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>379</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B130" t="s">
         <v>372</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C130" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
+    <row r="131" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>328</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B131" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+    <row r="132" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>329</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B132" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+    <row r="133" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>330</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B133" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+    <row r="134" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>122</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B134" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+    <row r="135" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>124</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B135" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+    <row r="136" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>126</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B136" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+    <row r="137" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>128</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B137" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+    <row r="138" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>626</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B138" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+    <row r="139" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>389</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B139" t="s">
         <v>396</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C139" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
+    <row r="140" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>390</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B140" t="s">
         <v>396</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C140" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
+    <row r="141" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>391</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B141" t="s">
         <v>396</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C141" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
+    <row r="142" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>392</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B142" t="s">
         <v>397</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C142" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
+    <row r="143" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>687</v>
+      </c>
+      <c r="B143" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>688</v>
+      </c>
+      <c r="B144" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>685</v>
+      </c>
+      <c r="B145" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>130</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B146" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
+    <row r="147" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>132</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B147" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
+    <row r="148" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>332</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B148" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
+    <row r="149" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>331</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B149" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
+    <row r="150" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>700</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B150" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
+    <row r="151" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>697</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B151" t="s">
         <v>701</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
+    <row r="152" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>698</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B152" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
+    <row r="153" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>464</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B153" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148" t="s">
+    <row r="154" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>465</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B154" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
+    <row r="155" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>472</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B155" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" t="s">
+    <row r="156" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>473</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B156" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151" t="s">
+    <row r="157" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>134</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B157" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A152" t="s">
+    <row r="158" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>458</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B158" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A153" t="s">
+    <row r="159" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>457</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B159" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A154" t="s">
+    <row r="160" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>459</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B160" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155" t="s">
+    <row r="161" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>461</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B161" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A156" t="s">
+    <row r="162" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>551</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B162" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A157" t="s">
+    <row r="163" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>470</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B163" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A158" t="s">
+    <row r="164" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>471</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B164" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A159" t="s">
+    <row r="165" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>467</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B165" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160" t="s">
+    <row r="166" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>468</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B166" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" t="s">
+    <row r="167" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>469</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B167" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" t="s">
+    <row r="168" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>466</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B168" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A163" t="s">
+    <row r="169" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>476</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B169" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" t="s">
+    <row r="170" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>477</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B170" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165" t="s">
+    <row r="171" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>478</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B171" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A166" t="s">
+    <row r="172" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>479</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B172" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A167" t="s">
+    <row r="173" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>481</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B173" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A168" t="s">
+    <row r="174" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>480</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B174" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A169" t="s">
+    <row r="175" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>474</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B175" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A170" t="s">
+    <row r="176" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>475</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B176" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
+    <row r="177" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>541</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B177" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A172" t="s">
+    <row r="178" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>543</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B178" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A173" t="s">
+    <row r="179" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>542</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B179" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A174" t="s">
+    <row r="180" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>136</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B180" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A175" t="s">
+    <row r="181" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>547</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B181" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A176" t="s">
+    <row r="182" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>535</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B182" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A177" t="s">
+    <row r="183" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>570</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B183" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A178" t="s">
+    <row r="184" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>571</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B184" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>727</v>
+      </c>
+      <c r="B185" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A179" t="s">
+    <row r="186" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>572</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B186" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A180" t="s">
+    <row r="187" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>573</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B187" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>728</v>
+      </c>
+      <c r="B188" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A181" t="s">
+    <row r="189" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>574</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B189" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A182" t="s">
+    <row r="190" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>575</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B190" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>729</v>
+      </c>
+      <c r="B191" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A183" t="s">
+    <row r="192" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>576</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B192" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A184" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>577</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B193" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>730</v>
+      </c>
+      <c r="B194" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A185" t="s">
+    <row r="195" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>144</v>
+      </c>
+      <c r="B195" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>145</v>
+      </c>
+      <c r="B196" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>673</v>
+      </c>
+      <c r="B197" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>677</v>
+      </c>
+      <c r="B198" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>678</v>
+      </c>
+      <c r="B199" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>146</v>
+      </c>
+      <c r="B200" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>148</v>
+      </c>
+      <c r="B201" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>537</v>
+      </c>
+      <c r="B202" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>643</v>
+      </c>
+      <c r="B203" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>644</v>
+      </c>
+      <c r="B204" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>650</v>
+      </c>
+      <c r="B205" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>707</v>
+      </c>
+      <c r="B206" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>708</v>
+      </c>
+      <c r="B207" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>150</v>
+      </c>
+      <c r="B208" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>152</v>
+      </c>
+      <c r="B209" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>154</v>
+      </c>
+      <c r="B210" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>156</v>
+      </c>
+      <c r="B211" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>158</v>
+      </c>
+      <c r="B212" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>160</v>
+      </c>
+      <c r="B213" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>162</v>
+      </c>
+      <c r="B214" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>164</v>
+      </c>
+      <c r="B215" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>166</v>
+      </c>
+      <c r="B216" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>168</v>
+      </c>
+      <c r="B217" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>170</v>
+      </c>
+      <c r="B218" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>172</v>
+      </c>
+      <c r="B219" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>174</v>
+      </c>
+      <c r="B220" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>176</v>
+      </c>
+      <c r="B221" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>178</v>
+      </c>
+      <c r="B222" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>180</v>
+      </c>
+      <c r="B223" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>182</v>
+      </c>
+      <c r="B224" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>184</v>
+      </c>
+      <c r="B225" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>403</v>
+      </c>
+      <c r="B226" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>408</v>
+      </c>
+      <c r="B227" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>409</v>
+      </c>
+      <c r="B228" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>628</v>
+      </c>
+      <c r="B229" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>630</v>
+      </c>
+      <c r="B230" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>435</v>
+      </c>
+      <c r="B231" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>437</v>
+      </c>
+      <c r="B232" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>439</v>
+      </c>
+      <c r="B233" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>413</v>
+      </c>
+      <c r="B234" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>420</v>
+      </c>
+      <c r="B235" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>422</v>
+      </c>
+      <c r="B236" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>186</v>
+      </c>
+      <c r="B237" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>188</v>
+      </c>
+      <c r="B238" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>557</v>
+      </c>
+      <c r="B239" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>424</v>
+      </c>
+      <c r="B240" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>432</v>
+      </c>
+      <c r="B241" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
         <v>578</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B242" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186" t="s">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
         <v>579</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B243" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>731</v>
+      </c>
+      <c r="B244" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A187" t="s">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
         <v>138</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B245" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A188" t="s">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
         <v>140</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B246" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189" t="s">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
         <v>142</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B247" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A190" t="s">
-        <v>144</v>
-      </c>
-      <c r="B190" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A191" t="s">
-        <v>145</v>
-      </c>
-      <c r="B191" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A192" t="s">
-        <v>673</v>
-      </c>
-      <c r="B192" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A193" t="s">
-        <v>677</v>
-      </c>
-      <c r="B193" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A194" t="s">
-        <v>678</v>
-      </c>
-      <c r="B194" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A195" t="s">
-        <v>146</v>
-      </c>
-      <c r="B195" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A196" t="s">
-        <v>148</v>
-      </c>
-      <c r="B196" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A197" t="s">
-        <v>537</v>
-      </c>
-      <c r="B197" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A198" t="s">
-        <v>643</v>
-      </c>
-      <c r="B198" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A199" t="s">
-        <v>644</v>
-      </c>
-      <c r="B199" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A200" t="s">
-        <v>650</v>
-      </c>
-      <c r="B200" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A201" t="s">
-        <v>707</v>
-      </c>
-      <c r="B201" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A202" t="s">
-        <v>708</v>
-      </c>
-      <c r="B202" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A203" t="s">
-        <v>150</v>
-      </c>
-      <c r="B203" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A204" t="s">
-        <v>152</v>
-      </c>
-      <c r="B204" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A205" t="s">
-        <v>154</v>
-      </c>
-      <c r="B205" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A206" t="s">
-        <v>156</v>
-      </c>
-      <c r="B206" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A207" t="s">
-        <v>158</v>
-      </c>
-      <c r="B207" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A208" t="s">
-        <v>160</v>
-      </c>
-      <c r="B208" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A209" t="s">
-        <v>162</v>
-      </c>
-      <c r="B209" t="s">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>432</v>
+      </c>
+      <c r="B248" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>560</v>
+      </c>
+      <c r="B249" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>561</v>
+      </c>
+      <c r="B250" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>721</v>
+      </c>
+      <c r="B251" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>562</v>
+      </c>
+      <c r="B252" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>563</v>
+      </c>
+      <c r="B253" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>720</v>
+      </c>
+      <c r="B254" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>564</v>
+      </c>
+      <c r="B255" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>565</v>
+      </c>
+      <c r="B256" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>719</v>
+      </c>
+      <c r="B257" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>566</v>
+      </c>
+      <c r="B258" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>567</v>
+      </c>
+      <c r="B259" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>718</v>
+      </c>
+      <c r="B260" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>568</v>
+      </c>
+      <c r="B261" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>569</v>
+      </c>
+      <c r="B262" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>717</v>
+      </c>
+      <c r="B263" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>190</v>
+      </c>
+      <c r="B264" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>192</v>
+      </c>
+      <c r="B265" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>194</v>
+      </c>
+      <c r="B266" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>196</v>
+      </c>
+      <c r="B267" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>198</v>
+      </c>
+      <c r="B268" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>674</v>
+      </c>
+      <c r="B269" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>675</v>
+      </c>
+      <c r="B270" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>676</v>
+      </c>
+      <c r="B271" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>200</v>
+      </c>
+      <c r="B272" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>202</v>
+      </c>
+      <c r="B273" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>539</v>
+      </c>
+      <c r="B274" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>639</v>
+      </c>
+      <c r="B275" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>640</v>
+      </c>
+      <c r="B276" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>648</v>
+      </c>
+      <c r="B277" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>703</v>
+      </c>
+      <c r="B278" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>704</v>
+      </c>
+      <c r="B279" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>204</v>
+      </c>
+      <c r="B280" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>206</v>
+      </c>
+      <c r="B281" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>208</v>
+      </c>
+      <c r="B282" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>210</v>
+      </c>
+      <c r="B283" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>212</v>
+      </c>
+      <c r="B284" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>214</v>
+      </c>
+      <c r="B285" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>216</v>
+      </c>
+      <c r="B286" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A210" t="s">
-        <v>164</v>
-      </c>
-      <c r="B210" t="s">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>217</v>
+      </c>
+      <c r="B287" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A211" t="s">
-        <v>166</v>
-      </c>
-      <c r="B211" t="s">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>218</v>
+      </c>
+      <c r="B288" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A212" t="s">
-        <v>168</v>
-      </c>
-      <c r="B212" t="s">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>219</v>
+      </c>
+      <c r="B289" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A213" t="s">
-        <v>170</v>
-      </c>
-      <c r="B213" t="s">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>220</v>
+      </c>
+      <c r="B290" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A214" t="s">
-        <v>172</v>
-      </c>
-      <c r="B214" t="s">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>221</v>
+      </c>
+      <c r="B291" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A215" t="s">
-        <v>174</v>
-      </c>
-      <c r="B215" t="s">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>222</v>
+      </c>
+      <c r="B292" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A216" t="s">
-        <v>176</v>
-      </c>
-      <c r="B216" t="s">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>223</v>
+      </c>
+      <c r="B293" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A217" t="s">
-        <v>178</v>
-      </c>
-      <c r="B217" t="s">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>224</v>
+      </c>
+      <c r="B294" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A218" t="s">
-        <v>180</v>
-      </c>
-      <c r="B218" t="s">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>225</v>
+      </c>
+      <c r="B295" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A219" t="s">
-        <v>182</v>
-      </c>
-      <c r="B219" t="s">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>226</v>
+      </c>
+      <c r="B296" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A220" t="s">
-        <v>184</v>
-      </c>
-      <c r="B220" t="s">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>227</v>
+      </c>
+      <c r="B297" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A221" t="s">
-        <v>403</v>
-      </c>
-      <c r="B221" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A222" t="s">
-        <v>408</v>
-      </c>
-      <c r="B222" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A223" t="s">
-        <v>409</v>
-      </c>
-      <c r="B223" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A224" t="s">
-        <v>628</v>
-      </c>
-      <c r="B224" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A225" t="s">
-        <v>630</v>
-      </c>
-      <c r="B225" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A226" t="s">
-        <v>435</v>
-      </c>
-      <c r="B226" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A227" t="s">
-        <v>437</v>
-      </c>
-      <c r="B227" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A228" t="s">
-        <v>439</v>
-      </c>
-      <c r="B228" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A229" t="s">
-        <v>413</v>
-      </c>
-      <c r="B229" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A230" t="s">
-        <v>420</v>
-      </c>
-      <c r="B230" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A231" t="s">
-        <v>422</v>
-      </c>
-      <c r="B231" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A232" t="s">
-        <v>186</v>
-      </c>
-      <c r="B232" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A233" t="s">
-        <v>188</v>
-      </c>
-      <c r="B233" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A234" t="s">
-        <v>557</v>
-      </c>
-      <c r="B234" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A235" t="s">
-        <v>424</v>
-      </c>
-      <c r="B235" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A236" t="s">
-        <v>432</v>
-      </c>
-      <c r="B236" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A237" t="s">
-        <v>432</v>
-      </c>
-      <c r="B237" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A238" t="s">
-        <v>560</v>
-      </c>
-      <c r="B238" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A239" t="s">
-        <v>561</v>
-      </c>
-      <c r="B239" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A240" t="s">
-        <v>562</v>
-      </c>
-      <c r="B240" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A241" t="s">
-        <v>563</v>
-      </c>
-      <c r="B241" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A242" t="s">
-        <v>564</v>
-      </c>
-      <c r="B242" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A243" t="s">
-        <v>565</v>
-      </c>
-      <c r="B243" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A244" t="s">
-        <v>566</v>
-      </c>
-      <c r="B244" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A245" t="s">
-        <v>567</v>
-      </c>
-      <c r="B245" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A246" t="s">
-        <v>568</v>
-      </c>
-      <c r="B246" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A247" t="s">
-        <v>569</v>
-      </c>
-      <c r="B247" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A248" t="s">
-        <v>190</v>
-      </c>
-      <c r="B248" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A249" t="s">
-        <v>192</v>
-      </c>
-      <c r="B249" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A250" t="s">
-        <v>194</v>
-      </c>
-      <c r="B250" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A251" t="s">
-        <v>196</v>
-      </c>
-      <c r="B251" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A252" t="s">
-        <v>198</v>
-      </c>
-      <c r="B252" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A253" t="s">
-        <v>674</v>
-      </c>
-      <c r="B253" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A254" t="s">
-        <v>675</v>
-      </c>
-      <c r="B254" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A255" t="s">
-        <v>676</v>
-      </c>
-      <c r="B255" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A256" t="s">
-        <v>200</v>
-      </c>
-      <c r="B256" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A257" t="s">
-        <v>202</v>
-      </c>
-      <c r="B257" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A258" t="s">
-        <v>539</v>
-      </c>
-      <c r="B258" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A259" t="s">
-        <v>639</v>
-      </c>
-      <c r="B259" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A260" t="s">
-        <v>640</v>
-      </c>
-      <c r="B260" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A261" t="s">
-        <v>648</v>
-      </c>
-      <c r="B261" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A262" t="s">
-        <v>703</v>
-      </c>
-      <c r="B262" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A263" t="s">
-        <v>704</v>
-      </c>
-      <c r="B263" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A264" t="s">
-        <v>204</v>
-      </c>
-      <c r="B264" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A265" t="s">
-        <v>206</v>
-      </c>
-      <c r="B265" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A266" t="s">
-        <v>208</v>
-      </c>
-      <c r="B266" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A267" t="s">
-        <v>210</v>
-      </c>
-      <c r="B267" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A268" t="s">
-        <v>212</v>
-      </c>
-      <c r="B268" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A269" t="s">
-        <v>214</v>
-      </c>
-      <c r="B269" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A270" t="s">
-        <v>216</v>
-      </c>
-      <c r="B270" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A271" t="s">
-        <v>217</v>
-      </c>
-      <c r="B271" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A272" t="s">
-        <v>218</v>
-      </c>
-      <c r="B272" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A273" t="s">
-        <v>219</v>
-      </c>
-      <c r="B273" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A274" t="s">
-        <v>220</v>
-      </c>
-      <c r="B274" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A275" t="s">
-        <v>221</v>
-      </c>
-      <c r="B275" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A276" t="s">
-        <v>222</v>
-      </c>
-      <c r="B276" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A277" t="s">
-        <v>223</v>
-      </c>
-      <c r="B277" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A278" t="s">
-        <v>224</v>
-      </c>
-      <c r="B278" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A279" t="s">
-        <v>225</v>
-      </c>
-      <c r="B279" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A280" t="s">
-        <v>226</v>
-      </c>
-      <c r="B280" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A281" t="s">
-        <v>227</v>
-      </c>
-      <c r="B281" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A282" t="s">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
         <v>402</v>
       </c>
-      <c r="B282" t="s">
+      <c r="B298" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A283" t="s">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
         <v>407</v>
       </c>
-      <c r="B283" t="s">
+      <c r="B299" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A284" t="s">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
         <v>410</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B300" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A285" t="s">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
         <v>631</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B301" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A286" t="s">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
         <v>633</v>
       </c>
-      <c r="B286" t="s">
+      <c r="B302" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A287" t="s">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
         <v>658</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B303" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A288" t="s">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
         <v>662</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B304" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A289" t="s">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
         <v>663</v>
       </c>
-      <c r="B289" t="s">
+      <c r="B305" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A290" t="s">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
         <v>434</v>
       </c>
-      <c r="B290" t="s">
+      <c r="B306" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A291" t="s">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
         <v>436</v>
       </c>
-      <c r="B291" t="s">
+      <c r="B307" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A292" t="s">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
         <v>438</v>
       </c>
-      <c r="B292" t="s">
+      <c r="B308" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A293" t="s">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
         <v>414</v>
       </c>
-      <c r="B293" t="s">
+      <c r="B309" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A294" t="s">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
         <v>421</v>
       </c>
-      <c r="B294" t="s">
+      <c r="B310" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A295" t="s">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
         <v>423</v>
       </c>
-      <c r="B295" t="s">
+      <c r="B311" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A296" t="s">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
         <v>228</v>
       </c>
-      <c r="B296" t="s">
+      <c r="B312" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A297" t="s">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
         <v>230</v>
       </c>
-      <c r="B297" t="s">
+      <c r="B313" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A298" t="s">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
         <v>556</v>
       </c>
-      <c r="B298" t="s">
+      <c r="B314" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A299" t="s">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
         <v>425</v>
       </c>
-      <c r="B299" t="s">
+      <c r="B315" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A300" t="s">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
         <v>430</v>
       </c>
-      <c r="B300" t="s">
+      <c r="B316" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A301" t="s">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
         <v>431</v>
       </c>
-      <c r="B301" t="s">
+      <c r="B317" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A302" t="s">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
         <v>232</v>
       </c>
-      <c r="B302" t="s">
+      <c r="B318" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A303" t="s">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
         <v>234</v>
       </c>
-      <c r="B303" t="s">
+      <c r="B319" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A304" t="s">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
         <v>236</v>
       </c>
-      <c r="B304" t="s">
+      <c r="B320" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A305" t="s">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
         <v>238</v>
       </c>
-      <c r="B305" t="s">
+      <c r="B321" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A306" t="s">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
         <v>240</v>
       </c>
-      <c r="B306" t="s">
+      <c r="B322" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A307" t="s">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
         <v>242</v>
       </c>
-      <c r="B307" t="s">
+      <c r="B323" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A308" t="s">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
         <v>244</v>
       </c>
-      <c r="B308" t="s">
+      <c r="B324" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A309" t="s">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
         <v>246</v>
       </c>
-      <c r="B309" t="s">
+      <c r="B325" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A310" t="s">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
         <v>248</v>
       </c>
-      <c r="B310" t="s">
+      <c r="B326" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A311" t="s">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
         <v>250</v>
       </c>
-      <c r="B311" t="s">
+      <c r="B327" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A312" t="s">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
         <v>252</v>
       </c>
-      <c r="B312" t="s">
+      <c r="B328" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A313" t="s">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
         <v>254</v>
       </c>
-      <c r="B313" t="s">
+      <c r="B329" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A314" t="s">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
         <v>256</v>
       </c>
-      <c r="B314" t="s">
+      <c r="B330" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A315" t="s">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
         <v>258</v>
       </c>
-      <c r="B315" t="s">
+      <c r="B331" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A316" t="s">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
         <v>260</v>
       </c>
-      <c r="B316" t="s">
+      <c r="B332" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A317" t="s">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
         <v>262</v>
       </c>
-      <c r="B317" t="s">
+      <c r="B333" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A318" t="s">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
         <v>264</v>
       </c>
-      <c r="B318" t="s">
+      <c r="B334" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A319" t="s">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
         <v>266</v>
       </c>
-      <c r="B319" t="s">
+      <c r="B335" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A320" t="s">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
         <v>268</v>
       </c>
-      <c r="B320" t="s">
+      <c r="B336" t="s">
         <v>269</v>
       </c>
-      <c r="C320" t="s">
+      <c r="C336" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A321" t="s">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
         <v>362</v>
       </c>
-      <c r="B321" t="s">
+      <c r="B337" t="s">
         <v>364</v>
       </c>
-      <c r="C321" t="s">
+      <c r="C337" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A322" t="s">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
         <v>270</v>
       </c>
-      <c r="B322" t="s">
+      <c r="B338" t="s">
         <v>271</v>
       </c>
-      <c r="C322" t="s">
+      <c r="C338" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A323" t="s">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
         <v>502</v>
       </c>
-      <c r="B323" t="s">
+      <c r="B339" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A324" t="s">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
         <v>272</v>
       </c>
-      <c r="B324" t="s">
+      <c r="B340" t="s">
         <v>653</v>
       </c>
-      <c r="C324" t="s">
+      <c r="C340" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A325" t="s">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
         <v>317</v>
       </c>
-      <c r="B325" t="s">
+      <c r="B341" t="s">
         <v>322</v>
       </c>
-      <c r="C325" t="s">
+      <c r="C341" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A326" t="s">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
         <v>318</v>
       </c>
-      <c r="B326" t="s">
+      <c r="B342" t="s">
         <v>321</v>
       </c>
-      <c r="C326" t="s">
+      <c r="C342" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A327" t="s">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
         <v>273</v>
       </c>
-      <c r="B327" t="s">
+      <c r="B343" t="s">
         <v>274</v>
       </c>
-      <c r="C327" t="s">
+      <c r="C343" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A328" t="s">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
         <v>289</v>
       </c>
-      <c r="B328" t="s">
+      <c r="B344" t="s">
         <v>304</v>
       </c>
-      <c r="C328" t="s">
+      <c r="C344" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A329" t="s">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
         <v>293</v>
       </c>
-      <c r="B329" t="s">
+      <c r="B345" t="s">
         <v>303</v>
       </c>
-      <c r="C329" t="s">
+      <c r="C345" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A330" t="s">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
         <v>275</v>
       </c>
-      <c r="B330" t="s">
+      <c r="B346" t="s">
         <v>276</v>
       </c>
-      <c r="C330" t="s">
+      <c r="C346" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A331" t="s">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
         <v>342</v>
       </c>
-      <c r="B331" t="s">
+      <c r="B347" t="s">
         <v>343</v>
       </c>
-      <c r="C331" t="s">
+      <c r="C347" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A332" t="s">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
         <v>315</v>
       </c>
-      <c r="B332" t="s">
+      <c r="B348" t="s">
         <v>323</v>
       </c>
-      <c r="C332" t="s">
+      <c r="C348" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A333" t="s">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
         <v>316</v>
       </c>
-      <c r="B333" t="s">
+      <c r="B349" t="s">
         <v>324</v>
       </c>
-      <c r="C333" t="s">
+      <c r="C349" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A334" t="s">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
         <v>360</v>
       </c>
-      <c r="B334" t="s">
+      <c r="B350" t="s">
         <v>366</v>
       </c>
-      <c r="C334" t="s">
+      <c r="C350" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A335" t="s">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
         <v>277</v>
       </c>
-      <c r="B335" t="s">
+      <c r="B351" t="s">
         <v>278</v>
       </c>
-      <c r="C335" t="s">
+      <c r="C351" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A336" t="s">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
         <v>361</v>
       </c>
-      <c r="B336" t="s">
+      <c r="B352" t="s">
         <v>367</v>
       </c>
-      <c r="C336" t="s">
+      <c r="C352" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A337" t="s">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
         <v>357</v>
       </c>
-      <c r="B337" t="s">
+      <c r="B353" t="s">
         <v>369</v>
       </c>
-      <c r="C337" t="s">
+      <c r="C353" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A338" t="s">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
         <v>279</v>
       </c>
-      <c r="B338" t="s">
+      <c r="B354" t="s">
         <v>280</v>
       </c>
-      <c r="C338" t="s">
+      <c r="C354" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A339" t="s">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
         <v>281</v>
       </c>
-      <c r="B339" t="s">
+      <c r="B355" t="s">
         <v>282</v>
       </c>
-      <c r="C339" t="s">
+      <c r="C355" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A340" t="s">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
         <v>292</v>
       </c>
-      <c r="B340" t="s">
+      <c r="B356" t="s">
         <v>297</v>
       </c>
-      <c r="C340" t="s">
+      <c r="C356" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A341" t="s">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
         <v>296</v>
       </c>
-      <c r="B341" t="s">
+      <c r="B357" t="s">
         <v>302</v>
       </c>
-      <c r="C341" t="s">
+      <c r="C357" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A342" t="s">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
         <v>635</v>
       </c>
-      <c r="B342" t="s">
+      <c r="B358" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A343" t="s">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
         <v>637</v>
       </c>
-      <c r="B343" t="s">
+      <c r="B359" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A344" t="s">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
         <v>393</v>
       </c>
-      <c r="B344" t="s">
+      <c r="B360" t="s">
         <v>398</v>
       </c>
-      <c r="C344" t="s">
+      <c r="C360" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A345" t="s">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
         <v>359</v>
       </c>
-      <c r="B345" t="s">
+      <c r="B361" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A346" t="s">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
         <v>283</v>
       </c>
-      <c r="B346" t="s">
+      <c r="B362" t="s">
         <v>284</v>
       </c>
-      <c r="C346" t="s">
+      <c r="C362" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A347" t="s">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
         <v>285</v>
       </c>
-      <c r="B347" t="s">
+      <c r="B363" t="s">
         <v>286</v>
       </c>
-      <c r="C347" t="s">
+      <c r="C363" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A348" t="s">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
         <v>291</v>
       </c>
-      <c r="B348" t="s">
+      <c r="B364" t="s">
         <v>298</v>
       </c>
-      <c r="C348" t="s">
+      <c r="C364" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A349" t="s">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
         <v>295</v>
       </c>
-      <c r="B349" t="s">
+      <c r="B365" t="s">
         <v>301</v>
       </c>
-      <c r="C349" t="s">
+      <c r="C365" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A350" t="s">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
         <v>287</v>
       </c>
-      <c r="B350" t="s">
+      <c r="B366" t="s">
         <v>288</v>
       </c>
-      <c r="C350" t="s">
+      <c r="C366" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A351" t="s">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
         <v>290</v>
       </c>
-      <c r="B351" t="s">
+      <c r="B367" t="s">
         <v>299</v>
       </c>
-      <c r="C351" t="s">
+      <c r="C367" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A352" t="s">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
         <v>294</v>
       </c>
-      <c r="B352" t="s">
+      <c r="B368" t="s">
         <v>300</v>
       </c>
-      <c r="C352" t="s">
+      <c r="C368" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A353" t="s">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
         <v>358</v>
       </c>
-      <c r="B353" t="s">
+      <c r="B369" t="s">
         <v>368</v>
       </c>
-      <c r="C353" t="s">
+      <c r="C369" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A354" t="s">
-        <v>687</v>
-      </c>
-      <c r="B354" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A355" t="s">
-        <v>688</v>
-      </c>
-      <c r="B355" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A356" t="s">
-        <v>685</v>
-      </c>
-      <c r="B356" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A357" t="s">
-        <v>689</v>
-      </c>
-      <c r="B357" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A358" t="s">
-        <v>690</v>
-      </c>
-      <c r="B358" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A359" t="s">
-        <v>686</v>
-      </c>
-      <c r="B359" t="s">
-        <v>695</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:K347">
-    <sortState ref="A2:K345">
-      <sortCondition ref="A1:A339"/>
+  <autoFilter ref="A1:K357">
+    <sortState ref="A2:K369">
+      <sortCondition ref="A1:A357"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6051,9 +6176,9 @@
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>384</v>
       </c>
@@ -6064,7 +6189,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>386</v>
       </c>
@@ -6072,7 +6197,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>387</v>
       </c>
@@ -6080,7 +6205,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>388</v>
       </c>
@@ -6088,7 +6213,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>389</v>
       </c>
@@ -6099,7 +6224,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>390</v>
       </c>
@@ -6110,7 +6235,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>391</v>
       </c>
@@ -6121,7 +6246,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>392</v>
       </c>
@@ -6132,7 +6257,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>393</v>
       </c>

</xml_diff>

<commit_message>
explosives tower tech refinement
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="12405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28790" windowHeight="12410"/>
   </bookViews>
   <sheets>
     <sheet name="rebalance_localizations" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="748">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -2219,6 +2219,54 @@
   </si>
   <si>
     <t>gui/menu/research/description/ammo_low_caliber_lvl4</t>
+  </si>
+  <si>
+    <t>Rocket Towers</t>
+  </si>
+  <si>
+    <t>Rocket Towers 2</t>
+  </si>
+  <si>
+    <t>Rocket Towers 3</t>
+  </si>
+  <si>
+    <t>Simple rocket powered granade defense towers</t>
+  </si>
+  <si>
+    <t>Artillery using indicidary rounds</t>
+  </si>
+  <si>
+    <t>Artillery utilizing acidic rounds</t>
+  </si>
+  <si>
+    <t>Incidiary Artillery</t>
+  </si>
+  <si>
+    <t>Acidic Artillery</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/towers_rocket_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/towers_rocket_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/towers_rocket</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/towers_artillery_acid</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/towers_artillery_napalm</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/towers_artillery_acid</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/towers_artillery_napalm</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/towers_rocket</t>
   </si>
 </sst>
 </file>
@@ -3043,20 +3091,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K369"/>
+  <dimension ref="A1:K377"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G172" sqref="G172"/>
+      <selection pane="bottomLeft" activeCell="A251" sqref="A251"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="54.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="54.1796875" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3088,7 +3136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3096,7 +3144,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3104,7 +3152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3112,7 +3160,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -3120,7 +3168,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>448</v>
       </c>
@@ -3128,7 +3176,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3136,7 +3184,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -3144,7 +3192,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -3152,7 +3200,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>590</v>
       </c>
@@ -3160,7 +3208,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -3168,7 +3216,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3176,7 +3224,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -3184,7 +3232,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>449</v>
       </c>
@@ -3192,7 +3240,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -3200,7 +3248,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3208,7 +3256,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -3216,7 +3264,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3224,7 +3272,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -3232,7 +3280,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -3240,7 +3288,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -3248,7 +3296,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -3256,7 +3304,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -3264,7 +3312,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -3272,7 +3320,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>503</v>
       </c>
@@ -3280,7 +3328,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>651</v>
       </c>
@@ -3288,7 +3336,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>504</v>
       </c>
@@ -3296,7 +3344,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -3304,7 +3352,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>381</v>
       </c>
@@ -3312,7 +3360,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>462</v>
       </c>
@@ -3320,7 +3368,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>345</v>
       </c>
@@ -3331,7 +3379,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>671</v>
       </c>
@@ -3339,7 +3387,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -3347,7 +3395,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -3355,7 +3403,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -3363,7 +3411,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>378</v>
       </c>
@@ -3374,7 +3422,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>327</v>
       </c>
@@ -3382,7 +3430,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>336</v>
       </c>
@@ -3390,7 +3438,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>337</v>
       </c>
@@ -3398,7 +3446,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>57</v>
       </c>
@@ -3406,7 +3454,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -3414,7 +3462,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>60</v>
       </c>
@@ -3422,7 +3470,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>61</v>
       </c>
@@ -3430,7 +3478,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -3438,7 +3486,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>64</v>
       </c>
@@ -3446,7 +3494,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>622</v>
       </c>
@@ -3454,7 +3502,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>624</v>
       </c>
@@ -3462,7 +3510,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>659</v>
       </c>
@@ -3470,7 +3518,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>667</v>
       </c>
@@ -3478,7 +3526,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>668</v>
       </c>
@@ -3486,7 +3534,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>384</v>
       </c>
@@ -3497,7 +3545,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>386</v>
       </c>
@@ -3505,7 +3553,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>387</v>
       </c>
@@ -3513,7 +3561,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>388</v>
       </c>
@@ -3521,7 +3569,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>689</v>
       </c>
@@ -3529,7 +3577,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>690</v>
       </c>
@@ -3537,7 +3585,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>686</v>
       </c>
@@ -3545,7 +3593,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>348</v>
       </c>
@@ -3556,7 +3604,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -3564,7 +3612,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -3572,7 +3620,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -3580,7 +3628,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -3588,7 +3636,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>714</v>
       </c>
@@ -3596,7 +3644,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>713</v>
       </c>
@@ -3604,7 +3652,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>712</v>
       </c>
@@ -3612,7 +3660,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -3620,7 +3668,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -3628,7 +3676,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>482</v>
       </c>
@@ -3636,7 +3684,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>483</v>
       </c>
@@ -3644,7 +3692,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>490</v>
       </c>
@@ -3652,7 +3700,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>491</v>
       </c>
@@ -3660,7 +3708,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -3668,7 +3716,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>455</v>
       </c>
@@ -3676,7 +3724,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>454</v>
       </c>
@@ -3684,7 +3732,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>456</v>
       </c>
@@ -3692,7 +3740,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>460</v>
       </c>
@@ -3700,7 +3748,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>554</v>
       </c>
@@ -3708,7 +3756,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>488</v>
       </c>
@@ -3716,7 +3764,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>489</v>
       </c>
@@ -3724,7 +3772,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>484</v>
       </c>
@@ -3732,7 +3780,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>486</v>
       </c>
@@ -3740,7 +3788,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>487</v>
       </c>
@@ -3748,7 +3796,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>485</v>
       </c>
@@ -3756,7 +3804,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>494</v>
       </c>
@@ -3764,7 +3812,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>495</v>
       </c>
@@ -3772,7 +3820,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>496</v>
       </c>
@@ -3780,7 +3828,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>497</v>
       </c>
@@ -3788,7 +3836,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>499</v>
       </c>
@@ -3796,7 +3844,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>498</v>
       </c>
@@ -3804,7 +3852,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>492</v>
       </c>
@@ -3812,7 +3860,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>493</v>
       </c>
@@ -3820,7 +3868,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>545</v>
       </c>
@@ -3828,7 +3876,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>546</v>
       </c>
@@ -3836,7 +3884,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>544</v>
       </c>
@@ -3844,7 +3892,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>77</v>
       </c>
@@ -3852,7 +3900,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>79</v>
       </c>
@@ -3860,7 +3908,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>81</v>
       </c>
@@ -3868,7 +3916,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>83</v>
       </c>
@@ -3876,7 +3924,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>85</v>
       </c>
@@ -3884,7 +3932,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>446</v>
       </c>
@@ -3892,7 +3940,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>87</v>
       </c>
@@ -3900,7 +3948,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>89</v>
       </c>
@@ -3908,7 +3956,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>91</v>
       </c>
@@ -3916,7 +3964,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>591</v>
       </c>
@@ -3924,7 +3972,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>92</v>
       </c>
@@ -3932,7 +3980,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>94</v>
       </c>
@@ -3940,7 +3988,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>96</v>
       </c>
@@ -3948,7 +3996,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>447</v>
       </c>
@@ -3956,7 +4004,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>98</v>
       </c>
@@ -3964,7 +4012,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>100</v>
       </c>
@@ -3972,7 +4020,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>102</v>
       </c>
@@ -3980,7 +4028,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>104</v>
       </c>
@@ -3988,7 +4036,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>106</v>
       </c>
@@ -3996,7 +4044,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>108</v>
       </c>
@@ -4004,7 +4052,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>110</v>
       </c>
@@ -4012,7 +4060,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>112</v>
       </c>
@@ -4020,7 +4068,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>114</v>
       </c>
@@ -4028,7 +4076,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -4036,7 +4084,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>500</v>
       </c>
@@ -4044,7 +4092,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>646</v>
       </c>
@@ -4052,7 +4100,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>501</v>
       </c>
@@ -4060,7 +4108,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>118</v>
       </c>
@@ -4068,7 +4116,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>380</v>
       </c>
@@ -4076,7 +4124,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>463</v>
       </c>
@@ -4084,7 +4132,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>346</v>
       </c>
@@ -4095,7 +4143,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>349</v>
       </c>
@@ -4106,7 +4154,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>350</v>
       </c>
@@ -4117,7 +4165,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>657</v>
       </c>
@@ -4125,7 +4173,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>120</v>
       </c>
@@ -4133,7 +4181,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>379</v>
       </c>
@@ -4144,7 +4192,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>328</v>
       </c>
@@ -4152,7 +4200,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>329</v>
       </c>
@@ -4160,7 +4208,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>330</v>
       </c>
@@ -4168,7 +4216,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>122</v>
       </c>
@@ -4176,7 +4224,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>124</v>
       </c>
@@ -4184,7 +4232,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>126</v>
       </c>
@@ -4192,7 +4240,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>128</v>
       </c>
@@ -4200,7 +4248,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>626</v>
       </c>
@@ -4208,7 +4256,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>389</v>
       </c>
@@ -4219,7 +4267,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>390</v>
       </c>
@@ -4230,7 +4278,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>391</v>
       </c>
@@ -4241,7 +4289,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>392</v>
       </c>
@@ -4252,7 +4300,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>687</v>
       </c>
@@ -4260,7 +4308,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>688</v>
       </c>
@@ -4268,7 +4316,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>685</v>
       </c>
@@ -4276,7 +4324,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>130</v>
       </c>
@@ -4284,7 +4332,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>132</v>
       </c>
@@ -4292,7 +4340,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>332</v>
       </c>
@@ -4300,7 +4348,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>331</v>
       </c>
@@ -4308,7 +4356,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>700</v>
       </c>
@@ -4316,7 +4364,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>697</v>
       </c>
@@ -4324,7 +4372,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>698</v>
       </c>
@@ -4332,7 +4380,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>464</v>
       </c>
@@ -4340,7 +4388,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>465</v>
       </c>
@@ -4348,7 +4396,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>472</v>
       </c>
@@ -4356,7 +4404,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>473</v>
       </c>
@@ -4364,7 +4412,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>134</v>
       </c>
@@ -4372,7 +4420,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>458</v>
       </c>
@@ -4380,7 +4428,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>457</v>
       </c>
@@ -4388,7 +4436,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>459</v>
       </c>
@@ -4396,7 +4444,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>461</v>
       </c>
@@ -4404,7 +4452,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>551</v>
       </c>
@@ -4412,7 +4460,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>470</v>
       </c>
@@ -4420,7 +4468,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>471</v>
       </c>
@@ -4428,7 +4476,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>467</v>
       </c>
@@ -4436,7 +4484,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>468</v>
       </c>
@@ -4444,7 +4492,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>469</v>
       </c>
@@ -4452,7 +4500,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>466</v>
       </c>
@@ -4460,7 +4508,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>476</v>
       </c>
@@ -4468,7 +4516,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>477</v>
       </c>
@@ -4476,7 +4524,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>478</v>
       </c>
@@ -4484,7 +4532,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>479</v>
       </c>
@@ -4492,7 +4540,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>481</v>
       </c>
@@ -4500,7 +4548,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>480</v>
       </c>
@@ -4508,7 +4556,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>474</v>
       </c>
@@ -4516,7 +4564,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>475</v>
       </c>
@@ -4524,7 +4572,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>541</v>
       </c>
@@ -4532,7 +4580,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>543</v>
       </c>
@@ -4540,7 +4588,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>542</v>
       </c>
@@ -4548,7 +4596,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>136</v>
       </c>
@@ -4556,7 +4604,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>547</v>
       </c>
@@ -4564,7 +4612,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>535</v>
       </c>
@@ -4572,7 +4620,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>570</v>
       </c>
@@ -4580,7 +4628,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>571</v>
       </c>
@@ -4588,7 +4636,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>727</v>
       </c>
@@ -4596,7 +4644,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>572</v>
       </c>
@@ -4604,7 +4652,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>573</v>
       </c>
@@ -4612,7 +4660,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>728</v>
       </c>
@@ -4620,7 +4668,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>574</v>
       </c>
@@ -4628,7 +4676,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>575</v>
       </c>
@@ -4636,7 +4684,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>729</v>
       </c>
@@ -4644,7 +4692,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>576</v>
       </c>
@@ -4652,7 +4700,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>577</v>
       </c>
@@ -4660,7 +4708,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>730</v>
       </c>
@@ -4668,7 +4716,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>144</v>
       </c>
@@ -4676,7 +4724,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>145</v>
       </c>
@@ -4684,7 +4732,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>673</v>
       </c>
@@ -4692,7 +4740,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>677</v>
       </c>
@@ -4700,7 +4748,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>678</v>
       </c>
@@ -4708,7 +4756,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>146</v>
       </c>
@@ -4716,7 +4764,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>148</v>
       </c>
@@ -4724,7 +4772,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>537</v>
       </c>
@@ -4732,7 +4780,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>643</v>
       </c>
@@ -4740,7 +4788,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>644</v>
       </c>
@@ -4748,7 +4796,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>650</v>
       </c>
@@ -4756,7 +4804,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>707</v>
       </c>
@@ -4764,7 +4812,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>708</v>
       </c>
@@ -4772,7 +4820,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>150</v>
       </c>
@@ -4780,7 +4828,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>152</v>
       </c>
@@ -4788,7 +4836,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>154</v>
       </c>
@@ -4796,7 +4844,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>156</v>
       </c>
@@ -4804,7 +4852,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>158</v>
       </c>
@@ -4812,7 +4860,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>160</v>
       </c>
@@ -4820,7 +4868,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>162</v>
       </c>
@@ -4828,7 +4876,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>164</v>
       </c>
@@ -4836,7 +4884,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>166</v>
       </c>
@@ -4844,7 +4892,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>168</v>
       </c>
@@ -4852,7 +4900,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>170</v>
       </c>
@@ -4860,7 +4908,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>172</v>
       </c>
@@ -4868,7 +4916,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>174</v>
       </c>
@@ -4876,7 +4924,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>176</v>
       </c>
@@ -4884,7 +4932,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>178</v>
       </c>
@@ -4892,7 +4940,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>180</v>
       </c>
@@ -4900,7 +4948,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>182</v>
       </c>
@@ -4908,7 +4956,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>184</v>
       </c>
@@ -4916,7 +4964,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>403</v>
       </c>
@@ -4924,7 +4972,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>408</v>
       </c>
@@ -4932,7 +4980,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>409</v>
       </c>
@@ -4940,7 +4988,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>628</v>
       </c>
@@ -4948,7 +4996,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>630</v>
       </c>
@@ -4956,7 +5004,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>435</v>
       </c>
@@ -4964,7 +5012,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>437</v>
       </c>
@@ -4972,7 +5020,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>439</v>
       </c>
@@ -4980,7 +5028,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>413</v>
       </c>
@@ -4988,7 +5036,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>420</v>
       </c>
@@ -4996,7 +5044,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>422</v>
       </c>
@@ -5004,7 +5052,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>186</v>
       </c>
@@ -5012,7 +5060,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>188</v>
       </c>
@@ -5020,7 +5068,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>557</v>
       </c>
@@ -5028,7 +5076,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>424</v>
       </c>
@@ -5036,7 +5084,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>432</v>
       </c>
@@ -5044,7 +5092,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>578</v>
       </c>
@@ -5052,7 +5100,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>579</v>
       </c>
@@ -5060,7 +5108,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>731</v>
       </c>
@@ -5068,7 +5116,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>138</v>
       </c>
@@ -5076,7 +5124,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>140</v>
       </c>
@@ -5084,7 +5132,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>142</v>
       </c>
@@ -5092,1075 +5140,1139 @@
         <v>143</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
+        <v>743</v>
+      </c>
+      <c r="B248" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A249" t="s">
+        <v>744</v>
+      </c>
+      <c r="B249" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A250" t="s">
+        <v>747</v>
+      </c>
+      <c r="B250" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A251" t="s">
         <v>432</v>
       </c>
-      <c r="B248" t="s">
+      <c r="B251" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A252" t="s">
         <v>560</v>
       </c>
-      <c r="B249" t="s">
+      <c r="B252" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A253" t="s">
         <v>561</v>
       </c>
-      <c r="B250" t="s">
+      <c r="B253" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A254" t="s">
         <v>721</v>
       </c>
-      <c r="B251" t="s">
+      <c r="B254" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
         <v>562</v>
       </c>
-      <c r="B252" t="s">
+      <c r="B255" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
         <v>563</v>
       </c>
-      <c r="B253" t="s">
+      <c r="B256" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
         <v>720</v>
       </c>
-      <c r="B254" t="s">
+      <c r="B257" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
         <v>564</v>
       </c>
-      <c r="B255" t="s">
+      <c r="B258" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
         <v>565</v>
       </c>
-      <c r="B256" t="s">
+      <c r="B259" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
         <v>719</v>
       </c>
-      <c r="B257" t="s">
+      <c r="B260" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
         <v>566</v>
       </c>
-      <c r="B258" t="s">
+      <c r="B261" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
         <v>567</v>
       </c>
-      <c r="B259" t="s">
+      <c r="B262" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" t="s">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
         <v>718</v>
       </c>
-      <c r="B260" t="s">
+      <c r="B263" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" t="s">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A264" t="s">
         <v>568</v>
       </c>
-      <c r="B261" t="s">
+      <c r="B264" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A265" t="s">
         <v>569</v>
       </c>
-      <c r="B262" t="s">
+      <c r="B265" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A266" t="s">
         <v>717</v>
       </c>
-      <c r="B263" t="s">
+      <c r="B266" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A267" t="s">
         <v>190</v>
       </c>
-      <c r="B264" t="s">
+      <c r="B267" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" t="s">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A268" t="s">
         <v>192</v>
       </c>
-      <c r="B265" t="s">
+      <c r="B268" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" t="s">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A269" t="s">
         <v>194</v>
       </c>
-      <c r="B266" t="s">
+      <c r="B269" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" t="s">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A270" t="s">
         <v>196</v>
       </c>
-      <c r="B267" t="s">
+      <c r="B270" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" t="s">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A271" t="s">
         <v>198</v>
       </c>
-      <c r="B268" t="s">
+      <c r="B271" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" t="s">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A272" t="s">
         <v>674</v>
       </c>
-      <c r="B269" t="s">
+      <c r="B272" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" t="s">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A273" t="s">
         <v>675</v>
       </c>
-      <c r="B270" t="s">
+      <c r="B273" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" t="s">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A274" t="s">
         <v>676</v>
       </c>
-      <c r="B271" t="s">
+      <c r="B274" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" t="s">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A275" t="s">
         <v>200</v>
       </c>
-      <c r="B272" t="s">
+      <c r="B275" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
         <v>202</v>
       </c>
-      <c r="B273" t="s">
+      <c r="B276" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A277" t="s">
         <v>539</v>
       </c>
-      <c r="B274" t="s">
+      <c r="B277" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" t="s">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A278" t="s">
         <v>639</v>
       </c>
-      <c r="B275" t="s">
+      <c r="B278" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A279" t="s">
         <v>640</v>
       </c>
-      <c r="B276" t="s">
+      <c r="B279" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A280" t="s">
         <v>648</v>
       </c>
-      <c r="B277" t="s">
+      <c r="B280" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A281" t="s">
         <v>703</v>
       </c>
-      <c r="B278" t="s">
+      <c r="B281" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A282" t="s">
         <v>704</v>
       </c>
-      <c r="B279" t="s">
+      <c r="B282" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A283" t="s">
         <v>204</v>
       </c>
-      <c r="B280" t="s">
+      <c r="B283" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A284" t="s">
         <v>206</v>
       </c>
-      <c r="B281" t="s">
+      <c r="B284" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A285" t="s">
         <v>208</v>
       </c>
-      <c r="B282" t="s">
+      <c r="B285" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A286" t="s">
         <v>210</v>
       </c>
-      <c r="B283" t="s">
+      <c r="B286" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A287" t="s">
         <v>212</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B287" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A288" t="s">
         <v>214</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B288" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A289" t="s">
         <v>216</v>
       </c>
-      <c r="B286" t="s">
+      <c r="B289" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A290" t="s">
         <v>217</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B290" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A291" t="s">
         <v>218</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B291" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A292" t="s">
         <v>219</v>
       </c>
-      <c r="B289" t="s">
+      <c r="B292" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A293" t="s">
         <v>220</v>
       </c>
-      <c r="B290" t="s">
+      <c r="B293" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A294" t="s">
         <v>221</v>
       </c>
-      <c r="B291" t="s">
+      <c r="B294" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A295" t="s">
         <v>222</v>
       </c>
-      <c r="B292" t="s">
+      <c r="B295" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A296" t="s">
         <v>223</v>
       </c>
-      <c r="B293" t="s">
+      <c r="B296" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A297" t="s">
         <v>224</v>
       </c>
-      <c r="B294" t="s">
+      <c r="B297" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A298" t="s">
         <v>225</v>
       </c>
-      <c r="B295" t="s">
+      <c r="B298" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A299" t="s">
         <v>226</v>
       </c>
-      <c r="B296" t="s">
+      <c r="B299" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A300" t="s">
         <v>227</v>
       </c>
-      <c r="B297" t="s">
+      <c r="B300" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A301" t="s">
         <v>402</v>
       </c>
-      <c r="B298" t="s">
+      <c r="B301" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A302" t="s">
         <v>407</v>
       </c>
-      <c r="B299" t="s">
+      <c r="B302" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A303" t="s">
         <v>410</v>
       </c>
-      <c r="B300" t="s">
+      <c r="B303" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" t="s">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A304" t="s">
         <v>631</v>
       </c>
-      <c r="B301" t="s">
+      <c r="B304" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" t="s">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A305" t="s">
         <v>633</v>
       </c>
-      <c r="B302" t="s">
+      <c r="B305" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" t="s">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A306" t="s">
         <v>658</v>
       </c>
-      <c r="B303" t="s">
+      <c r="B306" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" t="s">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A307" t="s">
         <v>662</v>
       </c>
-      <c r="B304" t="s">
+      <c r="B307" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" t="s">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A308" t="s">
         <v>663</v>
       </c>
-      <c r="B305" t="s">
+      <c r="B308" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306" t="s">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A309" t="s">
         <v>434</v>
       </c>
-      <c r="B306" t="s">
+      <c r="B309" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" t="s">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A310" t="s">
         <v>436</v>
       </c>
-      <c r="B307" t="s">
+      <c r="B310" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" t="s">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A311" t="s">
         <v>438</v>
       </c>
-      <c r="B308" t="s">
+      <c r="B311" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" t="s">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A312" t="s">
         <v>414</v>
       </c>
-      <c r="B309" t="s">
+      <c r="B312" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" t="s">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A313" t="s">
         <v>421</v>
       </c>
-      <c r="B310" t="s">
+      <c r="B313" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" t="s">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A314" t="s">
         <v>423</v>
       </c>
-      <c r="B311" t="s">
+      <c r="B314" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A315" t="s">
         <v>228</v>
       </c>
-      <c r="B312" t="s">
+      <c r="B315" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
         <v>230</v>
       </c>
-      <c r="B313" t="s">
+      <c r="B316" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A314" t="s">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
+        <v>745</v>
+      </c>
+      <c r="B317" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A318" t="s">
+        <v>746</v>
+      </c>
+      <c r="B318" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A319" t="s">
         <v>556</v>
       </c>
-      <c r="B314" t="s">
+      <c r="B319" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A315" t="s">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A320" t="s">
+        <v>742</v>
+      </c>
+      <c r="B320" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A321" t="s">
+        <v>740</v>
+      </c>
+      <c r="B321" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A322" t="s">
+        <v>741</v>
+      </c>
+      <c r="B322" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A323" t="s">
         <v>425</v>
       </c>
-      <c r="B315" t="s">
+      <c r="B323" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A316" t="s">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A324" t="s">
         <v>430</v>
       </c>
-      <c r="B316" t="s">
+      <c r="B324" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" t="s">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A325" t="s">
         <v>431</v>
       </c>
-      <c r="B317" t="s">
+      <c r="B325" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318" t="s">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A326" t="s">
         <v>232</v>
       </c>
-      <c r="B318" t="s">
+      <c r="B326" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319" t="s">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A327" t="s">
         <v>234</v>
       </c>
-      <c r="B319" t="s">
+      <c r="B327" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A320" t="s">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A328" t="s">
         <v>236</v>
       </c>
-      <c r="B320" t="s">
+      <c r="B328" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A321" t="s">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A329" t="s">
         <v>238</v>
       </c>
-      <c r="B321" t="s">
+      <c r="B329" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A322" t="s">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A330" t="s">
         <v>240</v>
       </c>
-      <c r="B322" t="s">
+      <c r="B330" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A323" t="s">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A331" t="s">
         <v>242</v>
       </c>
-      <c r="B323" t="s">
+      <c r="B331" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A324" t="s">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A332" t="s">
         <v>244</v>
       </c>
-      <c r="B324" t="s">
+      <c r="B332" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A325" t="s">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A333" t="s">
         <v>246</v>
       </c>
-      <c r="B325" t="s">
+      <c r="B333" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A326" t="s">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A334" t="s">
         <v>248</v>
       </c>
-      <c r="B326" t="s">
+      <c r="B334" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A327" t="s">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A335" t="s">
         <v>250</v>
       </c>
-      <c r="B327" t="s">
+      <c r="B335" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A328" t="s">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A336" t="s">
         <v>252</v>
       </c>
-      <c r="B328" t="s">
+      <c r="B336" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A329" t="s">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A337" t="s">
         <v>254</v>
       </c>
-      <c r="B329" t="s">
+      <c r="B337" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A330" t="s">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A338" t="s">
         <v>256</v>
       </c>
-      <c r="B330" t="s">
+      <c r="B338" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A331" t="s">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A339" t="s">
         <v>258</v>
       </c>
-      <c r="B331" t="s">
+      <c r="B339" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A332" t="s">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A340" t="s">
         <v>260</v>
       </c>
-      <c r="B332" t="s">
+      <c r="B340" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A333" t="s">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A341" t="s">
         <v>262</v>
       </c>
-      <c r="B333" t="s">
+      <c r="B341" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A334" t="s">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A342" t="s">
         <v>264</v>
       </c>
-      <c r="B334" t="s">
+      <c r="B342" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A335" t="s">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A343" t="s">
         <v>266</v>
       </c>
-      <c r="B335" t="s">
+      <c r="B343" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A336" t="s">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A344" t="s">
         <v>268</v>
       </c>
-      <c r="B336" t="s">
+      <c r="B344" t="s">
         <v>269</v>
       </c>
-      <c r="C336" t="s">
+      <c r="C344" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A337" t="s">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A345" t="s">
         <v>362</v>
       </c>
-      <c r="B337" t="s">
+      <c r="B345" t="s">
         <v>364</v>
       </c>
-      <c r="C337" t="s">
+      <c r="C345" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A338" t="s">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A346" t="s">
         <v>270</v>
       </c>
-      <c r="B338" t="s">
+      <c r="B346" t="s">
         <v>271</v>
       </c>
-      <c r="C338" t="s">
+      <c r="C346" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A339" t="s">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A347" t="s">
         <v>502</v>
       </c>
-      <c r="B339" t="s">
+      <c r="B347" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A340" t="s">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A348" t="s">
         <v>272</v>
       </c>
-      <c r="B340" t="s">
+      <c r="B348" t="s">
         <v>653</v>
       </c>
-      <c r="C340" t="s">
+      <c r="C348" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A341" t="s">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A349" t="s">
         <v>317</v>
       </c>
-      <c r="B341" t="s">
+      <c r="B349" t="s">
         <v>322</v>
       </c>
-      <c r="C341" t="s">
+      <c r="C349" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A342" t="s">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A350" t="s">
         <v>318</v>
       </c>
-      <c r="B342" t="s">
+      <c r="B350" t="s">
         <v>321</v>
       </c>
-      <c r="C342" t="s">
+      <c r="C350" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A343" t="s">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A351" t="s">
         <v>273</v>
       </c>
-      <c r="B343" t="s">
+      <c r="B351" t="s">
         <v>274</v>
       </c>
-      <c r="C343" t="s">
+      <c r="C351" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A344" t="s">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A352" t="s">
         <v>289</v>
       </c>
-      <c r="B344" t="s">
+      <c r="B352" t="s">
         <v>304</v>
       </c>
-      <c r="C344" t="s">
+      <c r="C352" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A345" t="s">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A353" t="s">
         <v>293</v>
       </c>
-      <c r="B345" t="s">
+      <c r="B353" t="s">
         <v>303</v>
       </c>
-      <c r="C345" t="s">
+      <c r="C353" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A346" t="s">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A354" t="s">
         <v>275</v>
       </c>
-      <c r="B346" t="s">
+      <c r="B354" t="s">
         <v>276</v>
       </c>
-      <c r="C346" t="s">
+      <c r="C354" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A347" t="s">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A355" t="s">
         <v>342</v>
       </c>
-      <c r="B347" t="s">
+      <c r="B355" t="s">
         <v>343</v>
       </c>
-      <c r="C347" t="s">
+      <c r="C355" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A348" t="s">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A356" t="s">
         <v>315</v>
       </c>
-      <c r="B348" t="s">
+      <c r="B356" t="s">
         <v>323</v>
       </c>
-      <c r="C348" t="s">
+      <c r="C356" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A349" t="s">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A357" t="s">
         <v>316</v>
       </c>
-      <c r="B349" t="s">
+      <c r="B357" t="s">
         <v>324</v>
       </c>
-      <c r="C349" t="s">
+      <c r="C357" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A350" t="s">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A358" t="s">
         <v>360</v>
       </c>
-      <c r="B350" t="s">
+      <c r="B358" t="s">
         <v>366</v>
       </c>
-      <c r="C350" t="s">
+      <c r="C358" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A351" t="s">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A359" t="s">
         <v>277</v>
       </c>
-      <c r="B351" t="s">
+      <c r="B359" t="s">
         <v>278</v>
       </c>
-      <c r="C351" t="s">
+      <c r="C359" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A360" t="s">
         <v>361</v>
       </c>
-      <c r="B352" t="s">
+      <c r="B360" t="s">
         <v>367</v>
       </c>
-      <c r="C352" t="s">
+      <c r="C360" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A353" t="s">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A361" t="s">
         <v>357</v>
       </c>
-      <c r="B353" t="s">
+      <c r="B361" t="s">
         <v>369</v>
       </c>
-      <c r="C353" t="s">
+      <c r="C361" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A354" t="s">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A362" t="s">
         <v>279</v>
       </c>
-      <c r="B354" t="s">
+      <c r="B362" t="s">
         <v>280</v>
       </c>
-      <c r="C354" t="s">
+      <c r="C362" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A355" t="s">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A363" t="s">
         <v>281</v>
       </c>
-      <c r="B355" t="s">
+      <c r="B363" t="s">
         <v>282</v>
       </c>
-      <c r="C355" t="s">
+      <c r="C363" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A356" t="s">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A364" t="s">
         <v>292</v>
       </c>
-      <c r="B356" t="s">
+      <c r="B364" t="s">
         <v>297</v>
       </c>
-      <c r="C356" t="s">
+      <c r="C364" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A357" t="s">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A365" t="s">
         <v>296</v>
       </c>
-      <c r="B357" t="s">
+      <c r="B365" t="s">
         <v>302</v>
       </c>
-      <c r="C357" t="s">
+      <c r="C365" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A358" t="s">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A366" t="s">
         <v>635</v>
       </c>
-      <c r="B358" t="s">
+      <c r="B366" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A359" t="s">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A367" t="s">
         <v>637</v>
       </c>
-      <c r="B359" t="s">
+      <c r="B367" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A360" t="s">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A368" t="s">
         <v>393</v>
       </c>
-      <c r="B360" t="s">
+      <c r="B368" t="s">
         <v>398</v>
       </c>
-      <c r="C360" t="s">
+      <c r="C368" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A361" t="s">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A369" t="s">
         <v>359</v>
       </c>
-      <c r="B361" t="s">
+      <c r="B369" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A370" t="s">
         <v>283</v>
       </c>
-      <c r="B362" t="s">
+      <c r="B370" t="s">
         <v>284</v>
       </c>
-      <c r="C362" t="s">
+      <c r="C370" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A363" t="s">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A371" t="s">
         <v>285</v>
       </c>
-      <c r="B363" t="s">
+      <c r="B371" t="s">
         <v>286</v>
       </c>
-      <c r="C363" t="s">
+      <c r="C371" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A364" t="s">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A372" t="s">
         <v>291</v>
       </c>
-      <c r="B364" t="s">
+      <c r="B372" t="s">
         <v>298</v>
       </c>
-      <c r="C364" t="s">
+      <c r="C372" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A365" t="s">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A373" t="s">
         <v>295</v>
       </c>
-      <c r="B365" t="s">
+      <c r="B373" t="s">
         <v>301</v>
       </c>
-      <c r="C365" t="s">
+      <c r="C373" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A366" t="s">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A374" t="s">
         <v>287</v>
       </c>
-      <c r="B366" t="s">
+      <c r="B374" t="s">
         <v>288</v>
       </c>
-      <c r="C366" t="s">
+      <c r="C374" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A367" t="s">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A375" t="s">
         <v>290</v>
       </c>
-      <c r="B367" t="s">
+      <c r="B375" t="s">
         <v>299</v>
       </c>
-      <c r="C367" t="s">
+      <c r="C375" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A368" t="s">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A376" t="s">
         <v>294</v>
       </c>
-      <c r="B368" t="s">
+      <c r="B376" t="s">
         <v>300</v>
       </c>
-      <c r="C368" t="s">
+      <c r="C376" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A369" t="s">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A377" t="s">
         <v>358</v>
       </c>
-      <c r="B369" t="s">
+      <c r="B377" t="s">
         <v>368</v>
       </c>
-      <c r="C369" t="s">
+      <c r="C377" t="s">
         <v>376</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K357">
-    <sortState ref="A2:K369">
+    <sortState ref="A2:K377">
       <sortCondition ref="A1:A357"/>
     </sortState>
   </autoFilter>
@@ -6176,9 +6288,9 @@
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>384</v>
       </c>
@@ -6189,7 +6301,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>386</v>
       </c>
@@ -6197,7 +6309,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>387</v>
       </c>
@@ -6205,7 +6317,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>388</v>
       </c>
@@ -6213,7 +6325,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>389</v>
       </c>
@@ -6224,7 +6336,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>390</v>
       </c>
@@ -6235,7 +6347,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>391</v>
       </c>
@@ -6246,7 +6358,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>392</v>
       </c>
@@ -6257,7 +6369,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>393</v>
       </c>

</xml_diff>

<commit_message>
tech-tree: split bio-gas production, moved synthethizer
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="767">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -175,9 +175,6 @@
     <t>gui/hud/building_description/biomass_water_press</t>
   </si>
   <si>
-    <t>Extracts water from wet biomass</t>
-  </si>
-  <si>
     <t>gui/hud/building_description/heavy_water_plant</t>
   </si>
   <si>
@@ -2267,6 +2264,66 @@
   </si>
   <si>
     <t>gui/menu/research/description/towers_rocket</t>
+  </si>
+  <si>
+    <t>Extracts sludge from biooil</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/biogas</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/biogas_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/biogas_lvl_3</t>
+  </si>
+  <si>
+    <t>Bioreactors</t>
+  </si>
+  <si>
+    <t>Bioreactors 2</t>
+  </si>
+  <si>
+    <t>Bioreactors 3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/biogas</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/biogas_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/biogas_lvl_3</t>
+  </si>
+  <si>
+    <t>Bioreactors process native biomass into flammable gases</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/rare_metals_storage</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/general_storage</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/rare_metals_storage</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/general_storage</t>
+  </si>
+  <si>
+    <t>General Storage</t>
+  </si>
+  <si>
+    <t>Storage facilities for rare metals</t>
+  </si>
+  <si>
+    <t>Storage facilities for various native solid materials</t>
+  </si>
+  <si>
+    <t>Improved bioreactors processes allow faster prodution of flammable gas</t>
+  </si>
+  <si>
+    <t>Optimized Bioreactors offer best flammable gases yield</t>
   </si>
 </sst>
 </file>
@@ -3091,11 +3148,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K377"/>
+  <dimension ref="A1:K387"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A251" sqref="A251"/>
+      <pane ySplit="1" topLeftCell="A356" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E384" sqref="E384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3170,10 +3227,10 @@
     </row>
     <row r="6" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3197,15 +3254,15 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B10" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3234,10 +3291,10 @@
     </row>
     <row r="14" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B14" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3322,26 +3379,26 @@
     </row>
     <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B25" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>650</v>
+      </c>
+      <c r="B26" t="s">
         <v>651</v>
-      </c>
-      <c r="B26" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B27" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3349,2930 +3406,3010 @@
         <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>747</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B29" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B30" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B31" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C31" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>670</v>
+      </c>
+      <c r="B32" t="s">
         <v>671</v>
-      </c>
-      <c r="B32" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" t="s">
         <v>51</v>
-      </c>
-      <c r="B33" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
         <v>53</v>
-      </c>
-      <c r="B34" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" t="s">
         <v>55</v>
-      </c>
-      <c r="B35" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B36" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C36" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B37" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B38" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B39" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
         <v>57</v>
-      </c>
-      <c r="B40" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" t="s">
         <v>61</v>
-      </c>
-      <c r="B43" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>621</v>
+      </c>
+      <c r="B46" t="s">
         <v>622</v>
-      </c>
-      <c r="B46" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>623</v>
+      </c>
+      <c r="B47" t="s">
         <v>624</v>
-      </c>
-      <c r="B47" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B48" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B49" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B50" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>383</v>
+      </c>
+      <c r="B51" t="s">
         <v>384</v>
       </c>
-      <c r="B51" t="s">
-        <v>385</v>
-      </c>
       <c r="C51" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B52" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B53" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B54" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B55" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B56" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B57" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B58" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C58" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" t="s">
         <v>65</v>
-      </c>
-      <c r="B59" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" t="s">
         <v>69</v>
-      </c>
-      <c r="B62" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B63" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B64" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B65" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" t="s">
         <v>71</v>
-      </c>
-      <c r="B66" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" t="s">
         <v>73</v>
-      </c>
-      <c r="B67" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B68" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B69" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B70" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B71" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" t="s">
         <v>75</v>
-      </c>
-      <c r="B72" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B73" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B74" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B75" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B76" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>553</v>
+      </c>
+      <c r="B77" t="s">
         <v>554</v>
-      </c>
-      <c r="B77" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B78" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B79" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B80" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B81" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B82" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B83" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B84" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B85" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B86" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B87" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B88" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B89" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B90" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B91" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B92" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B93" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B94" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
+        <v>76</v>
+      </c>
+      <c r="B95" t="s">
         <v>77</v>
-      </c>
-      <c r="B95" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>78</v>
+      </c>
+      <c r="B96" t="s">
         <v>79</v>
-      </c>
-      <c r="B96" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>80</v>
+      </c>
+      <c r="B97" t="s">
         <v>81</v>
-      </c>
-      <c r="B97" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
+        <v>82</v>
+      </c>
+      <c r="B98" t="s">
         <v>83</v>
-      </c>
-      <c r="B98" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>84</v>
+      </c>
+      <c r="B99" t="s">
         <v>85</v>
-      </c>
-      <c r="B99" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B100" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
+        <v>86</v>
+      </c>
+      <c r="B101" t="s">
         <v>87</v>
-      </c>
-      <c r="B101" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
+        <v>88</v>
+      </c>
+      <c r="B102" t="s">
         <v>89</v>
-      </c>
-      <c r="B102" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B103" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
+        <v>590</v>
+      </c>
+      <c r="B104" t="s">
         <v>591</v>
-      </c>
-      <c r="B104" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
+        <v>91</v>
+      </c>
+      <c r="B105" t="s">
         <v>92</v>
-      </c>
-      <c r="B105" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
+        <v>93</v>
+      </c>
+      <c r="B106" t="s">
         <v>94</v>
-      </c>
-      <c r="B106" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
+        <v>95</v>
+      </c>
+      <c r="B107" t="s">
         <v>96</v>
-      </c>
-      <c r="B107" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B108" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
+        <v>97</v>
+      </c>
+      <c r="B109" t="s">
         <v>98</v>
-      </c>
-      <c r="B109" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
+        <v>99</v>
+      </c>
+      <c r="B110" t="s">
         <v>100</v>
-      </c>
-      <c r="B110" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
+        <v>101</v>
+      </c>
+      <c r="B111" t="s">
         <v>102</v>
-      </c>
-      <c r="B111" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
+        <v>103</v>
+      </c>
+      <c r="B112" t="s">
         <v>104</v>
-      </c>
-      <c r="B112" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
+        <v>105</v>
+      </c>
+      <c r="B113" t="s">
         <v>106</v>
-      </c>
-      <c r="B113" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
+        <v>107</v>
+      </c>
+      <c r="B114" t="s">
         <v>108</v>
-      </c>
-      <c r="B114" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
+        <v>109</v>
+      </c>
+      <c r="B115" t="s">
         <v>110</v>
-      </c>
-      <c r="B115" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
+        <v>111</v>
+      </c>
+      <c r="B116" t="s">
         <v>112</v>
-      </c>
-      <c r="B116" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
+        <v>113</v>
+      </c>
+      <c r="B117" t="s">
         <v>114</v>
-      </c>
-      <c r="B117" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
+        <v>115</v>
+      </c>
+      <c r="B118" t="s">
         <v>116</v>
-      </c>
-      <c r="B118" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B119" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
+        <v>645</v>
+      </c>
+      <c r="B120" t="s">
         <v>646</v>
-      </c>
-      <c r="B120" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B121" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
+        <v>117</v>
+      </c>
+      <c r="B122" t="s">
         <v>118</v>
-      </c>
-      <c r="B122" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B123" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B124" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
+        <v>345</v>
+      </c>
+      <c r="B125" t="s">
         <v>346</v>
       </c>
-      <c r="B125" t="s">
-        <v>347</v>
-      </c>
       <c r="C125" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B126" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C126" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B127" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C127" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B128" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
+        <v>119</v>
+      </c>
+      <c r="B129" t="s">
         <v>120</v>
-      </c>
-      <c r="B129" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B130" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C130" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B131" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B132" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B133" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
+        <v>121</v>
+      </c>
+      <c r="B134" t="s">
         <v>122</v>
-      </c>
-      <c r="B134" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
+        <v>123</v>
+      </c>
+      <c r="B135" t="s">
         <v>124</v>
-      </c>
-      <c r="B135" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
+        <v>125</v>
+      </c>
+      <c r="B136" t="s">
         <v>126</v>
-      </c>
-      <c r="B136" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
+        <v>127</v>
+      </c>
+      <c r="B137" t="s">
         <v>128</v>
-      </c>
-      <c r="B137" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
+        <v>625</v>
+      </c>
+      <c r="B138" t="s">
         <v>626</v>
-      </c>
-      <c r="B138" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B139" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C139" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B140" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C140" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B141" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C141" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B142" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C142" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B143" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B144" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B145" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
+        <v>129</v>
+      </c>
+      <c r="B146" t="s">
         <v>130</v>
-      </c>
-      <c r="B146" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
+        <v>131</v>
+      </c>
+      <c r="B147" t="s">
         <v>132</v>
-      </c>
-      <c r="B147" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
+        <v>331</v>
+      </c>
+      <c r="B148" t="s">
         <v>332</v>
-      </c>
-      <c r="B148" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B149" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B150" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B151" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B152" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B153" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B154" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B155" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B156" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
+        <v>133</v>
+      </c>
+      <c r="B157" t="s">
         <v>134</v>
-      </c>
-      <c r="B157" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B158" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B159" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B160" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B161" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
+        <v>550</v>
+      </c>
+      <c r="B162" t="s">
         <v>551</v>
-      </c>
-      <c r="B162" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B163" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B164" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B165" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B166" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B167" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B168" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B169" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B170" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B171" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B172" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B173" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B174" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B175" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B176" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B177" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B178" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B179" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
+        <v>135</v>
+      </c>
+      <c r="B180" t="s">
         <v>136</v>
-      </c>
-      <c r="B180" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
+        <v>546</v>
+      </c>
+      <c r="B181" t="s">
         <v>547</v>
-      </c>
-      <c r="B181" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
+        <v>534</v>
+      </c>
+      <c r="B182" t="s">
         <v>535</v>
-      </c>
-      <c r="B182" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B183" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B184" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B185" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B186" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B187" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B188" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B189" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B190" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B191" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B192" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B193" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B194" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B195" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B196" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B197" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B198" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B199" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
+        <v>145</v>
+      </c>
+      <c r="B200" t="s">
         <v>146</v>
-      </c>
-      <c r="B200" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
+        <v>147</v>
+      </c>
+      <c r="B201" t="s">
         <v>148</v>
-      </c>
-      <c r="B201" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
+        <v>536</v>
+      </c>
+      <c r="B202" t="s">
         <v>537</v>
-      </c>
-      <c r="B202" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B203" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
+        <v>643</v>
+      </c>
+      <c r="B204" t="s">
         <v>644</v>
-      </c>
-      <c r="B204" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B205" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B206" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B207" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
+        <v>149</v>
+      </c>
+      <c r="B208" t="s">
         <v>150</v>
-      </c>
-      <c r="B208" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
+        <v>151</v>
+      </c>
+      <c r="B209" t="s">
         <v>152</v>
-      </c>
-      <c r="B209" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
+        <v>153</v>
+      </c>
+      <c r="B210" t="s">
         <v>154</v>
-      </c>
-      <c r="B210" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
+        <v>155</v>
+      </c>
+      <c r="B211" t="s">
         <v>156</v>
-      </c>
-      <c r="B211" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
+        <v>157</v>
+      </c>
+      <c r="B212" t="s">
         <v>158</v>
-      </c>
-      <c r="B212" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
+        <v>159</v>
+      </c>
+      <c r="B213" t="s">
         <v>160</v>
-      </c>
-      <c r="B213" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
+        <v>161</v>
+      </c>
+      <c r="B214" t="s">
         <v>162</v>
-      </c>
-      <c r="B214" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
+        <v>163</v>
+      </c>
+      <c r="B215" t="s">
         <v>164</v>
-      </c>
-      <c r="B215" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
+        <v>165</v>
+      </c>
+      <c r="B216" t="s">
         <v>166</v>
-      </c>
-      <c r="B216" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
+        <v>167</v>
+      </c>
+      <c r="B217" t="s">
         <v>168</v>
-      </c>
-      <c r="B217" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
+        <v>169</v>
+      </c>
+      <c r="B218" t="s">
         <v>170</v>
-      </c>
-      <c r="B218" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
+        <v>171</v>
+      </c>
+      <c r="B219" t="s">
         <v>172</v>
-      </c>
-      <c r="B219" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
+        <v>173</v>
+      </c>
+      <c r="B220" t="s">
         <v>174</v>
-      </c>
-      <c r="B220" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
+        <v>175</v>
+      </c>
+      <c r="B221" t="s">
         <v>176</v>
-      </c>
-      <c r="B221" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
+        <v>177</v>
+      </c>
+      <c r="B222" t="s">
         <v>178</v>
-      </c>
-      <c r="B222" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
+        <v>179</v>
+      </c>
+      <c r="B223" t="s">
         <v>180</v>
-      </c>
-      <c r="B223" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
+        <v>181</v>
+      </c>
+      <c r="B224" t="s">
         <v>182</v>
-      </c>
-      <c r="B224" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
+        <v>183</v>
+      </c>
+      <c r="B225" t="s">
         <v>184</v>
-      </c>
-      <c r="B225" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B226" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B227" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B228" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
+        <v>627</v>
+      </c>
+      <c r="B229" t="s">
         <v>628</v>
-      </c>
-      <c r="B229" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B230" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B231" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B232" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B233" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B234" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B235" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B236" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
+        <v>185</v>
+      </c>
+      <c r="B237" t="s">
         <v>186</v>
-      </c>
-      <c r="B237" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
+        <v>187</v>
+      </c>
+      <c r="B238" t="s">
         <v>188</v>
-      </c>
-      <c r="B238" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B239" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B240" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B241" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B242" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B243" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B244" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
+        <v>137</v>
+      </c>
+      <c r="B245" t="s">
         <v>138</v>
-      </c>
-      <c r="B245" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
+        <v>139</v>
+      </c>
+      <c r="B246" t="s">
         <v>140</v>
-      </c>
-      <c r="B246" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
+        <v>141</v>
+      </c>
+      <c r="B247" t="s">
         <v>142</v>
-      </c>
-      <c r="B247" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>743</v>
+        <v>754</v>
       </c>
       <c r="B248" t="s">
-        <v>737</v>
+        <v>757</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>744</v>
+        <v>755</v>
       </c>
       <c r="B249" t="s">
-        <v>736</v>
+        <v>765</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>747</v>
+        <v>756</v>
       </c>
       <c r="B250" t="s">
-        <v>735</v>
+        <v>766</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>432</v>
+        <v>761</v>
       </c>
       <c r="B251" t="s">
-        <v>433</v>
+        <v>764</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>560</v>
+        <v>760</v>
       </c>
       <c r="B252" t="s">
-        <v>580</v>
+        <v>763</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>561</v>
+        <v>742</v>
       </c>
       <c r="B253" t="s">
-        <v>722</v>
+        <v>736</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>721</v>
+        <v>743</v>
       </c>
       <c r="B254" t="s">
-        <v>583</v>
+        <v>735</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>562</v>
+        <v>746</v>
       </c>
       <c r="B255" t="s">
-        <v>586</v>
+        <v>734</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>563</v>
+        <v>431</v>
       </c>
       <c r="B256" t="s">
-        <v>723</v>
+        <v>432</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>720</v>
+        <v>559</v>
       </c>
       <c r="B257" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B258" t="s">
-        <v>581</v>
+        <v>721</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>565</v>
+        <v>720</v>
       </c>
       <c r="B259" t="s">
-        <v>724</v>
+        <v>582</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>719</v>
+        <v>561</v>
       </c>
       <c r="B260" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B261" t="s">
-        <v>587</v>
+        <v>722</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>567</v>
+        <v>719</v>
       </c>
       <c r="B262" t="s">
-        <v>725</v>
+        <v>587</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>718</v>
+        <v>563</v>
       </c>
       <c r="B263" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B264" t="s">
-        <v>582</v>
+        <v>723</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>569</v>
+        <v>718</v>
       </c>
       <c r="B265" t="s">
-        <v>726</v>
+        <v>583</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>717</v>
+        <v>565</v>
       </c>
       <c r="B266" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>190</v>
+        <v>566</v>
       </c>
       <c r="B267" t="s">
-        <v>191</v>
+        <v>724</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>192</v>
+        <v>717</v>
       </c>
       <c r="B268" t="s">
-        <v>193</v>
+        <v>588</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>194</v>
+        <v>567</v>
       </c>
       <c r="B269" t="s">
-        <v>195</v>
+        <v>581</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>196</v>
+        <v>568</v>
       </c>
       <c r="B270" t="s">
-        <v>197</v>
+        <v>725</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>198</v>
+        <v>716</v>
       </c>
       <c r="B271" t="s">
-        <v>199</v>
+        <v>584</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>674</v>
+        <v>189</v>
       </c>
       <c r="B272" t="s">
-        <v>679</v>
+        <v>190</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>675</v>
+        <v>191</v>
       </c>
       <c r="B273" t="s">
-        <v>683</v>
+        <v>192</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>676</v>
+        <v>193</v>
       </c>
       <c r="B274" t="s">
-        <v>684</v>
+        <v>194</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B275" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B276" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>539</v>
+        <v>673</v>
       </c>
       <c r="B277" t="s">
-        <v>540</v>
+        <v>678</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>639</v>
+        <v>674</v>
       </c>
       <c r="B278" t="s">
-        <v>641</v>
+        <v>682</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>640</v>
+        <v>675</v>
       </c>
       <c r="B279" t="s">
-        <v>642</v>
+        <v>683</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>648</v>
+        <v>199</v>
       </c>
       <c r="B280" t="s">
-        <v>649</v>
+        <v>200</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>703</v>
+        <v>201</v>
       </c>
       <c r="B281" t="s">
-        <v>705</v>
+        <v>202</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>704</v>
+        <v>748</v>
       </c>
       <c r="B282" t="s">
-        <v>706</v>
+        <v>751</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>204</v>
+        <v>749</v>
       </c>
       <c r="B283" t="s">
-        <v>205</v>
+        <v>752</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>206</v>
+        <v>750</v>
       </c>
       <c r="B284" t="s">
-        <v>207</v>
+        <v>753</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>208</v>
+        <v>538</v>
       </c>
       <c r="B285" t="s">
-        <v>209</v>
+        <v>539</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>210</v>
+        <v>638</v>
       </c>
       <c r="B286" t="s">
-        <v>211</v>
+        <v>640</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>212</v>
+        <v>639</v>
       </c>
       <c r="B287" t="s">
-        <v>213</v>
+        <v>641</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>214</v>
+        <v>647</v>
       </c>
       <c r="B288" t="s">
-        <v>215</v>
+        <v>648</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>216</v>
+        <v>702</v>
       </c>
       <c r="B289" t="s">
-        <v>163</v>
+        <v>704</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>217</v>
+        <v>703</v>
       </c>
       <c r="B290" t="s">
-        <v>165</v>
+        <v>705</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>218</v>
+        <v>759</v>
       </c>
       <c r="B291" t="s">
-        <v>167</v>
+        <v>762</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="B292" t="s">
-        <v>169</v>
+        <v>204</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="B293" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B294" t="s">
-        <v>173</v>
+        <v>208</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="B295" t="s">
-        <v>175</v>
+        <v>210</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="B296" t="s">
-        <v>177</v>
+        <v>212</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="B297" t="s">
-        <v>179</v>
+        <v>214</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B298" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="B299" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B300" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>402</v>
+        <v>218</v>
       </c>
       <c r="B301" t="s">
-        <v>404</v>
+        <v>168</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>407</v>
+        <v>219</v>
       </c>
       <c r="B302" t="s">
-        <v>405</v>
+        <v>170</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>410</v>
+        <v>220</v>
       </c>
       <c r="B303" t="s">
-        <v>406</v>
+        <v>172</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>631</v>
+        <v>221</v>
       </c>
       <c r="B304" t="s">
-        <v>632</v>
+        <v>174</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>633</v>
+        <v>222</v>
       </c>
       <c r="B305" t="s">
-        <v>634</v>
+        <v>176</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>658</v>
+        <v>223</v>
       </c>
       <c r="B306" t="s">
-        <v>661</v>
+        <v>178</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>662</v>
+        <v>224</v>
       </c>
       <c r="B307" t="s">
-        <v>664</v>
+        <v>180</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>663</v>
+        <v>225</v>
       </c>
       <c r="B308" t="s">
-        <v>669</v>
+        <v>182</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>434</v>
+        <v>226</v>
       </c>
       <c r="B309" t="s">
-        <v>440</v>
+        <v>184</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>436</v>
+        <v>401</v>
       </c>
       <c r="B310" t="s">
-        <v>441</v>
+        <v>403</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>438</v>
+        <v>406</v>
       </c>
       <c r="B311" t="s">
-        <v>442</v>
+        <v>404</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B312" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>421</v>
+        <v>630</v>
       </c>
       <c r="B313" t="s">
-        <v>418</v>
+        <v>631</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>423</v>
+        <v>632</v>
       </c>
       <c r="B314" t="s">
-        <v>419</v>
+        <v>633</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>228</v>
+        <v>657</v>
       </c>
       <c r="B315" t="s">
-        <v>229</v>
+        <v>660</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>230</v>
+        <v>661</v>
       </c>
       <c r="B316" t="s">
-        <v>231</v>
+        <v>663</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>745</v>
+        <v>662</v>
       </c>
       <c r="B317" t="s">
-        <v>739</v>
+        <v>668</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>746</v>
+        <v>433</v>
       </c>
       <c r="B318" t="s">
-        <v>738</v>
+        <v>439</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>556</v>
+        <v>435</v>
       </c>
       <c r="B319" t="s">
-        <v>558</v>
+        <v>440</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>742</v>
+        <v>437</v>
       </c>
       <c r="B320" t="s">
-        <v>732</v>
+        <v>441</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>740</v>
+        <v>758</v>
       </c>
       <c r="B321" t="s">
-        <v>733</v>
+        <v>691</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>741</v>
+        <v>413</v>
       </c>
       <c r="B322" t="s">
-        <v>734</v>
+        <v>414</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="B323" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B324" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>431</v>
+        <v>227</v>
       </c>
       <c r="B325" t="s">
-        <v>429</v>
+        <v>228</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B326" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>234</v>
+        <v>744</v>
       </c>
       <c r="B327" t="s">
-        <v>235</v>
+        <v>738</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>236</v>
+        <v>745</v>
       </c>
       <c r="B328" t="s">
-        <v>237</v>
+        <v>737</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>238</v>
+        <v>555</v>
       </c>
       <c r="B329" t="s">
-        <v>239</v>
+        <v>557</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>240</v>
+        <v>741</v>
       </c>
       <c r="B330" t="s">
-        <v>241</v>
+        <v>731</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>242</v>
+        <v>739</v>
       </c>
       <c r="B331" t="s">
-        <v>243</v>
+        <v>732</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>244</v>
+        <v>740</v>
       </c>
       <c r="B332" t="s">
-        <v>245</v>
+        <v>733</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>246</v>
+        <v>424</v>
       </c>
       <c r="B333" t="s">
-        <v>247</v>
+        <v>425</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>248</v>
+        <v>429</v>
       </c>
       <c r="B334" t="s">
-        <v>249</v>
+        <v>427</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>250</v>
+        <v>430</v>
       </c>
       <c r="B335" t="s">
-        <v>251</v>
+        <v>428</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
+        <v>231</v>
+      </c>
+      <c r="B336" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A337" t="s">
+        <v>233</v>
+      </c>
+      <c r="B337" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A338" t="s">
+        <v>235</v>
+      </c>
+      <c r="B338" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A339" t="s">
+        <v>237</v>
+      </c>
+      <c r="B339" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A340" t="s">
+        <v>239</v>
+      </c>
+      <c r="B340" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A341" t="s">
+        <v>241</v>
+      </c>
+      <c r="B341" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A342" t="s">
+        <v>243</v>
+      </c>
+      <c r="B342" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A343" t="s">
+        <v>245</v>
+      </c>
+      <c r="B343" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A344" t="s">
+        <v>247</v>
+      </c>
+      <c r="B344" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A345" t="s">
+        <v>249</v>
+      </c>
+      <c r="B345" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A346" t="s">
+        <v>251</v>
+      </c>
+      <c r="B346" t="s">
         <v>252</v>
       </c>
-      <c r="B336" t="s">
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A347" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A337" t="s">
+      <c r="B347" t="s">
         <v>254</v>
       </c>
-      <c r="B337" t="s">
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A348" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A338" t="s">
+      <c r="B348" t="s">
         <v>256</v>
       </c>
-      <c r="B338" t="s">
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A349" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A339" t="s">
+      <c r="B349" t="s">
         <v>258</v>
       </c>
-      <c r="B339" t="s">
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A350" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A340" t="s">
+      <c r="B350" t="s">
         <v>260</v>
       </c>
-      <c r="B340" t="s">
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A351" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A341" t="s">
+      <c r="B351" t="s">
         <v>262</v>
       </c>
-      <c r="B341" t="s">
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A352" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A342" t="s">
+      <c r="B352" t="s">
         <v>264</v>
-      </c>
-      <c r="B342" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A343" t="s">
-        <v>266</v>
-      </c>
-      <c r="B343" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A344" t="s">
-        <v>268</v>
-      </c>
-      <c r="B344" t="s">
-        <v>269</v>
-      </c>
-      <c r="C344" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A345" t="s">
-        <v>362</v>
-      </c>
-      <c r="B345" t="s">
-        <v>364</v>
-      </c>
-      <c r="C345" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A346" t="s">
-        <v>270</v>
-      </c>
-      <c r="B346" t="s">
-        <v>271</v>
-      </c>
-      <c r="C346" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A347" t="s">
-        <v>502</v>
-      </c>
-      <c r="B347" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A348" t="s">
-        <v>272</v>
-      </c>
-      <c r="B348" t="s">
-        <v>653</v>
-      </c>
-      <c r="C348" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A349" t="s">
-        <v>317</v>
-      </c>
-      <c r="B349" t="s">
-        <v>322</v>
-      </c>
-      <c r="C349" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A350" t="s">
-        <v>318</v>
-      </c>
-      <c r="B350" t="s">
-        <v>321</v>
-      </c>
-      <c r="C350" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A351" t="s">
-        <v>273</v>
-      </c>
-      <c r="B351" t="s">
-        <v>274</v>
-      </c>
-      <c r="C351" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A352" t="s">
-        <v>289</v>
-      </c>
-      <c r="B352" t="s">
-        <v>304</v>
-      </c>
-      <c r="C352" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>293</v>
+        <v>265</v>
       </c>
       <c r="B353" t="s">
-        <v>303</v>
-      </c>
-      <c r="C353" t="s">
-        <v>306</v>
+        <v>266</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B354" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C354" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>342</v>
+        <v>361</v>
       </c>
       <c r="B355" t="s">
-        <v>343</v>
+        <v>363</v>
       </c>
       <c r="C355" t="s">
-        <v>344</v>
+        <v>362</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>315</v>
+        <v>269</v>
       </c>
       <c r="B356" t="s">
-        <v>323</v>
+        <v>270</v>
       </c>
       <c r="C356" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>316</v>
+        <v>501</v>
       </c>
       <c r="B357" t="s">
-        <v>324</v>
-      </c>
-      <c r="C357" t="s">
-        <v>326</v>
+        <v>509</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>360</v>
+        <v>271</v>
       </c>
       <c r="B358" t="s">
-        <v>366</v>
+        <v>652</v>
       </c>
       <c r="C358" t="s">
-        <v>370</v>
+        <v>653</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>277</v>
+        <v>316</v>
       </c>
       <c r="B359" t="s">
-        <v>278</v>
+        <v>321</v>
       </c>
       <c r="C359" t="s">
-        <v>278</v>
+        <v>318</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>361</v>
+        <v>317</v>
       </c>
       <c r="B360" t="s">
-        <v>367</v>
+        <v>320</v>
       </c>
       <c r="C360" t="s">
-        <v>371</v>
+        <v>324</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>357</v>
+        <v>272</v>
       </c>
       <c r="B361" t="s">
-        <v>369</v>
+        <v>273</v>
       </c>
       <c r="C361" t="s">
-        <v>377</v>
+        <v>273</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="B362" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="C362" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="B363" t="s">
-        <v>282</v>
+        <v>302</v>
       </c>
       <c r="C363" t="s">
-        <v>282</v>
+        <v>305</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="B364" t="s">
-        <v>297</v>
+        <v>275</v>
       </c>
       <c r="C364" t="s">
-        <v>305</v>
+        <v>275</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>296</v>
+        <v>341</v>
       </c>
       <c r="B365" t="s">
-        <v>302</v>
+        <v>342</v>
       </c>
       <c r="C365" t="s">
-        <v>309</v>
+        <v>343</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>635</v>
+        <v>314</v>
       </c>
       <c r="B366" t="s">
-        <v>636</v>
+        <v>322</v>
+      </c>
+      <c r="C366" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>637</v>
+        <v>315</v>
       </c>
       <c r="B367" t="s">
-        <v>638</v>
+        <v>323</v>
+      </c>
+      <c r="C367" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>393</v>
+        <v>359</v>
       </c>
       <c r="B368" t="s">
-        <v>398</v>
+        <v>365</v>
       </c>
       <c r="C368" t="s">
-        <v>399</v>
+        <v>369</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>359</v>
+        <v>276</v>
       </c>
       <c r="B369" t="s">
-        <v>365</v>
+        <v>277</v>
+      </c>
+      <c r="C369" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>283</v>
+        <v>360</v>
       </c>
       <c r="B370" t="s">
-        <v>284</v>
+        <v>366</v>
       </c>
       <c r="C370" t="s">
-        <v>355</v>
+        <v>370</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>285</v>
+        <v>356</v>
       </c>
       <c r="B371" t="s">
-        <v>286</v>
+        <v>368</v>
       </c>
       <c r="C371" t="s">
-        <v>286</v>
+        <v>376</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="B372" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="C372" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="B373" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="C373" t="s">
-        <v>311</v>
+        <v>281</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B374" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="C374" t="s">
-        <v>288</v>
+        <v>304</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="B375" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C375" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>294</v>
+        <v>634</v>
       </c>
       <c r="B376" t="s">
-        <v>300</v>
-      </c>
-      <c r="C376" t="s">
-        <v>313</v>
+        <v>635</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
+        <v>636</v>
+      </c>
+      <c r="B377" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A378" t="s">
+        <v>392</v>
+      </c>
+      <c r="B378" t="s">
+        <v>397</v>
+      </c>
+      <c r="C378" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A379" t="s">
         <v>358</v>
       </c>
-      <c r="B377" t="s">
-        <v>368</v>
-      </c>
-      <c r="C377" t="s">
-        <v>376</v>
+      <c r="B379" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A380" t="s">
+        <v>282</v>
+      </c>
+      <c r="B380" t="s">
+        <v>283</v>
+      </c>
+      <c r="C380" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A381" t="s">
+        <v>284</v>
+      </c>
+      <c r="B381" t="s">
+        <v>285</v>
+      </c>
+      <c r="C381" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A382" t="s">
+        <v>290</v>
+      </c>
+      <c r="B382" t="s">
+        <v>297</v>
+      </c>
+      <c r="C382" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A383" t="s">
+        <v>294</v>
+      </c>
+      <c r="B383" t="s">
+        <v>300</v>
+      </c>
+      <c r="C383" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A384" t="s">
+        <v>286</v>
+      </c>
+      <c r="B384" t="s">
+        <v>287</v>
+      </c>
+      <c r="C384" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A385" t="s">
+        <v>289</v>
+      </c>
+      <c r="B385" t="s">
+        <v>298</v>
+      </c>
+      <c r="C385" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A386" t="s">
+        <v>293</v>
+      </c>
+      <c r="B386" t="s">
+        <v>299</v>
+      </c>
+      <c r="C386" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A387" t="s">
+        <v>357</v>
+      </c>
+      <c r="B387" t="s">
+        <v>367</v>
+      </c>
+      <c r="C387" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K357">
-    <sortState ref="A2:K377">
+    <sortState ref="A2:K387">
       <sortCondition ref="A1:A357"/>
     </sortState>
   </autoFilter>
@@ -6292,92 +6429,92 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B1" t="s">
         <v>384</v>
       </c>
-      <c r="B1" t="s">
-        <v>385</v>
-      </c>
       <c r="C1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C9" t="s">
         <v>398</v>
-      </c>
-      <c r="C9" t="s">
-        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some tower research splitting
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28790" windowHeight="12410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="rebalance_localizations" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="780">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -2251,18 +2251,6 @@
     <t>gui/menu/research/name/towers_rocket</t>
   </si>
   <si>
-    <t>gui/menu/research/description/towers_artillery_acid</t>
-  </si>
-  <si>
-    <t>gui/menu/research/description/towers_artillery_napalm</t>
-  </si>
-  <si>
-    <t>gui/menu/research/name/towers_artillery_acid</t>
-  </si>
-  <si>
-    <t>gui/menu/research/name/towers_artillery_napalm</t>
-  </si>
-  <si>
     <t>gui/menu/research/description/towers_rocket</t>
   </si>
   <si>
@@ -2324,6 +2312,57 @@
   </si>
   <si>
     <t>Optimized Bioreactors offer best flammable gases yield</t>
+  </si>
+  <si>
+    <t>Defense platform utilizing surrounding liquids for cooling</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/tower_water_minigun</t>
+  </si>
+  <si>
+    <t>Enviormental Cooled Defense Platforms</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/tower_water_minigun</t>
+  </si>
+  <si>
+    <t>Cannon utilizing acidic rounds</t>
+  </si>
+  <si>
+    <t>Canon using indicidary rounds</t>
+  </si>
+  <si>
+    <t>Canon using cryo rounds</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/tower_artillery_acid</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/tower_artillery_napalm</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/tower_cannon_acid</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/tower_cannon_cryo</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/tower_cannon_incindiary</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/tower_artillery_acid</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/tower_artillery_napalm</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/tower_cannon_acid</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/tower_cannon_cryo</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/tower_cannon_incindiary</t>
   </si>
 </sst>
 </file>
@@ -3148,20 +3187,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K387"/>
+  <dimension ref="A1:K395"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A356" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E384" sqref="E384"/>
+      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C325" sqref="C325"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.1796875" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3193,7 +3232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3201,7 +3240,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3209,7 +3248,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3217,7 +3256,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -3225,7 +3264,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>447</v>
       </c>
@@ -3233,7 +3272,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3241,7 +3280,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -3249,7 +3288,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -3257,7 +3296,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>589</v>
       </c>
@@ -3265,7 +3304,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -3273,7 +3312,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3281,7 +3320,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -3289,7 +3328,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>448</v>
       </c>
@@ -3297,7 +3336,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -3305,7 +3344,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3313,7 +3352,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -3321,7 +3360,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3329,7 +3368,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -3337,7 +3376,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -3345,7 +3384,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -3353,7 +3392,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -3361,7 +3400,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -3369,7 +3408,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -3377,7 +3416,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>502</v>
       </c>
@@ -3385,7 +3424,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>650</v>
       </c>
@@ -3393,7 +3432,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>503</v>
       </c>
@@ -3401,15 +3440,15 @@
         <v>532</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>380</v>
       </c>
@@ -3417,7 +3456,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>461</v>
       </c>
@@ -3425,7 +3464,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>344</v>
       </c>
@@ -3436,7 +3475,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>670</v>
       </c>
@@ -3444,7 +3483,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -3452,7 +3491,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -3460,7 +3499,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -3468,7 +3507,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>377</v>
       </c>
@@ -3479,7 +3518,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>326</v>
       </c>
@@ -3487,7 +3526,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>335</v>
       </c>
@@ -3495,7 +3534,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>336</v>
       </c>
@@ -3503,7 +3542,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -3511,7 +3550,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -3519,7 +3558,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>59</v>
       </c>
@@ -3527,7 +3566,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -3535,7 +3574,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>62</v>
       </c>
@@ -3543,7 +3582,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -3551,7 +3590,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>621</v>
       </c>
@@ -3559,7 +3598,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>623</v>
       </c>
@@ -3567,7 +3606,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>658</v>
       </c>
@@ -3575,7 +3614,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>666</v>
       </c>
@@ -3583,7 +3622,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>667</v>
       </c>
@@ -3591,7 +3630,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>383</v>
       </c>
@@ -3602,7 +3641,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>385</v>
       </c>
@@ -3610,7 +3649,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>386</v>
       </c>
@@ -3618,7 +3657,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>387</v>
       </c>
@@ -3626,7 +3665,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>688</v>
       </c>
@@ -3634,7 +3673,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>689</v>
       </c>
@@ -3642,7 +3681,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>685</v>
       </c>
@@ -3650,7 +3689,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>347</v>
       </c>
@@ -3661,7 +3700,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -3669,7 +3708,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -3677,7 +3716,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -3685,7 +3724,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -3693,7 +3732,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>713</v>
       </c>
@@ -3701,7 +3740,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>712</v>
       </c>
@@ -3709,7 +3748,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>711</v>
       </c>
@@ -3717,7 +3756,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -3725,7 +3764,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -3733,7 +3772,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>481</v>
       </c>
@@ -3741,7 +3780,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>482</v>
       </c>
@@ -3749,7 +3788,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>489</v>
       </c>
@@ -3757,7 +3796,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>490</v>
       </c>
@@ -3765,7 +3804,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -3773,7 +3812,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>454</v>
       </c>
@@ -3781,7 +3820,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>453</v>
       </c>
@@ -3789,7 +3828,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>455</v>
       </c>
@@ -3797,7 +3836,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>459</v>
       </c>
@@ -3805,7 +3844,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>553</v>
       </c>
@@ -3813,7 +3852,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>487</v>
       </c>
@@ -3821,7 +3860,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>488</v>
       </c>
@@ -3829,7 +3868,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>483</v>
       </c>
@@ -3837,7 +3876,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>485</v>
       </c>
@@ -3845,7 +3884,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>486</v>
       </c>
@@ -3853,7 +3892,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>484</v>
       </c>
@@ -3861,7 +3900,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>493</v>
       </c>
@@ -3869,7 +3908,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>494</v>
       </c>
@@ -3877,7 +3916,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>495</v>
       </c>
@@ -3885,7 +3924,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>496</v>
       </c>
@@ -3893,7 +3932,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>498</v>
       </c>
@@ -3901,7 +3940,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>497</v>
       </c>
@@ -3909,7 +3948,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>491</v>
       </c>
@@ -3917,7 +3956,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>492</v>
       </c>
@@ -3925,7 +3964,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>544</v>
       </c>
@@ -3933,7 +3972,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>545</v>
       </c>
@@ -3941,7 +3980,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>543</v>
       </c>
@@ -3949,7 +3988,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>76</v>
       </c>
@@ -3957,7 +3996,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>78</v>
       </c>
@@ -3965,7 +4004,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>80</v>
       </c>
@@ -3973,7 +4012,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>82</v>
       </c>
@@ -3981,7 +4020,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>84</v>
       </c>
@@ -3989,7 +4028,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>445</v>
       </c>
@@ -3997,7 +4036,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>86</v>
       </c>
@@ -4005,7 +4044,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>88</v>
       </c>
@@ -4013,7 +4052,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>90</v>
       </c>
@@ -4021,7 +4060,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>590</v>
       </c>
@@ -4029,7 +4068,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>91</v>
       </c>
@@ -4037,7 +4076,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>93</v>
       </c>
@@ -4045,7 +4084,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>95</v>
       </c>
@@ -4053,7 +4092,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>446</v>
       </c>
@@ -4061,7 +4100,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>97</v>
       </c>
@@ -4069,7 +4108,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>99</v>
       </c>
@@ -4077,7 +4116,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>101</v>
       </c>
@@ -4085,7 +4124,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>103</v>
       </c>
@@ -4093,7 +4132,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>105</v>
       </c>
@@ -4101,7 +4140,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>107</v>
       </c>
@@ -4109,7 +4148,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>109</v>
       </c>
@@ -4117,7 +4156,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>111</v>
       </c>
@@ -4125,7 +4164,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>113</v>
       </c>
@@ -4133,7 +4172,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>115</v>
       </c>
@@ -4141,7 +4180,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>499</v>
       </c>
@@ -4149,7 +4188,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>645</v>
       </c>
@@ -4157,7 +4196,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>500</v>
       </c>
@@ -4165,7 +4204,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>117</v>
       </c>
@@ -4173,7 +4212,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>379</v>
       </c>
@@ -4181,7 +4220,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>462</v>
       </c>
@@ -4189,7 +4228,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>345</v>
       </c>
@@ -4200,7 +4239,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>348</v>
       </c>
@@ -4211,7 +4250,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>349</v>
       </c>
@@ -4222,7 +4261,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>656</v>
       </c>
@@ -4230,7 +4269,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>119</v>
       </c>
@@ -4238,7 +4277,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>378</v>
       </c>
@@ -4249,7 +4288,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>327</v>
       </c>
@@ -4257,7 +4296,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>328</v>
       </c>
@@ -4265,7 +4304,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>329</v>
       </c>
@@ -4273,7 +4312,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>121</v>
       </c>
@@ -4281,7 +4320,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>123</v>
       </c>
@@ -4289,7 +4328,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>125</v>
       </c>
@@ -4297,7 +4336,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>127</v>
       </c>
@@ -4305,7 +4344,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>625</v>
       </c>
@@ -4313,7 +4352,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>388</v>
       </c>
@@ -4324,7 +4363,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>389</v>
       </c>
@@ -4335,7 +4374,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>390</v>
       </c>
@@ -4346,7 +4385,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>391</v>
       </c>
@@ -4357,7 +4396,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>686</v>
       </c>
@@ -4365,7 +4404,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>687</v>
       </c>
@@ -4373,7 +4412,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>684</v>
       </c>
@@ -4381,7 +4420,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>129</v>
       </c>
@@ -4389,7 +4428,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>131</v>
       </c>
@@ -4397,7 +4436,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>331</v>
       </c>
@@ -4405,7 +4444,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>330</v>
       </c>
@@ -4413,7 +4452,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>699</v>
       </c>
@@ -4421,7 +4460,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>696</v>
       </c>
@@ -4429,7 +4468,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>697</v>
       </c>
@@ -4437,7 +4476,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>463</v>
       </c>
@@ -4445,7 +4484,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>464</v>
       </c>
@@ -4453,7 +4492,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>471</v>
       </c>
@@ -4461,7 +4500,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>472</v>
       </c>
@@ -4469,7 +4508,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>133</v>
       </c>
@@ -4477,7 +4516,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>457</v>
       </c>
@@ -4485,7 +4524,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>456</v>
       </c>
@@ -4493,7 +4532,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>458</v>
       </c>
@@ -4501,7 +4540,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>460</v>
       </c>
@@ -4509,7 +4548,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>550</v>
       </c>
@@ -4517,7 +4556,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>469</v>
       </c>
@@ -4525,7 +4564,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>470</v>
       </c>
@@ -4533,7 +4572,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>466</v>
       </c>
@@ -4541,7 +4580,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>467</v>
       </c>
@@ -4549,7 +4588,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>468</v>
       </c>
@@ -4557,7 +4596,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>465</v>
       </c>
@@ -4565,7 +4604,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>475</v>
       </c>
@@ -4573,7 +4612,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>476</v>
       </c>
@@ -4581,7 +4620,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>477</v>
       </c>
@@ -4589,7 +4628,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>478</v>
       </c>
@@ -4597,7 +4636,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>480</v>
       </c>
@@ -4605,7 +4644,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>479</v>
       </c>
@@ -4613,7 +4652,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>473</v>
       </c>
@@ -4621,7 +4660,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>474</v>
       </c>
@@ -4629,7 +4668,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>540</v>
       </c>
@@ -4637,7 +4676,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>542</v>
       </c>
@@ -4645,7 +4684,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>541</v>
       </c>
@@ -4653,7 +4692,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>135</v>
       </c>
@@ -4661,7 +4700,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>546</v>
       </c>
@@ -4669,7 +4708,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>534</v>
       </c>
@@ -4677,7 +4716,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>569</v>
       </c>
@@ -4685,7 +4724,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>570</v>
       </c>
@@ -4693,7 +4732,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>726</v>
       </c>
@@ -4701,7 +4740,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>571</v>
       </c>
@@ -4709,7 +4748,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>572</v>
       </c>
@@ -4717,7 +4756,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>727</v>
       </c>
@@ -4725,7 +4764,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>573</v>
       </c>
@@ -4733,7 +4772,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>574</v>
       </c>
@@ -4741,7 +4780,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>728</v>
       </c>
@@ -4749,7 +4788,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>575</v>
       </c>
@@ -4757,7 +4796,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>576</v>
       </c>
@@ -4765,7 +4804,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>729</v>
       </c>
@@ -4773,7 +4812,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>143</v>
       </c>
@@ -4781,7 +4820,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>144</v>
       </c>
@@ -4789,7 +4828,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>672</v>
       </c>
@@ -4797,7 +4836,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>676</v>
       </c>
@@ -4805,7 +4844,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>677</v>
       </c>
@@ -4813,7 +4852,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="14.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>145</v>
       </c>
@@ -4821,7 +4860,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>147</v>
       </c>
@@ -4829,7 +4868,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>536</v>
       </c>
@@ -4837,7 +4876,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>642</v>
       </c>
@@ -4845,7 +4884,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>643</v>
       </c>
@@ -4853,7 +4892,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>649</v>
       </c>
@@ -4861,7 +4900,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>706</v>
       </c>
@@ -4869,7 +4908,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>707</v>
       </c>
@@ -4877,7 +4916,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>149</v>
       </c>
@@ -4885,7 +4924,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>151</v>
       </c>
@@ -4893,7 +4932,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>153</v>
       </c>
@@ -4901,7 +4940,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>155</v>
       </c>
@@ -4909,7 +4948,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>157</v>
       </c>
@@ -4917,7 +4956,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>159</v>
       </c>
@@ -4925,7 +4964,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>161</v>
       </c>
@@ -4933,7 +4972,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>163</v>
       </c>
@@ -4941,7 +4980,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>165</v>
       </c>
@@ -4949,7 +4988,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>167</v>
       </c>
@@ -4957,7 +4996,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>169</v>
       </c>
@@ -4965,7 +5004,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>171</v>
       </c>
@@ -4973,7 +5012,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>173</v>
       </c>
@@ -4981,7 +5020,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>175</v>
       </c>
@@ -4989,7 +5028,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>177</v>
       </c>
@@ -4997,7 +5036,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>179</v>
       </c>
@@ -5005,7 +5044,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>181</v>
       </c>
@@ -5013,7 +5052,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>183</v>
       </c>
@@ -5021,7 +5060,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>402</v>
       </c>
@@ -5029,7 +5068,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>407</v>
       </c>
@@ -5037,7 +5076,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>408</v>
       </c>
@@ -5045,7 +5084,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>627</v>
       </c>
@@ -5053,7 +5092,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>629</v>
       </c>
@@ -5061,7 +5100,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>434</v>
       </c>
@@ -5069,7 +5108,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>436</v>
       </c>
@@ -5077,7 +5116,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>438</v>
       </c>
@@ -5085,7 +5124,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>412</v>
       </c>
@@ -5093,7 +5132,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>419</v>
       </c>
@@ -5101,7 +5140,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>421</v>
       </c>
@@ -5109,7 +5148,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>185</v>
       </c>
@@ -5117,7 +5156,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>187</v>
       </c>
@@ -5125,7 +5164,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>556</v>
       </c>
@@ -5133,7 +5172,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>423</v>
       </c>
@@ -5141,7 +5180,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>431</v>
       </c>
@@ -5149,7 +5188,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>577</v>
       </c>
@@ -5157,7 +5196,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>578</v>
       </c>
@@ -5165,7 +5204,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>730</v>
       </c>
@@ -5173,7 +5212,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>137</v>
       </c>
@@ -5181,7 +5220,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>139</v>
       </c>
@@ -5189,7 +5228,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>141</v>
       </c>
@@ -5197,1219 +5236,1283 @@
         <v>142</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
+        <v>750</v>
+      </c>
+      <c r="B248" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>751</v>
+      </c>
+      <c r="B249" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>752</v>
+      </c>
+      <c r="B250" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>757</v>
+      </c>
+      <c r="B251" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>756</v>
+      </c>
+      <c r="B252" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>764</v>
+      </c>
+      <c r="B253" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>770</v>
+      </c>
+      <c r="B254" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>771</v>
+      </c>
+      <c r="B255" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>772</v>
+      </c>
+      <c r="B256" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>773</v>
+      </c>
+      <c r="B257" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>774</v>
+      </c>
+      <c r="B258" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>742</v>
+      </c>
+      <c r="B259" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>431</v>
+      </c>
+      <c r="B260" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>559</v>
+      </c>
+      <c r="B261" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>560</v>
+      </c>
+      <c r="B262" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>720</v>
+      </c>
+      <c r="B263" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>561</v>
+      </c>
+      <c r="B264" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>562</v>
+      </c>
+      <c r="B265" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>719</v>
+      </c>
+      <c r="B266" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>563</v>
+      </c>
+      <c r="B267" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>564</v>
+      </c>
+      <c r="B268" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>718</v>
+      </c>
+      <c r="B269" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>565</v>
+      </c>
+      <c r="B270" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>566</v>
+      </c>
+      <c r="B271" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>717</v>
+      </c>
+      <c r="B272" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>567</v>
+      </c>
+      <c r="B273" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>568</v>
+      </c>
+      <c r="B274" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>716</v>
+      </c>
+      <c r="B275" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>189</v>
+      </c>
+      <c r="B276" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>191</v>
+      </c>
+      <c r="B277" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>193</v>
+      </c>
+      <c r="B278" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>195</v>
+      </c>
+      <c r="B279" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>197</v>
+      </c>
+      <c r="B280" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>673</v>
+      </c>
+      <c r="B281" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>674</v>
+      </c>
+      <c r="B282" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>675</v>
+      </c>
+      <c r="B283" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>199</v>
+      </c>
+      <c r="B284" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>201</v>
+      </c>
+      <c r="B285" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>744</v>
+      </c>
+      <c r="B286" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>745</v>
+      </c>
+      <c r="B287" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>746</v>
+      </c>
+      <c r="B288" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>538</v>
+      </c>
+      <c r="B289" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>638</v>
+      </c>
+      <c r="B290" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>639</v>
+      </c>
+      <c r="B291" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>647</v>
+      </c>
+      <c r="B292" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>702</v>
+      </c>
+      <c r="B293" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>703</v>
+      </c>
+      <c r="B294" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>755</v>
+      </c>
+      <c r="B295" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>203</v>
+      </c>
+      <c r="B296" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>205</v>
+      </c>
+      <c r="B297" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>207</v>
+      </c>
+      <c r="B298" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>209</v>
+      </c>
+      <c r="B299" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>211</v>
+      </c>
+      <c r="B300" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>213</v>
+      </c>
+      <c r="B301" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>215</v>
+      </c>
+      <c r="B302" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>216</v>
+      </c>
+      <c r="B303" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>217</v>
+      </c>
+      <c r="B304" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>218</v>
+      </c>
+      <c r="B305" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>219</v>
+      </c>
+      <c r="B306" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>220</v>
+      </c>
+      <c r="B307" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>221</v>
+      </c>
+      <c r="B308" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>222</v>
+      </c>
+      <c r="B309" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>223</v>
+      </c>
+      <c r="B310" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>224</v>
+      </c>
+      <c r="B311" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>225</v>
+      </c>
+      <c r="B312" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>226</v>
+      </c>
+      <c r="B313" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>401</v>
+      </c>
+      <c r="B314" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>406</v>
+      </c>
+      <c r="B315" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>409</v>
+      </c>
+      <c r="B316" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>630</v>
+      </c>
+      <c r="B317" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>632</v>
+      </c>
+      <c r="B318" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>657</v>
+      </c>
+      <c r="B319" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>661</v>
+      </c>
+      <c r="B320" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>662</v>
+      </c>
+      <c r="B321" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>433</v>
+      </c>
+      <c r="B322" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>435</v>
+      </c>
+      <c r="B323" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>437</v>
+      </c>
+      <c r="B324" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
         <v>754</v>
       </c>
-      <c r="B248" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A249" t="s">
-        <v>755</v>
-      </c>
-      <c r="B249" t="s">
+      <c r="B325" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>413</v>
+      </c>
+      <c r="B326" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>420</v>
+      </c>
+      <c r="B327" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>422</v>
+      </c>
+      <c r="B328" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>227</v>
+      </c>
+      <c r="B329" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>229</v>
+      </c>
+      <c r="B330" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>766</v>
+      </c>
+      <c r="B331" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A250" t="s">
-        <v>756</v>
-      </c>
-      <c r="B250" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A251" t="s">
-        <v>761</v>
-      </c>
-      <c r="B251" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A252" t="s">
-        <v>760</v>
-      </c>
-      <c r="B252" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A253" t="s">
-        <v>742</v>
-      </c>
-      <c r="B253" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A254" t="s">
-        <v>743</v>
-      </c>
-      <c r="B254" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A255" t="s">
-        <v>746</v>
-      </c>
-      <c r="B255" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A256" t="s">
-        <v>431</v>
-      </c>
-      <c r="B256" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A257" t="s">
-        <v>559</v>
-      </c>
-      <c r="B257" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A258" t="s">
-        <v>560</v>
-      </c>
-      <c r="B258" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A259" t="s">
-        <v>720</v>
-      </c>
-      <c r="B259" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A260" t="s">
-        <v>561</v>
-      </c>
-      <c r="B260" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A261" t="s">
-        <v>562</v>
-      </c>
-      <c r="B261" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A262" t="s">
-        <v>719</v>
-      </c>
-      <c r="B262" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A263" t="s">
-        <v>563</v>
-      </c>
-      <c r="B263" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A264" t="s">
-        <v>564</v>
-      </c>
-      <c r="B264" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A265" t="s">
-        <v>718</v>
-      </c>
-      <c r="B265" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A266" t="s">
-        <v>565</v>
-      </c>
-      <c r="B266" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A267" t="s">
-        <v>566</v>
-      </c>
-      <c r="B267" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A268" t="s">
-        <v>717</v>
-      </c>
-      <c r="B268" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A269" t="s">
-        <v>567</v>
-      </c>
-      <c r="B269" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A270" t="s">
-        <v>568</v>
-      </c>
-      <c r="B270" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A271" t="s">
-        <v>716</v>
-      </c>
-      <c r="B271" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A272" t="s">
-        <v>189</v>
-      </c>
-      <c r="B272" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A273" t="s">
-        <v>191</v>
-      </c>
-      <c r="B273" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A274" t="s">
-        <v>193</v>
-      </c>
-      <c r="B274" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A275" t="s">
-        <v>195</v>
-      </c>
-      <c r="B275" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A276" t="s">
-        <v>197</v>
-      </c>
-      <c r="B276" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A277" t="s">
-        <v>673</v>
-      </c>
-      <c r="B277" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A278" t="s">
-        <v>674</v>
-      </c>
-      <c r="B278" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A279" t="s">
-        <v>675</v>
-      </c>
-      <c r="B279" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A280" t="s">
-        <v>199</v>
-      </c>
-      <c r="B280" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A281" t="s">
-        <v>201</v>
-      </c>
-      <c r="B281" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A282" t="s">
-        <v>748</v>
-      </c>
-      <c r="B282" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A283" t="s">
-        <v>749</v>
-      </c>
-      <c r="B283" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A284" t="s">
-        <v>750</v>
-      </c>
-      <c r="B284" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A285" t="s">
-        <v>538</v>
-      </c>
-      <c r="B285" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A286" t="s">
-        <v>638</v>
-      </c>
-      <c r="B286" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A287" t="s">
-        <v>639</v>
-      </c>
-      <c r="B287" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A288" t="s">
-        <v>647</v>
-      </c>
-      <c r="B288" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A289" t="s">
-        <v>702</v>
-      </c>
-      <c r="B289" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A290" t="s">
-        <v>703</v>
-      </c>
-      <c r="B290" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A291" t="s">
-        <v>759</v>
-      </c>
-      <c r="B291" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A292" t="s">
-        <v>203</v>
-      </c>
-      <c r="B292" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A293" t="s">
-        <v>205</v>
-      </c>
-      <c r="B293" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A294" t="s">
-        <v>207</v>
-      </c>
-      <c r="B294" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A295" t="s">
-        <v>209</v>
-      </c>
-      <c r="B295" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A296" t="s">
-        <v>211</v>
-      </c>
-      <c r="B296" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A297" t="s">
-        <v>213</v>
-      </c>
-      <c r="B297" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A298" t="s">
-        <v>215</v>
-      </c>
-      <c r="B298" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A299" t="s">
-        <v>216</v>
-      </c>
-      <c r="B299" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A300" t="s">
-        <v>217</v>
-      </c>
-      <c r="B300" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A301" t="s">
-        <v>218</v>
-      </c>
-      <c r="B301" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A302" t="s">
-        <v>219</v>
-      </c>
-      <c r="B302" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A303" t="s">
-        <v>220</v>
-      </c>
-      <c r="B303" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A304" t="s">
-        <v>221</v>
-      </c>
-      <c r="B304" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A305" t="s">
-        <v>222</v>
-      </c>
-      <c r="B305" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A306" t="s">
-        <v>223</v>
-      </c>
-      <c r="B306" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A307" t="s">
-        <v>224</v>
-      </c>
-      <c r="B307" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A308" t="s">
-        <v>225</v>
-      </c>
-      <c r="B308" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A309" t="s">
-        <v>226</v>
-      </c>
-      <c r="B309" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A310" t="s">
-        <v>401</v>
-      </c>
-      <c r="B310" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A311" t="s">
-        <v>406</v>
-      </c>
-      <c r="B311" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A312" t="s">
-        <v>409</v>
-      </c>
-      <c r="B312" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A313" t="s">
-        <v>630</v>
-      </c>
-      <c r="B313" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A314" t="s">
-        <v>632</v>
-      </c>
-      <c r="B314" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A315" t="s">
-        <v>657</v>
-      </c>
-      <c r="B315" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A316" t="s">
-        <v>661</v>
-      </c>
-      <c r="B316" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A317" t="s">
-        <v>662</v>
-      </c>
-      <c r="B317" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A318" t="s">
-        <v>433</v>
-      </c>
-      <c r="B318" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A319" t="s">
-        <v>435</v>
-      </c>
-      <c r="B319" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A320" t="s">
-        <v>437</v>
-      </c>
-      <c r="B320" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A321" t="s">
-        <v>758</v>
-      </c>
-      <c r="B321" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A322" t="s">
-        <v>413</v>
-      </c>
-      <c r="B322" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A323" t="s">
-        <v>420</v>
-      </c>
-      <c r="B323" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A324" t="s">
-        <v>422</v>
-      </c>
-      <c r="B324" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A325" t="s">
-        <v>227</v>
-      </c>
-      <c r="B325" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A326" t="s">
-        <v>229</v>
-      </c>
-      <c r="B326" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A327" t="s">
-        <v>744</v>
-      </c>
-      <c r="B327" t="s">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>775</v>
+      </c>
+      <c r="B332" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A328" t="s">
-        <v>745</v>
-      </c>
-      <c r="B328" t="s">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>776</v>
+      </c>
+      <c r="B333" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A329" t="s">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>777</v>
+      </c>
+      <c r="B334" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>778</v>
+      </c>
+      <c r="B335" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>779</v>
+      </c>
+      <c r="B336" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
         <v>555</v>
       </c>
-      <c r="B329" t="s">
+      <c r="B337" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A330" t="s">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
         <v>741</v>
       </c>
-      <c r="B330" t="s">
+      <c r="B338" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A331" t="s">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
         <v>739</v>
       </c>
-      <c r="B331" t="s">
+      <c r="B339" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A332" t="s">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
         <v>740</v>
       </c>
-      <c r="B332" t="s">
+      <c r="B340" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A333" t="s">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
         <v>424</v>
       </c>
-      <c r="B333" t="s">
+      <c r="B341" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A334" t="s">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
         <v>429</v>
       </c>
-      <c r="B334" t="s">
+      <c r="B342" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A335" t="s">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
         <v>430</v>
       </c>
-      <c r="B335" t="s">
+      <c r="B343" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A336" t="s">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
         <v>231</v>
       </c>
-      <c r="B336" t="s">
+      <c r="B344" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A337" t="s">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
         <v>233</v>
       </c>
-      <c r="B337" t="s">
+      <c r="B345" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A338" t="s">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
         <v>235</v>
       </c>
-      <c r="B338" t="s">
+      <c r="B346" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A339" t="s">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
         <v>237</v>
       </c>
-      <c r="B339" t="s">
+      <c r="B347" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A340" t="s">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
         <v>239</v>
       </c>
-      <c r="B340" t="s">
+      <c r="B348" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A341" t="s">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
         <v>241</v>
       </c>
-      <c r="B341" t="s">
+      <c r="B349" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A342" t="s">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
         <v>243</v>
       </c>
-      <c r="B342" t="s">
+      <c r="B350" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A343" t="s">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
         <v>245</v>
       </c>
-      <c r="B343" t="s">
+      <c r="B351" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A344" t="s">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
         <v>247</v>
       </c>
-      <c r="B344" t="s">
+      <c r="B352" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A345" t="s">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
         <v>249</v>
       </c>
-      <c r="B345" t="s">
+      <c r="B353" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A346" t="s">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
         <v>251</v>
       </c>
-      <c r="B346" t="s">
+      <c r="B354" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A347" t="s">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
         <v>253</v>
       </c>
-      <c r="B347" t="s">
+      <c r="B355" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A348" t="s">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
         <v>255</v>
       </c>
-      <c r="B348" t="s">
+      <c r="B356" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A349" t="s">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
         <v>257</v>
       </c>
-      <c r="B349" t="s">
+      <c r="B357" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A350" t="s">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
         <v>259</v>
       </c>
-      <c r="B350" t="s">
+      <c r="B358" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A351" t="s">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
         <v>261</v>
       </c>
-      <c r="B351" t="s">
+      <c r="B359" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A352" t="s">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
         <v>263</v>
       </c>
-      <c r="B352" t="s">
+      <c r="B360" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A353" t="s">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
         <v>265</v>
       </c>
-      <c r="B353" t="s">
+      <c r="B361" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A354" t="s">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
         <v>267</v>
       </c>
-      <c r="B354" t="s">
+      <c r="B362" t="s">
         <v>268</v>
       </c>
-      <c r="C354" t="s">
+      <c r="C362" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A355" t="s">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
         <v>361</v>
       </c>
-      <c r="B355" t="s">
+      <c r="B363" t="s">
         <v>363</v>
       </c>
-      <c r="C355" t="s">
+      <c r="C363" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A356" t="s">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
         <v>269</v>
       </c>
-      <c r="B356" t="s">
+      <c r="B364" t="s">
         <v>270</v>
       </c>
-      <c r="C356" t="s">
+      <c r="C364" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A357" t="s">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
         <v>501</v>
       </c>
-      <c r="B357" t="s">
+      <c r="B365" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A358" t="s">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
         <v>271</v>
       </c>
-      <c r="B358" t="s">
+      <c r="B366" t="s">
         <v>652</v>
       </c>
-      <c r="C358" t="s">
+      <c r="C366" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A359" t="s">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
         <v>316</v>
       </c>
-      <c r="B359" t="s">
+      <c r="B367" t="s">
         <v>321</v>
       </c>
-      <c r="C359" t="s">
+      <c r="C367" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A360" t="s">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
         <v>317</v>
       </c>
-      <c r="B360" t="s">
+      <c r="B368" t="s">
         <v>320</v>
       </c>
-      <c r="C360" t="s">
+      <c r="C368" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A361" t="s">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
         <v>272</v>
       </c>
-      <c r="B361" t="s">
+      <c r="B369" t="s">
         <v>273</v>
       </c>
-      <c r="C361" t="s">
+      <c r="C369" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A362" t="s">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
         <v>288</v>
       </c>
-      <c r="B362" t="s">
+      <c r="B370" t="s">
         <v>303</v>
       </c>
-      <c r="C362" t="s">
+      <c r="C370" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A363" t="s">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
         <v>292</v>
       </c>
-      <c r="B363" t="s">
+      <c r="B371" t="s">
         <v>302</v>
       </c>
-      <c r="C363" t="s">
+      <c r="C371" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A364" t="s">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
         <v>274</v>
       </c>
-      <c r="B364" t="s">
+      <c r="B372" t="s">
         <v>275</v>
       </c>
-      <c r="C364" t="s">
+      <c r="C372" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A365" t="s">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
         <v>341</v>
       </c>
-      <c r="B365" t="s">
+      <c r="B373" t="s">
         <v>342</v>
       </c>
-      <c r="C365" t="s">
+      <c r="C373" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A366" t="s">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
         <v>314</v>
       </c>
-      <c r="B366" t="s">
+      <c r="B374" t="s">
         <v>322</v>
       </c>
-      <c r="C366" t="s">
+      <c r="C374" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A367" t="s">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
         <v>315</v>
       </c>
-      <c r="B367" t="s">
+      <c r="B375" t="s">
         <v>323</v>
       </c>
-      <c r="C367" t="s">
+      <c r="C375" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A368" t="s">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
         <v>359</v>
       </c>
-      <c r="B368" t="s">
+      <c r="B376" t="s">
         <v>365</v>
       </c>
-      <c r="C368" t="s">
+      <c r="C376" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A369" t="s">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
         <v>276</v>
       </c>
-      <c r="B369" t="s">
+      <c r="B377" t="s">
         <v>277</v>
       </c>
-      <c r="C369" t="s">
+      <c r="C377" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A370" t="s">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
         <v>360</v>
       </c>
-      <c r="B370" t="s">
+      <c r="B378" t="s">
         <v>366</v>
       </c>
-      <c r="C370" t="s">
+      <c r="C378" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A371" t="s">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
         <v>356</v>
       </c>
-      <c r="B371" t="s">
+      <c r="B379" t="s">
         <v>368</v>
       </c>
-      <c r="C371" t="s">
+      <c r="C379" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A372" t="s">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
         <v>278</v>
       </c>
-      <c r="B372" t="s">
+      <c r="B380" t="s">
         <v>279</v>
       </c>
-      <c r="C372" t="s">
+      <c r="C380" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A373" t="s">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
         <v>280</v>
       </c>
-      <c r="B373" t="s">
+      <c r="B381" t="s">
         <v>281</v>
       </c>
-      <c r="C373" t="s">
+      <c r="C381" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A374" t="s">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
         <v>291</v>
       </c>
-      <c r="B374" t="s">
+      <c r="B382" t="s">
         <v>296</v>
       </c>
-      <c r="C374" t="s">
+      <c r="C382" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A375" t="s">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
         <v>295</v>
       </c>
-      <c r="B375" t="s">
+      <c r="B383" t="s">
         <v>301</v>
       </c>
-      <c r="C375" t="s">
+      <c r="C383" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A376" t="s">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
         <v>634</v>
       </c>
-      <c r="B376" t="s">
+      <c r="B384" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A377" t="s">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
         <v>636</v>
       </c>
-      <c r="B377" t="s">
+      <c r="B385" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A378" t="s">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
         <v>392</v>
       </c>
-      <c r="B378" t="s">
+      <c r="B386" t="s">
         <v>397</v>
       </c>
-      <c r="C378" t="s">
+      <c r="C386" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A379" t="s">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
         <v>358</v>
       </c>
-      <c r="B379" t="s">
+      <c r="B387" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A380" t="s">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
         <v>282</v>
       </c>
-      <c r="B380" t="s">
+      <c r="B388" t="s">
         <v>283</v>
       </c>
-      <c r="C380" t="s">
+      <c r="C388" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A381" t="s">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
         <v>284</v>
       </c>
-      <c r="B381" t="s">
+      <c r="B389" t="s">
         <v>285</v>
       </c>
-      <c r="C381" t="s">
+      <c r="C389" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A382" t="s">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
         <v>290</v>
       </c>
-      <c r="B382" t="s">
+      <c r="B390" t="s">
         <v>297</v>
       </c>
-      <c r="C382" t="s">
+      <c r="C390" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A383" t="s">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
         <v>294</v>
       </c>
-      <c r="B383" t="s">
+      <c r="B391" t="s">
         <v>300</v>
       </c>
-      <c r="C383" t="s">
+      <c r="C391" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A384" t="s">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
         <v>286</v>
       </c>
-      <c r="B384" t="s">
+      <c r="B392" t="s">
         <v>287</v>
       </c>
-      <c r="C384" t="s">
+      <c r="C392" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A385" t="s">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
         <v>289</v>
       </c>
-      <c r="B385" t="s">
+      <c r="B393" t="s">
         <v>298</v>
       </c>
-      <c r="C385" t="s">
+      <c r="C393" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A386" t="s">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
         <v>293</v>
       </c>
-      <c r="B386" t="s">
+      <c r="B394" t="s">
         <v>299</v>
       </c>
-      <c r="C386" t="s">
+      <c r="C394" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A387" t="s">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
         <v>357</v>
       </c>
-      <c r="B387" t="s">
+      <c r="B395" t="s">
         <v>367</v>
       </c>
-      <c r="C387" t="s">
+      <c r="C395" t="s">
         <v>375</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K357">
-    <sortState ref="A2:K387">
+    <sortState ref="A2:K395">
       <sortCondition ref="A1:A357"/>
     </sortState>
   </autoFilter>
@@ -6425,9 +6528,9 @@
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>383</v>
       </c>
@@ -6438,7 +6541,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>385</v>
       </c>
@@ -6446,7 +6549,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>386</v>
       </c>
@@ -6454,7 +6557,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>387</v>
       </c>
@@ -6462,7 +6565,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>388</v>
       </c>
@@ -6473,7 +6576,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>389</v>
       </c>
@@ -6484,7 +6587,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>390</v>
       </c>
@@ -6495,7 +6598,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>391</v>
       </c>
@@ -6506,7 +6609,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>392</v>
       </c>

</xml_diff>

<commit_message>
tech tree standard mech weapons split-up
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="12405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28790" windowHeight="12410"/>
   </bookViews>
   <sheets>
     <sheet name="rebalance_localizations" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$357</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$393</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="835">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -2363,6 +2363,171 @@
   </si>
   <si>
     <t>gui/menu/research/name/tower_cannon_incindiary</t>
+  </si>
+  <si>
+    <t>Granade Launcher - Andvanced</t>
+  </si>
+  <si>
+    <t>Granade Launcher - Superior</t>
+  </si>
+  <si>
+    <t>Granade Launcher - Extreme</t>
+  </si>
+  <si>
+    <t>Rocket Launcher - Andvanced</t>
+  </si>
+  <si>
+    <t>Rocket Launcher - Superior</t>
+  </si>
+  <si>
+    <t>Rocket Launcher - Extreme</t>
+  </si>
+  <si>
+    <t>Mine Layer - Andvanced</t>
+  </si>
+  <si>
+    <t>Mine Layer - Superior</t>
+  </si>
+  <si>
+    <t>Mine Layer - Extreme</t>
+  </si>
+  <si>
+    <t>90mm Cannon - Andvanced</t>
+  </si>
+  <si>
+    <t>90mm Cannon - Superior</t>
+  </si>
+  <si>
+    <t>90mm Cannon - Extreme</t>
+  </si>
+  <si>
+    <t>Burst Rifle - Andvanced</t>
+  </si>
+  <si>
+    <t>Burst Rifle - Superior</t>
+  </si>
+  <si>
+    <t>Burst Rifle - Extreme</t>
+  </si>
+  <si>
+    <t>Shotgun - Andvanced</t>
+  </si>
+  <si>
+    <t>Shotgun - Superior</t>
+  </si>
+  <si>
+    <t>Shotgun - Extreme</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_burst_rifle_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_burst_rifle_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_burst_rifle_lvl_4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_granade_launcher_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_granade_launcher_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_granade_launcher_lvl_4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_mine_layer_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_mine_layer_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_mine_layer_lvl_4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_shotgun_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_shotgun_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_shotgun_lvl_4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_sniper_rifle_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_sniper_rifle_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_sniper_rifle_lvl_4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_rocket_launcher_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_rocket_launcher_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/mech_weapons_rocket_launcher_lvl_4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/well_contruction_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_burst_rifle_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_burst_rifle_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_burst_rifle_lvl_4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_granade_launcher_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_granade_launcher_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_granade_launcher_lvl_4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_mine_layer_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_mine_layer_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_mine_layer_lvl_4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_rocket_launcher_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_rocket_launcher_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_rocket_launcher_lvl_4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_shotgun_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_shotgun_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_shotgun_lvl_4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_sniper_rifle_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_sniper_rifle_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/mech_weapons_sniper_rifle_lvl_4</t>
   </si>
 </sst>
 </file>
@@ -3187,20 +3352,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K395"/>
+  <dimension ref="A1:K431"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C325" sqref="C325"/>
+      <pane ySplit="1" topLeftCell="A389" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="54.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="65.453125" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3232,7 +3397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3240,7 +3405,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3248,7 +3413,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3256,7 +3421,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -3264,7 +3429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>447</v>
       </c>
@@ -3272,7 +3437,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3280,7 +3445,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -3288,7 +3453,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -3296,7 +3461,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>589</v>
       </c>
@@ -3304,7 +3469,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -3312,7 +3477,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3320,7 +3485,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -3328,7 +3493,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>448</v>
       </c>
@@ -3336,7 +3501,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -3344,7 +3509,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3352,7 +3517,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -3360,7 +3525,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -3368,7 +3533,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -3376,7 +3541,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -3384,7 +3549,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -3392,7 +3557,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -3400,7 +3565,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -3408,7 +3573,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -3416,7 +3581,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>502</v>
       </c>
@@ -3424,7 +3589,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>650</v>
       </c>
@@ -3432,7 +3597,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>503</v>
       </c>
@@ -3440,7 +3605,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -3448,7 +3613,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>380</v>
       </c>
@@ -3456,7 +3621,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>461</v>
       </c>
@@ -3464,7 +3629,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>344</v>
       </c>
@@ -3475,7 +3640,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>670</v>
       </c>
@@ -3483,7 +3648,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -3491,7 +3656,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -3499,7 +3664,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -3507,7 +3672,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>377</v>
       </c>
@@ -3518,7 +3683,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>326</v>
       </c>
@@ -3526,7 +3691,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>335</v>
       </c>
@@ -3534,7 +3699,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>336</v>
       </c>
@@ -3542,7 +3707,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -3550,7 +3715,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -3558,7 +3723,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>59</v>
       </c>
@@ -3566,7 +3731,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -3574,7 +3739,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>62</v>
       </c>
@@ -3582,7 +3747,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -3590,7 +3755,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>621</v>
       </c>
@@ -3598,7 +3763,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>623</v>
       </c>
@@ -3606,7 +3771,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>658</v>
       </c>
@@ -3614,7 +3779,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>666</v>
       </c>
@@ -3622,7 +3787,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>667</v>
       </c>
@@ -3630,7 +3795,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>383</v>
       </c>
@@ -3641,7 +3806,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>385</v>
       </c>
@@ -3649,7 +3814,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>386</v>
       </c>
@@ -3657,7 +3822,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>387</v>
       </c>
@@ -3665,7 +3830,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>688</v>
       </c>
@@ -3673,7 +3838,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>689</v>
       </c>
@@ -3681,7 +3846,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>685</v>
       </c>
@@ -3689,7 +3854,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>347</v>
       </c>
@@ -3700,7 +3865,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -3708,7 +3873,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -3716,7 +3881,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -3724,7 +3889,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -3732,7 +3897,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>713</v>
       </c>
@@ -3740,7 +3905,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>712</v>
       </c>
@@ -3748,7 +3913,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>711</v>
       </c>
@@ -3756,7 +3921,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -3764,7 +3929,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -3772,7 +3937,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>481</v>
       </c>
@@ -3780,7 +3945,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>482</v>
       </c>
@@ -3788,7 +3953,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>489</v>
       </c>
@@ -3796,7 +3961,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>490</v>
       </c>
@@ -3804,7 +3969,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -3812,7 +3977,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>454</v>
       </c>
@@ -3820,7 +3985,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>453</v>
       </c>
@@ -3828,7 +3993,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>455</v>
       </c>
@@ -3836,7 +4001,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>459</v>
       </c>
@@ -3844,7 +4009,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>553</v>
       </c>
@@ -3852,7 +4017,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>487</v>
       </c>
@@ -3860,7 +4025,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>488</v>
       </c>
@@ -3868,7 +4033,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>483</v>
       </c>
@@ -3876,7 +4041,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>485</v>
       </c>
@@ -3884,7 +4049,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>486</v>
       </c>
@@ -3892,7 +4057,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>484</v>
       </c>
@@ -3900,7 +4065,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>493</v>
       </c>
@@ -3908,7 +4073,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>494</v>
       </c>
@@ -3916,7 +4081,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>495</v>
       </c>
@@ -3924,7 +4089,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>496</v>
       </c>
@@ -3932,7 +4097,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>498</v>
       </c>
@@ -3940,7 +4105,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>497</v>
       </c>
@@ -3948,7 +4113,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>491</v>
       </c>
@@ -3956,7 +4121,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>492</v>
       </c>
@@ -3964,7 +4129,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>544</v>
       </c>
@@ -3972,7 +4137,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>545</v>
       </c>
@@ -3980,7 +4145,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>543</v>
       </c>
@@ -3988,7 +4153,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>76</v>
       </c>
@@ -3996,7 +4161,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>78</v>
       </c>
@@ -4004,7 +4169,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>80</v>
       </c>
@@ -4012,7 +4177,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>82</v>
       </c>
@@ -4020,7 +4185,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>84</v>
       </c>
@@ -4028,7 +4193,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>445</v>
       </c>
@@ -4036,7 +4201,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>86</v>
       </c>
@@ -4044,7 +4209,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>88</v>
       </c>
@@ -4052,7 +4217,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>90</v>
       </c>
@@ -4060,7 +4225,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>590</v>
       </c>
@@ -4068,7 +4233,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>91</v>
       </c>
@@ -4076,7 +4241,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>93</v>
       </c>
@@ -4084,7 +4249,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>95</v>
       </c>
@@ -4092,7 +4257,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>446</v>
       </c>
@@ -4100,7 +4265,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>97</v>
       </c>
@@ -4108,7 +4273,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>99</v>
       </c>
@@ -4116,7 +4281,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>101</v>
       </c>
@@ -4124,7 +4289,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>103</v>
       </c>
@@ -4132,7 +4297,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>105</v>
       </c>
@@ -4140,7 +4305,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>107</v>
       </c>
@@ -4148,7 +4313,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>109</v>
       </c>
@@ -4156,7 +4321,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>111</v>
       </c>
@@ -4164,7 +4329,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>113</v>
       </c>
@@ -4172,7 +4337,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>115</v>
       </c>
@@ -4180,7 +4345,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>499</v>
       </c>
@@ -4188,7 +4353,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>645</v>
       </c>
@@ -4196,7 +4361,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>500</v>
       </c>
@@ -4204,7 +4369,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>117</v>
       </c>
@@ -4212,7 +4377,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>379</v>
       </c>
@@ -4220,7 +4385,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>462</v>
       </c>
@@ -4228,7 +4393,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>345</v>
       </c>
@@ -4239,7 +4404,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>348</v>
       </c>
@@ -4250,7 +4415,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>349</v>
       </c>
@@ -4261,7 +4426,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>656</v>
       </c>
@@ -4269,7 +4434,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>119</v>
       </c>
@@ -4277,7 +4442,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>378</v>
       </c>
@@ -4288,7 +4453,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>327</v>
       </c>
@@ -4296,7 +4461,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>328</v>
       </c>
@@ -4304,7 +4469,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>329</v>
       </c>
@@ -4312,7 +4477,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>121</v>
       </c>
@@ -4320,7 +4485,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>123</v>
       </c>
@@ -4328,7 +4493,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>125</v>
       </c>
@@ -4336,7 +4501,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>127</v>
       </c>
@@ -4344,7 +4509,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>625</v>
       </c>
@@ -4352,7 +4517,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>388</v>
       </c>
@@ -4363,7 +4528,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>389</v>
       </c>
@@ -4374,7 +4539,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>390</v>
       </c>
@@ -4385,7 +4550,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>391</v>
       </c>
@@ -4396,7 +4561,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>686</v>
       </c>
@@ -4404,7 +4569,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>687</v>
       </c>
@@ -4412,7 +4577,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>684</v>
       </c>
@@ -4420,7 +4585,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>129</v>
       </c>
@@ -4428,7 +4593,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>131</v>
       </c>
@@ -4436,7 +4601,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>331</v>
       </c>
@@ -4444,7 +4609,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>330</v>
       </c>
@@ -4452,7 +4617,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>699</v>
       </c>
@@ -4460,7 +4625,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>696</v>
       </c>
@@ -4468,7 +4633,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>697</v>
       </c>
@@ -4476,7 +4641,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>463</v>
       </c>
@@ -4484,7 +4649,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>464</v>
       </c>
@@ -4492,7 +4657,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>471</v>
       </c>
@@ -4500,7 +4665,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>472</v>
       </c>
@@ -4508,7 +4673,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>133</v>
       </c>
@@ -4516,7 +4681,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>457</v>
       </c>
@@ -4524,7 +4689,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>456</v>
       </c>
@@ -4532,7 +4697,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>458</v>
       </c>
@@ -4540,7 +4705,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>460</v>
       </c>
@@ -4548,7 +4713,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>550</v>
       </c>
@@ -4556,7 +4721,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>469</v>
       </c>
@@ -4564,7 +4729,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>470</v>
       </c>
@@ -4572,7 +4737,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>466</v>
       </c>
@@ -4580,7 +4745,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>467</v>
       </c>
@@ -4588,7 +4753,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>468</v>
       </c>
@@ -4596,7 +4761,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>465</v>
       </c>
@@ -4604,7 +4769,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>475</v>
       </c>
@@ -4612,7 +4777,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>476</v>
       </c>
@@ -4620,7 +4785,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>477</v>
       </c>
@@ -4628,7 +4793,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>478</v>
       </c>
@@ -4636,7 +4801,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>480</v>
       </c>
@@ -4644,7 +4809,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>479</v>
       </c>
@@ -4652,7 +4817,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>473</v>
       </c>
@@ -4660,7 +4825,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>474</v>
       </c>
@@ -4668,7 +4833,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>540</v>
       </c>
@@ -4676,7 +4841,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>542</v>
       </c>
@@ -4684,7 +4849,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>541</v>
       </c>
@@ -4692,7 +4857,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>135</v>
       </c>
@@ -4700,7 +4865,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>546</v>
       </c>
@@ -4708,7 +4873,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>534</v>
       </c>
@@ -4716,7 +4881,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>569</v>
       </c>
@@ -4724,7 +4889,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>570</v>
       </c>
@@ -4732,7 +4897,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>726</v>
       </c>
@@ -4740,7 +4905,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>571</v>
       </c>
@@ -4748,7 +4913,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>572</v>
       </c>
@@ -4756,7 +4921,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>727</v>
       </c>
@@ -4764,7 +4929,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>573</v>
       </c>
@@ -4772,7 +4937,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>574</v>
       </c>
@@ -4780,7 +4945,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>728</v>
       </c>
@@ -4788,7 +4953,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>575</v>
       </c>
@@ -4796,7 +4961,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>576</v>
       </c>
@@ -4804,7 +4969,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>729</v>
       </c>
@@ -4812,1708 +4977,1996 @@
         <v>588</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
+        <v>577</v>
+      </c>
+      <c r="B195" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>578</v>
+      </c>
+      <c r="B196" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>730</v>
+      </c>
+      <c r="B197" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>137</v>
+      </c>
+      <c r="B198" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>139</v>
+      </c>
+      <c r="B199" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>141</v>
+      </c>
+      <c r="B200" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
         <v>143</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B201" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
         <v>144</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B202" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
         <v>672</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B203" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
         <v>676</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B204" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
         <v>677</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B205" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
         <v>145</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B206" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
         <v>147</v>
       </c>
-      <c r="B201" t="s">
+      <c r="B207" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>750</v>
+      </c>
+      <c r="B208" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>751</v>
+      </c>
+      <c r="B209" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>752</v>
+      </c>
+      <c r="B210" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
         <v>536</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B211" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
         <v>642</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B212" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
         <v>643</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B213" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
         <v>649</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B214" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
         <v>706</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B215" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
         <v>707</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B216" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>757</v>
+      </c>
+      <c r="B217" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
         <v>149</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B218" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
         <v>151</v>
       </c>
-      <c r="B209" t="s">
+      <c r="B219" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
         <v>153</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B220" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
         <v>155</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B221" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
         <v>157</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B222" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
         <v>159</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B223" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
         <v>161</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B224" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
         <v>163</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B225" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
         <v>165</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B226" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
         <v>167</v>
       </c>
-      <c r="B217" t="s">
+      <c r="B227" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
         <v>169</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B228" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
         <v>171</v>
       </c>
-      <c r="B219" t="s">
+      <c r="B229" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
         <v>173</v>
       </c>
-      <c r="B220" t="s">
+      <c r="B230" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
         <v>175</v>
       </c>
-      <c r="B221" t="s">
+      <c r="B231" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
         <v>177</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B232" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
         <v>179</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B233" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
         <v>181</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B234" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A235" t="s">
         <v>183</v>
       </c>
-      <c r="B225" t="s">
+      <c r="B235" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
+        <v>798</v>
+      </c>
+      <c r="B236" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
+        <v>799</v>
+      </c>
+      <c r="B237" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A238" t="s">
+        <v>800</v>
+      </c>
+      <c r="B238" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A239" t="s">
+        <v>801</v>
+      </c>
+      <c r="B239" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A240" t="s">
+        <v>802</v>
+      </c>
+      <c r="B240" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
+        <v>803</v>
+      </c>
+      <c r="B241" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A242" t="s">
+        <v>804</v>
+      </c>
+      <c r="B242" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A243" t="s">
+        <v>805</v>
+      </c>
+      <c r="B243" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A244" t="s">
+        <v>806</v>
+      </c>
+      <c r="B244" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A245" t="s">
+        <v>813</v>
+      </c>
+      <c r="B245" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A246" t="s">
+        <v>814</v>
+      </c>
+      <c r="B246" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
+        <v>815</v>
+      </c>
+      <c r="B247" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A248" t="s">
+        <v>807</v>
+      </c>
+      <c r="B248" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A249" t="s">
+        <v>808</v>
+      </c>
+      <c r="B249" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A250" t="s">
+        <v>809</v>
+      </c>
+      <c r="B250" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A251" t="s">
+        <v>810</v>
+      </c>
+      <c r="B251" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A252" t="s">
+        <v>811</v>
+      </c>
+      <c r="B252" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A253" t="s">
+        <v>812</v>
+      </c>
+      <c r="B253" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A254" t="s">
         <v>402</v>
       </c>
-      <c r="B226" t="s">
+      <c r="B254" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
         <v>407</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B255" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
         <v>408</v>
       </c>
-      <c r="B228" t="s">
+      <c r="B256" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
         <v>627</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B257" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
         <v>629</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B258" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
         <v>434</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B259" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
         <v>436</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B260" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
         <v>438</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B261" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
+        <v>756</v>
+      </c>
+      <c r="B262" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
         <v>412</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B263" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A264" t="s">
         <v>419</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B264" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A265" t="s">
         <v>421</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B265" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A266" t="s">
         <v>185</v>
       </c>
-      <c r="B237" t="s">
+      <c r="B266" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A267" t="s">
         <v>187</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B267" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A268" t="s">
+        <v>770</v>
+      </c>
+      <c r="B268" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A269" t="s">
+        <v>771</v>
+      </c>
+      <c r="B269" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A270" t="s">
+        <v>772</v>
+      </c>
+      <c r="B270" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A271" t="s">
+        <v>773</v>
+      </c>
+      <c r="B271" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A272" t="s">
+        <v>774</v>
+      </c>
+      <c r="B272" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A273" t="s">
+        <v>764</v>
+      </c>
+      <c r="B273" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A274" t="s">
         <v>556</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B274" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A275" t="s">
+        <v>742</v>
+      </c>
+      <c r="B275" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
         <v>423</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B276" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A277" t="s">
+        <v>816</v>
+      </c>
+      <c r="B277" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A278" t="s">
         <v>431</v>
       </c>
-      <c r="B241" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>577</v>
-      </c>
-      <c r="B242" t="s">
+      <c r="B278" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A279" t="s">
+        <v>559</v>
+      </c>
+      <c r="B279" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A280" t="s">
+        <v>560</v>
+      </c>
+      <c r="B280" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A281" t="s">
+        <v>720</v>
+      </c>
+      <c r="B281" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A282" t="s">
+        <v>561</v>
+      </c>
+      <c r="B282" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A283" t="s">
+        <v>562</v>
+      </c>
+      <c r="B283" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A284" t="s">
+        <v>719</v>
+      </c>
+      <c r="B284" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A285" t="s">
+        <v>563</v>
+      </c>
+      <c r="B285" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A286" t="s">
+        <v>564</v>
+      </c>
+      <c r="B286" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A287" t="s">
+        <v>718</v>
+      </c>
+      <c r="B287" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A288" t="s">
+        <v>565</v>
+      </c>
+      <c r="B288" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A289" t="s">
+        <v>566</v>
+      </c>
+      <c r="B289" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A290" t="s">
+        <v>717</v>
+      </c>
+      <c r="B290" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A291" t="s">
+        <v>567</v>
+      </c>
+      <c r="B291" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>578</v>
-      </c>
-      <c r="B243" t="s">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A292" t="s">
+        <v>568</v>
+      </c>
+      <c r="B292" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>730</v>
-      </c>
-      <c r="B244" t="s">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A293" t="s">
+        <v>716</v>
+      </c>
+      <c r="B293" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>137</v>
-      </c>
-      <c r="B245" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>139</v>
-      </c>
-      <c r="B246" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>141</v>
-      </c>
-      <c r="B247" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>750</v>
-      </c>
-      <c r="B248" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>751</v>
-      </c>
-      <c r="B249" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>752</v>
-      </c>
-      <c r="B250" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>757</v>
-      </c>
-      <c r="B251" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>756</v>
-      </c>
-      <c r="B252" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>764</v>
-      </c>
-      <c r="B253" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>770</v>
-      </c>
-      <c r="B254" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
-        <v>771</v>
-      </c>
-      <c r="B255" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>772</v>
-      </c>
-      <c r="B256" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A257" t="s">
-        <v>773</v>
-      </c>
-      <c r="B257" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
-        <v>774</v>
-      </c>
-      <c r="B258" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
-        <v>742</v>
-      </c>
-      <c r="B259" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A260" t="s">
-        <v>431</v>
-      </c>
-      <c r="B260" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A261" t="s">
-        <v>559</v>
-      </c>
-      <c r="B261" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
-        <v>560</v>
-      </c>
-      <c r="B262" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
-        <v>720</v>
-      </c>
-      <c r="B263" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
-        <v>561</v>
-      </c>
-      <c r="B264" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" t="s">
-        <v>562</v>
-      </c>
-      <c r="B265" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" t="s">
-        <v>719</v>
-      </c>
-      <c r="B266" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" t="s">
-        <v>563</v>
-      </c>
-      <c r="B267" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" t="s">
-        <v>564</v>
-      </c>
-      <c r="B268" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" t="s">
-        <v>718</v>
-      </c>
-      <c r="B269" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" t="s">
-        <v>565</v>
-      </c>
-      <c r="B270" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" t="s">
-        <v>566</v>
-      </c>
-      <c r="B271" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" t="s">
-        <v>717</v>
-      </c>
-      <c r="B272" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>567</v>
-      </c>
-      <c r="B273" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
-        <v>568</v>
-      </c>
-      <c r="B274" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" t="s">
-        <v>716</v>
-      </c>
-      <c r="B275" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A294" t="s">
         <v>189</v>
       </c>
-      <c r="B276" t="s">
+      <c r="B294" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A295" t="s">
         <v>191</v>
       </c>
-      <c r="B277" t="s">
+      <c r="B295" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A296" t="s">
         <v>193</v>
       </c>
-      <c r="B278" t="s">
+      <c r="B296" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A297" t="s">
         <v>195</v>
       </c>
-      <c r="B279" t="s">
+      <c r="B297" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A298" t="s">
         <v>197</v>
       </c>
-      <c r="B280" t="s">
+      <c r="B298" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A299" t="s">
         <v>673</v>
       </c>
-      <c r="B281" t="s">
+      <c r="B299" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A300" t="s">
         <v>674</v>
       </c>
-      <c r="B282" t="s">
+      <c r="B300" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A301" t="s">
         <v>675</v>
       </c>
-      <c r="B283" t="s">
+      <c r="B301" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A302" t="s">
         <v>199</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B302" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A303" t="s">
         <v>201</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B303" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A304" t="s">
         <v>744</v>
       </c>
-      <c r="B286" t="s">
+      <c r="B304" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A305" t="s">
         <v>745</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B305" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A306" t="s">
         <v>746</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B306" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A307" t="s">
         <v>538</v>
       </c>
-      <c r="B289" t="s">
+      <c r="B307" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A308" t="s">
         <v>638</v>
       </c>
-      <c r="B290" t="s">
+      <c r="B308" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A309" t="s">
         <v>639</v>
       </c>
-      <c r="B291" t="s">
+      <c r="B309" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A310" t="s">
         <v>647</v>
       </c>
-      <c r="B292" t="s">
+      <c r="B310" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A311" t="s">
         <v>702</v>
       </c>
-      <c r="B293" t="s">
+      <c r="B311" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A312" t="s">
         <v>703</v>
       </c>
-      <c r="B294" t="s">
+      <c r="B312" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A313" t="s">
         <v>755</v>
       </c>
-      <c r="B295" t="s">
+      <c r="B313" t="s">
         <v>758</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A314" t="s">
         <v>203</v>
       </c>
-      <c r="B296" t="s">
+      <c r="B314" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A315" t="s">
         <v>205</v>
       </c>
-      <c r="B297" t="s">
+      <c r="B315" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
         <v>207</v>
       </c>
-      <c r="B298" t="s">
+      <c r="B316" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
         <v>209</v>
       </c>
-      <c r="B299" t="s">
+      <c r="B317" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A318" t="s">
         <v>211</v>
       </c>
-      <c r="B300" t="s">
+      <c r="B318" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" t="s">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A319" t="s">
         <v>213</v>
       </c>
-      <c r="B301" t="s">
+      <c r="B319" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" t="s">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A320" t="s">
         <v>215</v>
       </c>
-      <c r="B302" t="s">
+      <c r="B320" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A303" t="s">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A321" t="s">
         <v>216</v>
       </c>
-      <c r="B303" t="s">
+      <c r="B321" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A304" t="s">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A322" t="s">
         <v>217</v>
       </c>
-      <c r="B304" t="s">
+      <c r="B322" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" t="s">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A323" t="s">
         <v>218</v>
       </c>
-      <c r="B305" t="s">
+      <c r="B323" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A306" t="s">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A324" t="s">
         <v>219</v>
       </c>
-      <c r="B306" t="s">
+      <c r="B324" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A307" t="s">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A325" t="s">
         <v>220</v>
       </c>
-      <c r="B307" t="s">
+      <c r="B325" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A308" t="s">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A326" t="s">
         <v>221</v>
       </c>
-      <c r="B308" t="s">
+      <c r="B326" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" t="s">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A327" t="s">
         <v>222</v>
       </c>
-      <c r="B309" t="s">
+      <c r="B327" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" t="s">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A328" t="s">
         <v>223</v>
       </c>
-      <c r="B310" t="s">
+      <c r="B328" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" t="s">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A329" t="s">
         <v>224</v>
       </c>
-      <c r="B311" t="s">
+      <c r="B329" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A330" t="s">
         <v>225</v>
       </c>
-      <c r="B312" t="s">
+      <c r="B330" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A331" t="s">
         <v>226</v>
       </c>
-      <c r="B313" t="s">
+      <c r="B331" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A314" t="s">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A332" t="s">
+        <v>817</v>
+      </c>
+      <c r="B332" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A333" t="s">
+        <v>818</v>
+      </c>
+      <c r="B333" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A334" t="s">
+        <v>819</v>
+      </c>
+      <c r="B334" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A335" t="s">
+        <v>820</v>
+      </c>
+      <c r="B335" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A336" t="s">
+        <v>821</v>
+      </c>
+      <c r="B336" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A337" t="s">
+        <v>822</v>
+      </c>
+      <c r="B337" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A338" t="s">
+        <v>823</v>
+      </c>
+      <c r="B338" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A339" t="s">
+        <v>824</v>
+      </c>
+      <c r="B339" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A340" t="s">
+        <v>825</v>
+      </c>
+      <c r="B340" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A341" t="s">
+        <v>826</v>
+      </c>
+      <c r="B341" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A342" t="s">
+        <v>827</v>
+      </c>
+      <c r="B342" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A343" t="s">
+        <v>828</v>
+      </c>
+      <c r="B343" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A344" t="s">
+        <v>829</v>
+      </c>
+      <c r="B344" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A345" t="s">
+        <v>830</v>
+      </c>
+      <c r="B345" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A346" t="s">
+        <v>831</v>
+      </c>
+      <c r="B346" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A347" t="s">
+        <v>832</v>
+      </c>
+      <c r="B347" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A348" t="s">
+        <v>833</v>
+      </c>
+      <c r="B348" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A349" t="s">
+        <v>834</v>
+      </c>
+      <c r="B349" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A350" t="s">
         <v>401</v>
       </c>
-      <c r="B314" t="s">
+      <c r="B350" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A315" t="s">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A351" t="s">
         <v>406</v>
       </c>
-      <c r="B315" t="s">
+      <c r="B351" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A316" t="s">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A352" t="s">
         <v>409</v>
       </c>
-      <c r="B316" t="s">
+      <c r="B352" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A317" t="s">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A353" t="s">
         <v>630</v>
       </c>
-      <c r="B317" t="s">
+      <c r="B353" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A318" t="s">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A354" t="s">
         <v>632</v>
       </c>
-      <c r="B318" t="s">
+      <c r="B354" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A319" t="s">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A355" t="s">
         <v>657</v>
       </c>
-      <c r="B319" t="s">
+      <c r="B355" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A320" t="s">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A356" t="s">
         <v>661</v>
       </c>
-      <c r="B320" t="s">
+      <c r="B356" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A321" t="s">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A357" t="s">
         <v>662</v>
       </c>
-      <c r="B321" t="s">
+      <c r="B357" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A322" t="s">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A358" t="s">
         <v>433</v>
       </c>
-      <c r="B322" t="s">
+      <c r="B358" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A323" t="s">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A359" t="s">
         <v>435</v>
       </c>
-      <c r="B323" t="s">
+      <c r="B359" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A324" t="s">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A360" t="s">
         <v>437</v>
       </c>
-      <c r="B324" t="s">
+      <c r="B360" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" t="s">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A361" t="s">
         <v>754</v>
       </c>
-      <c r="B325" t="s">
+      <c r="B361" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" t="s">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A362" t="s">
         <v>413</v>
       </c>
-      <c r="B326" t="s">
+      <c r="B362" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327" t="s">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A363" t="s">
         <v>420</v>
       </c>
-      <c r="B327" t="s">
+      <c r="B363" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" t="s">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A364" t="s">
         <v>422</v>
       </c>
-      <c r="B328" t="s">
+      <c r="B364" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" t="s">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A365" t="s">
         <v>227</v>
       </c>
-      <c r="B329" t="s">
+      <c r="B365" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" t="s">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A366" t="s">
         <v>229</v>
       </c>
-      <c r="B330" t="s">
+      <c r="B366" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" t="s">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A367" t="s">
+        <v>775</v>
+      </c>
+      <c r="B367" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A368" t="s">
+        <v>776</v>
+      </c>
+      <c r="B368" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A369" t="s">
+        <v>777</v>
+      </c>
+      <c r="B369" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A370" t="s">
+        <v>778</v>
+      </c>
+      <c r="B370" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A371" t="s">
+        <v>779</v>
+      </c>
+      <c r="B371" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A372" t="s">
         <v>766</v>
       </c>
-      <c r="B331" t="s">
+      <c r="B372" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" t="s">
-        <v>775</v>
-      </c>
-      <c r="B332" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" t="s">
-        <v>776</v>
-      </c>
-      <c r="B333" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" t="s">
-        <v>777</v>
-      </c>
-      <c r="B334" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A335" t="s">
-        <v>778</v>
-      </c>
-      <c r="B335" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A336" t="s">
-        <v>779</v>
-      </c>
-      <c r="B336" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A337" t="s">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A373" t="s">
         <v>555</v>
       </c>
-      <c r="B337" t="s">
+      <c r="B373" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A338" t="s">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A374" t="s">
         <v>741</v>
       </c>
-      <c r="B338" t="s">
+      <c r="B374" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A339" t="s">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A375" t="s">
         <v>739</v>
       </c>
-      <c r="B339" t="s">
+      <c r="B375" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A340" t="s">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A376" t="s">
         <v>740</v>
       </c>
-      <c r="B340" t="s">
+      <c r="B376" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A341" t="s">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A377" t="s">
         <v>424</v>
       </c>
-      <c r="B341" t="s">
+      <c r="B377" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A342" t="s">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A378" t="s">
         <v>429</v>
       </c>
-      <c r="B342" t="s">
+      <c r="B378" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A343" t="s">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A379" t="s">
         <v>430</v>
       </c>
-      <c r="B343" t="s">
+      <c r="B379" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A344" t="s">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A380" t="s">
         <v>231</v>
       </c>
-      <c r="B344" t="s">
+      <c r="B380" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A345" t="s">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A381" t="s">
         <v>233</v>
       </c>
-      <c r="B345" t="s">
+      <c r="B381" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A346" t="s">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A382" t="s">
         <v>235</v>
       </c>
-      <c r="B346" t="s">
+      <c r="B382" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A347" t="s">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A383" t="s">
         <v>237</v>
       </c>
-      <c r="B347" t="s">
+      <c r="B383" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A348" t="s">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A384" t="s">
         <v>239</v>
       </c>
-      <c r="B348" t="s">
+      <c r="B384" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A349" t="s">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A385" t="s">
         <v>241</v>
       </c>
-      <c r="B349" t="s">
+      <c r="B385" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A350" t="s">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A386" t="s">
         <v>243</v>
       </c>
-      <c r="B350" t="s">
+      <c r="B386" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A351" t="s">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A387" t="s">
         <v>245</v>
       </c>
-      <c r="B351" t="s">
+      <c r="B387" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A388" t="s">
         <v>247</v>
       </c>
-      <c r="B352" t="s">
+      <c r="B388" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A353" t="s">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A389" t="s">
         <v>249</v>
       </c>
-      <c r="B353" t="s">
+      <c r="B389" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A354" t="s">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A390" t="s">
         <v>251</v>
       </c>
-      <c r="B354" t="s">
+      <c r="B390" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A355" t="s">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A391" t="s">
         <v>253</v>
       </c>
-      <c r="B355" t="s">
+      <c r="B391" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A356" t="s">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A392" t="s">
         <v>255</v>
       </c>
-      <c r="B356" t="s">
+      <c r="B392" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A357" t="s">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A393" t="s">
         <v>257</v>
       </c>
-      <c r="B357" t="s">
+      <c r="B393" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A358" t="s">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A394" t="s">
         <v>259</v>
       </c>
-      <c r="B358" t="s">
+      <c r="B394" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A359" t="s">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A395" t="s">
         <v>261</v>
       </c>
-      <c r="B359" t="s">
+      <c r="B395" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A360" t="s">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A396" t="s">
         <v>263</v>
       </c>
-      <c r="B360" t="s">
+      <c r="B396" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A361" t="s">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A397" t="s">
         <v>265</v>
       </c>
-      <c r="B361" t="s">
+      <c r="B397" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A398" t="s">
         <v>267</v>
       </c>
-      <c r="B362" t="s">
+      <c r="B398" t="s">
         <v>268</v>
       </c>
-      <c r="C362" t="s">
+      <c r="C398" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A363" t="s">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A399" t="s">
         <v>361</v>
       </c>
-      <c r="B363" t="s">
+      <c r="B399" t="s">
         <v>363</v>
       </c>
-      <c r="C363" t="s">
+      <c r="C399" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A364" t="s">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A400" t="s">
         <v>269</v>
       </c>
-      <c r="B364" t="s">
+      <c r="B400" t="s">
         <v>270</v>
       </c>
-      <c r="C364" t="s">
+      <c r="C400" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A365" t="s">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A401" t="s">
         <v>501</v>
       </c>
-      <c r="B365" t="s">
+      <c r="B401" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A366" t="s">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A402" t="s">
         <v>271</v>
       </c>
-      <c r="B366" t="s">
+      <c r="B402" t="s">
         <v>652</v>
       </c>
-      <c r="C366" t="s">
+      <c r="C402" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A367" t="s">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A403" t="s">
         <v>316</v>
       </c>
-      <c r="B367" t="s">
+      <c r="B403" t="s">
         <v>321</v>
       </c>
-      <c r="C367" t="s">
+      <c r="C403" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A368" t="s">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A404" t="s">
         <v>317</v>
       </c>
-      <c r="B368" t="s">
+      <c r="B404" t="s">
         <v>320</v>
       </c>
-      <c r="C368" t="s">
+      <c r="C404" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A369" t="s">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A405" t="s">
         <v>272</v>
       </c>
-      <c r="B369" t="s">
+      <c r="B405" t="s">
         <v>273</v>
       </c>
-      <c r="C369" t="s">
+      <c r="C405" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A370" t="s">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A406" t="s">
         <v>288</v>
       </c>
-      <c r="B370" t="s">
+      <c r="B406" t="s">
         <v>303</v>
       </c>
-      <c r="C370" t="s">
+      <c r="C406" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A371" t="s">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A407" t="s">
         <v>292</v>
       </c>
-      <c r="B371" t="s">
+      <c r="B407" t="s">
         <v>302</v>
       </c>
-      <c r="C371" t="s">
+      <c r="C407" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A372" t="s">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A408" t="s">
         <v>274</v>
       </c>
-      <c r="B372" t="s">
+      <c r="B408" t="s">
         <v>275</v>
       </c>
-      <c r="C372" t="s">
+      <c r="C408" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A373" t="s">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A409" t="s">
         <v>341</v>
       </c>
-      <c r="B373" t="s">
+      <c r="B409" t="s">
         <v>342</v>
       </c>
-      <c r="C373" t="s">
+      <c r="C409" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A374" t="s">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A410" t="s">
         <v>314</v>
       </c>
-      <c r="B374" t="s">
+      <c r="B410" t="s">
         <v>322</v>
       </c>
-      <c r="C374" t="s">
+      <c r="C410" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A375" t="s">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A411" t="s">
         <v>315</v>
       </c>
-      <c r="B375" t="s">
+      <c r="B411" t="s">
         <v>323</v>
       </c>
-      <c r="C375" t="s">
+      <c r="C411" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A376" t="s">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A412" t="s">
         <v>359</v>
       </c>
-      <c r="B376" t="s">
+      <c r="B412" t="s">
         <v>365</v>
       </c>
-      <c r="C376" t="s">
+      <c r="C412" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A377" t="s">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A413" t="s">
         <v>276</v>
       </c>
-      <c r="B377" t="s">
+      <c r="B413" t="s">
         <v>277</v>
       </c>
-      <c r="C377" t="s">
+      <c r="C413" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A378" t="s">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A414" t="s">
         <v>360</v>
       </c>
-      <c r="B378" t="s">
+      <c r="B414" t="s">
         <v>366</v>
       </c>
-      <c r="C378" t="s">
+      <c r="C414" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A379" t="s">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A415" t="s">
         <v>356</v>
       </c>
-      <c r="B379" t="s">
+      <c r="B415" t="s">
         <v>368</v>
       </c>
-      <c r="C379" t="s">
+      <c r="C415" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A380" t="s">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A416" t="s">
         <v>278</v>
       </c>
-      <c r="B380" t="s">
+      <c r="B416" t="s">
         <v>279</v>
       </c>
-      <c r="C380" t="s">
+      <c r="C416" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A381" t="s">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A417" t="s">
         <v>280</v>
       </c>
-      <c r="B381" t="s">
+      <c r="B417" t="s">
         <v>281</v>
       </c>
-      <c r="C381" t="s">
+      <c r="C417" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A382" t="s">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A418" t="s">
         <v>291</v>
       </c>
-      <c r="B382" t="s">
+      <c r="B418" t="s">
         <v>296</v>
       </c>
-      <c r="C382" t="s">
+      <c r="C418" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A383" t="s">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A419" t="s">
         <v>295</v>
       </c>
-      <c r="B383" t="s">
+      <c r="B419" t="s">
         <v>301</v>
       </c>
-      <c r="C383" t="s">
+      <c r="C419" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A384" t="s">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A420" t="s">
         <v>634</v>
       </c>
-      <c r="B384" t="s">
+      <c r="B420" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A385" t="s">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A421" t="s">
         <v>636</v>
       </c>
-      <c r="B385" t="s">
+      <c r="B421" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A386" t="s">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A422" t="s">
         <v>392</v>
       </c>
-      <c r="B386" t="s">
+      <c r="B422" t="s">
         <v>397</v>
       </c>
-      <c r="C386" t="s">
+      <c r="C422" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A387" t="s">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A423" t="s">
         <v>358</v>
       </c>
-      <c r="B387" t="s">
+      <c r="B423" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A388" t="s">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A424" t="s">
         <v>282</v>
       </c>
-      <c r="B388" t="s">
+      <c r="B424" t="s">
         <v>283</v>
       </c>
-      <c r="C388" t="s">
+      <c r="C424" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A389" t="s">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A425" t="s">
         <v>284</v>
       </c>
-      <c r="B389" t="s">
+      <c r="B425" t="s">
         <v>285</v>
       </c>
-      <c r="C389" t="s">
+      <c r="C425" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A390" t="s">
+    <row r="426" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A426" t="s">
         <v>290</v>
       </c>
-      <c r="B390" t="s">
+      <c r="B426" t="s">
         <v>297</v>
       </c>
-      <c r="C390" t="s">
+      <c r="C426" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A391" t="s">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A427" t="s">
         <v>294</v>
       </c>
-      <c r="B391" t="s">
+      <c r="B427" t="s">
         <v>300</v>
       </c>
-      <c r="C391" t="s">
+      <c r="C427" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A392" t="s">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A428" t="s">
         <v>286</v>
       </c>
-      <c r="B392" t="s">
+      <c r="B428" t="s">
         <v>287</v>
       </c>
-      <c r="C392" t="s">
+      <c r="C428" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A393" t="s">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A429" t="s">
         <v>289</v>
       </c>
-      <c r="B393" t="s">
+      <c r="B429" t="s">
         <v>298</v>
       </c>
-      <c r="C393" t="s">
+      <c r="C429" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A394" t="s">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A430" t="s">
         <v>293</v>
       </c>
-      <c r="B394" t="s">
+      <c r="B430" t="s">
         <v>299</v>
       </c>
-      <c r="C394" t="s">
+      <c r="C430" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A395" t="s">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A431" t="s">
         <v>357</v>
       </c>
-      <c r="B395" t="s">
+      <c r="B431" t="s">
         <v>367</v>
       </c>
-      <c r="C395" t="s">
+      <c r="C431" t="s">
         <v>375</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K357">
-    <sortState ref="A2:K395">
-      <sortCondition ref="A1:A357"/>
+  <autoFilter ref="A1:K393">
+    <sortState ref="A2:K431">
+      <sortCondition ref="A1:A393"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6528,9 +6981,9 @@
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>383</v>
       </c>
@@ -6541,7 +6994,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>385</v>
       </c>
@@ -6549,7 +7002,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>386</v>
       </c>
@@ -6557,7 +7010,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>387</v>
       </c>
@@ -6565,7 +7018,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>388</v>
       </c>
@@ -6576,7 +7029,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>389</v>
       </c>
@@ -6587,7 +7040,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>390</v>
       </c>
@@ -6598,7 +7051,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>391</v>
       </c>
@@ -6609,7 +7062,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>392</v>
       </c>

</xml_diff>

<commit_message>
working on cannon towers
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$393</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$400</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="835">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="846">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -2528,6 +2528,39 @@
   </si>
   <si>
     <t>gui/menu/research/name/mech_weapons_sniper_rifle_lvl_4</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/tower_cannon_cooled</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/tower_cannon_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/tower_cannon_lvl_3</t>
+  </si>
+  <si>
+    <t>90mm Gun Tower - Advanced</t>
+  </si>
+  <si>
+    <t>90mm Gun Tower - Extreme</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_cannon_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/tower_cannon_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/tower_cannon_cooled</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/tower_cannon_cooled_lvl_2</t>
+  </si>
+  <si>
+    <t>Cooling for cannons to improve the rate of fire</t>
+  </si>
+  <si>
+    <t>Advanceed cooling for cannons to maximize the rate of fire</t>
   </si>
 </sst>
 </file>
@@ -3352,11 +3385,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K431"/>
+  <dimension ref="A1:K438"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A389" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4715,327 +4748,327 @@
     </row>
     <row r="162" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>550</v>
+        <v>840</v>
       </c>
       <c r="B162" t="s">
-        <v>551</v>
+        <v>838</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>469</v>
+        <v>841</v>
       </c>
       <c r="B163" t="s">
-        <v>613</v>
+        <v>839</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>470</v>
+        <v>550</v>
       </c>
       <c r="B164" t="s">
-        <v>614</v>
+        <v>551</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="B165" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B166" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B167" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B168" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="B169" t="s">
-        <v>505</v>
+        <v>617</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
       <c r="B170" t="s">
-        <v>602</v>
+        <v>618</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B171" t="s">
-        <v>603</v>
+        <v>505</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B172" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B173" t="s">
-        <v>506</v>
+        <v>603</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B174" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="B175" t="s">
-        <v>605</v>
+        <v>506</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="B176" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>540</v>
+        <v>473</v>
       </c>
       <c r="B177" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>542</v>
+        <v>474</v>
       </c>
       <c r="B178" t="s">
-        <v>552</v>
+        <v>606</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B179" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>135</v>
+        <v>542</v>
       </c>
       <c r="B180" t="s">
-        <v>136</v>
+        <v>552</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="B181" t="s">
-        <v>547</v>
+        <v>607</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>534</v>
+        <v>135</v>
       </c>
       <c r="B182" t="s">
-        <v>535</v>
+        <v>136</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>569</v>
+        <v>546</v>
       </c>
       <c r="B183" t="s">
-        <v>579</v>
+        <v>547</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>570</v>
+        <v>534</v>
       </c>
       <c r="B184" t="s">
-        <v>721</v>
+        <v>535</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>726</v>
+        <v>569</v>
       </c>
       <c r="B185" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B186" t="s">
-        <v>585</v>
+        <v>721</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>572</v>
+        <v>726</v>
       </c>
       <c r="B187" t="s">
-        <v>722</v>
+        <v>582</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>727</v>
+        <v>571</v>
       </c>
       <c r="B188" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B189" t="s">
-        <v>580</v>
+        <v>722</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>574</v>
+        <v>727</v>
       </c>
       <c r="B190" t="s">
-        <v>723</v>
+        <v>587</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>728</v>
+        <v>573</v>
       </c>
       <c r="B191" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B192" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>576</v>
+        <v>728</v>
       </c>
       <c r="B193" t="s">
-        <v>724</v>
+        <v>583</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>729</v>
+        <v>575</v>
       </c>
       <c r="B194" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B195" t="s">
-        <v>581</v>
+        <v>724</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>578</v>
+        <v>729</v>
       </c>
       <c r="B196" t="s">
-        <v>725</v>
+        <v>588</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>730</v>
+        <v>577</v>
       </c>
       <c r="B197" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>137</v>
+        <v>578</v>
       </c>
       <c r="B198" t="s">
-        <v>138</v>
+        <v>725</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>139</v>
+        <v>730</v>
       </c>
       <c r="B199" t="s">
-        <v>140</v>
+        <v>584</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
+        <v>137</v>
+      </c>
+      <c r="B200" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>139</v>
+      </c>
+      <c r="B201" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
         <v>141</v>
-      </c>
-      <c r="B200" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A201" t="s">
-        <v>143</v>
-      </c>
-      <c r="B201" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A202" t="s">
-        <v>144</v>
       </c>
       <c r="B202" t="s">
         <v>142</v>
@@ -5043,1930 +5076,1986 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>672</v>
+        <v>143</v>
       </c>
       <c r="B203" t="s">
-        <v>679</v>
+        <v>142</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>676</v>
+        <v>144</v>
       </c>
       <c r="B204" t="s">
-        <v>680</v>
+        <v>142</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="B205" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>145</v>
+        <v>676</v>
       </c>
       <c r="B206" t="s">
-        <v>146</v>
+        <v>680</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>147</v>
+        <v>677</v>
       </c>
       <c r="B207" t="s">
-        <v>148</v>
+        <v>681</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>750</v>
+        <v>145</v>
       </c>
       <c r="B208" t="s">
-        <v>753</v>
+        <v>146</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>751</v>
+        <v>147</v>
       </c>
       <c r="B209" t="s">
-        <v>761</v>
+        <v>148</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B210" t="s">
-        <v>762</v>
+        <v>753</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>536</v>
+        <v>751</v>
       </c>
       <c r="B211" t="s">
-        <v>537</v>
+        <v>761</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>642</v>
+        <v>752</v>
       </c>
       <c r="B212" t="s">
-        <v>654</v>
+        <v>762</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>643</v>
+        <v>536</v>
       </c>
       <c r="B213" t="s">
-        <v>644</v>
+        <v>537</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="B214" t="s">
-        <v>708</v>
+        <v>654</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>706</v>
+        <v>643</v>
       </c>
       <c r="B215" t="s">
-        <v>709</v>
+        <v>644</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>707</v>
+        <v>649</v>
       </c>
       <c r="B216" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>757</v>
+        <v>706</v>
       </c>
       <c r="B217" t="s">
-        <v>760</v>
+        <v>709</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>149</v>
+        <v>707</v>
       </c>
       <c r="B218" t="s">
-        <v>150</v>
+        <v>710</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>151</v>
+        <v>757</v>
       </c>
       <c r="B219" t="s">
-        <v>152</v>
+        <v>760</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B220" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B221" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B222" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B223" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B224" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B225" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B226" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B227" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B228" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B229" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B230" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B231" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B232" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B233" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B234" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B235" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>798</v>
+        <v>181</v>
       </c>
       <c r="B236" t="s">
-        <v>792</v>
+        <v>182</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>799</v>
+        <v>183</v>
       </c>
       <c r="B237" t="s">
-        <v>793</v>
+        <v>184</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B238" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B239" t="s">
-        <v>780</v>
+        <v>793</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B240" t="s">
-        <v>781</v>
+        <v>794</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B241" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B242" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B243" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B244" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>813</v>
+        <v>805</v>
       </c>
       <c r="B245" t="s">
-        <v>783</v>
+        <v>787</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>814</v>
+        <v>806</v>
       </c>
       <c r="B246" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B247" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>807</v>
+        <v>814</v>
       </c>
       <c r="B248" t="s">
-        <v>795</v>
+        <v>784</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>808</v>
+        <v>815</v>
       </c>
       <c r="B249" t="s">
-        <v>796</v>
+        <v>785</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B250" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B251" t="s">
-        <v>789</v>
+        <v>796</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B252" t="s">
-        <v>790</v>
+        <v>797</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B253" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>402</v>
+        <v>811</v>
       </c>
       <c r="B254" t="s">
-        <v>619</v>
+        <v>790</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>407</v>
+        <v>812</v>
       </c>
       <c r="B255" t="s">
-        <v>411</v>
+        <v>791</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="B256" t="s">
-        <v>410</v>
+        <v>619</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>627</v>
+        <v>407</v>
       </c>
       <c r="B257" t="s">
-        <v>628</v>
+        <v>411</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>629</v>
+        <v>408</v>
       </c>
       <c r="B258" t="s">
-        <v>628</v>
+        <v>410</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>434</v>
+        <v>627</v>
       </c>
       <c r="B259" t="s">
-        <v>442</v>
+        <v>628</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>436</v>
+        <v>629</v>
       </c>
       <c r="B260" t="s">
-        <v>443</v>
+        <v>628</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B261" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>756</v>
+        <v>436</v>
       </c>
       <c r="B262" t="s">
-        <v>759</v>
+        <v>443</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>412</v>
+        <v>438</v>
       </c>
       <c r="B263" t="s">
-        <v>415</v>
+        <v>444</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>419</v>
+        <v>756</v>
       </c>
       <c r="B264" t="s">
-        <v>416</v>
+        <v>759</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="B265" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>185</v>
+        <v>419</v>
       </c>
       <c r="B266" t="s">
-        <v>186</v>
+        <v>416</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>187</v>
+        <v>421</v>
       </c>
       <c r="B267" t="s">
-        <v>188</v>
+        <v>416</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>770</v>
+        <v>185</v>
       </c>
       <c r="B268" t="s">
-        <v>736</v>
+        <v>186</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>771</v>
+        <v>187</v>
       </c>
       <c r="B269" t="s">
-        <v>735</v>
+        <v>188</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="B270" t="s">
-        <v>767</v>
+        <v>736</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="B271" t="s">
-        <v>769</v>
+        <v>735</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B272" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>764</v>
+        <v>842</v>
       </c>
       <c r="B273" t="s">
-        <v>763</v>
+        <v>844</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>556</v>
+        <v>843</v>
       </c>
       <c r="B274" t="s">
-        <v>558</v>
+        <v>845</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>742</v>
+        <v>773</v>
       </c>
       <c r="B275" t="s">
-        <v>734</v>
+        <v>769</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>423</v>
+        <v>774</v>
       </c>
       <c r="B276" t="s">
-        <v>426</v>
+        <v>768</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>816</v>
+        <v>764</v>
       </c>
       <c r="B277" t="s">
-        <v>620</v>
+        <v>763</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>431</v>
+        <v>556</v>
       </c>
       <c r="B278" t="s">
-        <v>432</v>
+        <v>558</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>559</v>
+        <v>742</v>
       </c>
       <c r="B279" t="s">
-        <v>579</v>
+        <v>734</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>560</v>
+        <v>423</v>
       </c>
       <c r="B280" t="s">
-        <v>721</v>
+        <v>426</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>720</v>
+        <v>816</v>
       </c>
       <c r="B281" t="s">
-        <v>582</v>
+        <v>620</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>561</v>
+        <v>431</v>
       </c>
       <c r="B282" t="s">
-        <v>585</v>
+        <v>432</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B283" t="s">
-        <v>722</v>
+        <v>579</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>719</v>
+        <v>560</v>
       </c>
       <c r="B284" t="s">
-        <v>587</v>
+        <v>721</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>563</v>
+        <v>720</v>
       </c>
       <c r="B285" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B286" t="s">
-        <v>723</v>
+        <v>585</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>718</v>
+        <v>562</v>
       </c>
       <c r="B287" t="s">
-        <v>583</v>
+        <v>722</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>565</v>
+        <v>719</v>
       </c>
       <c r="B288" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B289" t="s">
-        <v>724</v>
+        <v>580</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>717</v>
+        <v>564</v>
       </c>
       <c r="B290" t="s">
-        <v>588</v>
+        <v>723</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>567</v>
+        <v>718</v>
       </c>
       <c r="B291" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B292" t="s">
-        <v>725</v>
+        <v>586</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>716</v>
+        <v>566</v>
       </c>
       <c r="B293" t="s">
-        <v>584</v>
+        <v>724</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>189</v>
+        <v>717</v>
       </c>
       <c r="B294" t="s">
-        <v>190</v>
+        <v>588</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>191</v>
+        <v>567</v>
       </c>
       <c r="B295" t="s">
-        <v>192</v>
+        <v>581</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>193</v>
+        <v>568</v>
       </c>
       <c r="B296" t="s">
-        <v>194</v>
+        <v>725</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>195</v>
+        <v>716</v>
       </c>
       <c r="B297" t="s">
-        <v>196</v>
+        <v>584</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B298" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>673</v>
+        <v>191</v>
       </c>
       <c r="B299" t="s">
-        <v>678</v>
+        <v>192</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>674</v>
+        <v>193</v>
       </c>
       <c r="B300" t="s">
-        <v>682</v>
+        <v>194</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>675</v>
+        <v>195</v>
       </c>
       <c r="B301" t="s">
-        <v>683</v>
+        <v>196</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B302" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>201</v>
+        <v>673</v>
       </c>
       <c r="B303" t="s">
-        <v>202</v>
+        <v>678</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>744</v>
+        <v>674</v>
       </c>
       <c r="B304" t="s">
-        <v>747</v>
+        <v>682</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>745</v>
+        <v>675</v>
       </c>
       <c r="B305" t="s">
-        <v>748</v>
+        <v>683</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>746</v>
+        <v>199</v>
       </c>
       <c r="B306" t="s">
-        <v>749</v>
+        <v>200</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>538</v>
+        <v>201</v>
       </c>
       <c r="B307" t="s">
-        <v>539</v>
+        <v>202</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>638</v>
+        <v>744</v>
       </c>
       <c r="B308" t="s">
-        <v>640</v>
+        <v>747</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>639</v>
+        <v>745</v>
       </c>
       <c r="B309" t="s">
-        <v>641</v>
+        <v>748</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>647</v>
+        <v>746</v>
       </c>
       <c r="B310" t="s">
-        <v>648</v>
+        <v>749</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>702</v>
+        <v>538</v>
       </c>
       <c r="B311" t="s">
-        <v>704</v>
+        <v>539</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>703</v>
+        <v>638</v>
       </c>
       <c r="B312" t="s">
-        <v>705</v>
+        <v>640</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>755</v>
+        <v>639</v>
       </c>
       <c r="B313" t="s">
-        <v>758</v>
+        <v>641</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>203</v>
+        <v>647</v>
       </c>
       <c r="B314" t="s">
-        <v>204</v>
+        <v>648</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>205</v>
+        <v>702</v>
       </c>
       <c r="B315" t="s">
-        <v>206</v>
+        <v>704</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>207</v>
+        <v>703</v>
       </c>
       <c r="B316" t="s">
-        <v>208</v>
+        <v>705</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>209</v>
+        <v>755</v>
       </c>
       <c r="B317" t="s">
-        <v>210</v>
+        <v>758</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B318" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B319" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B320" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B321" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B322" t="s">
-        <v>166</v>
+        <v>212</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B323" t="s">
-        <v>168</v>
+        <v>214</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B324" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B325" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B326" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B327" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B328" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B329" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B330" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B331" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>817</v>
+        <v>223</v>
       </c>
       <c r="B332" t="s">
-        <v>792</v>
+        <v>178</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>818</v>
+        <v>224</v>
       </c>
       <c r="B333" t="s">
-        <v>793</v>
+        <v>180</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>819</v>
+        <v>225</v>
       </c>
       <c r="B334" t="s">
-        <v>794</v>
+        <v>182</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>820</v>
+        <v>226</v>
       </c>
       <c r="B335" t="s">
-        <v>780</v>
+        <v>184</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="B336" t="s">
-        <v>781</v>
+        <v>792</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B337" t="s">
-        <v>782</v>
+        <v>793</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="B338" t="s">
-        <v>786</v>
+        <v>794</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="B339" t="s">
-        <v>787</v>
+        <v>780</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="B340" t="s">
-        <v>788</v>
+        <v>781</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="B341" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B342" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="B343" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="B344" t="s">
-        <v>795</v>
+        <v>788</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="B345" t="s">
-        <v>796</v>
+        <v>783</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="B346" t="s">
-        <v>797</v>
+        <v>784</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="B347" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="B348" t="s">
-        <v>790</v>
+        <v>795</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B349" t="s">
-        <v>791</v>
+        <v>796</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>401</v>
+        <v>831</v>
       </c>
       <c r="B350" t="s">
-        <v>403</v>
+        <v>797</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>406</v>
+        <v>832</v>
       </c>
       <c r="B351" t="s">
-        <v>404</v>
+        <v>789</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>409</v>
+        <v>833</v>
       </c>
       <c r="B352" t="s">
-        <v>405</v>
+        <v>790</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>630</v>
+        <v>834</v>
       </c>
       <c r="B353" t="s">
-        <v>631</v>
+        <v>791</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>632</v>
+        <v>401</v>
       </c>
       <c r="B354" t="s">
-        <v>633</v>
+        <v>403</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>657</v>
+        <v>406</v>
       </c>
       <c r="B355" t="s">
-        <v>660</v>
+        <v>404</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>661</v>
+        <v>409</v>
       </c>
       <c r="B356" t="s">
-        <v>663</v>
+        <v>405</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>662</v>
+        <v>630</v>
       </c>
       <c r="B357" t="s">
-        <v>668</v>
+        <v>631</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>433</v>
+        <v>632</v>
       </c>
       <c r="B358" t="s">
-        <v>439</v>
+        <v>633</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>435</v>
+        <v>657</v>
       </c>
       <c r="B359" t="s">
-        <v>440</v>
+        <v>660</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>437</v>
+        <v>661</v>
       </c>
       <c r="B360" t="s">
-        <v>441</v>
+        <v>663</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>754</v>
+        <v>662</v>
       </c>
       <c r="B361" t="s">
-        <v>691</v>
+        <v>668</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>413</v>
+        <v>433</v>
       </c>
       <c r="B362" t="s">
-        <v>414</v>
+        <v>439</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>420</v>
+        <v>435</v>
       </c>
       <c r="B363" t="s">
-        <v>417</v>
+        <v>440</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>422</v>
+        <v>437</v>
       </c>
       <c r="B364" t="s">
-        <v>418</v>
+        <v>441</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>227</v>
+        <v>754</v>
       </c>
       <c r="B365" t="s">
-        <v>228</v>
+        <v>691</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>229</v>
+        <v>413</v>
       </c>
       <c r="B366" t="s">
-        <v>230</v>
+        <v>414</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>775</v>
+        <v>420</v>
       </c>
       <c r="B367" t="s">
-        <v>738</v>
+        <v>417</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>776</v>
+        <v>422</v>
       </c>
       <c r="B368" t="s">
-        <v>737</v>
+        <v>418</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>777</v>
+        <v>227</v>
       </c>
       <c r="B369" t="s">
-        <v>612</v>
+        <v>228</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>778</v>
+        <v>229</v>
       </c>
       <c r="B370" t="s">
-        <v>596</v>
+        <v>230</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="B371" t="s">
-        <v>597</v>
+        <v>738</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="B372" t="s">
-        <v>765</v>
+        <v>737</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>555</v>
+        <v>777</v>
       </c>
       <c r="B373" t="s">
-        <v>557</v>
+        <v>612</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>741</v>
+        <v>835</v>
       </c>
       <c r="B374" t="s">
-        <v>731</v>
+        <v>595</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>739</v>
+        <v>778</v>
       </c>
       <c r="B375" t="s">
-        <v>732</v>
+        <v>596</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>740</v>
+        <v>779</v>
       </c>
       <c r="B376" t="s">
-        <v>733</v>
+        <v>597</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>424</v>
+        <v>836</v>
       </c>
       <c r="B377" t="s">
-        <v>425</v>
+        <v>838</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>429</v>
+        <v>837</v>
       </c>
       <c r="B378" t="s">
-        <v>427</v>
+        <v>839</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>430</v>
+        <v>766</v>
       </c>
       <c r="B379" t="s">
-        <v>428</v>
+        <v>765</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>231</v>
+        <v>555</v>
       </c>
       <c r="B380" t="s">
-        <v>232</v>
+        <v>557</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>233</v>
+        <v>741</v>
       </c>
       <c r="B381" t="s">
-        <v>234</v>
+        <v>731</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>235</v>
+        <v>739</v>
       </c>
       <c r="B382" t="s">
-        <v>236</v>
+        <v>732</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>237</v>
+        <v>740</v>
       </c>
       <c r="B383" t="s">
-        <v>238</v>
+        <v>733</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
+        <v>424</v>
+      </c>
+      <c r="B384" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A385" t="s">
+        <v>429</v>
+      </c>
+      <c r="B385" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A386" t="s">
+        <v>430</v>
+      </c>
+      <c r="B386" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A387" t="s">
+        <v>231</v>
+      </c>
+      <c r="B387" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A388" t="s">
+        <v>233</v>
+      </c>
+      <c r="B388" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A389" t="s">
+        <v>235</v>
+      </c>
+      <c r="B389" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A390" t="s">
+        <v>237</v>
+      </c>
+      <c r="B390" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A391" t="s">
         <v>239</v>
       </c>
-      <c r="B384" t="s">
+      <c r="B391" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A385" t="s">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A392" t="s">
         <v>241</v>
       </c>
-      <c r="B385" t="s">
+      <c r="B392" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A386" t="s">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A393" t="s">
         <v>243</v>
       </c>
-      <c r="B386" t="s">
+      <c r="B393" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A387" t="s">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A394" t="s">
         <v>245</v>
       </c>
-      <c r="B387" t="s">
+      <c r="B394" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A388" t="s">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A395" t="s">
         <v>247</v>
       </c>
-      <c r="B388" t="s">
+      <c r="B395" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A389" t="s">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A396" t="s">
         <v>249</v>
       </c>
-      <c r="B389" t="s">
+      <c r="B396" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A390" t="s">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A397" t="s">
         <v>251</v>
       </c>
-      <c r="B390" t="s">
+      <c r="B397" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A391" t="s">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A398" t="s">
         <v>253</v>
       </c>
-      <c r="B391" t="s">
+      <c r="B398" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A392" t="s">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A399" t="s">
         <v>255</v>
       </c>
-      <c r="B392" t="s">
+      <c r="B399" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A393" t="s">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A400" t="s">
         <v>257</v>
       </c>
-      <c r="B393" t="s">
+      <c r="B400" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A394" t="s">
-        <v>259</v>
-      </c>
-      <c r="B394" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A395" t="s">
-        <v>261</v>
-      </c>
-      <c r="B395" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A396" t="s">
-        <v>263</v>
-      </c>
-      <c r="B396" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A397" t="s">
-        <v>265</v>
-      </c>
-      <c r="B397" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A398" t="s">
-        <v>267</v>
-      </c>
-      <c r="B398" t="s">
-        <v>268</v>
-      </c>
-      <c r="C398" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A399" t="s">
-        <v>361</v>
-      </c>
-      <c r="B399" t="s">
-        <v>363</v>
-      </c>
-      <c r="C399" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A400" t="s">
-        <v>269</v>
-      </c>
-      <c r="B400" t="s">
-        <v>270</v>
-      </c>
-      <c r="C400" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>501</v>
+        <v>259</v>
       </c>
       <c r="B401" t="s">
-        <v>509</v>
+        <v>260</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B402" t="s">
-        <v>652</v>
-      </c>
-      <c r="C402" t="s">
-        <v>653</v>
+        <v>262</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>316</v>
+        <v>263</v>
       </c>
       <c r="B403" t="s">
-        <v>321</v>
-      </c>
-      <c r="C403" t="s">
-        <v>318</v>
+        <v>264</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>317</v>
+        <v>265</v>
       </c>
       <c r="B404" t="s">
-        <v>320</v>
-      </c>
-      <c r="C404" t="s">
-        <v>324</v>
+        <v>266</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B405" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C405" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>288</v>
+        <v>361</v>
       </c>
       <c r="B406" t="s">
-        <v>303</v>
+        <v>363</v>
       </c>
       <c r="C406" t="s">
-        <v>306</v>
+        <v>362</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="B407" t="s">
-        <v>302</v>
+        <v>270</v>
       </c>
       <c r="C407" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>274</v>
+        <v>501</v>
       </c>
       <c r="B408" t="s">
-        <v>275</v>
-      </c>
-      <c r="C408" t="s">
-        <v>275</v>
+        <v>509</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>341</v>
+        <v>271</v>
       </c>
       <c r="B409" t="s">
-        <v>342</v>
+        <v>652</v>
       </c>
       <c r="C409" t="s">
-        <v>343</v>
+        <v>653</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B410" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C410" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B411" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C411" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>359</v>
+        <v>272</v>
       </c>
       <c r="B412" t="s">
-        <v>365</v>
+        <v>273</v>
       </c>
       <c r="C412" t="s">
-        <v>369</v>
+        <v>273</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="B413" t="s">
-        <v>277</v>
+        <v>303</v>
       </c>
       <c r="C413" t="s">
-        <v>277</v>
+        <v>306</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>360</v>
+        <v>292</v>
       </c>
       <c r="B414" t="s">
-        <v>366</v>
+        <v>302</v>
       </c>
       <c r="C414" t="s">
-        <v>370</v>
+        <v>305</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>356</v>
+        <v>274</v>
       </c>
       <c r="B415" t="s">
-        <v>368</v>
+        <v>275</v>
       </c>
       <c r="C415" t="s">
-        <v>376</v>
+        <v>275</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>278</v>
+        <v>341</v>
       </c>
       <c r="B416" t="s">
-        <v>279</v>
+        <v>342</v>
       </c>
       <c r="C416" t="s">
-        <v>313</v>
+        <v>343</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>280</v>
+        <v>314</v>
       </c>
       <c r="B417" t="s">
-        <v>281</v>
+        <v>322</v>
       </c>
       <c r="C417" t="s">
-        <v>281</v>
+        <v>319</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
-        <v>291</v>
+        <v>315</v>
       </c>
       <c r="B418" t="s">
-        <v>296</v>
+        <v>323</v>
       </c>
       <c r="C418" t="s">
-        <v>304</v>
+        <v>325</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
-        <v>295</v>
+        <v>359</v>
       </c>
       <c r="B419" t="s">
-        <v>301</v>
+        <v>365</v>
       </c>
       <c r="C419" t="s">
-        <v>308</v>
+        <v>369</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
-        <v>634</v>
+        <v>276</v>
       </c>
       <c r="B420" t="s">
-        <v>635</v>
+        <v>277</v>
+      </c>
+      <c r="C420" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
-        <v>636</v>
+        <v>360</v>
       </c>
       <c r="B421" t="s">
-        <v>637</v>
+        <v>366</v>
+      </c>
+      <c r="C421" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
-        <v>392</v>
+        <v>356</v>
       </c>
       <c r="B422" t="s">
-        <v>397</v>
+        <v>368</v>
       </c>
       <c r="C422" t="s">
-        <v>398</v>
+        <v>376</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
-        <v>358</v>
+        <v>278</v>
       </c>
       <c r="B423" t="s">
-        <v>364</v>
+        <v>279</v>
+      </c>
+      <c r="C423" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B424" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C424" t="s">
-        <v>354</v>
+        <v>281</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="B425" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="C425" t="s">
-        <v>285</v>
+        <v>304</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="B426" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C426" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
-        <v>294</v>
+        <v>634</v>
       </c>
       <c r="B427" t="s">
-        <v>300</v>
-      </c>
-      <c r="C427" t="s">
-        <v>310</v>
+        <v>635</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
-        <v>286</v>
+        <v>636</v>
       </c>
       <c r="B428" t="s">
-        <v>287</v>
-      </c>
-      <c r="C428" t="s">
-        <v>287</v>
+        <v>637</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
-        <v>289</v>
+        <v>392</v>
       </c>
       <c r="B429" t="s">
-        <v>298</v>
+        <v>397</v>
       </c>
       <c r="C429" t="s">
-        <v>311</v>
+        <v>398</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
-        <v>293</v>
+        <v>358</v>
       </c>
       <c r="B430" t="s">
-        <v>299</v>
-      </c>
-      <c r="C430" t="s">
-        <v>312</v>
+        <v>364</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
+        <v>282</v>
+      </c>
+      <c r="B431" t="s">
+        <v>283</v>
+      </c>
+      <c r="C431" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A432" t="s">
+        <v>284</v>
+      </c>
+      <c r="B432" t="s">
+        <v>285</v>
+      </c>
+      <c r="C432" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A433" t="s">
+        <v>290</v>
+      </c>
+      <c r="B433" t="s">
+        <v>297</v>
+      </c>
+      <c r="C433" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A434" t="s">
+        <v>294</v>
+      </c>
+      <c r="B434" t="s">
+        <v>300</v>
+      </c>
+      <c r="C434" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A435" t="s">
+        <v>286</v>
+      </c>
+      <c r="B435" t="s">
+        <v>287</v>
+      </c>
+      <c r="C435" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A436" t="s">
+        <v>289</v>
+      </c>
+      <c r="B436" t="s">
+        <v>298</v>
+      </c>
+      <c r="C436" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A437" t="s">
+        <v>293</v>
+      </c>
+      <c r="B437" t="s">
+        <v>299</v>
+      </c>
+      <c r="C437" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A438" t="s">
         <v>357</v>
       </c>
-      <c r="B431" t="s">
+      <c r="B438" t="s">
         <v>367</v>
       </c>
-      <c r="C431" t="s">
+      <c r="C438" t="s">
         <v>375</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K393">
-    <sortState ref="A2:K431">
-      <sortCondition ref="A1:A393"/>
+  <autoFilter ref="A1:K400">
+    <sortState ref="A2:K438">
+      <sortCondition ref="A1:A400"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added underground storage + tech tree gas split up
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$400</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$415</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="872">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -2561,6 +2561,84 @@
   </si>
   <si>
     <t>Advanceed cooling for cannons to maximize the rate of fire</t>
+  </si>
+  <si>
+    <t>gui/hud/building_description/solid_material_storage_underground</t>
+  </si>
+  <si>
+    <t>Underground storage facility for all solid materials</t>
+  </si>
+  <si>
+    <t>gui/hud/building_name/solid_material_storage_underground</t>
+  </si>
+  <si>
+    <t>Underground Storage</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/solid_material_storage_underground</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/solid_material_storage_underground</t>
+  </si>
+  <si>
+    <t>Enables construction of underground storage with enormous capacity</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/gas_filtering_lvl2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/gas_filtering_lvl3</t>
+  </si>
+  <si>
+    <t>Gas Filtering 2</t>
+  </si>
+  <si>
+    <t>Gas Filtering 3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/gas_filtering_lvl3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/gas_filtering_lvl2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/ai_hub_lvl2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/ai_hub_lvl3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/fire_control_station</t>
+  </si>
+  <si>
+    <t>AI Hub - Cooled</t>
+  </si>
+  <si>
+    <t>AI Hub - Supercooled</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/ai_hub_lvl2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/ai_hub_lvl3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/fire_control_station</t>
+  </si>
+  <si>
+    <t>This technology survails the surroundings for threats and enables intelligent defense buildings control to save resources</t>
+  </si>
+  <si>
+    <t>Improved computation capacity by cooling</t>
+  </si>
+  <si>
+    <t>Improved computation capacity by advanced cooling</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/ai_hub</t>
+  </si>
+  <si>
+    <t>AI Hub</t>
   </si>
 </sst>
 </file>
@@ -3385,11 +3463,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K438"/>
+  <dimension ref="A1:K453"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A312" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B323" sqref="B323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3889,26 +3967,26 @@
     </row>
     <row r="58" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>347</v>
+        <v>846</v>
       </c>
       <c r="B58" t="s">
-        <v>351</v>
-      </c>
-      <c r="C58" t="s">
-        <v>355</v>
+        <v>847</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>347</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>351</v>
+      </c>
+      <c r="C59" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
         <v>65</v>
@@ -3916,7 +3994,7 @@
     </row>
     <row r="61" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B61" t="s">
         <v>65</v>
@@ -3924,522 +4002,519 @@
     </row>
     <row r="62" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>713</v>
+        <v>68</v>
       </c>
       <c r="B63" t="s">
-        <v>655</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B64" t="s">
-        <v>714</v>
+        <v>655</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B65" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>711</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>715</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>481</v>
+        <v>72</v>
       </c>
       <c r="B68" t="s">
-        <v>511</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B69" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="B70" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B71" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>490</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
+        <v>519</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>454</v>
+        <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>531</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B74" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B75" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B76" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>553</v>
+        <v>459</v>
       </c>
       <c r="B77" t="s">
-        <v>554</v>
+        <v>530</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>487</v>
+        <v>553</v>
       </c>
       <c r="B78" t="s">
-        <v>516</v>
+        <v>554</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B79" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="B80" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B81" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B82" t="s">
-        <v>610</v>
+        <v>515</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>486</v>
+      </c>
+      <c r="B83" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>484</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>513</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>493</v>
-      </c>
-      <c r="B84" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B85" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B86" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
+        <v>495</v>
+      </c>
+      <c r="B87" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>496</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>525</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>498</v>
-      </c>
-      <c r="B88" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B89" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="B90" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B91" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>544</v>
+        <v>492</v>
       </c>
       <c r="B92" t="s">
-        <v>548</v>
+        <v>521</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B93" t="s">
-        <v>611</v>
+        <v>548</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B94" t="s">
-        <v>549</v>
+        <v>611</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>76</v>
+        <v>543</v>
       </c>
       <c r="B95" t="s">
-        <v>77</v>
+        <v>549</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B96" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B97" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B98" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B99" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>445</v>
+        <v>84</v>
       </c>
       <c r="B100" t="s">
-        <v>449</v>
+        <v>85</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>86</v>
+        <v>445</v>
       </c>
       <c r="B101" t="s">
-        <v>87</v>
+        <v>449</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B102" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B103" t="s">
-        <v>592</v>
+        <v>89</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>590</v>
+        <v>90</v>
       </c>
       <c r="B104" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>91</v>
+        <v>590</v>
       </c>
       <c r="B105" t="s">
-        <v>92</v>
+        <v>591</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B106" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B107" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>446</v>
+        <v>95</v>
       </c>
       <c r="B108" t="s">
-        <v>450</v>
+        <v>96</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>97</v>
+        <v>446</v>
       </c>
       <c r="B109" t="s">
-        <v>98</v>
+        <v>450</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B110" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B111" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B112" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B113" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B114" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B115" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B116" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B117" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B118" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>499</v>
+        <v>115</v>
       </c>
       <c r="B119" t="s">
-        <v>507</v>
+        <v>116</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>645</v>
+        <v>499</v>
       </c>
       <c r="B120" t="s">
-        <v>646</v>
+        <v>507</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>500</v>
+        <v>645</v>
       </c>
       <c r="B121" t="s">
-        <v>508</v>
+        <v>646</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
+        <v>500</v>
+      </c>
+      <c r="B122" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>117</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
-        <v>379</v>
-      </c>
-      <c r="B123" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>462</v>
+        <v>379</v>
       </c>
       <c r="B124" t="s">
-        <v>504</v>
+        <v>381</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>345</v>
+        <v>462</v>
       </c>
       <c r="B125" t="s">
-        <v>346</v>
-      </c>
-      <c r="C125" t="s">
-        <v>352</v>
+        <v>504</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B126" t="s">
         <v>346</v>
@@ -4450,7 +4525,7 @@
     </row>
     <row r="127" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B127" t="s">
         <v>346</v>
@@ -4461,109 +4536,109 @@
     </row>
     <row r="128" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>656</v>
+        <v>349</v>
       </c>
       <c r="B128" t="s">
-        <v>659</v>
+        <v>346</v>
+      </c>
+      <c r="C128" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>119</v>
+        <v>656</v>
       </c>
       <c r="B129" t="s">
-        <v>120</v>
+        <v>659</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>378</v>
+        <v>119</v>
       </c>
       <c r="B130" t="s">
-        <v>371</v>
-      </c>
-      <c r="C130" t="s">
-        <v>373</v>
+        <v>120</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>327</v>
+        <v>378</v>
       </c>
       <c r="B131" t="s">
-        <v>334</v>
+        <v>371</v>
+      </c>
+      <c r="C131" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B132" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B133" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>121</v>
+        <v>329</v>
       </c>
       <c r="B134" t="s">
-        <v>122</v>
+        <v>340</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B135" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B136" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B137" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>625</v>
+        <v>127</v>
       </c>
       <c r="B138" t="s">
-        <v>626</v>
+        <v>128</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>388</v>
+        <v>625</v>
       </c>
       <c r="B139" t="s">
-        <v>395</v>
-      </c>
-      <c r="C139" t="s">
-        <v>399</v>
+        <v>626</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B140" t="s">
         <v>395</v>
@@ -4574,7 +4649,7 @@
     </row>
     <row r="141" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B141" t="s">
         <v>395</v>
@@ -4585,2477 +4660,2600 @@
     </row>
     <row r="142" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B142" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C142" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>686</v>
+        <v>391</v>
       </c>
       <c r="B143" t="s">
-        <v>690</v>
+        <v>396</v>
+      </c>
+      <c r="C143" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B144" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="B145" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>129</v>
+        <v>684</v>
       </c>
       <c r="B146" t="s">
-        <v>130</v>
+        <v>691</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>131</v>
+        <v>848</v>
       </c>
       <c r="B147" t="s">
-        <v>132</v>
+        <v>849</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>331</v>
+        <v>129</v>
       </c>
       <c r="B148" t="s">
-        <v>332</v>
+        <v>130</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>330</v>
+        <v>131</v>
       </c>
       <c r="B149" t="s">
-        <v>333</v>
+        <v>132</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>699</v>
+        <v>331</v>
       </c>
       <c r="B150" t="s">
-        <v>698</v>
+        <v>332</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>696</v>
+        <v>330</v>
       </c>
       <c r="B151" t="s">
-        <v>700</v>
+        <v>333</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B152" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>463</v>
+        <v>696</v>
       </c>
       <c r="B153" t="s">
-        <v>601</v>
+        <v>700</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>464</v>
+        <v>697</v>
       </c>
       <c r="B154" t="s">
-        <v>600</v>
+        <v>701</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="B155" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="B156" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>133</v>
+        <v>471</v>
       </c>
       <c r="B157" t="s">
-        <v>134</v>
+        <v>599</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>457</v>
+        <v>472</v>
       </c>
       <c r="B158" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>456</v>
+        <v>133</v>
       </c>
       <c r="B159" t="s">
-        <v>595</v>
+        <v>134</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B160" t="s">
-        <v>596</v>
+        <v>612</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B161" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>840</v>
+        <v>458</v>
       </c>
       <c r="B162" t="s">
-        <v>838</v>
+        <v>596</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>841</v>
+        <v>460</v>
       </c>
       <c r="B163" t="s">
-        <v>839</v>
+        <v>597</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>550</v>
+        <v>840</v>
       </c>
       <c r="B164" t="s">
-        <v>551</v>
+        <v>838</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>469</v>
+        <v>841</v>
       </c>
       <c r="B165" t="s">
-        <v>613</v>
+        <v>839</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>470</v>
+        <v>550</v>
       </c>
       <c r="B166" t="s">
-        <v>614</v>
+        <v>551</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="B167" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B168" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B169" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B170" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="B171" t="s">
-        <v>505</v>
+        <v>617</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
       <c r="B172" t="s">
-        <v>602</v>
+        <v>618</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B173" t="s">
-        <v>603</v>
+        <v>505</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B174" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B175" t="s">
-        <v>506</v>
+        <v>603</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B176" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="B177" t="s">
-        <v>605</v>
+        <v>506</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="B178" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>540</v>
+        <v>473</v>
       </c>
       <c r="B179" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>542</v>
+        <v>474</v>
       </c>
       <c r="B180" t="s">
-        <v>552</v>
+        <v>606</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B181" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>135</v>
+        <v>542</v>
       </c>
       <c r="B182" t="s">
-        <v>136</v>
+        <v>552</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="B183" t="s">
-        <v>547</v>
+        <v>607</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>534</v>
+        <v>135</v>
       </c>
       <c r="B184" t="s">
-        <v>535</v>
+        <v>136</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>569</v>
+        <v>546</v>
       </c>
       <c r="B185" t="s">
-        <v>579</v>
+        <v>547</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>570</v>
+        <v>534</v>
       </c>
       <c r="B186" t="s">
-        <v>721</v>
+        <v>535</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>726</v>
+        <v>864</v>
       </c>
       <c r="B187" t="s">
-        <v>582</v>
+        <v>868</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>571</v>
+        <v>865</v>
       </c>
       <c r="B188" t="s">
-        <v>585</v>
+        <v>869</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B189" t="s">
-        <v>722</v>
+        <v>579</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>727</v>
+        <v>570</v>
       </c>
       <c r="B190" t="s">
-        <v>587</v>
+        <v>721</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>573</v>
+        <v>726</v>
       </c>
       <c r="B191" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B192" t="s">
-        <v>723</v>
+        <v>585</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>728</v>
+        <v>572</v>
       </c>
       <c r="B193" t="s">
-        <v>583</v>
+        <v>722</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>575</v>
+        <v>727</v>
       </c>
       <c r="B194" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B195" t="s">
-        <v>724</v>
+        <v>580</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>729</v>
+        <v>574</v>
       </c>
       <c r="B196" t="s">
-        <v>588</v>
+        <v>723</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>577</v>
+        <v>728</v>
       </c>
       <c r="B197" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B198" t="s">
-        <v>725</v>
+        <v>586</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>730</v>
+        <v>576</v>
       </c>
       <c r="B199" t="s">
-        <v>584</v>
+        <v>724</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>137</v>
+        <v>729</v>
       </c>
       <c r="B200" t="s">
-        <v>138</v>
+        <v>588</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>139</v>
+        <v>577</v>
       </c>
       <c r="B201" t="s">
-        <v>140</v>
+        <v>581</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>141</v>
+        <v>578</v>
       </c>
       <c r="B202" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>143</v>
+        <v>730</v>
       </c>
       <c r="B203" t="s">
-        <v>142</v>
+        <v>584</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
+        <v>137</v>
+      </c>
+      <c r="B204" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>139</v>
+      </c>
+      <c r="B205" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>141</v>
+      </c>
+      <c r="B206" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>143</v>
+      </c>
+      <c r="B207" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
         <v>144</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B208" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A205" t="s">
+    <row r="209" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
         <v>672</v>
       </c>
-      <c r="B205" t="s">
+      <c r="B209" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A206" t="s">
+    <row r="210" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
         <v>676</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B210" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A207" t="s">
+    <row r="211" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
         <v>677</v>
       </c>
-      <c r="B207" t="s">
+      <c r="B211" t="s">
         <v>681</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A208" t="s">
-        <v>145</v>
-      </c>
-      <c r="B208" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A209" t="s">
-        <v>147</v>
-      </c>
-      <c r="B209" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A210" t="s">
-        <v>750</v>
-      </c>
-      <c r="B210" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A211" t="s">
-        <v>751</v>
-      </c>
-      <c r="B211" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>752</v>
+        <v>145</v>
       </c>
       <c r="B212" t="s">
-        <v>762</v>
+        <v>146</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>536</v>
+        <v>147</v>
       </c>
       <c r="B213" t="s">
-        <v>537</v>
+        <v>148</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>642</v>
+        <v>750</v>
       </c>
       <c r="B214" t="s">
-        <v>654</v>
+        <v>753</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>643</v>
+        <v>751</v>
       </c>
       <c r="B215" t="s">
-        <v>644</v>
+        <v>761</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>649</v>
+        <v>752</v>
       </c>
       <c r="B216" t="s">
-        <v>708</v>
+        <v>762</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>706</v>
+        <v>536</v>
       </c>
       <c r="B217" t="s">
-        <v>709</v>
+        <v>537</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>707</v>
+        <v>642</v>
       </c>
       <c r="B218" t="s">
-        <v>710</v>
+        <v>654</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>757</v>
+        <v>643</v>
       </c>
       <c r="B219" t="s">
-        <v>760</v>
+        <v>644</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>149</v>
+        <v>649</v>
       </c>
       <c r="B220" t="s">
-        <v>150</v>
+        <v>708</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>151</v>
+        <v>706</v>
       </c>
       <c r="B221" t="s">
-        <v>152</v>
+        <v>709</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>153</v>
+        <v>707</v>
       </c>
       <c r="B222" t="s">
-        <v>154</v>
+        <v>710</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>155</v>
+        <v>866</v>
       </c>
       <c r="B223" t="s">
-        <v>156</v>
+        <v>867</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>157</v>
+        <v>858</v>
       </c>
       <c r="B224" t="s">
-        <v>158</v>
+        <v>855</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>159</v>
+        <v>857</v>
       </c>
       <c r="B225" t="s">
-        <v>160</v>
+        <v>856</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>161</v>
+        <v>757</v>
       </c>
       <c r="B226" t="s">
-        <v>162</v>
+        <v>760</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B227" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="B228" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B229" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B230" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B231" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="B232" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B233" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B234" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="B235" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="B236" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="B237" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>798</v>
+        <v>171</v>
       </c>
       <c r="B238" t="s">
-        <v>792</v>
+        <v>172</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>799</v>
+        <v>173</v>
       </c>
       <c r="B239" t="s">
-        <v>793</v>
+        <v>174</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="B240" t="s">
-        <v>794</v>
+        <v>176</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>801</v>
+        <v>177</v>
       </c>
       <c r="B241" t="s">
-        <v>780</v>
+        <v>178</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>802</v>
+        <v>179</v>
       </c>
       <c r="B242" t="s">
-        <v>781</v>
+        <v>180</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>803</v>
+        <v>181</v>
       </c>
       <c r="B243" t="s">
-        <v>782</v>
+        <v>182</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>804</v>
+        <v>183</v>
       </c>
       <c r="B244" t="s">
-        <v>786</v>
+        <v>184</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>805</v>
+        <v>798</v>
       </c>
       <c r="B245" t="s">
-        <v>787</v>
+        <v>792</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>806</v>
+        <v>799</v>
       </c>
       <c r="B246" t="s">
-        <v>788</v>
+        <v>793</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>813</v>
+        <v>800</v>
       </c>
       <c r="B247" t="s">
-        <v>783</v>
+        <v>794</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="B248" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>815</v>
+        <v>802</v>
       </c>
       <c r="B249" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="B250" t="s">
-        <v>795</v>
+        <v>782</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="B251" t="s">
-        <v>796</v>
+        <v>786</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="B252" t="s">
-        <v>797</v>
+        <v>787</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B253" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="B254" t="s">
-        <v>790</v>
+        <v>783</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="B255" t="s">
-        <v>791</v>
+        <v>784</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>402</v>
+        <v>815</v>
       </c>
       <c r="B256" t="s">
-        <v>619</v>
+        <v>785</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>407</v>
+        <v>807</v>
       </c>
       <c r="B257" t="s">
-        <v>411</v>
+        <v>795</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>408</v>
+        <v>808</v>
       </c>
       <c r="B258" t="s">
-        <v>410</v>
+        <v>796</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>627</v>
+        <v>809</v>
       </c>
       <c r="B259" t="s">
-        <v>628</v>
+        <v>797</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>629</v>
+        <v>810</v>
       </c>
       <c r="B260" t="s">
-        <v>628</v>
+        <v>789</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>434</v>
+        <v>811</v>
       </c>
       <c r="B261" t="s">
-        <v>442</v>
+        <v>790</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>436</v>
+        <v>812</v>
       </c>
       <c r="B262" t="s">
-        <v>443</v>
+        <v>791</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>438</v>
+        <v>402</v>
       </c>
       <c r="B263" t="s">
-        <v>444</v>
+        <v>619</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>756</v>
+        <v>407</v>
       </c>
       <c r="B264" t="s">
-        <v>759</v>
+        <v>411</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B265" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>419</v>
+        <v>627</v>
       </c>
       <c r="B266" t="s">
-        <v>416</v>
+        <v>628</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>421</v>
+        <v>629</v>
       </c>
       <c r="B267" t="s">
-        <v>416</v>
+        <v>628</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>185</v>
+        <v>434</v>
       </c>
       <c r="B268" t="s">
-        <v>186</v>
+        <v>442</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>187</v>
+        <v>436</v>
       </c>
       <c r="B269" t="s">
-        <v>188</v>
+        <v>443</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>770</v>
+        <v>438</v>
       </c>
       <c r="B270" t="s">
-        <v>736</v>
+        <v>444</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>771</v>
+        <v>756</v>
       </c>
       <c r="B271" t="s">
-        <v>735</v>
+        <v>759</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>772</v>
+        <v>412</v>
       </c>
       <c r="B272" t="s">
-        <v>767</v>
+        <v>415</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>842</v>
+        <v>419</v>
       </c>
       <c r="B273" t="s">
-        <v>844</v>
+        <v>416</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>843</v>
+        <v>421</v>
       </c>
       <c r="B274" t="s">
-        <v>845</v>
+        <v>416</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>773</v>
+        <v>850</v>
       </c>
       <c r="B275" t="s">
-        <v>769</v>
+        <v>852</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>774</v>
+        <v>185</v>
       </c>
       <c r="B276" t="s">
-        <v>768</v>
+        <v>186</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>764</v>
+        <v>187</v>
       </c>
       <c r="B277" t="s">
-        <v>763</v>
+        <v>188</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>556</v>
+        <v>770</v>
       </c>
       <c r="B278" t="s">
-        <v>558</v>
+        <v>736</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>742</v>
+        <v>771</v>
       </c>
       <c r="B279" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>423</v>
+        <v>772</v>
       </c>
       <c r="B280" t="s">
-        <v>426</v>
+        <v>767</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>816</v>
+        <v>842</v>
       </c>
       <c r="B281" t="s">
-        <v>620</v>
+        <v>844</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>431</v>
+        <v>843</v>
       </c>
       <c r="B282" t="s">
-        <v>432</v>
+        <v>845</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>559</v>
+        <v>773</v>
       </c>
       <c r="B283" t="s">
-        <v>579</v>
+        <v>769</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>560</v>
+        <v>774</v>
       </c>
       <c r="B284" t="s">
-        <v>721</v>
+        <v>768</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>720</v>
+        <v>764</v>
       </c>
       <c r="B285" t="s">
-        <v>582</v>
+        <v>763</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="B286" t="s">
-        <v>585</v>
+        <v>558</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>562</v>
+        <v>742</v>
       </c>
       <c r="B287" t="s">
-        <v>722</v>
+        <v>734</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>719</v>
+        <v>423</v>
       </c>
       <c r="B288" t="s">
-        <v>587</v>
+        <v>426</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>563</v>
+        <v>816</v>
       </c>
       <c r="B289" t="s">
-        <v>580</v>
+        <v>620</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>564</v>
+        <v>431</v>
       </c>
       <c r="B290" t="s">
-        <v>723</v>
+        <v>432</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>718</v>
+        <v>870</v>
       </c>
       <c r="B291" t="s">
-        <v>583</v>
+        <v>871</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>565</v>
+        <v>859</v>
       </c>
       <c r="B292" t="s">
-        <v>586</v>
+        <v>862</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>566</v>
+        <v>860</v>
       </c>
       <c r="B293" t="s">
-        <v>724</v>
+        <v>863</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>717</v>
+        <v>559</v>
       </c>
       <c r="B294" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="B295" t="s">
-        <v>581</v>
+        <v>721</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>568</v>
+        <v>720</v>
       </c>
       <c r="B296" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>716</v>
+        <v>561</v>
       </c>
       <c r="B297" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>189</v>
+        <v>562</v>
       </c>
       <c r="B298" t="s">
-        <v>190</v>
+        <v>722</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>191</v>
+        <v>719</v>
       </c>
       <c r="B299" t="s">
-        <v>192</v>
+        <v>587</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>193</v>
+        <v>563</v>
       </c>
       <c r="B300" t="s">
-        <v>194</v>
+        <v>580</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>195</v>
+        <v>564</v>
       </c>
       <c r="B301" t="s">
-        <v>196</v>
+        <v>723</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>197</v>
+        <v>718</v>
       </c>
       <c r="B302" t="s">
-        <v>198</v>
+        <v>583</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>673</v>
+        <v>565</v>
       </c>
       <c r="B303" t="s">
-        <v>678</v>
+        <v>586</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>674</v>
+        <v>566</v>
       </c>
       <c r="B304" t="s">
-        <v>682</v>
+        <v>724</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>675</v>
+        <v>717</v>
       </c>
       <c r="B305" t="s">
-        <v>683</v>
+        <v>588</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>199</v>
+        <v>567</v>
       </c>
       <c r="B306" t="s">
-        <v>200</v>
+        <v>581</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>201</v>
+        <v>568</v>
       </c>
       <c r="B307" t="s">
-        <v>202</v>
+        <v>725</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>744</v>
+        <v>716</v>
       </c>
       <c r="B308" t="s">
-        <v>747</v>
+        <v>584</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>745</v>
+        <v>189</v>
       </c>
       <c r="B309" t="s">
-        <v>748</v>
+        <v>190</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>746</v>
+        <v>191</v>
       </c>
       <c r="B310" t="s">
-        <v>749</v>
+        <v>192</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>538</v>
+        <v>193</v>
       </c>
       <c r="B311" t="s">
-        <v>539</v>
+        <v>194</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>638</v>
+        <v>195</v>
       </c>
       <c r="B312" t="s">
-        <v>640</v>
+        <v>196</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>639</v>
+        <v>197</v>
       </c>
       <c r="B313" t="s">
-        <v>641</v>
+        <v>198</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>647</v>
+        <v>673</v>
       </c>
       <c r="B314" t="s">
-        <v>648</v>
+        <v>678</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>702</v>
+        <v>674</v>
       </c>
       <c r="B315" t="s">
-        <v>704</v>
+        <v>682</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>703</v>
+        <v>675</v>
       </c>
       <c r="B316" t="s">
-        <v>705</v>
+        <v>683</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>755</v>
+        <v>199</v>
       </c>
       <c r="B317" t="s">
-        <v>758</v>
+        <v>200</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B318" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>205</v>
+        <v>744</v>
       </c>
       <c r="B319" t="s">
-        <v>206</v>
+        <v>747</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>207</v>
+        <v>745</v>
       </c>
       <c r="B320" t="s">
-        <v>208</v>
+        <v>748</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>209</v>
+        <v>746</v>
       </c>
       <c r="B321" t="s">
-        <v>210</v>
+        <v>749</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>211</v>
+        <v>538</v>
       </c>
       <c r="B322" t="s">
-        <v>212</v>
+        <v>539</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>213</v>
+        <v>638</v>
       </c>
       <c r="B323" t="s">
-        <v>214</v>
+        <v>640</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>215</v>
+        <v>639</v>
       </c>
       <c r="B324" t="s">
-        <v>162</v>
+        <v>641</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>216</v>
+        <v>647</v>
       </c>
       <c r="B325" t="s">
-        <v>164</v>
+        <v>648</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>217</v>
+        <v>702</v>
       </c>
       <c r="B326" t="s">
-        <v>166</v>
+        <v>704</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>218</v>
+        <v>703</v>
       </c>
       <c r="B327" t="s">
-        <v>168</v>
+        <v>705</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>219</v>
+        <v>861</v>
       </c>
       <c r="B328" t="s">
-        <v>170</v>
+        <v>504</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>220</v>
+        <v>853</v>
       </c>
       <c r="B329" t="s">
-        <v>172</v>
+        <v>855</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>221</v>
+        <v>854</v>
       </c>
       <c r="B330" t="s">
-        <v>174</v>
+        <v>856</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>222</v>
+        <v>755</v>
       </c>
       <c r="B331" t="s">
-        <v>176</v>
+        <v>758</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="B332" t="s">
-        <v>178</v>
+        <v>204</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="B333" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="B334" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="B335" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>817</v>
+        <v>211</v>
       </c>
       <c r="B336" t="s">
-        <v>792</v>
+        <v>212</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>818</v>
+        <v>213</v>
       </c>
       <c r="B337" t="s">
-        <v>793</v>
+        <v>214</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>819</v>
+        <v>215</v>
       </c>
       <c r="B338" t="s">
-        <v>794</v>
+        <v>162</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>820</v>
+        <v>216</v>
       </c>
       <c r="B339" t="s">
-        <v>780</v>
+        <v>164</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>821</v>
+        <v>217</v>
       </c>
       <c r="B340" t="s">
-        <v>781</v>
+        <v>166</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>822</v>
+        <v>218</v>
       </c>
       <c r="B341" t="s">
-        <v>782</v>
+        <v>168</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>823</v>
+        <v>219</v>
       </c>
       <c r="B342" t="s">
-        <v>786</v>
+        <v>170</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>824</v>
+        <v>220</v>
       </c>
       <c r="B343" t="s">
-        <v>787</v>
+        <v>172</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
-        <v>825</v>
+        <v>221</v>
       </c>
       <c r="B344" t="s">
-        <v>788</v>
+        <v>174</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>826</v>
+        <v>222</v>
       </c>
       <c r="B345" t="s">
-        <v>783</v>
+        <v>176</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>827</v>
+        <v>223</v>
       </c>
       <c r="B346" t="s">
-        <v>784</v>
+        <v>178</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>828</v>
+        <v>224</v>
       </c>
       <c r="B347" t="s">
-        <v>785</v>
+        <v>180</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>829</v>
+        <v>225</v>
       </c>
       <c r="B348" t="s">
-        <v>795</v>
+        <v>182</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>830</v>
+        <v>226</v>
       </c>
       <c r="B349" t="s">
-        <v>796</v>
+        <v>184</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>831</v>
+        <v>817</v>
       </c>
       <c r="B350" t="s">
-        <v>797</v>
+        <v>792</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>832</v>
+        <v>818</v>
       </c>
       <c r="B351" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>833</v>
+        <v>819</v>
       </c>
       <c r="B352" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>834</v>
+        <v>820</v>
       </c>
       <c r="B353" t="s">
-        <v>791</v>
+        <v>780</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>401</v>
+        <v>821</v>
       </c>
       <c r="B354" t="s">
-        <v>403</v>
+        <v>781</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>406</v>
+        <v>822</v>
       </c>
       <c r="B355" t="s">
-        <v>404</v>
+        <v>782</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>409</v>
+        <v>823</v>
       </c>
       <c r="B356" t="s">
-        <v>405</v>
+        <v>786</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>630</v>
+        <v>824</v>
       </c>
       <c r="B357" t="s">
-        <v>631</v>
+        <v>787</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>632</v>
+        <v>825</v>
       </c>
       <c r="B358" t="s">
-        <v>633</v>
+        <v>788</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>657</v>
+        <v>826</v>
       </c>
       <c r="B359" t="s">
-        <v>660</v>
+        <v>783</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>661</v>
+        <v>827</v>
       </c>
       <c r="B360" t="s">
-        <v>663</v>
+        <v>784</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>662</v>
+        <v>828</v>
       </c>
       <c r="B361" t="s">
-        <v>668</v>
+        <v>785</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>433</v>
+        <v>829</v>
       </c>
       <c r="B362" t="s">
-        <v>439</v>
+        <v>795</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>435</v>
+        <v>830</v>
       </c>
       <c r="B363" t="s">
-        <v>440</v>
+        <v>796</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>437</v>
+        <v>831</v>
       </c>
       <c r="B364" t="s">
-        <v>441</v>
+        <v>797</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>754</v>
+        <v>832</v>
       </c>
       <c r="B365" t="s">
-        <v>691</v>
+        <v>789</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>413</v>
+        <v>833</v>
       </c>
       <c r="B366" t="s">
-        <v>414</v>
+        <v>790</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>420</v>
+        <v>834</v>
       </c>
       <c r="B367" t="s">
-        <v>417</v>
+        <v>791</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="B368" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>227</v>
+        <v>406</v>
       </c>
       <c r="B369" t="s">
-        <v>228</v>
+        <v>404</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>229</v>
+        <v>409</v>
       </c>
       <c r="B370" t="s">
-        <v>230</v>
+        <v>405</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>775</v>
+        <v>630</v>
       </c>
       <c r="B371" t="s">
-        <v>738</v>
+        <v>631</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>776</v>
+        <v>632</v>
       </c>
       <c r="B372" t="s">
-        <v>737</v>
+        <v>633</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>777</v>
+        <v>657</v>
       </c>
       <c r="B373" t="s">
-        <v>612</v>
+        <v>660</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>835</v>
+        <v>661</v>
       </c>
       <c r="B374" t="s">
-        <v>595</v>
+        <v>663</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>778</v>
+        <v>662</v>
       </c>
       <c r="B375" t="s">
-        <v>596</v>
+        <v>668</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>779</v>
+        <v>433</v>
       </c>
       <c r="B376" t="s">
-        <v>597</v>
+        <v>439</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>836</v>
+        <v>435</v>
       </c>
       <c r="B377" t="s">
-        <v>838</v>
+        <v>440</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>837</v>
+        <v>437</v>
       </c>
       <c r="B378" t="s">
-        <v>839</v>
+        <v>441</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>766</v>
+        <v>754</v>
       </c>
       <c r="B379" t="s">
-        <v>765</v>
+        <v>691</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>555</v>
+        <v>413</v>
       </c>
       <c r="B380" t="s">
-        <v>557</v>
+        <v>414</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>741</v>
+        <v>420</v>
       </c>
       <c r="B381" t="s">
-        <v>731</v>
+        <v>417</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>739</v>
+        <v>422</v>
       </c>
       <c r="B382" t="s">
-        <v>732</v>
+        <v>418</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>740</v>
+        <v>851</v>
       </c>
       <c r="B383" t="s">
-        <v>733</v>
+        <v>849</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>424</v>
+        <v>227</v>
       </c>
       <c r="B384" t="s">
-        <v>425</v>
+        <v>228</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>429</v>
+        <v>229</v>
       </c>
       <c r="B385" t="s">
-        <v>427</v>
+        <v>230</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>430</v>
+        <v>775</v>
       </c>
       <c r="B386" t="s">
-        <v>428</v>
+        <v>738</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>231</v>
+        <v>776</v>
       </c>
       <c r="B387" t="s">
-        <v>232</v>
+        <v>737</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>233</v>
+        <v>777</v>
       </c>
       <c r="B388" t="s">
-        <v>234</v>
+        <v>612</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>235</v>
+        <v>835</v>
       </c>
       <c r="B389" t="s">
-        <v>236</v>
+        <v>595</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>237</v>
+        <v>778</v>
       </c>
       <c r="B390" t="s">
-        <v>238</v>
+        <v>596</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>239</v>
+        <v>779</v>
       </c>
       <c r="B391" t="s">
-        <v>240</v>
+        <v>597</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>241</v>
+        <v>836</v>
       </c>
       <c r="B392" t="s">
-        <v>242</v>
+        <v>838</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>243</v>
+        <v>837</v>
       </c>
       <c r="B393" t="s">
-        <v>244</v>
+        <v>839</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>245</v>
+        <v>766</v>
       </c>
       <c r="B394" t="s">
-        <v>246</v>
+        <v>765</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>247</v>
+        <v>555</v>
       </c>
       <c r="B395" t="s">
-        <v>248</v>
+        <v>557</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>249</v>
+        <v>741</v>
       </c>
       <c r="B396" t="s">
-        <v>250</v>
+        <v>731</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>251</v>
+        <v>739</v>
       </c>
       <c r="B397" t="s">
-        <v>252</v>
+        <v>732</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>253</v>
+        <v>740</v>
       </c>
       <c r="B398" t="s">
-        <v>254</v>
+        <v>733</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>255</v>
+        <v>424</v>
       </c>
       <c r="B399" t="s">
-        <v>256</v>
+        <v>425</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
+        <v>429</v>
+      </c>
+      <c r="B400" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A401" t="s">
+        <v>430</v>
+      </c>
+      <c r="B401" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A402" t="s">
+        <v>231</v>
+      </c>
+      <c r="B402" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A403" t="s">
+        <v>233</v>
+      </c>
+      <c r="B403" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A404" t="s">
+        <v>235</v>
+      </c>
+      <c r="B404" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A405" t="s">
+        <v>237</v>
+      </c>
+      <c r="B405" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A406" t="s">
+        <v>239</v>
+      </c>
+      <c r="B406" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A407" t="s">
+        <v>241</v>
+      </c>
+      <c r="B407" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A408" t="s">
+        <v>243</v>
+      </c>
+      <c r="B408" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A409" t="s">
+        <v>245</v>
+      </c>
+      <c r="B409" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A410" t="s">
+        <v>247</v>
+      </c>
+      <c r="B410" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A411" t="s">
+        <v>249</v>
+      </c>
+      <c r="B411" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A412" t="s">
+        <v>251</v>
+      </c>
+      <c r="B412" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A413" t="s">
+        <v>253</v>
+      </c>
+      <c r="B413" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A414" t="s">
+        <v>255</v>
+      </c>
+      <c r="B414" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A415" t="s">
         <v>257</v>
       </c>
-      <c r="B400" t="s">
+      <c r="B415" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A401" t="s">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A416" t="s">
         <v>259</v>
       </c>
-      <c r="B401" t="s">
+      <c r="B416" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A402" t="s">
-        <v>261</v>
-      </c>
-      <c r="B402" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A403" t="s">
-        <v>263</v>
-      </c>
-      <c r="B403" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A404" t="s">
-        <v>265</v>
-      </c>
-      <c r="B404" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A405" t="s">
-        <v>267</v>
-      </c>
-      <c r="B405" t="s">
-        <v>268</v>
-      </c>
-      <c r="C405" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A406" t="s">
-        <v>361</v>
-      </c>
-      <c r="B406" t="s">
-        <v>363</v>
-      </c>
-      <c r="C406" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A407" t="s">
-        <v>269</v>
-      </c>
-      <c r="B407" t="s">
-        <v>270</v>
-      </c>
-      <c r="C407" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A408" t="s">
-        <v>501</v>
-      </c>
-      <c r="B408" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A409" t="s">
-        <v>271</v>
-      </c>
-      <c r="B409" t="s">
-        <v>652</v>
-      </c>
-      <c r="C409" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A410" t="s">
-        <v>316</v>
-      </c>
-      <c r="B410" t="s">
-        <v>321</v>
-      </c>
-      <c r="C410" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A411" t="s">
-        <v>317</v>
-      </c>
-      <c r="B411" t="s">
-        <v>320</v>
-      </c>
-      <c r="C411" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A412" t="s">
-        <v>272</v>
-      </c>
-      <c r="B412" t="s">
-        <v>273</v>
-      </c>
-      <c r="C412" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A413" t="s">
-        <v>288</v>
-      </c>
-      <c r="B413" t="s">
-        <v>303</v>
-      </c>
-      <c r="C413" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A414" t="s">
-        <v>292</v>
-      </c>
-      <c r="B414" t="s">
-        <v>302</v>
-      </c>
-      <c r="C414" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A415" t="s">
-        <v>274</v>
-      </c>
-      <c r="B415" t="s">
-        <v>275</v>
-      </c>
-      <c r="C415" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A416" t="s">
-        <v>341</v>
-      </c>
-      <c r="B416" t="s">
-        <v>342</v>
-      </c>
-      <c r="C416" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>314</v>
+        <v>261</v>
       </c>
       <c r="B417" t="s">
-        <v>322</v>
-      </c>
-      <c r="C417" t="s">
-        <v>319</v>
+        <v>262</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
-        <v>315</v>
+        <v>263</v>
       </c>
       <c r="B418" t="s">
-        <v>323</v>
-      </c>
-      <c r="C418" t="s">
-        <v>325</v>
+        <v>264</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
-        <v>359</v>
+        <v>265</v>
       </c>
       <c r="B419" t="s">
-        <v>365</v>
-      </c>
-      <c r="C419" t="s">
-        <v>369</v>
+        <v>266</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B420" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C420" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B421" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C421" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
-        <v>356</v>
+        <v>269</v>
       </c>
       <c r="B422" t="s">
-        <v>368</v>
+        <v>270</v>
       </c>
       <c r="C422" t="s">
-        <v>376</v>
+        <v>307</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
-        <v>278</v>
+        <v>501</v>
       </c>
       <c r="B423" t="s">
-        <v>279</v>
-      </c>
-      <c r="C423" t="s">
-        <v>313</v>
+        <v>509</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B424" t="s">
-        <v>281</v>
+        <v>652</v>
       </c>
       <c r="C424" t="s">
-        <v>281</v>
+        <v>653</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
       <c r="B425" t="s">
-        <v>296</v>
+        <v>321</v>
       </c>
       <c r="C425" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
-        <v>295</v>
+        <v>317</v>
       </c>
       <c r="B426" t="s">
-        <v>301</v>
+        <v>320</v>
       </c>
       <c r="C426" t="s">
-        <v>308</v>
+        <v>324</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
-        <v>634</v>
+        <v>272</v>
       </c>
       <c r="B427" t="s">
-        <v>635</v>
+        <v>273</v>
+      </c>
+      <c r="C427" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
-        <v>636</v>
+        <v>288</v>
       </c>
       <c r="B428" t="s">
-        <v>637</v>
+        <v>303</v>
+      </c>
+      <c r="C428" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
-        <v>392</v>
+        <v>292</v>
       </c>
       <c r="B429" t="s">
-        <v>397</v>
+        <v>302</v>
       </c>
       <c r="C429" t="s">
-        <v>398</v>
+        <v>305</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
-        <v>358</v>
+        <v>274</v>
       </c>
       <c r="B430" t="s">
-        <v>364</v>
+        <v>275</v>
+      </c>
+      <c r="C430" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
-        <v>282</v>
+        <v>341</v>
       </c>
       <c r="B431" t="s">
-        <v>283</v>
+        <v>342</v>
       </c>
       <c r="C431" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
-        <v>284</v>
+        <v>314</v>
       </c>
       <c r="B432" t="s">
-        <v>285</v>
+        <v>322</v>
       </c>
       <c r="C432" t="s">
-        <v>285</v>
+        <v>319</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
       <c r="B433" t="s">
-        <v>297</v>
+        <v>323</v>
       </c>
       <c r="C433" t="s">
-        <v>309</v>
+        <v>325</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
-        <v>294</v>
+        <v>359</v>
       </c>
       <c r="B434" t="s">
-        <v>300</v>
+        <v>365</v>
       </c>
       <c r="C434" t="s">
-        <v>310</v>
+        <v>369</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B435" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C435" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
-        <v>289</v>
+        <v>360</v>
       </c>
       <c r="B436" t="s">
-        <v>298</v>
+        <v>366</v>
       </c>
       <c r="C436" t="s">
-        <v>311</v>
+        <v>370</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
-        <v>293</v>
+        <v>356</v>
       </c>
       <c r="B437" t="s">
-        <v>299</v>
+        <v>368</v>
       </c>
       <c r="C437" t="s">
-        <v>312</v>
+        <v>376</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
+        <v>278</v>
+      </c>
+      <c r="B438" t="s">
+        <v>279</v>
+      </c>
+      <c r="C438" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A439" t="s">
+        <v>280</v>
+      </c>
+      <c r="B439" t="s">
+        <v>281</v>
+      </c>
+      <c r="C439" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A440" t="s">
+        <v>291</v>
+      </c>
+      <c r="B440" t="s">
+        <v>296</v>
+      </c>
+      <c r="C440" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A441" t="s">
+        <v>295</v>
+      </c>
+      <c r="B441" t="s">
+        <v>301</v>
+      </c>
+      <c r="C441" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A442" t="s">
+        <v>634</v>
+      </c>
+      <c r="B442" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A443" t="s">
+        <v>636</v>
+      </c>
+      <c r="B443" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A444" t="s">
+        <v>392</v>
+      </c>
+      <c r="B444" t="s">
+        <v>397</v>
+      </c>
+      <c r="C444" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A445" t="s">
+        <v>358</v>
+      </c>
+      <c r="B445" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A446" t="s">
+        <v>282</v>
+      </c>
+      <c r="B446" t="s">
+        <v>283</v>
+      </c>
+      <c r="C446" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A447" t="s">
+        <v>284</v>
+      </c>
+      <c r="B447" t="s">
+        <v>285</v>
+      </c>
+      <c r="C447" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A448" t="s">
+        <v>290</v>
+      </c>
+      <c r="B448" t="s">
+        <v>297</v>
+      </c>
+      <c r="C448" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A449" t="s">
+        <v>294</v>
+      </c>
+      <c r="B449" t="s">
+        <v>300</v>
+      </c>
+      <c r="C449" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A450" t="s">
+        <v>286</v>
+      </c>
+      <c r="B450" t="s">
+        <v>287</v>
+      </c>
+      <c r="C450" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A451" t="s">
+        <v>289</v>
+      </c>
+      <c r="B451" t="s">
+        <v>298</v>
+      </c>
+      <c r="C451" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A452" t="s">
+        <v>293</v>
+      </c>
+      <c r="B452" t="s">
+        <v>299</v>
+      </c>
+      <c r="C452" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A453" t="s">
         <v>357</v>
       </c>
-      <c r="B438" t="s">
+      <c r="B453" t="s">
         <v>367</v>
       </c>
-      <c r="C438" t="s">
+      <c r="C453" t="s">
         <v>375</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K400">
-    <sortState ref="A2:K438">
-      <sortCondition ref="A1:A400"/>
+  <autoFilter ref="A1:K415">
+    <sortState ref="A2:K453">
+      <sortCondition ref="A1:A415"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added more deepvein (vent) resource nodes
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="882">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -2639,6 +2639,36 @@
   </si>
   <si>
     <t>AI Hub</t>
+  </si>
+  <si>
+    <t>resource_name/plasma_charged_deepvein</t>
+  </si>
+  <si>
+    <t>resource_name/plasma_deepvein</t>
+  </si>
+  <si>
+    <t>resource_name/fluorine_deepvein</t>
+  </si>
+  <si>
+    <t>resource_name/nitric_acid_deepvein</t>
+  </si>
+  <si>
+    <t>resource_name/resin_deepvein</t>
+  </si>
+  <si>
+    <t>Fluorine Vent</t>
+  </si>
+  <si>
+    <t>Charged Plasma Vent</t>
+  </si>
+  <si>
+    <t>Plasma Vent</t>
+  </si>
+  <si>
+    <t>Nitric acid well</t>
+  </si>
+  <si>
+    <t>Resin well</t>
   </si>
 </sst>
 </file>
@@ -3463,11 +3493,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K453"/>
+  <dimension ref="A1:K458"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A312" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B323" sqref="B323"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7019,240 +7049,280 @@
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
-        <v>314</v>
+        <v>874</v>
       </c>
       <c r="B432" t="s">
-        <v>322</v>
-      </c>
-      <c r="C432" t="s">
-        <v>319</v>
+        <v>877</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B433" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C433" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
-        <v>359</v>
+        <v>315</v>
       </c>
       <c r="B434" t="s">
-        <v>365</v>
+        <v>323</v>
       </c>
       <c r="C434" t="s">
-        <v>369</v>
+        <v>325</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
-        <v>276</v>
+        <v>359</v>
       </c>
       <c r="B435" t="s">
-        <v>277</v>
+        <v>365</v>
       </c>
       <c r="C435" t="s">
-        <v>277</v>
+        <v>369</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
-        <v>360</v>
+        <v>276</v>
       </c>
       <c r="B436" t="s">
-        <v>366</v>
+        <v>277</v>
       </c>
       <c r="C436" t="s">
-        <v>370</v>
+        <v>277</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="B437" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C437" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
-        <v>278</v>
+        <v>356</v>
       </c>
       <c r="B438" t="s">
-        <v>279</v>
+        <v>368</v>
       </c>
       <c r="C438" t="s">
-        <v>313</v>
+        <v>376</v>
       </c>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B439" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C439" t="s">
-        <v>281</v>
+        <v>313</v>
       </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
-        <v>291</v>
+        <v>875</v>
       </c>
       <c r="B440" t="s">
-        <v>296</v>
-      </c>
-      <c r="C440" t="s">
-        <v>304</v>
+        <v>880</v>
       </c>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="B441" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="C441" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
-        <v>634</v>
+        <v>291</v>
       </c>
       <c r="B442" t="s">
-        <v>635</v>
+        <v>296</v>
+      </c>
+      <c r="C442" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
-        <v>636</v>
+        <v>295</v>
       </c>
       <c r="B443" t="s">
-        <v>637</v>
+        <v>301</v>
+      </c>
+      <c r="C443" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
-        <v>392</v>
+        <v>634</v>
       </c>
       <c r="B444" t="s">
-        <v>397</v>
-      </c>
-      <c r="C444" t="s">
-        <v>398</v>
+        <v>635</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
-        <v>358</v>
+        <v>636</v>
       </c>
       <c r="B445" t="s">
-        <v>364</v>
+        <v>637</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
-        <v>282</v>
+        <v>872</v>
       </c>
       <c r="B446" t="s">
-        <v>283</v>
-      </c>
-      <c r="C446" t="s">
-        <v>354</v>
+        <v>878</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
-        <v>284</v>
+        <v>873</v>
       </c>
       <c r="B447" t="s">
-        <v>285</v>
-      </c>
-      <c r="C447" t="s">
-        <v>285</v>
+        <v>879</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
-        <v>290</v>
+        <v>392</v>
       </c>
       <c r="B448" t="s">
-        <v>297</v>
+        <v>397</v>
       </c>
       <c r="C448" t="s">
-        <v>309</v>
+        <v>398</v>
       </c>
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
-        <v>294</v>
+        <v>876</v>
       </c>
       <c r="B449" t="s">
-        <v>300</v>
-      </c>
-      <c r="C449" t="s">
-        <v>310</v>
+        <v>881</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
-        <v>286</v>
+        <v>358</v>
       </c>
       <c r="B450" t="s">
-        <v>287</v>
-      </c>
-      <c r="C450" t="s">
-        <v>287</v>
+        <v>364</v>
       </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B451" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="C451" t="s">
-        <v>311</v>
+        <v>354</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B452" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="C452" t="s">
-        <v>312</v>
+        <v>285</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
+        <v>290</v>
+      </c>
+      <c r="B453" t="s">
+        <v>297</v>
+      </c>
+      <c r="C453" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A454" t="s">
+        <v>294</v>
+      </c>
+      <c r="B454" t="s">
+        <v>300</v>
+      </c>
+      <c r="C454" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A455" t="s">
+        <v>286</v>
+      </c>
+      <c r="B455" t="s">
+        <v>287</v>
+      </c>
+      <c r="C455" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A456" t="s">
+        <v>289</v>
+      </c>
+      <c r="B456" t="s">
+        <v>298</v>
+      </c>
+      <c r="C456" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A457" t="s">
+        <v>293</v>
+      </c>
+      <c r="B457" t="s">
+        <v>299</v>
+      </c>
+      <c r="C457" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A458" t="s">
         <v>357</v>
       </c>
-      <c r="B453" t="s">
+      <c r="B458" t="s">
         <v>367</v>
       </c>
-      <c r="C453" t="s">
+      <c r="C458" t="s">
         <v>375</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K415">
-    <sortState ref="A2:K453">
+    <sortState ref="A2:K458">
       <sortCondition ref="A1:A415"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
artillery (and flamer) tower rebalance
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$415</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$419</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="895">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -2669,6 +2669,45 @@
   </si>
   <si>
     <t>Resin well</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/towers_artillery_propelled</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/towers_artillery_propelled_lvl_2</t>
+  </si>
+  <si>
+    <t>Artillery towers using rocket propelled granades to expand range</t>
+  </si>
+  <si>
+    <t>Propelled Artillery</t>
+  </si>
+  <si>
+    <t>Propelled Artillery - Advanced</t>
+  </si>
+  <si>
+    <t>Burst Rifle - Advanced</t>
+  </si>
+  <si>
+    <t>Granade Launcher - Advanced</t>
+  </si>
+  <si>
+    <t>Mine Layer - Advanced</t>
+  </si>
+  <si>
+    <t>Rocket Launcher - Advanced</t>
+  </si>
+  <si>
+    <t>Shotgun - Advanced</t>
+  </si>
+  <si>
+    <t>90mm Cannon - Advanced</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/towers_artillery_propelled_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/towers_artillery_propelled</t>
   </si>
 </sst>
 </file>
@@ -3493,11 +3532,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K458"/>
+  <dimension ref="A1:K462"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5848,1482 +5887,1514 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>556</v>
+        <v>882</v>
       </c>
       <c r="B286" t="s">
-        <v>558</v>
+        <v>884</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>742</v>
+        <v>883</v>
       </c>
       <c r="B287" t="s">
-        <v>734</v>
+        <v>884</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>423</v>
+        <v>556</v>
       </c>
       <c r="B288" t="s">
-        <v>426</v>
+        <v>558</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>816</v>
+        <v>742</v>
       </c>
       <c r="B289" t="s">
-        <v>620</v>
+        <v>734</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="B290" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>870</v>
+        <v>816</v>
       </c>
       <c r="B291" t="s">
-        <v>871</v>
+        <v>620</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>859</v>
+        <v>431</v>
       </c>
       <c r="B292" t="s">
-        <v>862</v>
+        <v>432</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>860</v>
+        <v>870</v>
       </c>
       <c r="B293" t="s">
-        <v>863</v>
+        <v>871</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>559</v>
+        <v>859</v>
       </c>
       <c r="B294" t="s">
-        <v>579</v>
+        <v>862</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>560</v>
+        <v>860</v>
       </c>
       <c r="B295" t="s">
-        <v>721</v>
+        <v>863</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>720</v>
+        <v>559</v>
       </c>
       <c r="B296" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B297" t="s">
-        <v>585</v>
+        <v>721</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>562</v>
+        <v>720</v>
       </c>
       <c r="B298" t="s">
-        <v>722</v>
+        <v>582</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>719</v>
+        <v>561</v>
       </c>
       <c r="B299" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B300" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>564</v>
+        <v>719</v>
       </c>
       <c r="B301" t="s">
-        <v>723</v>
+        <v>587</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>718</v>
+        <v>563</v>
       </c>
       <c r="B302" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B303" t="s">
-        <v>586</v>
+        <v>723</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>566</v>
+        <v>718</v>
       </c>
       <c r="B304" t="s">
-        <v>724</v>
+        <v>583</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>717</v>
+        <v>565</v>
       </c>
       <c r="B305" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B306" t="s">
-        <v>581</v>
+        <v>724</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>568</v>
+        <v>717</v>
       </c>
       <c r="B307" t="s">
-        <v>725</v>
+        <v>588</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>716</v>
+        <v>567</v>
       </c>
       <c r="B308" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>189</v>
+        <v>568</v>
       </c>
       <c r="B309" t="s">
-        <v>190</v>
+        <v>725</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>191</v>
+        <v>716</v>
       </c>
       <c r="B310" t="s">
-        <v>192</v>
+        <v>584</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B311" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B312" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B313" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>673</v>
+        <v>195</v>
       </c>
       <c r="B314" t="s">
-        <v>678</v>
+        <v>196</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>674</v>
+        <v>197</v>
       </c>
       <c r="B315" t="s">
-        <v>682</v>
+        <v>198</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B316" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>199</v>
+        <v>674</v>
       </c>
       <c r="B317" t="s">
-        <v>200</v>
+        <v>682</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>201</v>
+        <v>675</v>
       </c>
       <c r="B318" t="s">
-        <v>202</v>
+        <v>683</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>744</v>
+        <v>199</v>
       </c>
       <c r="B319" t="s">
-        <v>747</v>
+        <v>200</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>745</v>
+        <v>201</v>
       </c>
       <c r="B320" t="s">
-        <v>748</v>
+        <v>202</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B321" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>538</v>
+        <v>745</v>
       </c>
       <c r="B322" t="s">
-        <v>539</v>
+        <v>748</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>638</v>
+        <v>746</v>
       </c>
       <c r="B323" t="s">
-        <v>640</v>
+        <v>749</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>639</v>
+        <v>538</v>
       </c>
       <c r="B324" t="s">
-        <v>641</v>
+        <v>539</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
       <c r="B325" t="s">
-        <v>648</v>
+        <v>640</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>702</v>
+        <v>639</v>
       </c>
       <c r="B326" t="s">
-        <v>704</v>
+        <v>641</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>703</v>
+        <v>647</v>
       </c>
       <c r="B327" t="s">
-        <v>705</v>
+        <v>648</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>861</v>
+        <v>702</v>
       </c>
       <c r="B328" t="s">
-        <v>504</v>
+        <v>704</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>853</v>
+        <v>703</v>
       </c>
       <c r="B329" t="s">
-        <v>855</v>
+        <v>705</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>854</v>
+        <v>861</v>
       </c>
       <c r="B330" t="s">
-        <v>856</v>
+        <v>504</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>755</v>
+        <v>853</v>
       </c>
       <c r="B331" t="s">
-        <v>758</v>
+        <v>855</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>203</v>
+        <v>854</v>
       </c>
       <c r="B332" t="s">
-        <v>204</v>
+        <v>856</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>205</v>
+        <v>755</v>
       </c>
       <c r="B333" t="s">
-        <v>206</v>
+        <v>758</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B334" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B335" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B336" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B337" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B338" t="s">
-        <v>162</v>
+        <v>212</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B339" t="s">
-        <v>164</v>
+        <v>214</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B340" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B341" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B342" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B343" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B344" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B345" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B346" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B347" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B348" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B349" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>817</v>
+        <v>225</v>
       </c>
       <c r="B350" t="s">
-        <v>792</v>
+        <v>182</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>818</v>
+        <v>226</v>
       </c>
       <c r="B351" t="s">
-        <v>793</v>
+        <v>184</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B352" t="s">
-        <v>794</v>
+        <v>887</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B353" t="s">
-        <v>780</v>
+        <v>793</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B354" t="s">
-        <v>781</v>
+        <v>794</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B355" t="s">
-        <v>782</v>
+        <v>888</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="B356" t="s">
-        <v>786</v>
+        <v>781</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B357" t="s">
-        <v>787</v>
+        <v>782</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="B358" t="s">
-        <v>788</v>
+        <v>889</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B359" t="s">
-        <v>783</v>
+        <v>787</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B360" t="s">
-        <v>784</v>
+        <v>788</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B361" t="s">
-        <v>785</v>
+        <v>890</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B362" t="s">
-        <v>795</v>
+        <v>784</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B363" t="s">
-        <v>796</v>
+        <v>785</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B364" t="s">
-        <v>797</v>
+        <v>891</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B365" t="s">
-        <v>789</v>
+        <v>796</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B366" t="s">
-        <v>790</v>
+        <v>797</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B367" t="s">
-        <v>791</v>
+        <v>892</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>401</v>
+        <v>833</v>
       </c>
       <c r="B368" t="s">
-        <v>403</v>
+        <v>790</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>406</v>
+        <v>834</v>
       </c>
       <c r="B369" t="s">
-        <v>404</v>
+        <v>791</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="B370" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>630</v>
+        <v>406</v>
       </c>
       <c r="B371" t="s">
-        <v>631</v>
+        <v>404</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>632</v>
+        <v>409</v>
       </c>
       <c r="B372" t="s">
-        <v>633</v>
+        <v>405</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>657</v>
+        <v>630</v>
       </c>
       <c r="B373" t="s">
-        <v>660</v>
+        <v>631</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>661</v>
+        <v>632</v>
       </c>
       <c r="B374" t="s">
-        <v>663</v>
+        <v>633</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="B375" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>433</v>
+        <v>661</v>
       </c>
       <c r="B376" t="s">
-        <v>439</v>
+        <v>663</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>435</v>
+        <v>662</v>
       </c>
       <c r="B377" t="s">
-        <v>440</v>
+        <v>668</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B378" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>754</v>
+        <v>435</v>
       </c>
       <c r="B379" t="s">
-        <v>691</v>
+        <v>440</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>413</v>
+        <v>437</v>
       </c>
       <c r="B380" t="s">
-        <v>414</v>
+        <v>441</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>420</v>
+        <v>754</v>
       </c>
       <c r="B381" t="s">
-        <v>417</v>
+        <v>691</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="B382" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>851</v>
+        <v>420</v>
       </c>
       <c r="B383" t="s">
-        <v>849</v>
+        <v>417</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>227</v>
+        <v>422</v>
       </c>
       <c r="B384" t="s">
-        <v>228</v>
+        <v>418</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>229</v>
+        <v>851</v>
       </c>
       <c r="B385" t="s">
-        <v>230</v>
+        <v>849</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>775</v>
+        <v>227</v>
       </c>
       <c r="B386" t="s">
-        <v>738</v>
+        <v>228</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>776</v>
+        <v>229</v>
       </c>
       <c r="B387" t="s">
-        <v>737</v>
+        <v>230</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B388" t="s">
-        <v>612</v>
+        <v>738</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>835</v>
+        <v>776</v>
       </c>
       <c r="B389" t="s">
-        <v>595</v>
+        <v>737</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B390" t="s">
-        <v>596</v>
+        <v>612</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>779</v>
+        <v>835</v>
       </c>
       <c r="B391" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>836</v>
+        <v>778</v>
       </c>
       <c r="B392" t="s">
-        <v>838</v>
+        <v>596</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>837</v>
+        <v>779</v>
       </c>
       <c r="B393" t="s">
-        <v>839</v>
+        <v>597</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>766</v>
+        <v>836</v>
       </c>
       <c r="B394" t="s">
-        <v>765</v>
+        <v>838</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>555</v>
+        <v>837</v>
       </c>
       <c r="B395" t="s">
-        <v>557</v>
+        <v>839</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>741</v>
+        <v>766</v>
       </c>
       <c r="B396" t="s">
-        <v>731</v>
+        <v>765</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>739</v>
+        <v>894</v>
       </c>
       <c r="B397" t="s">
-        <v>732</v>
+        <v>885</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>740</v>
+        <v>893</v>
       </c>
       <c r="B398" t="s">
-        <v>733</v>
+        <v>886</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>424</v>
+        <v>555</v>
       </c>
       <c r="B399" t="s">
-        <v>425</v>
+        <v>557</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>429</v>
+        <v>741</v>
       </c>
       <c r="B400" t="s">
-        <v>427</v>
+        <v>731</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>430</v>
+        <v>739</v>
       </c>
       <c r="B401" t="s">
-        <v>428</v>
+        <v>732</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>231</v>
+        <v>740</v>
       </c>
       <c r="B402" t="s">
-        <v>232</v>
+        <v>733</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>233</v>
+        <v>424</v>
       </c>
       <c r="B403" t="s">
-        <v>234</v>
+        <v>425</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>235</v>
+        <v>429</v>
       </c>
       <c r="B404" t="s">
-        <v>236</v>
+        <v>427</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>237</v>
+        <v>430</v>
       </c>
       <c r="B405" t="s">
-        <v>238</v>
+        <v>428</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B406" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B407" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B408" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B409" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B410" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B411" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B412" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B413" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B414" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B415" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B416" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B417" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B418" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B419" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B420" t="s">
-        <v>268</v>
-      </c>
-      <c r="C420" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
-        <v>361</v>
+        <v>261</v>
       </c>
       <c r="B421" t="s">
-        <v>363</v>
-      </c>
-      <c r="C421" t="s">
-        <v>362</v>
+        <v>262</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B422" t="s">
-        <v>270</v>
-      </c>
-      <c r="C422" t="s">
-        <v>307</v>
+        <v>264</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
-        <v>501</v>
+        <v>265</v>
       </c>
       <c r="B423" t="s">
-        <v>509</v>
+        <v>266</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B424" t="s">
-        <v>652</v>
+        <v>268</v>
       </c>
       <c r="C424" t="s">
-        <v>653</v>
+        <v>268</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
-        <v>316</v>
+        <v>361</v>
       </c>
       <c r="B425" t="s">
-        <v>321</v>
+        <v>363</v>
       </c>
       <c r="C425" t="s">
-        <v>318</v>
+        <v>362</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
-        <v>317</v>
+        <v>269</v>
       </c>
       <c r="B426" t="s">
-        <v>320</v>
+        <v>270</v>
       </c>
       <c r="C426" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
-        <v>272</v>
+        <v>501</v>
       </c>
       <c r="B427" t="s">
-        <v>273</v>
-      </c>
-      <c r="C427" t="s">
-        <v>273</v>
+        <v>509</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="B428" t="s">
-        <v>303</v>
+        <v>652</v>
       </c>
       <c r="C428" t="s">
-        <v>306</v>
+        <v>653</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
-        <v>292</v>
+        <v>316</v>
       </c>
       <c r="B429" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="C429" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
-        <v>274</v>
+        <v>317</v>
       </c>
       <c r="B430" t="s">
-        <v>275</v>
+        <v>320</v>
       </c>
       <c r="C430" t="s">
-        <v>275</v>
+        <v>324</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
-        <v>341</v>
+        <v>272</v>
       </c>
       <c r="B431" t="s">
-        <v>342</v>
+        <v>273</v>
       </c>
       <c r="C431" t="s">
-        <v>343</v>
+        <v>273</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
-        <v>874</v>
+        <v>288</v>
       </c>
       <c r="B432" t="s">
-        <v>877</v>
+        <v>303</v>
+      </c>
+      <c r="C432" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>314</v>
+        <v>292</v>
       </c>
       <c r="B433" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="C433" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
-        <v>315</v>
+        <v>274</v>
       </c>
       <c r="B434" t="s">
-        <v>323</v>
+        <v>275</v>
       </c>
       <c r="C434" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="B435" t="s">
-        <v>365</v>
+        <v>342</v>
       </c>
       <c r="C435" t="s">
-        <v>369</v>
+        <v>343</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
-        <v>276</v>
+        <v>874</v>
       </c>
       <c r="B436" t="s">
-        <v>277</v>
-      </c>
-      <c r="C436" t="s">
-        <v>277</v>
+        <v>877</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
-        <v>360</v>
+        <v>314</v>
       </c>
       <c r="B437" t="s">
-        <v>366</v>
+        <v>322</v>
       </c>
       <c r="C437" t="s">
-        <v>370</v>
+        <v>319</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
-        <v>356</v>
+        <v>315</v>
       </c>
       <c r="B438" t="s">
-        <v>368</v>
+        <v>323</v>
       </c>
       <c r="C438" t="s">
-        <v>376</v>
+        <v>325</v>
       </c>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
-        <v>278</v>
+        <v>359</v>
       </c>
       <c r="B439" t="s">
-        <v>279</v>
+        <v>365</v>
       </c>
       <c r="C439" t="s">
-        <v>313</v>
+        <v>369</v>
       </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
-        <v>875</v>
+        <v>276</v>
       </c>
       <c r="B440" t="s">
-        <v>880</v>
+        <v>277</v>
+      </c>
+      <c r="C440" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
-        <v>280</v>
+        <v>360</v>
       </c>
       <c r="B441" t="s">
-        <v>281</v>
+        <v>366</v>
       </c>
       <c r="C441" t="s">
-        <v>281</v>
+        <v>370</v>
       </c>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
-        <v>291</v>
+        <v>356</v>
       </c>
       <c r="B442" t="s">
-        <v>296</v>
+        <v>368</v>
       </c>
       <c r="C442" t="s">
-        <v>304</v>
+        <v>376</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="B443" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="C443" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
-        <v>634</v>
+        <v>875</v>
       </c>
       <c r="B444" t="s">
-        <v>635</v>
+        <v>880</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
-        <v>636</v>
+        <v>280</v>
       </c>
       <c r="B445" t="s">
-        <v>637</v>
+        <v>281</v>
+      </c>
+      <c r="C445" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
-        <v>872</v>
+        <v>291</v>
       </c>
       <c r="B446" t="s">
-        <v>878</v>
+        <v>296</v>
+      </c>
+      <c r="C446" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
-        <v>873</v>
+        <v>295</v>
       </c>
       <c r="B447" t="s">
-        <v>879</v>
+        <v>301</v>
+      </c>
+      <c r="C447" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
-        <v>392</v>
+        <v>634</v>
       </c>
       <c r="B448" t="s">
-        <v>397</v>
-      </c>
-      <c r="C448" t="s">
-        <v>398</v>
+        <v>635</v>
       </c>
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
-        <v>876</v>
+        <v>636</v>
       </c>
       <c r="B449" t="s">
-        <v>881</v>
+        <v>637</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
-        <v>358</v>
+        <v>872</v>
       </c>
       <c r="B450" t="s">
-        <v>364</v>
+        <v>878</v>
       </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
-        <v>282</v>
+        <v>873</v>
       </c>
       <c r="B451" t="s">
-        <v>283</v>
-      </c>
-      <c r="C451" t="s">
-        <v>354</v>
+        <v>879</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
-        <v>284</v>
+        <v>392</v>
       </c>
       <c r="B452" t="s">
-        <v>285</v>
+        <v>397</v>
       </c>
       <c r="C452" t="s">
-        <v>285</v>
+        <v>398</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
-        <v>290</v>
+        <v>876</v>
       </c>
       <c r="B453" t="s">
-        <v>297</v>
-      </c>
-      <c r="C453" t="s">
-        <v>309</v>
+        <v>881</v>
       </c>
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
-        <v>294</v>
+        <v>358</v>
       </c>
       <c r="B454" t="s">
-        <v>300</v>
-      </c>
-      <c r="C454" t="s">
-        <v>310</v>
+        <v>364</v>
       </c>
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B455" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C455" t="s">
-        <v>287</v>
+        <v>354</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B456" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="C456" t="s">
-        <v>311</v>
+        <v>285</v>
       </c>
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B457" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C457" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
+        <v>294</v>
+      </c>
+      <c r="B458" t="s">
+        <v>300</v>
+      </c>
+      <c r="C458" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A459" t="s">
+        <v>286</v>
+      </c>
+      <c r="B459" t="s">
+        <v>287</v>
+      </c>
+      <c r="C459" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A460" t="s">
+        <v>289</v>
+      </c>
+      <c r="B460" t="s">
+        <v>298</v>
+      </c>
+      <c r="C460" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A461" t="s">
+        <v>293</v>
+      </c>
+      <c r="B461" t="s">
+        <v>299</v>
+      </c>
+      <c r="C461" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A462" t="s">
         <v>357</v>
       </c>
-      <c r="B458" t="s">
+      <c r="B462" t="s">
         <v>367</v>
       </c>
-      <c r="C458" t="s">
+      <c r="C462" t="s">
         <v>375</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K415">
-    <sortState ref="A2:K458">
-      <sortCondition ref="A1:A415"/>
+  <autoFilter ref="A1:K419">
+    <sortState ref="A2:K462">
+      <sortCondition ref="A1:A419"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
split mines and heavy artillery
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$419</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$469</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="909">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -721,111 +721,57 @@
     <t>resource_name/ammo_mech_energy_cell_lvl2</t>
   </si>
   <si>
-    <t>Energy cell advanced</t>
-  </si>
-  <si>
     <t>resource_name/ammo_mech_energy_cell_lvl3</t>
   </si>
   <si>
-    <t>Energy cell top end</t>
-  </si>
-  <si>
     <t>resource_name/ammo_mech_explosive_lvl2</t>
   </si>
   <si>
-    <t>Explosive advanced M</t>
-  </si>
-  <si>
     <t>resource_name/ammo_mech_explosive_lvl3</t>
   </si>
   <si>
-    <t>Explosive top end M</t>
-  </si>
-  <si>
     <t>resource_name/ammo_mech_high_caliber_lvl2</t>
   </si>
   <si>
-    <t>High caliber advanced M</t>
-  </si>
-  <si>
     <t>resource_name/ammo_mech_high_caliber_lvl3</t>
   </si>
   <si>
-    <t>High caliber top end M</t>
-  </si>
-  <si>
     <t>resource_name/ammo_mech_liquid_lvl2</t>
   </si>
   <si>
-    <t>Liquid advanced M</t>
-  </si>
-  <si>
     <t>resource_name/ammo_mech_liquid_lvl3</t>
   </si>
   <si>
-    <t>Liquid top end M</t>
-  </si>
-  <si>
     <t>resource_name/ammo_mech_low_caliber_lvl2</t>
   </si>
   <si>
-    <t>Low caliber advanced M</t>
-  </si>
-  <si>
     <t>resource_name/ammo_mech_low_caliber_lvl3</t>
   </si>
   <si>
-    <t>Low caliber top end M</t>
-  </si>
-  <si>
     <t>resource_name/ammo_tower_explosive_lvl2</t>
   </si>
   <si>
-    <t>Explosive advanced</t>
-  </si>
-  <si>
     <t>resource_name/ammo_tower_explosive_lvl3</t>
   </si>
   <si>
-    <t>Explosive top end</t>
-  </si>
-  <si>
     <t>resource_name/ammo_tower_high_caliber_lvl2</t>
   </si>
   <si>
-    <t>High caliber advanced</t>
-  </si>
-  <si>
     <t>resource_name/ammo_tower_high_caliber_lvl3</t>
   </si>
   <si>
-    <t>High caliber top end</t>
-  </si>
-  <si>
     <t>resource_name/ammo_tower_liquid_lvl2</t>
   </si>
   <si>
-    <t>Liquid advanced</t>
-  </si>
-  <si>
     <t>resource_name/ammo_tower_liquid_lvl3</t>
   </si>
   <si>
-    <t>Liquid top end</t>
-  </si>
-  <si>
     <t>resource_name/ammo_tower_low_caliber_lvl2</t>
   </si>
   <si>
-    <t>Low caliber advanced</t>
-  </si>
-  <si>
     <t>resource_name/ammo_tower_low_caliber_lvl3</t>
   </si>
   <si>
-    <t>Low caliber top end</t>
-  </si>
-  <si>
     <t>resource_name/ammonium</t>
   </si>
   <si>
@@ -2708,6 +2654,102 @@
   </si>
   <si>
     <t>gui/menu/research/name/towers_artillery_propelled</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/towers_mines_lvl1</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/towers_mines_lvl2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/towers_mines_lvl3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/towers_mines_lvl1</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/towers_mines_lvl2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/towers_mines_lvl3</t>
+  </si>
+  <si>
+    <t>Mining Towers 3</t>
+  </si>
+  <si>
+    <t>Mining Towers 2</t>
+  </si>
+  <si>
+    <t>Mining Towers 1</t>
+  </si>
+  <si>
+    <t>The Mine Layer Tower uses automated mine drones to block incoming enemy waves</t>
+  </si>
+  <si>
+    <t>Optimized blueprint allow the Riftbreaker to build more robust version of the Mine Layer Tower</t>
+  </si>
+  <si>
+    <t>Perfected blueprint allow the Riftbreaker to the most soffistaiced version of the Mine Layer Tower</t>
+  </si>
+  <si>
+    <t>Ammunition buildings:</t>
+  </si>
+  <si>
+    <t>gui/menu/planetary_scanner/base_info_buildings_ammo</t>
+  </si>
+  <si>
+    <t>High caliber &lt;img="gui/hud/building_info_mech"&gt; top end</t>
+  </si>
+  <si>
+    <t>High caliber &lt;img="gui/hud/building_info_mech"&gt; advanced</t>
+  </si>
+  <si>
+    <t>Explosive &lt;img="gui/hud/building_info_mech"&gt; top end</t>
+  </si>
+  <si>
+    <t>Explosive &lt;img="gui/hud/building_info_mech"&gt; advanced</t>
+  </si>
+  <si>
+    <t>Energy cell &lt;img="gui/hud/building_info_mech"&gt; top end</t>
+  </si>
+  <si>
+    <t>Energy cell &lt;img="gui/hud/building_info_mech"&gt; advanced</t>
+  </si>
+  <si>
+    <t>Liquid &lt;img="gui/hud/building_info_mech"&gt; advanced</t>
+  </si>
+  <si>
+    <t>Liquid &lt;img="gui/hud/building_info_mech"&gt; top end</t>
+  </si>
+  <si>
+    <t>Low caliber &lt;img="gui/hud/building_info_mech"&gt; advanced</t>
+  </si>
+  <si>
+    <t>Low caliber &lt;img="gui/hud/building_info_mech"&gt; top end</t>
+  </si>
+  <si>
+    <t>Explosive &lt;img="gui/hud/building_info_tower"&gt; top end</t>
+  </si>
+  <si>
+    <t>High caliber &lt;img="gui/hud/building_info_tower"&gt; advanced</t>
+  </si>
+  <si>
+    <t>High caliber &lt;img="gui/hud/building_info_tower"&gt; top end</t>
+  </si>
+  <si>
+    <t>Liquid &lt;img="gui/hud/building_info_tower"&gt; top end</t>
+  </si>
+  <si>
+    <t>Low caliber &lt;img="gui/hud/building_info_tower"&gt; advanced</t>
+  </si>
+  <si>
+    <t>Low caliber &lt;img="gui/hud/building_info_tower"&gt; top end</t>
+  </si>
+  <si>
+    <t>Liquid &lt;img="gui/hud/building_info_tower"&gt; advanced</t>
+  </si>
+  <si>
+    <t>Explosive &lt;img="gui/hud/building_info_tower"&gt; advanced</t>
   </si>
 </sst>
 </file>
@@ -3532,11 +3574,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K462"/>
+  <dimension ref="A1:K469"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3611,10 +3653,10 @@
     </row>
     <row r="6" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
       <c r="B6" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3638,15 +3680,15 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>593</v>
+        <v>575</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>589</v>
+        <v>571</v>
       </c>
       <c r="B10" t="s">
-        <v>594</v>
+        <v>576</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3675,10 +3717,10 @@
     </row>
     <row r="14" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
       <c r="B14" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3763,26 +3805,26 @@
     </row>
     <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>502</v>
+        <v>484</v>
       </c>
       <c r="B25" t="s">
-        <v>533</v>
+        <v>515</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>650</v>
+        <v>632</v>
       </c>
       <c r="B26" t="s">
-        <v>651</v>
+        <v>633</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>503</v>
+        <v>485</v>
       </c>
       <c r="B27" t="s">
-        <v>532</v>
+        <v>514</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3790,42 +3832,42 @@
         <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>743</v>
+        <v>725</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="B29" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>461</v>
+        <v>443</v>
       </c>
       <c r="B30" t="s">
-        <v>510</v>
+        <v>492</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>344</v>
+        <v>326</v>
       </c>
       <c r="B31" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="C31" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>670</v>
+        <v>652</v>
       </c>
       <c r="B32" t="s">
-        <v>671</v>
+        <v>653</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3854,37 +3896,37 @@
     </row>
     <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="B36" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="C36" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="B37" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="B38" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="B39" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3937,120 +3979,120 @@
     </row>
     <row r="46" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>621</v>
+        <v>603</v>
       </c>
       <c r="B46" t="s">
-        <v>622</v>
+        <v>604</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>623</v>
+        <v>605</v>
       </c>
       <c r="B47" t="s">
-        <v>624</v>
+        <v>606</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>658</v>
+        <v>640</v>
       </c>
       <c r="B48" t="s">
-        <v>664</v>
+        <v>646</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>666</v>
+        <v>648</v>
       </c>
       <c r="B49" t="s">
-        <v>665</v>
+        <v>647</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>667</v>
+        <v>649</v>
       </c>
       <c r="B50" t="s">
-        <v>669</v>
+        <v>651</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="B51" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="C51" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="B52" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="B53" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="B54" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>688</v>
+        <v>670</v>
       </c>
       <c r="B55" t="s">
-        <v>695</v>
+        <v>677</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>689</v>
+        <v>671</v>
       </c>
       <c r="B56" t="s">
-        <v>693</v>
+        <v>675</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>685</v>
+        <v>667</v>
       </c>
       <c r="B57" t="s">
-        <v>694</v>
+        <v>676</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>846</v>
+        <v>828</v>
       </c>
       <c r="B58" t="s">
-        <v>847</v>
+        <v>829</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="B59" t="s">
-        <v>351</v>
+        <v>333</v>
       </c>
       <c r="C59" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4087,26 +4129,26 @@
     </row>
     <row r="64" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>713</v>
+        <v>695</v>
       </c>
       <c r="B64" t="s">
-        <v>655</v>
+        <v>637</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>712</v>
+        <v>694</v>
       </c>
       <c r="B65" t="s">
-        <v>714</v>
+        <v>696</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>711</v>
+        <v>693</v>
       </c>
       <c r="B66" t="s">
-        <v>715</v>
+        <v>697</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4127,34 +4169,34 @@
     </row>
     <row r="69" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>481</v>
+        <v>463</v>
       </c>
       <c r="B69" t="s">
-        <v>511</v>
+        <v>493</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>482</v>
+        <v>464</v>
       </c>
       <c r="B70" t="s">
-        <v>512</v>
+        <v>494</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>489</v>
+        <v>471</v>
       </c>
       <c r="B71" t="s">
-        <v>518</v>
+        <v>500</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>490</v>
+        <v>472</v>
       </c>
       <c r="B72" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4167,178 +4209,178 @@
     </row>
     <row r="74" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
       <c r="B74" t="s">
-        <v>531</v>
+        <v>513</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="B75" t="s">
-        <v>528</v>
+        <v>510</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="B76" t="s">
-        <v>529</v>
+        <v>511</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>459</v>
+        <v>441</v>
       </c>
       <c r="B77" t="s">
-        <v>530</v>
+        <v>512</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>553</v>
+        <v>535</v>
       </c>
       <c r="B78" t="s">
-        <v>554</v>
+        <v>536</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>487</v>
+        <v>469</v>
       </c>
       <c r="B79" t="s">
-        <v>516</v>
+        <v>498</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>488</v>
+        <v>470</v>
       </c>
       <c r="B80" t="s">
-        <v>517</v>
+        <v>499</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>483</v>
+        <v>465</v>
       </c>
       <c r="B81" t="s">
-        <v>514</v>
+        <v>496</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>485</v>
+        <v>467</v>
       </c>
       <c r="B82" t="s">
-        <v>515</v>
+        <v>497</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>486</v>
+        <v>468</v>
       </c>
       <c r="B83" t="s">
-        <v>610</v>
+        <v>592</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>484</v>
+        <v>466</v>
       </c>
       <c r="B84" t="s">
-        <v>513</v>
+        <v>495</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>493</v>
+        <v>475</v>
       </c>
       <c r="B85" t="s">
-        <v>522</v>
+        <v>504</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="B86" t="s">
-        <v>523</v>
+        <v>505</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>495</v>
+        <v>477</v>
       </c>
       <c r="B87" t="s">
-        <v>524</v>
+        <v>506</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>496</v>
+        <v>478</v>
       </c>
       <c r="B88" t="s">
-        <v>525</v>
+        <v>507</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>498</v>
+        <v>480</v>
       </c>
       <c r="B89" t="s">
-        <v>527</v>
+        <v>509</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>497</v>
+        <v>479</v>
       </c>
       <c r="B90" t="s">
-        <v>526</v>
+        <v>508</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>491</v>
+        <v>473</v>
       </c>
       <c r="B91" t="s">
-        <v>520</v>
+        <v>502</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>492</v>
+        <v>474</v>
       </c>
       <c r="B92" t="s">
-        <v>521</v>
+        <v>503</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>544</v>
+        <v>526</v>
       </c>
       <c r="B93" t="s">
-        <v>548</v>
+        <v>530</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>545</v>
+        <v>527</v>
       </c>
       <c r="B94" t="s">
-        <v>611</v>
+        <v>593</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>543</v>
+        <v>525</v>
       </c>
       <c r="B95" t="s">
-        <v>549</v>
+        <v>531</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4383,10 +4425,10 @@
     </row>
     <row r="101" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="B101" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4410,15 +4452,15 @@
         <v>90</v>
       </c>
       <c r="B104" t="s">
-        <v>592</v>
+        <v>574</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
       <c r="B105" t="s">
-        <v>591</v>
+        <v>573</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4447,10 +4489,10 @@
     </row>
     <row r="109" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
       <c r="B109" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4535,26 +4577,26 @@
     </row>
     <row r="120" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>499</v>
+        <v>481</v>
       </c>
       <c r="B120" t="s">
-        <v>507</v>
+        <v>489</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>645</v>
+        <v>627</v>
       </c>
       <c r="B121" t="s">
-        <v>646</v>
+        <v>628</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>500</v>
+        <v>482</v>
       </c>
       <c r="B122" t="s">
-        <v>508</v>
+        <v>490</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -4567,59 +4609,59 @@
     </row>
     <row r="124" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="B124" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="B125" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
       <c r="B126" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
       <c r="C126" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="B127" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
       <c r="C127" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>349</v>
+        <v>331</v>
       </c>
       <c r="B128" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
       <c r="C128" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>656</v>
+        <v>638</v>
       </c>
       <c r="B129" t="s">
-        <v>659</v>
+        <v>641</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4632,37 +4674,37 @@
     </row>
     <row r="131" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="B131" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="C131" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="B132" t="s">
-        <v>334</v>
+        <v>316</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="B133" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="B134" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4699,86 +4741,86 @@
     </row>
     <row r="139" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>625</v>
+        <v>607</v>
       </c>
       <c r="B139" t="s">
-        <v>626</v>
+        <v>608</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="B140" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="C140" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="B141" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="C141" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="B142" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="C142" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="B143" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="C143" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>686</v>
+        <v>668</v>
       </c>
       <c r="B144" t="s">
-        <v>690</v>
+        <v>672</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>687</v>
+        <v>669</v>
       </c>
       <c r="B145" t="s">
-        <v>692</v>
+        <v>674</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>684</v>
+        <v>666</v>
       </c>
       <c r="B146" t="s">
-        <v>691</v>
+        <v>673</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>848</v>
+        <v>830</v>
       </c>
       <c r="B147" t="s">
-        <v>849</v>
+        <v>831</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4799,74 +4841,74 @@
     </row>
     <row r="150" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="B150" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="B151" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>699</v>
+        <v>681</v>
       </c>
       <c r="B152" t="s">
-        <v>698</v>
+        <v>680</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>696</v>
+        <v>678</v>
       </c>
       <c r="B153" t="s">
-        <v>700</v>
+        <v>682</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>697</v>
+        <v>679</v>
       </c>
       <c r="B154" t="s">
-        <v>701</v>
+        <v>683</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>463</v>
+        <v>445</v>
       </c>
       <c r="B155" t="s">
-        <v>601</v>
+        <v>583</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>464</v>
+        <v>446</v>
       </c>
       <c r="B156" t="s">
-        <v>600</v>
+        <v>582</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>471</v>
+        <v>453</v>
       </c>
       <c r="B157" t="s">
-        <v>599</v>
+        <v>581</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>472</v>
+        <v>454</v>
       </c>
       <c r="B158" t="s">
-        <v>598</v>
+        <v>580</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4879,194 +4921,194 @@
     </row>
     <row r="160" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
       <c r="B160" t="s">
-        <v>612</v>
+        <v>594</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
       <c r="B161" t="s">
-        <v>595</v>
+        <v>577</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
       <c r="B162" t="s">
-        <v>596</v>
+        <v>578</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>460</v>
+        <v>442</v>
       </c>
       <c r="B163" t="s">
-        <v>597</v>
+        <v>579</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>840</v>
+        <v>822</v>
       </c>
       <c r="B164" t="s">
-        <v>838</v>
+        <v>820</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>841</v>
+        <v>823</v>
       </c>
       <c r="B165" t="s">
-        <v>839</v>
+        <v>821</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>550</v>
+        <v>532</v>
       </c>
       <c r="B166" t="s">
-        <v>551</v>
+        <v>533</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="B167" t="s">
-        <v>613</v>
+        <v>595</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>470</v>
+        <v>452</v>
       </c>
       <c r="B168" t="s">
-        <v>614</v>
+        <v>596</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>466</v>
+        <v>448</v>
       </c>
       <c r="B169" t="s">
-        <v>615</v>
+        <v>597</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>467</v>
+        <v>449</v>
       </c>
       <c r="B170" t="s">
-        <v>616</v>
+        <v>598</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>468</v>
+        <v>450</v>
       </c>
       <c r="B171" t="s">
-        <v>617</v>
+        <v>599</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
       <c r="B172" t="s">
-        <v>618</v>
+        <v>600</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>475</v>
+        <v>457</v>
       </c>
       <c r="B173" t="s">
-        <v>505</v>
+        <v>487</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>476</v>
+        <v>458</v>
       </c>
       <c r="B174" t="s">
-        <v>602</v>
+        <v>584</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="B175" t="s">
-        <v>603</v>
+        <v>585</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>478</v>
+        <v>460</v>
       </c>
       <c r="B176" t="s">
-        <v>604</v>
+        <v>586</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>480</v>
+        <v>462</v>
       </c>
       <c r="B177" t="s">
-        <v>506</v>
+        <v>488</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>479</v>
+        <v>461</v>
       </c>
       <c r="B178" t="s">
-        <v>609</v>
+        <v>591</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>473</v>
+        <v>455</v>
       </c>
       <c r="B179" t="s">
-        <v>605</v>
+        <v>587</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="B180" t="s">
-        <v>606</v>
+        <v>588</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>540</v>
+        <v>522</v>
       </c>
       <c r="B181" t="s">
-        <v>608</v>
+        <v>590</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>542</v>
+        <v>524</v>
       </c>
       <c r="B182" t="s">
-        <v>552</v>
+        <v>534</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>541</v>
+        <v>523</v>
       </c>
       <c r="B183" t="s">
-        <v>607</v>
+        <v>589</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5079,183 +5121,183 @@
     </row>
     <row r="185" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>546</v>
+        <v>528</v>
       </c>
       <c r="B185" t="s">
-        <v>547</v>
+        <v>529</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>534</v>
+        <v>516</v>
       </c>
       <c r="B186" t="s">
-        <v>535</v>
+        <v>517</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>864</v>
+        <v>890</v>
       </c>
       <c r="B187" t="s">
-        <v>868</v>
+        <v>889</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>865</v>
+        <v>846</v>
       </c>
       <c r="B188" t="s">
-        <v>869</v>
+        <v>850</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>569</v>
+        <v>847</v>
       </c>
       <c r="B189" t="s">
-        <v>579</v>
+        <v>851</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>570</v>
+        <v>551</v>
       </c>
       <c r="B190" t="s">
-        <v>721</v>
+        <v>561</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>726</v>
+        <v>552</v>
       </c>
       <c r="B191" t="s">
-        <v>582</v>
+        <v>703</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>571</v>
+        <v>708</v>
       </c>
       <c r="B192" t="s">
-        <v>585</v>
+        <v>564</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>572</v>
+        <v>553</v>
       </c>
       <c r="B193" t="s">
-        <v>722</v>
+        <v>567</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>727</v>
+        <v>554</v>
       </c>
       <c r="B194" t="s">
-        <v>587</v>
+        <v>704</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>573</v>
+        <v>709</v>
       </c>
       <c r="B195" t="s">
-        <v>580</v>
+        <v>569</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>574</v>
+        <v>555</v>
       </c>
       <c r="B196" t="s">
-        <v>723</v>
+        <v>562</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>728</v>
+        <v>556</v>
       </c>
       <c r="B197" t="s">
-        <v>583</v>
+        <v>705</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>575</v>
+        <v>710</v>
       </c>
       <c r="B198" t="s">
-        <v>586</v>
+        <v>565</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>576</v>
+        <v>557</v>
       </c>
       <c r="B199" t="s">
-        <v>724</v>
+        <v>568</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>729</v>
+        <v>558</v>
       </c>
       <c r="B200" t="s">
-        <v>588</v>
+        <v>706</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>577</v>
+        <v>711</v>
       </c>
       <c r="B201" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>578</v>
+        <v>559</v>
       </c>
       <c r="B202" t="s">
-        <v>725</v>
+        <v>563</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>730</v>
+        <v>560</v>
       </c>
       <c r="B203" t="s">
-        <v>584</v>
+        <v>707</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>137</v>
+        <v>712</v>
       </c>
       <c r="B204" t="s">
-        <v>138</v>
+        <v>566</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B205" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B206" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B207" t="s">
         <v>142</v>
@@ -5263,7 +5305,7 @@
     </row>
     <row r="208" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B208" t="s">
         <v>142</v>
@@ -5271,2130 +5313,2186 @@
     </row>
     <row r="209" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>672</v>
+        <v>144</v>
       </c>
       <c r="B209" t="s">
-        <v>679</v>
+        <v>142</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>676</v>
+        <v>654</v>
       </c>
       <c r="B210" t="s">
-        <v>680</v>
+        <v>661</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>677</v>
+        <v>658</v>
       </c>
       <c r="B211" t="s">
-        <v>681</v>
+        <v>662</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>145</v>
+        <v>659</v>
       </c>
       <c r="B212" t="s">
-        <v>146</v>
+        <v>663</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B213" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>750</v>
+        <v>147</v>
       </c>
       <c r="B214" t="s">
-        <v>753</v>
+        <v>148</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>751</v>
+        <v>732</v>
       </c>
       <c r="B215" t="s">
-        <v>761</v>
+        <v>735</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>752</v>
+        <v>733</v>
       </c>
       <c r="B216" t="s">
-        <v>762</v>
+        <v>743</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>536</v>
+        <v>734</v>
       </c>
       <c r="B217" t="s">
-        <v>537</v>
+        <v>744</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>642</v>
+        <v>518</v>
       </c>
       <c r="B218" t="s">
-        <v>654</v>
+        <v>519</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>643</v>
+        <v>624</v>
       </c>
       <c r="B219" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>649</v>
+        <v>625</v>
       </c>
       <c r="B220" t="s">
-        <v>708</v>
+        <v>626</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>706</v>
+        <v>631</v>
       </c>
       <c r="B221" t="s">
-        <v>709</v>
+        <v>690</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>707</v>
+        <v>688</v>
       </c>
       <c r="B222" t="s">
-        <v>710</v>
+        <v>691</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>866</v>
+        <v>689</v>
       </c>
       <c r="B223" t="s">
-        <v>867</v>
+        <v>692</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>858</v>
+        <v>848</v>
       </c>
       <c r="B224" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>857</v>
+        <v>840</v>
       </c>
       <c r="B225" t="s">
-        <v>856</v>
+        <v>837</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>757</v>
+        <v>839</v>
       </c>
       <c r="B226" t="s">
-        <v>760</v>
+        <v>838</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>149</v>
+        <v>739</v>
       </c>
       <c r="B227" t="s">
-        <v>150</v>
+        <v>742</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B228" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B229" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B230" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B231" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B232" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B233" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B234" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B235" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B236" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B237" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B238" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B239" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B240" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B241" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B242" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B243" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B244" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>798</v>
+        <v>183</v>
       </c>
       <c r="B245" t="s">
-        <v>792</v>
+        <v>184</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>799</v>
+        <v>780</v>
       </c>
       <c r="B246" t="s">
-        <v>793</v>
+        <v>774</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>800</v>
+        <v>781</v>
       </c>
       <c r="B247" t="s">
-        <v>794</v>
+        <v>775</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>801</v>
+        <v>782</v>
       </c>
       <c r="B248" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>802</v>
+        <v>783</v>
       </c>
       <c r="B249" t="s">
-        <v>781</v>
+        <v>762</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>803</v>
+        <v>784</v>
       </c>
       <c r="B250" t="s">
-        <v>782</v>
+        <v>763</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>804</v>
+        <v>785</v>
       </c>
       <c r="B251" t="s">
-        <v>786</v>
+        <v>764</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>805</v>
+        <v>786</v>
       </c>
       <c r="B252" t="s">
-        <v>787</v>
+        <v>768</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>806</v>
+        <v>787</v>
       </c>
       <c r="B253" t="s">
-        <v>788</v>
+        <v>769</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>813</v>
+        <v>788</v>
       </c>
       <c r="B254" t="s">
-        <v>783</v>
+        <v>770</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>814</v>
+        <v>795</v>
       </c>
       <c r="B255" t="s">
-        <v>784</v>
+        <v>765</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>815</v>
+        <v>796</v>
       </c>
       <c r="B256" t="s">
-        <v>785</v>
+        <v>766</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>807</v>
+        <v>797</v>
       </c>
       <c r="B257" t="s">
-        <v>795</v>
+        <v>767</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>808</v>
+        <v>789</v>
       </c>
       <c r="B258" t="s">
-        <v>796</v>
+        <v>777</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>809</v>
+        <v>790</v>
       </c>
       <c r="B259" t="s">
-        <v>797</v>
+        <v>778</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>810</v>
+        <v>791</v>
       </c>
       <c r="B260" t="s">
-        <v>789</v>
+        <v>779</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>811</v>
+        <v>792</v>
       </c>
       <c r="B261" t="s">
-        <v>790</v>
+        <v>771</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>812</v>
+        <v>793</v>
       </c>
       <c r="B262" t="s">
-        <v>791</v>
+        <v>772</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>402</v>
+        <v>794</v>
       </c>
       <c r="B263" t="s">
-        <v>619</v>
+        <v>773</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>407</v>
+        <v>384</v>
       </c>
       <c r="B264" t="s">
-        <v>411</v>
+        <v>601</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>408</v>
+        <v>389</v>
       </c>
       <c r="B265" t="s">
-        <v>410</v>
+        <v>393</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>627</v>
+        <v>390</v>
       </c>
       <c r="B266" t="s">
-        <v>628</v>
+        <v>392</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>629</v>
+        <v>609</v>
       </c>
       <c r="B267" t="s">
-        <v>628</v>
+        <v>610</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>434</v>
+        <v>611</v>
       </c>
       <c r="B268" t="s">
-        <v>442</v>
+        <v>610</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>436</v>
+        <v>416</v>
       </c>
       <c r="B269" t="s">
-        <v>443</v>
+        <v>424</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="B270" t="s">
-        <v>444</v>
+        <v>425</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>756</v>
+        <v>420</v>
       </c>
       <c r="B271" t="s">
-        <v>759</v>
+        <v>426</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>412</v>
+        <v>738</v>
       </c>
       <c r="B272" t="s">
-        <v>415</v>
+        <v>741</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>419</v>
+        <v>394</v>
       </c>
       <c r="B273" t="s">
-        <v>416</v>
+        <v>397</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>421</v>
+        <v>401</v>
       </c>
       <c r="B274" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>850</v>
+        <v>403</v>
       </c>
       <c r="B275" t="s">
-        <v>852</v>
+        <v>398</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>185</v>
+        <v>832</v>
       </c>
       <c r="B276" t="s">
-        <v>186</v>
+        <v>834</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B277" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>770</v>
+        <v>187</v>
       </c>
       <c r="B278" t="s">
-        <v>736</v>
+        <v>188</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>771</v>
+        <v>752</v>
       </c>
       <c r="B279" t="s">
-        <v>735</v>
+        <v>718</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>772</v>
+        <v>753</v>
       </c>
       <c r="B280" t="s">
-        <v>767</v>
+        <v>717</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>842</v>
+        <v>754</v>
       </c>
       <c r="B281" t="s">
-        <v>844</v>
+        <v>749</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>843</v>
+        <v>824</v>
       </c>
       <c r="B282" t="s">
-        <v>845</v>
+        <v>826</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>773</v>
+        <v>825</v>
       </c>
       <c r="B283" t="s">
-        <v>769</v>
+        <v>827</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>774</v>
+        <v>755</v>
       </c>
       <c r="B284" t="s">
-        <v>768</v>
+        <v>751</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="B285" t="s">
-        <v>763</v>
+        <v>750</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>882</v>
+        <v>746</v>
       </c>
       <c r="B286" t="s">
-        <v>884</v>
+        <v>745</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>883</v>
+        <v>864</v>
       </c>
       <c r="B287" t="s">
-        <v>884</v>
+        <v>866</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>556</v>
+        <v>865</v>
       </c>
       <c r="B288" t="s">
-        <v>558</v>
+        <v>866</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>742</v>
+        <v>538</v>
       </c>
       <c r="B289" t="s">
-        <v>734</v>
+        <v>540</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>423</v>
+        <v>877</v>
       </c>
       <c r="B290" t="s">
-        <v>426</v>
+        <v>886</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>816</v>
+        <v>878</v>
       </c>
       <c r="B291" t="s">
-        <v>620</v>
+        <v>887</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>431</v>
+        <v>879</v>
       </c>
       <c r="B292" t="s">
-        <v>432</v>
+        <v>888</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>870</v>
+        <v>724</v>
       </c>
       <c r="B293" t="s">
-        <v>871</v>
+        <v>716</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>859</v>
+        <v>405</v>
       </c>
       <c r="B294" t="s">
-        <v>862</v>
+        <v>408</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>860</v>
+        <v>798</v>
       </c>
       <c r="B295" t="s">
-        <v>863</v>
+        <v>602</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>559</v>
+        <v>413</v>
       </c>
       <c r="B296" t="s">
-        <v>579</v>
+        <v>414</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>560</v>
+        <v>852</v>
       </c>
       <c r="B297" t="s">
-        <v>721</v>
+        <v>853</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>720</v>
+        <v>841</v>
       </c>
       <c r="B298" t="s">
-        <v>582</v>
+        <v>844</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>561</v>
+        <v>842</v>
       </c>
       <c r="B299" t="s">
-        <v>585</v>
+        <v>845</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>562</v>
+        <v>541</v>
       </c>
       <c r="B300" t="s">
-        <v>722</v>
+        <v>561</v>
       </c>
     </row>
     <row r="301" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>719</v>
+        <v>542</v>
       </c>
       <c r="B301" t="s">
-        <v>587</v>
+        <v>703</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>563</v>
+        <v>702</v>
       </c>
       <c r="B302" t="s">
-        <v>580</v>
+        <v>564</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>564</v>
+        <v>543</v>
       </c>
       <c r="B303" t="s">
-        <v>723</v>
+        <v>567</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>718</v>
+        <v>544</v>
       </c>
       <c r="B304" t="s">
-        <v>583</v>
+        <v>704</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>565</v>
+        <v>701</v>
       </c>
       <c r="B305" t="s">
-        <v>586</v>
+        <v>569</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>566</v>
+        <v>545</v>
       </c>
       <c r="B306" t="s">
-        <v>724</v>
+        <v>562</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>717</v>
+        <v>546</v>
       </c>
       <c r="B307" t="s">
-        <v>588</v>
+        <v>705</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>567</v>
+        <v>700</v>
       </c>
       <c r="B308" t="s">
-        <v>581</v>
+        <v>565</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
+        <v>547</v>
+      </c>
+      <c r="B309" t="s">
         <v>568</v>
-      </c>
-      <c r="B309" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>716</v>
+        <v>548</v>
       </c>
       <c r="B310" t="s">
-        <v>584</v>
+        <v>706</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>189</v>
+        <v>699</v>
       </c>
       <c r="B311" t="s">
-        <v>190</v>
+        <v>570</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>191</v>
+        <v>549</v>
       </c>
       <c r="B312" t="s">
-        <v>192</v>
+        <v>563</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>193</v>
+        <v>550</v>
       </c>
       <c r="B313" t="s">
-        <v>194</v>
+        <v>707</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>195</v>
+        <v>698</v>
       </c>
       <c r="B314" t="s">
-        <v>196</v>
+        <v>566</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B315" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>673</v>
+        <v>191</v>
       </c>
       <c r="B316" t="s">
-        <v>678</v>
+        <v>192</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>674</v>
+        <v>193</v>
       </c>
       <c r="B317" t="s">
-        <v>682</v>
+        <v>194</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>675</v>
+        <v>195</v>
       </c>
       <c r="B318" t="s">
-        <v>683</v>
+        <v>196</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B319" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>201</v>
+        <v>655</v>
       </c>
       <c r="B320" t="s">
-        <v>202</v>
+        <v>660</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>744</v>
+        <v>656</v>
       </c>
       <c r="B321" t="s">
-        <v>747</v>
+        <v>664</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>745</v>
+        <v>657</v>
       </c>
       <c r="B322" t="s">
-        <v>748</v>
+        <v>665</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>746</v>
+        <v>199</v>
       </c>
       <c r="B323" t="s">
-        <v>749</v>
+        <v>200</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>538</v>
+        <v>201</v>
       </c>
       <c r="B324" t="s">
-        <v>539</v>
+        <v>202</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>638</v>
+        <v>726</v>
       </c>
       <c r="B325" t="s">
-        <v>640</v>
+        <v>729</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>639</v>
+        <v>727</v>
       </c>
       <c r="B326" t="s">
-        <v>641</v>
+        <v>730</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>647</v>
+        <v>728</v>
       </c>
       <c r="B327" t="s">
-        <v>648</v>
+        <v>731</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>702</v>
+        <v>520</v>
       </c>
       <c r="B328" t="s">
-        <v>704</v>
+        <v>521</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>703</v>
+        <v>620</v>
       </c>
       <c r="B329" t="s">
-        <v>705</v>
+        <v>622</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>861</v>
+        <v>621</v>
       </c>
       <c r="B330" t="s">
-        <v>504</v>
+        <v>623</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>853</v>
+        <v>629</v>
       </c>
       <c r="B331" t="s">
-        <v>855</v>
+        <v>630</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>854</v>
+        <v>684</v>
       </c>
       <c r="B332" t="s">
-        <v>856</v>
+        <v>686</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>755</v>
+        <v>685</v>
       </c>
       <c r="B333" t="s">
-        <v>758</v>
+        <v>687</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>203</v>
+        <v>843</v>
       </c>
       <c r="B334" t="s">
-        <v>204</v>
+        <v>486</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>205</v>
+        <v>835</v>
       </c>
       <c r="B335" t="s">
-        <v>206</v>
+        <v>837</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>207</v>
+        <v>836</v>
       </c>
       <c r="B336" t="s">
-        <v>208</v>
+        <v>838</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>209</v>
+        <v>737</v>
       </c>
       <c r="B337" t="s">
-        <v>210</v>
+        <v>740</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B338" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B339" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B340" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B341" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B342" t="s">
-        <v>166</v>
+        <v>212</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B343" t="s">
-        <v>168</v>
+        <v>214</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B344" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B345" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B346" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B347" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B348" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B349" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B350" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B351" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>817</v>
+        <v>223</v>
       </c>
       <c r="B352" t="s">
-        <v>887</v>
+        <v>178</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>818</v>
+        <v>224</v>
       </c>
       <c r="B353" t="s">
-        <v>793</v>
+        <v>180</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>819</v>
+        <v>225</v>
       </c>
       <c r="B354" t="s">
-        <v>794</v>
+        <v>182</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>820</v>
+        <v>226</v>
       </c>
       <c r="B355" t="s">
-        <v>888</v>
+        <v>184</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>821</v>
+        <v>799</v>
       </c>
       <c r="B356" t="s">
-        <v>781</v>
+        <v>869</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>822</v>
+        <v>800</v>
       </c>
       <c r="B357" t="s">
-        <v>782</v>
+        <v>775</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>823</v>
+        <v>801</v>
       </c>
       <c r="B358" t="s">
-        <v>889</v>
+        <v>776</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>824</v>
+        <v>802</v>
       </c>
       <c r="B359" t="s">
-        <v>787</v>
+        <v>870</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>825</v>
+        <v>803</v>
       </c>
       <c r="B360" t="s">
-        <v>788</v>
+        <v>763</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>826</v>
+        <v>804</v>
       </c>
       <c r="B361" t="s">
-        <v>890</v>
+        <v>764</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>827</v>
+        <v>805</v>
       </c>
       <c r="B362" t="s">
-        <v>784</v>
+        <v>871</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>828</v>
+        <v>806</v>
       </c>
       <c r="B363" t="s">
-        <v>785</v>
+        <v>769</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>829</v>
+        <v>807</v>
       </c>
       <c r="B364" t="s">
-        <v>891</v>
+        <v>770</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>830</v>
+        <v>808</v>
       </c>
       <c r="B365" t="s">
-        <v>796</v>
+        <v>872</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>831</v>
+        <v>809</v>
       </c>
       <c r="B366" t="s">
-        <v>797</v>
+        <v>766</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>832</v>
+        <v>810</v>
       </c>
       <c r="B367" t="s">
-        <v>892</v>
+        <v>767</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>833</v>
+        <v>811</v>
       </c>
       <c r="B368" t="s">
-        <v>790</v>
+        <v>873</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>834</v>
+        <v>812</v>
       </c>
       <c r="B369" t="s">
-        <v>791</v>
+        <v>778</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>401</v>
+        <v>813</v>
       </c>
       <c r="B370" t="s">
-        <v>403</v>
+        <v>779</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>406</v>
+        <v>814</v>
       </c>
       <c r="B371" t="s">
-        <v>404</v>
+        <v>874</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>409</v>
+        <v>815</v>
       </c>
       <c r="B372" t="s">
-        <v>405</v>
+        <v>772</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>630</v>
+        <v>816</v>
       </c>
       <c r="B373" t="s">
-        <v>631</v>
+        <v>773</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>632</v>
+        <v>383</v>
       </c>
       <c r="B374" t="s">
-        <v>633</v>
+        <v>385</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>657</v>
+        <v>388</v>
       </c>
       <c r="B375" t="s">
-        <v>660</v>
+        <v>386</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>661</v>
+        <v>391</v>
       </c>
       <c r="B376" t="s">
-        <v>663</v>
+        <v>387</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>662</v>
+        <v>612</v>
       </c>
       <c r="B377" t="s">
-        <v>668</v>
+        <v>613</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>433</v>
+        <v>614</v>
       </c>
       <c r="B378" t="s">
-        <v>439</v>
+        <v>615</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>435</v>
+        <v>639</v>
       </c>
       <c r="B379" t="s">
-        <v>440</v>
+        <v>642</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>437</v>
+        <v>643</v>
       </c>
       <c r="B380" t="s">
-        <v>441</v>
+        <v>645</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>754</v>
+        <v>644</v>
       </c>
       <c r="B381" t="s">
-        <v>691</v>
+        <v>650</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B382" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B383" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B384" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>851</v>
+        <v>736</v>
       </c>
       <c r="B385" t="s">
-        <v>849</v>
+        <v>673</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>227</v>
+        <v>395</v>
       </c>
       <c r="B386" t="s">
-        <v>228</v>
+        <v>396</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>229</v>
+        <v>402</v>
       </c>
       <c r="B387" t="s">
-        <v>230</v>
+        <v>399</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>775</v>
+        <v>404</v>
       </c>
       <c r="B388" t="s">
-        <v>738</v>
+        <v>400</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>776</v>
+        <v>833</v>
       </c>
       <c r="B389" t="s">
-        <v>737</v>
+        <v>831</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>777</v>
+        <v>227</v>
       </c>
       <c r="B390" t="s">
-        <v>612</v>
+        <v>228</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>835</v>
+        <v>229</v>
       </c>
       <c r="B391" t="s">
-        <v>595</v>
+        <v>230</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>778</v>
+        <v>757</v>
       </c>
       <c r="B392" t="s">
-        <v>596</v>
+        <v>720</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>779</v>
+        <v>758</v>
       </c>
       <c r="B393" t="s">
-        <v>597</v>
+        <v>719</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>836</v>
+        <v>759</v>
       </c>
       <c r="B394" t="s">
-        <v>838</v>
+        <v>594</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>837</v>
+        <v>817</v>
       </c>
       <c r="B395" t="s">
-        <v>839</v>
+        <v>577</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="B396" t="s">
-        <v>765</v>
+        <v>578</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>894</v>
+        <v>761</v>
       </c>
       <c r="B397" t="s">
-        <v>885</v>
+        <v>579</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>893</v>
+        <v>818</v>
       </c>
       <c r="B398" t="s">
-        <v>886</v>
+        <v>820</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>555</v>
+        <v>819</v>
       </c>
       <c r="B399" t="s">
-        <v>557</v>
+        <v>821</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>741</v>
+        <v>748</v>
       </c>
       <c r="B400" t="s">
-        <v>731</v>
+        <v>747</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>739</v>
+        <v>876</v>
       </c>
       <c r="B401" t="s">
-        <v>732</v>
+        <v>867</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>740</v>
+        <v>875</v>
       </c>
       <c r="B402" t="s">
-        <v>733</v>
+        <v>868</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>424</v>
+        <v>537</v>
       </c>
       <c r="B403" t="s">
-        <v>425</v>
+        <v>539</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>429</v>
+        <v>880</v>
       </c>
       <c r="B404" t="s">
-        <v>427</v>
+        <v>885</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>430</v>
+        <v>881</v>
       </c>
       <c r="B405" t="s">
-        <v>428</v>
+        <v>884</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>231</v>
+        <v>882</v>
       </c>
       <c r="B406" t="s">
-        <v>232</v>
+        <v>883</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>233</v>
+        <v>723</v>
       </c>
       <c r="B407" t="s">
-        <v>234</v>
+        <v>713</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>235</v>
+        <v>721</v>
       </c>
       <c r="B408" t="s">
-        <v>236</v>
+        <v>714</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>237</v>
+        <v>722</v>
       </c>
       <c r="B409" t="s">
-        <v>238</v>
+        <v>715</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>239</v>
+        <v>406</v>
       </c>
       <c r="B410" t="s">
-        <v>240</v>
+        <v>407</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>241</v>
+        <v>411</v>
       </c>
       <c r="B411" t="s">
-        <v>242</v>
+        <v>409</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>243</v>
+        <v>412</v>
       </c>
       <c r="B412" t="s">
-        <v>244</v>
+        <v>410</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="B413" t="s">
-        <v>246</v>
+        <v>896</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="B414" t="s">
-        <v>248</v>
+        <v>895</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="B415" t="s">
-        <v>250</v>
+        <v>894</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="B416" t="s">
-        <v>252</v>
+        <v>893</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="B417" t="s">
-        <v>254</v>
+        <v>892</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="B418" t="s">
-        <v>256</v>
+        <v>891</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="B419" t="s">
-        <v>258</v>
+        <v>897</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="B420" t="s">
-        <v>260</v>
+        <v>898</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="B421" t="s">
-        <v>262</v>
+        <v>899</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="B422" t="s">
-        <v>264</v>
+        <v>900</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="B423" t="s">
-        <v>266</v>
+        <v>908</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="B424" t="s">
-        <v>268</v>
-      </c>
-      <c r="C424" t="s">
-        <v>268</v>
+        <v>901</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
-        <v>361</v>
+        <v>243</v>
       </c>
       <c r="B425" t="s">
-        <v>363</v>
-      </c>
-      <c r="C425" t="s">
-        <v>362</v>
+        <v>902</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
       <c r="B426" t="s">
-        <v>270</v>
-      </c>
-      <c r="C426" t="s">
-        <v>307</v>
+        <v>903</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
-        <v>501</v>
+        <v>245</v>
       </c>
       <c r="B427" t="s">
-        <v>509</v>
+        <v>907</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="B428" t="s">
-        <v>652</v>
-      </c>
-      <c r="C428" t="s">
-        <v>653</v>
+        <v>904</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
-        <v>316</v>
+        <v>247</v>
       </c>
       <c r="B429" t="s">
-        <v>321</v>
-      </c>
-      <c r="C429" t="s">
-        <v>318</v>
+        <v>905</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
-        <v>317</v>
+        <v>248</v>
       </c>
       <c r="B430" t="s">
-        <v>320</v>
-      </c>
-      <c r="C430" t="s">
-        <v>324</v>
+        <v>906</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="B431" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="C431" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
-        <v>288</v>
+        <v>343</v>
       </c>
       <c r="B432" t="s">
-        <v>303</v>
+        <v>345</v>
       </c>
       <c r="C432" t="s">
-        <v>306</v>
+        <v>344</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>292</v>
+        <v>251</v>
       </c>
       <c r="B433" t="s">
-        <v>302</v>
+        <v>252</v>
       </c>
       <c r="C433" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
-        <v>274</v>
+        <v>483</v>
       </c>
       <c r="B434" t="s">
-        <v>275</v>
-      </c>
-      <c r="C434" t="s">
-        <v>275</v>
+        <v>491</v>
       </c>
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
-        <v>341</v>
+        <v>253</v>
       </c>
       <c r="B435" t="s">
-        <v>342</v>
+        <v>634</v>
       </c>
       <c r="C435" t="s">
-        <v>343</v>
+        <v>635</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
-        <v>874</v>
+        <v>298</v>
       </c>
       <c r="B436" t="s">
-        <v>877</v>
+        <v>303</v>
+      </c>
+      <c r="C436" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="B437" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="C437" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
-        <v>315</v>
+        <v>254</v>
       </c>
       <c r="B438" t="s">
-        <v>323</v>
+        <v>255</v>
       </c>
       <c r="C438" t="s">
-        <v>325</v>
+        <v>255</v>
       </c>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
-        <v>359</v>
+        <v>270</v>
       </c>
       <c r="B439" t="s">
-        <v>365</v>
+        <v>285</v>
       </c>
       <c r="C439" t="s">
-        <v>369</v>
+        <v>288</v>
       </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B440" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="C440" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
-        <v>360</v>
+        <v>256</v>
       </c>
       <c r="B441" t="s">
-        <v>366</v>
+        <v>257</v>
       </c>
       <c r="C441" t="s">
-        <v>370</v>
+        <v>257</v>
       </c>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
-        <v>356</v>
+        <v>323</v>
       </c>
       <c r="B442" t="s">
-        <v>368</v>
+        <v>324</v>
       </c>
       <c r="C442" t="s">
-        <v>376</v>
+        <v>325</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
-        <v>278</v>
+        <v>856</v>
       </c>
       <c r="B443" t="s">
-        <v>279</v>
-      </c>
-      <c r="C443" t="s">
-        <v>313</v>
+        <v>859</v>
       </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
-        <v>875</v>
+        <v>296</v>
       </c>
       <c r="B444" t="s">
-        <v>880</v>
+        <v>304</v>
+      </c>
+      <c r="C444" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
-        <v>280</v>
+        <v>297</v>
       </c>
       <c r="B445" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="C445" t="s">
-        <v>281</v>
+        <v>307</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
-        <v>291</v>
+        <v>341</v>
       </c>
       <c r="B446" t="s">
-        <v>296</v>
+        <v>347</v>
       </c>
       <c r="C446" t="s">
-        <v>304</v>
+        <v>351</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
-        <v>295</v>
+        <v>258</v>
       </c>
       <c r="B447" t="s">
-        <v>301</v>
+        <v>259</v>
       </c>
       <c r="C447" t="s">
-        <v>308</v>
+        <v>259</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
-        <v>634</v>
+        <v>342</v>
       </c>
       <c r="B448" t="s">
-        <v>635</v>
+        <v>348</v>
+      </c>
+      <c r="C448" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
-        <v>636</v>
+        <v>338</v>
       </c>
       <c r="B449" t="s">
-        <v>637</v>
+        <v>350</v>
+      </c>
+      <c r="C449" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
-        <v>872</v>
+        <v>260</v>
       </c>
       <c r="B450" t="s">
-        <v>878</v>
+        <v>261</v>
+      </c>
+      <c r="C450" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
-        <v>873</v>
+        <v>857</v>
       </c>
       <c r="B451" t="s">
-        <v>879</v>
+        <v>862</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
-        <v>392</v>
+        <v>262</v>
       </c>
       <c r="B452" t="s">
-        <v>397</v>
+        <v>263</v>
       </c>
       <c r="C452" t="s">
-        <v>398</v>
+        <v>263</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
-        <v>876</v>
+        <v>273</v>
       </c>
       <c r="B453" t="s">
-        <v>881</v>
+        <v>278</v>
+      </c>
+      <c r="C453" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
-        <v>358</v>
+        <v>277</v>
       </c>
       <c r="B454" t="s">
-        <v>364</v>
+        <v>283</v>
+      </c>
+      <c r="C454" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
-        <v>282</v>
+        <v>616</v>
       </c>
       <c r="B455" t="s">
-        <v>283</v>
-      </c>
-      <c r="C455" t="s">
-        <v>354</v>
+        <v>617</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
-        <v>284</v>
+        <v>618</v>
       </c>
       <c r="B456" t="s">
-        <v>285</v>
-      </c>
-      <c r="C456" t="s">
-        <v>285</v>
+        <v>619</v>
       </c>
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
-        <v>290</v>
+        <v>854</v>
       </c>
       <c r="B457" t="s">
-        <v>297</v>
-      </c>
-      <c r="C457" t="s">
-        <v>309</v>
+        <v>860</v>
       </c>
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
-        <v>294</v>
+        <v>855</v>
       </c>
       <c r="B458" t="s">
-        <v>300</v>
-      </c>
-      <c r="C458" t="s">
-        <v>310</v>
+        <v>861</v>
       </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
-        <v>286</v>
+        <v>374</v>
       </c>
       <c r="B459" t="s">
-        <v>287</v>
+        <v>379</v>
       </c>
       <c r="C459" t="s">
-        <v>287</v>
+        <v>380</v>
       </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A460" t="s">
-        <v>289</v>
+        <v>858</v>
       </c>
       <c r="B460" t="s">
-        <v>298</v>
-      </c>
-      <c r="C460" t="s">
-        <v>311</v>
+        <v>863</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A461" t="s">
-        <v>293</v>
+        <v>340</v>
       </c>
       <c r="B461" t="s">
-        <v>299</v>
-      </c>
-      <c r="C461" t="s">
-        <v>312</v>
+        <v>346</v>
       </c>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A462" t="s">
+        <v>264</v>
+      </c>
+      <c r="B462" t="s">
+        <v>265</v>
+      </c>
+      <c r="C462" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A463" t="s">
+        <v>266</v>
+      </c>
+      <c r="B463" t="s">
+        <v>267</v>
+      </c>
+      <c r="C463" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A464" t="s">
+        <v>272</v>
+      </c>
+      <c r="B464" t="s">
+        <v>279</v>
+      </c>
+      <c r="C464" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A465" t="s">
+        <v>276</v>
+      </c>
+      <c r="B465" t="s">
+        <v>282</v>
+      </c>
+      <c r="C465" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A466" t="s">
+        <v>268</v>
+      </c>
+      <c r="B466" t="s">
+        <v>269</v>
+      </c>
+      <c r="C466" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A467" t="s">
+        <v>271</v>
+      </c>
+      <c r="B467" t="s">
+        <v>280</v>
+      </c>
+      <c r="C467" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A468" t="s">
+        <v>275</v>
+      </c>
+      <c r="B468" t="s">
+        <v>281</v>
+      </c>
+      <c r="C468" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A469" t="s">
+        <v>339</v>
+      </c>
+      <c r="B469" t="s">
+        <v>349</v>
+      </c>
+      <c r="C469" t="s">
         <v>357</v>
       </c>
-      <c r="B462" t="s">
-        <v>367</v>
-      </c>
-      <c r="C462" t="s">
-        <v>375</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K419">
-    <sortState ref="A2:K462">
-      <sortCondition ref="A1:A419"/>
+  <autoFilter ref="A1:K469">
+    <sortState ref="A2:K469">
+      <sortCondition ref="A1:A469"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7413,92 +7511,92 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="B1" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="C1" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="B2" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="B3" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="B4" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="B5" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="C5" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="B6" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="C6" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="B7" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="C7" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="B8" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="C8" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
       <c r="B9" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="C9" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added rare metals converters
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$518</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">rebalance_localizations!$A$1:$K$571</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="1077">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -3127,15 +3127,6 @@
     <t>gui/menu/research/description/resource_converter_titanium</t>
   </si>
   <si>
-    <t>gui/menu/research/resource_converter_cobalt</t>
-  </si>
-  <si>
-    <t>gui/menu/research/resource_converter_palladium</t>
-  </si>
-  <si>
-    <t>gui/menu/research/resource_converter_titanium</t>
-  </si>
-  <si>
     <t>Metallic Morphing - Cobalt</t>
   </si>
   <si>
@@ -3172,9 +3163,6 @@
     <t>gui/menu/research/description/fire_control_station_artillery</t>
   </si>
   <si>
-    <t>gui/menu/research/fire_control_station_artillery</t>
-  </si>
-  <si>
     <t>Powers up/down long range artillery towers depending on if enemies are in vicinity or not. Much wieder detection range then regular fire control stations</t>
   </si>
   <si>
@@ -3203,6 +3191,69 @@
   </si>
   <si>
     <t>Advanced techniques applying tanzanite allows for a more efficient mass seperation of isotopes</t>
+  </si>
+  <si>
+    <t>resource_name/reagent_compressed</t>
+  </si>
+  <si>
+    <t>resource_name/solvent_compressed</t>
+  </si>
+  <si>
+    <t>resource_name/nitric_acid_compressed</t>
+  </si>
+  <si>
+    <t>resource_name/fluorine_compressed</t>
+  </si>
+  <si>
+    <t>resource_name/deuterium_compressed</t>
+  </si>
+  <si>
+    <t>resource_name/magma_metal_compressed</t>
+  </si>
+  <si>
+    <t>resource_name/petroleum_compressed</t>
+  </si>
+  <si>
+    <t>Packaged Reagent</t>
+  </si>
+  <si>
+    <t>Packaged Solvent</t>
+  </si>
+  <si>
+    <t>Packaged Petroleum</t>
+  </si>
+  <si>
+    <t>Packaged N.Acid</t>
+  </si>
+  <si>
+    <t>Liquid Fluorine</t>
+  </si>
+  <si>
+    <t>Liquid Deuterium</t>
+  </si>
+  <si>
+    <t>You don't want to know</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/fire_control_station_artillery</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/resource_converter_cobalt</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/resource_converter_palladium</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/resource_converter_titanium</t>
+  </si>
+  <si>
+    <t>Uses morphiums ability to transition between elements to convert iron into cobalt</t>
+  </si>
+  <si>
+    <t>Uses morphium ability to transition between elements to convert cobalt into palladium</t>
+  </si>
+  <si>
+    <t>Uses morphium ability to transition between elements to convert cobalt into titanium</t>
   </si>
 </sst>
 </file>
@@ -4045,11 +4096,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K564"/>
+  <dimension ref="A1:K571"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A555" sqref="A555"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4357,10 +4408,10 @@
     </row>
     <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>1046</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4569,7 +4620,7 @@
         <v>1025</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4577,7 +4628,7 @@
         <v>1029</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4585,7 +4636,7 @@
         <v>1030</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5217,10 +5268,10 @@
     </row>
     <row r="141" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>1047</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>1051</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5396,7 +5447,7 @@
         <v>1026</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5404,7 +5455,7 @@
         <v>1027</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5412,7 +5463,7 @@
         <v>1028</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -6289,10 +6340,10 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.35">
@@ -6748,7 +6799,7 @@
         <v>1031</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>1045</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.35">
@@ -6756,7 +6807,7 @@
         <v>1032</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>1043</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6764,7 +6815,7 @@
         <v>1033</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>1044</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.35">
@@ -6937,18 +6988,18 @@
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="B353" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
       <c r="B354" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.35">
@@ -6977,474 +7028,474 @@
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>1049</v>
+        <v>846</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>1051</v>
+        <v>847</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>846</v>
+        <v>835</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>847</v>
+        <v>838</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>836</v>
+        <v>537</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>839</v>
+        <v>557</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>557</v>
+        <v>699</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>538</v>
+        <v>698</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>699</v>
+        <v>560</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>698</v>
+        <v>539</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>563</v>
+        <v>700</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>540</v>
+        <v>697</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>700</v>
+        <v>565</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>697</v>
+        <v>541</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>558</v>
+        <v>701</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>542</v>
+        <v>696</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>701</v>
+        <v>561</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>696</v>
+        <v>543</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>564</v>
+        <v>702</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>544</v>
+        <v>695</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>702</v>
+        <v>566</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>695</v>
+        <v>545</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>559</v>
+        <v>703</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>546</v>
+        <v>694</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>703</v>
+        <v>562</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>694</v>
+        <v>187</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>562</v>
+        <v>188</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>195</v>
+        <v>651</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>196</v>
+        <v>656</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>656</v>
+        <v>660</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>653</v>
+        <v>197</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>661</v>
+        <v>198</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>199</v>
+        <v>722</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>200</v>
+        <v>725</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>724</v>
+        <v>516</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>727</v>
+        <v>517</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>516</v>
+        <v>616</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>517</v>
+        <v>618</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>617</v>
+        <v>1020</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>619</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>1020</v>
+        <v>996</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>1021</v>
+        <v>999</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>998</v>
+        <v>981</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>1001</v>
+        <v>985</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>984</v>
+        <v>625</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>988</v>
+        <v>626</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>625</v>
+        <v>680</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>626</v>
+        <v>682</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>681</v>
+        <v>935</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>683</v>
+        <v>931</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>935</v>
+        <v>948</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>931</v>
+        <v>951</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>948</v>
+        <v>955</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>951</v>
+        <v>958</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>955</v>
+        <v>934</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>958</v>
+        <v>930</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>934</v>
+        <v>949</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>930</v>
+        <v>952</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>949</v>
+        <v>956</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>952</v>
+        <v>959</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>956</v>
+        <v>972</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>959</v>
+        <v>933</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>933</v>
+        <v>953</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>953</v>
+        <v>960</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>974</v>
+        <v>936</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>960</v>
+        <v>932</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>936</v>
+        <v>950</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>932</v>
+        <v>954</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>950</v>
+        <v>957</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>954</v>
+        <v>961</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>957</v>
+        <v>837</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>961</v>
+        <v>482</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>837</v>
+        <v>1070</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>482</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.35">
@@ -7921,258 +7972,258 @@
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A476" t="s">
-        <v>922</v>
+        <v>1071</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>923</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A477" t="s">
-        <v>920</v>
+        <v>1072</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>924</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A478" t="s">
-        <v>921</v>
+        <v>1073</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>925</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A479" t="s">
-        <v>827</v>
+        <v>922</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>825</v>
+        <v>923</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A480" t="s">
-        <v>225</v>
+        <v>920</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>226</v>
+        <v>924</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A481" t="s">
-        <v>227</v>
+        <v>921</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>228</v>
+        <v>925</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A482" t="s">
-        <v>752</v>
+        <v>827</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>715</v>
+        <v>825</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A483" t="s">
-        <v>753</v>
+        <v>225</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>590</v>
+        <v>226</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A484" t="s">
-        <v>811</v>
+        <v>227</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>573</v>
+        <v>228</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>574</v>
+        <v>715</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A486" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>575</v>
+        <v>590</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A487" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>814</v>
+        <v>573</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A488" t="s">
-        <v>813</v>
+        <v>754</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>815</v>
+        <v>574</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A489" t="s">
-        <v>744</v>
+        <v>755</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>743</v>
+        <v>575</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A490" t="s">
-        <v>979</v>
+        <v>812</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>716</v>
+        <v>814</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A491" t="s">
-        <v>870</v>
+        <v>813</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>861</v>
+        <v>815</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A492" t="s">
-        <v>869</v>
+        <v>744</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>862</v>
+        <v>743</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A493" t="s">
-        <v>533</v>
+        <v>979</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>535</v>
+        <v>716</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A494" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>879</v>
+        <v>861</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A495" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>878</v>
+        <v>862</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A496" t="s">
-        <v>876</v>
+        <v>533</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>877</v>
+        <v>535</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A497" t="s">
-        <v>719</v>
+        <v>874</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>709</v>
+        <v>879</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A498" t="s">
-        <v>717</v>
+        <v>875</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>710</v>
+        <v>878</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A499" t="s">
-        <v>718</v>
+        <v>876</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>711</v>
+        <v>877</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A500" t="s">
-        <v>1054</v>
-      </c>
-      <c r="B500" t="s">
-        <v>1059</v>
+        <v>719</v>
+      </c>
+      <c r="B500" s="1" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A501" t="s">
-        <v>1055</v>
-      </c>
-      <c r="B501" t="s">
-        <v>1058</v>
+        <v>717</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A502" t="s">
-        <v>402</v>
+        <v>718</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>403</v>
+        <v>711</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A503" t="s">
-        <v>407</v>
-      </c>
-      <c r="B503" s="1" t="s">
-        <v>405</v>
+        <v>1050</v>
+      </c>
+      <c r="B503" t="s">
+        <v>1052</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A504" t="s">
-        <v>408</v>
-      </c>
-      <c r="B504" s="1" t="s">
-        <v>406</v>
+        <v>1051</v>
+      </c>
+      <c r="B504" t="s">
+        <v>1053</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A505" t="s">
-        <v>1034</v>
+        <v>402</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1037</v>
+        <v>403</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A506" t="s">
-        <v>1035</v>
+        <v>407</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1038</v>
+        <v>405</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A507" t="s">
-        <v>1036</v>
+        <v>408</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>1039</v>
+        <v>406</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.35">
@@ -8439,292 +8490,348 @@
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A537" t="s">
-        <v>319</v>
+        <v>1060</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C537" s="2" t="s">
-        <v>321</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="538" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A538" t="s">
-        <v>850</v>
+        <v>319</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>853</v>
+        <v>320</v>
+      </c>
+      <c r="C538" s="2" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A539" t="s">
-        <v>294</v>
+        <v>1059</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C539" s="2" t="s">
-        <v>299</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A540" t="s">
-        <v>295</v>
+        <v>850</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="C540" s="2" t="s">
-        <v>305</v>
+        <v>853</v>
       </c>
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A541" t="s">
-        <v>337</v>
+        <v>294</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>343</v>
+        <v>302</v>
       </c>
       <c r="C541" s="2" t="s">
-        <v>347</v>
+        <v>299</v>
       </c>
     </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A542" t="s">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>257</v>
+        <v>303</v>
       </c>
       <c r="C542" s="2" t="s">
-        <v>257</v>
+        <v>305</v>
       </c>
     </row>
     <row r="543" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A543" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C543" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="544" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A544" t="s">
-        <v>334</v>
+        <v>256</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>346</v>
+        <v>257</v>
       </c>
       <c r="C544" s="2" t="s">
-        <v>354</v>
+        <v>257</v>
       </c>
     </row>
     <row r="545" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A545" t="s">
-        <v>258</v>
+        <v>1061</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C545" s="2" t="s">
-        <v>293</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="546" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A546" t="s">
-        <v>851</v>
+        <v>338</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>856</v>
+        <v>344</v>
+      </c>
+      <c r="C546" s="2" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="547" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A547" t="s">
-        <v>260</v>
+        <v>334</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>261</v>
+        <v>346</v>
       </c>
       <c r="C547" s="2" t="s">
-        <v>261</v>
+        <v>354</v>
       </c>
     </row>
     <row r="548" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A548" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="C548" s="2" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A549" t="s">
-        <v>275</v>
+        <v>1058</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="C549" s="2" t="s">
-        <v>288</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="550" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A550" t="s">
-        <v>612</v>
+        <v>851</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>613</v>
+        <v>856</v>
       </c>
     </row>
     <row r="551" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A551" t="s">
-        <v>614</v>
+        <v>260</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>615</v>
+        <v>261</v>
+      </c>
+      <c r="C551" s="2" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A552" t="s">
-        <v>848</v>
+        <v>271</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>854</v>
+        <v>276</v>
+      </c>
+      <c r="C552" s="2" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A553" t="s">
-        <v>849</v>
+        <v>275</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>855</v>
+        <v>281</v>
+      </c>
+      <c r="C553" s="2" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="554" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A554" t="s">
-        <v>370</v>
+        <v>612</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="C554" s="2" t="s">
-        <v>376</v>
+        <v>613</v>
       </c>
     </row>
     <row r="555" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A555" t="s">
-        <v>852</v>
+        <v>1062</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>857</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="556" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A556" t="s">
-        <v>336</v>
+        <v>614</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>342</v>
+        <v>615</v>
       </c>
     </row>
     <row r="557" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A557" t="s">
-        <v>262</v>
+        <v>848</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="C557" s="2" t="s">
-        <v>332</v>
+        <v>854</v>
       </c>
     </row>
     <row r="558" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A558" t="s">
-        <v>264</v>
+        <v>849</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C558" s="2" t="s">
-        <v>265</v>
+        <v>855</v>
       </c>
     </row>
     <row r="559" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A559" t="s">
-        <v>270</v>
+        <v>370</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>277</v>
+        <v>375</v>
       </c>
       <c r="C559" s="2" t="s">
-        <v>289</v>
+        <v>376</v>
       </c>
     </row>
     <row r="560" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A560" t="s">
-        <v>274</v>
+        <v>1056</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="C560" s="2" t="s">
-        <v>290</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="561" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A561" t="s">
-        <v>266</v>
+        <v>852</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C561" s="2" t="s">
-        <v>267</v>
+        <v>857</v>
       </c>
     </row>
     <row r="562" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A562" t="s">
-        <v>269</v>
+        <v>336</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C562" s="2" t="s">
-        <v>291</v>
+        <v>342</v>
       </c>
     </row>
     <row r="563" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A563" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="C563" s="2" t="s">
-        <v>292</v>
+        <v>332</v>
       </c>
     </row>
     <row r="564" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A564" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A565" t="s">
+        <v>264</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C565" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A566" t="s">
+        <v>270</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C566" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A567" t="s">
+        <v>274</v>
+      </c>
+      <c r="B567" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C567" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="568" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A568" t="s">
+        <v>266</v>
+      </c>
+      <c r="B568" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C568" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="569" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A569" t="s">
+        <v>269</v>
+      </c>
+      <c r="B569" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C569" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="570" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A570" t="s">
+        <v>273</v>
+      </c>
+      <c r="B570" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C570" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="571" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A571" t="s">
         <v>335</v>
       </c>
-      <c r="B564" s="1" t="s">
+      <c r="B571" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C564" s="2" t="s">
+      <c r="C571" s="2" t="s">
         <v>353</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K518">
-    <sortState ref="A2:K564">
-      <sortCondition ref="A1:A518"/>
+  <autoFilter ref="A1:K571">
+    <sortState ref="A2:K571">
+      <sortCondition ref="A1:A571"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8734,10 +8841,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B14"/>
+      <selection activeCell="A10" sqref="A10:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8788,36 +8895,60 @@
         <v>846</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1063</v>
+      </c>
+    </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1053</v>
+        <v>1057</v>
       </c>
       <c r="B11" t="s">
-        <v>1057</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1052</v>
+        <v>1058</v>
       </c>
       <c r="B12" t="s">
-        <v>1056</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1054</v>
+        <v>1059</v>
       </c>
       <c r="B13" t="s">
-        <v>1059</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>1055</v>
+        <v>1060</v>
       </c>
       <c r="B14" t="s">
-        <v>1058</v>
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1069</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new ammonium production to tech tree
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="1090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="1098">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -3293,6 +3293,30 @@
   </si>
   <si>
     <t>Improved Haber Process</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/ammonium_extraction_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/ammonium_extraction</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/ammonium_extraction_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/ammonium_extraction</t>
+  </si>
+  <si>
+    <t>Ammonium Extraction</t>
+  </si>
+  <si>
+    <t>Advanced Ammonium Extraction</t>
+  </si>
+  <si>
+    <t>Extracts Ammonium from nitrate rich natural sources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracts Ammonium from nitrate rich natural sources. </t>
   </si>
 </sst>
 </file>
@@ -4135,11 +4159,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K578"/>
+  <dimension ref="A1:K582"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A341" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C369" sqref="C369"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I580" sqref="I580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6083,55 +6107,55 @@
     </row>
     <row r="235" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>1077</v>
+        <v>1093</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>1087</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>1078</v>
+        <v>1092</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>1086</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>135</v>
+        <v>1077</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>136</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>137</v>
+        <v>1078</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>138</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B241" s="1" t="s">
         <v>140</v>
@@ -6139,111 +6163,111 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>650</v>
+        <v>141</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>657</v>
+        <v>140</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>654</v>
+        <v>142</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>658</v>
+        <v>140</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>143</v>
+        <v>654</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>144</v>
+        <v>658</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>145</v>
+        <v>655</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>146</v>
+        <v>659</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>728</v>
+        <v>143</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>731</v>
+        <v>144</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>729</v>
+        <v>145</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>739</v>
+        <v>146</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>740</v>
+        <v>731</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>514</v>
+        <v>729</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>515</v>
+        <v>739</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>620</v>
+        <v>730</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>632</v>
+        <v>740</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>621</v>
+        <v>514</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>622</v>
+        <v>515</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>1022</v>
+        <v>620</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>1018</v>
+        <v>632</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>1009</v>
+        <v>621</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>1018</v>
+        <v>622</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>1010</v>
+        <v>1022</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>1018</v>
@@ -6251,7 +6275,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>1018</v>
@@ -6259,23 +6283,23 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>1003</v>
+        <v>1010</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>1004</v>
+        <v>1011</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>1019</v>
@@ -6283,7 +6307,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>1019</v>
@@ -6291,47 +6315,47 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>627</v>
+        <v>1002</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>686</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>684</v>
+        <v>1005</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>687</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>685</v>
+        <v>627</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>938</v>
+        <v>684</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>944</v>
+        <v>687</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>962</v>
+        <v>685</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>944</v>
+        <v>688</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>966</v>
+        <v>938</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>944</v>
@@ -6339,23 +6363,23 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>937</v>
+        <v>962</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>970</v>
+        <v>944</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>963</v>
+        <v>966</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>970</v>
+        <v>944</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>967</v>
+        <v>937</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>970</v>
@@ -6363,23 +6387,23 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>945</v>
+        <v>963</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>968</v>
+        <v>945</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>971</v>
@@ -6387,23 +6411,23 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>939</v>
+        <v>964</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>943</v>
+        <v>971</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>965</v>
+        <v>968</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>943</v>
+        <v>971</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>969</v>
+        <v>939</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>943</v>
@@ -6411,375 +6435,375 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>842</v>
+        <v>965</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>843</v>
+        <v>943</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>1045</v>
+        <v>969</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>1046</v>
+        <v>943</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>834</v>
+        <v>842</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>831</v>
+        <v>843</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>833</v>
+        <v>1045</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>832</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>735</v>
+        <v>834</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>738</v>
+        <v>831</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>147</v>
+        <v>833</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>148</v>
+        <v>832</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>149</v>
+        <v>735</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>150</v>
+        <v>738</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>774</v>
+        <v>179</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>768</v>
+        <v>180</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>775</v>
+        <v>181</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>769</v>
+        <v>182</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>757</v>
+        <v>770</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>763</v>
+        <v>758</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>759</v>
+        <v>763</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
-        <v>790</v>
+        <v>782</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>760</v>
+        <v>764</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
-        <v>783</v>
+        <v>790</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>771</v>
+        <v>760</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
-        <v>784</v>
+        <v>791</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>772</v>
+        <v>761</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>765</v>
+        <v>772</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>766</v>
+        <v>773</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>380</v>
+        <v>787</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>597</v>
+        <v>766</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>385</v>
+        <v>788</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>389</v>
+        <v>767</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>388</v>
+        <v>597</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>1006</v>
+        <v>385</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>1017</v>
+        <v>389</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>1007</v>
+        <v>386</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>1017</v>
+        <v>388</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="B322" s="1" t="s">
         <v>1017</v>
@@ -6787,7 +6811,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>1015</v>
+        <v>1007</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>1017</v>
@@ -6795,7 +6819,7 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>1016</v>
+        <v>1008</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>1017</v>
@@ -6803,119 +6827,119 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>605</v>
+        <v>1015</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>606</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>607</v>
+        <v>1016</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>606</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>412</v>
+        <v>605</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>420</v>
+        <v>606</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>414</v>
+        <v>607</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>421</v>
+        <v>606</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>734</v>
+        <v>414</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>737</v>
+        <v>421</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>390</v>
+        <v>416</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>393</v>
+        <v>422</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>397</v>
+        <v>734</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>394</v>
+        <v>737</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>1031</v>
+        <v>397</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>1074</v>
+        <v>394</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>1032</v>
+        <v>399</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>1075</v>
+        <v>394</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>919</v>
+        <v>1032</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>926</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>918</v>
+        <v>1033</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>915</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="B339" s="1" t="s">
         <v>926</v>
@@ -6923,2009 +6947,2041 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>826</v>
+        <v>918</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>828</v>
+        <v>915</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>183</v>
+        <v>917</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>184</v>
+        <v>926</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>185</v>
+        <v>826</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>186</v>
+        <v>828</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>748</v>
+        <v>183</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>713</v>
+        <v>184</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
-        <v>749</v>
+        <v>185</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>745</v>
+        <v>186</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>818</v>
+        <v>748</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>820</v>
+        <v>713</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>819</v>
+        <v>749</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>821</v>
+        <v>745</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>750</v>
+        <v>818</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>747</v>
+        <v>820</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>751</v>
+        <v>819</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>746</v>
+        <v>821</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>742</v>
+        <v>750</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>741</v>
+        <v>747</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>980</v>
+        <v>751</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>714</v>
+        <v>746</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>858</v>
+        <v>742</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>860</v>
+        <v>741</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>859</v>
+        <v>980</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>860</v>
+        <v>714</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>534</v>
+        <v>858</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>536</v>
+        <v>860</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>871</v>
+        <v>859</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>880</v>
+        <v>860</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>872</v>
+        <v>534</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>881</v>
+        <v>536</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>720</v>
+        <v>872</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>712</v>
+        <v>881</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>1048</v>
+        <v>873</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>1055</v>
+        <v>882</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>1049</v>
+        <v>720</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>1054</v>
+        <v>712</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>401</v>
+        <v>1048</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>404</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>792</v>
+        <v>1049</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>598</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>846</v>
+        <v>792</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>847</v>
+        <v>598</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>835</v>
+        <v>409</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>838</v>
+        <v>410</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>836</v>
+        <v>846</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>839</v>
+        <v>847</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>537</v>
+        <v>835</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>557</v>
+        <v>838</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>538</v>
+        <v>836</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>699</v>
+        <v>839</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>698</v>
+        <v>537</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>563</v>
+        <v>699</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>540</v>
+        <v>698</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>700</v>
+        <v>560</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>697</v>
+        <v>539</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>558</v>
+        <v>700</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>542</v>
+        <v>697</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>701</v>
+        <v>565</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>696</v>
+        <v>541</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>564</v>
+        <v>701</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>544</v>
+        <v>696</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>702</v>
+        <v>561</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>695</v>
+        <v>543</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>559</v>
+        <v>702</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>546</v>
+        <v>695</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>703</v>
+        <v>566</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>694</v>
+        <v>545</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>1079</v>
+        <v>546</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>1088</v>
+        <v>703</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>1080</v>
+        <v>694</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>1089</v>
+        <v>562</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>187</v>
+        <v>1091</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>188</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>189</v>
+        <v>1090</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>190</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>191</v>
+        <v>1079</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>192</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>193</v>
+        <v>1080</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>194</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>651</v>
+        <v>189</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>656</v>
+        <v>190</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>652</v>
+        <v>191</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>660</v>
+        <v>192</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>653</v>
+        <v>193</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>661</v>
+        <v>194</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>199</v>
+        <v>651</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>200</v>
+        <v>656</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>722</v>
+        <v>652</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>725</v>
+        <v>660</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>723</v>
+        <v>653</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>726</v>
+        <v>661</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>724</v>
+        <v>197</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>727</v>
+        <v>198</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>516</v>
+        <v>199</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>517</v>
+        <v>200</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>616</v>
+        <v>722</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>618</v>
+        <v>725</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>617</v>
+        <v>723</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>619</v>
+        <v>726</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>1020</v>
+        <v>724</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>1021</v>
+        <v>727</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>996</v>
+        <v>516</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>999</v>
+        <v>517</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>997</v>
+        <v>616</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>1000</v>
+        <v>618</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>998</v>
+        <v>617</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>1001</v>
+        <v>619</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>981</v>
+        <v>1020</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>985</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>982</v>
+        <v>996</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>987</v>
+        <v>999</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>983</v>
+        <v>997</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>986</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>984</v>
+        <v>998</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>988</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>625</v>
+        <v>981</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>626</v>
+        <v>985</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>680</v>
+        <v>982</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>682</v>
+        <v>987</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>681</v>
+        <v>983</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>683</v>
+        <v>986</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>935</v>
+        <v>984</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>931</v>
+        <v>988</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>948</v>
+        <v>625</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>951</v>
+        <v>626</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>955</v>
+        <v>680</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>958</v>
+        <v>682</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>934</v>
+        <v>681</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>930</v>
+        <v>683</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>949</v>
+        <v>935</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>952</v>
+        <v>931</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>956</v>
+        <v>948</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>959</v>
+        <v>951</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>972</v>
+        <v>955</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>933</v>
+        <v>958</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>973</v>
+        <v>934</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>953</v>
+        <v>930</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
-        <v>974</v>
+        <v>949</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>960</v>
+        <v>952</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
-        <v>936</v>
+        <v>956</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>932</v>
+        <v>959</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
-        <v>950</v>
+        <v>972</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>954</v>
+        <v>933</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
-        <v>957</v>
+        <v>973</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>961</v>
+        <v>953</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
-        <v>837</v>
+        <v>974</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>482</v>
+        <v>960</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
-        <v>1070</v>
+        <v>936</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>1047</v>
+        <v>932</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
-        <v>829</v>
+        <v>950</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>831</v>
+        <v>954</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
-        <v>830</v>
+        <v>957</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>832</v>
+        <v>961</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
-        <v>733</v>
+        <v>837</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>736</v>
+        <v>482</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
-        <v>201</v>
+        <v>1070</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>202</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
-        <v>203</v>
+        <v>829</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>204</v>
+        <v>831</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
-        <v>205</v>
+        <v>830</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>206</v>
+        <v>832</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
-        <v>207</v>
+        <v>733</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>208</v>
+        <v>736</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>160</v>
+        <v>206</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>164</v>
+        <v>210</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>166</v>
+        <v>212</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
-        <v>793</v>
+        <v>221</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>863</v>
+        <v>176</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
-        <v>794</v>
+        <v>222</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>769</v>
+        <v>178</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
-        <v>795</v>
+        <v>223</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>770</v>
+        <v>180</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
-        <v>796</v>
+        <v>224</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>864</v>
+        <v>182</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>757</v>
+        <v>863</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>758</v>
+        <v>769</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>865</v>
+        <v>770</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>763</v>
+        <v>864</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>866</v>
+        <v>758</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>760</v>
+        <v>865</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>867</v>
+        <v>764</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>772</v>
+        <v>866</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>773</v>
+        <v>760</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A460" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>868</v>
+        <v>761</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A461" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>766</v>
+        <v>867</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A462" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>767</v>
+        <v>772</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A463" t="s">
-        <v>379</v>
+        <v>807</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>381</v>
+        <v>773</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A464" t="s">
-        <v>384</v>
+        <v>808</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>382</v>
+        <v>868</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A465" t="s">
-        <v>387</v>
+        <v>809</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>383</v>
+        <v>766</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A466" t="s">
-        <v>994</v>
+        <v>810</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>992</v>
+        <v>767</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A467" t="s">
-        <v>989</v>
+        <v>379</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>993</v>
+        <v>381</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A468" t="s">
-        <v>990</v>
+        <v>384</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>995</v>
+        <v>382</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A469" t="s">
-        <v>991</v>
+        <v>387</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>1012</v>
+        <v>383</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A470" t="s">
-        <v>1013</v>
+        <v>994</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>1014</v>
+        <v>992</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A471" t="s">
-        <v>608</v>
+        <v>989</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>609</v>
+        <v>993</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A472" t="s">
-        <v>610</v>
+        <v>990</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>611</v>
+        <v>995</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A473" t="s">
-        <v>635</v>
+        <v>991</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>638</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A474" t="s">
-        <v>639</v>
+        <v>1013</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>641</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A475" t="s">
-        <v>640</v>
+        <v>608</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>646</v>
+        <v>609</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A476" t="s">
-        <v>411</v>
+        <v>610</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>417</v>
+        <v>611</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A477" t="s">
-        <v>413</v>
+        <v>635</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>418</v>
+        <v>638</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A478" t="s">
-        <v>415</v>
+        <v>639</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>419</v>
+        <v>641</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A479" t="s">
-        <v>732</v>
+        <v>640</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>669</v>
+        <v>646</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A480" t="s">
-        <v>391</v>
+        <v>411</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>392</v>
+        <v>417</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A481" t="s">
-        <v>398</v>
+        <v>413</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>395</v>
+        <v>418</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A482" t="s">
-        <v>400</v>
+        <v>415</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>396</v>
+        <v>419</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A483" t="s">
-        <v>1071</v>
+        <v>732</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>1034</v>
+        <v>669</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A484" t="s">
-        <v>1072</v>
+        <v>391</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>1035</v>
+        <v>392</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
-        <v>1073</v>
+        <v>398</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>1036</v>
+        <v>395</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A486" t="s">
-        <v>922</v>
+        <v>400</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>923</v>
+        <v>396</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A487" t="s">
-        <v>920</v>
+        <v>1071</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>924</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A488" t="s">
-        <v>921</v>
+        <v>1072</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>925</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A489" t="s">
-        <v>827</v>
+        <v>1073</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>825</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A490" t="s">
-        <v>225</v>
+        <v>922</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>226</v>
+        <v>923</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A491" t="s">
-        <v>227</v>
+        <v>920</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>228</v>
+        <v>924</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A492" t="s">
-        <v>752</v>
+        <v>921</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>715</v>
+        <v>925</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A493" t="s">
-        <v>753</v>
+        <v>827</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>590</v>
+        <v>825</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A494" t="s">
-        <v>811</v>
+        <v>225</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>573</v>
+        <v>226</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A495" t="s">
-        <v>754</v>
+        <v>227</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>574</v>
+        <v>228</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A496" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>575</v>
+        <v>715</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A497" t="s">
-        <v>812</v>
+        <v>753</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>814</v>
+        <v>590</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A498" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>815</v>
+        <v>573</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A499" t="s">
-        <v>744</v>
+        <v>754</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>743</v>
+        <v>574</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A500" t="s">
-        <v>979</v>
+        <v>755</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>716</v>
+        <v>575</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A501" t="s">
-        <v>870</v>
+        <v>812</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>861</v>
+        <v>814</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A502" t="s">
-        <v>869</v>
+        <v>813</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>862</v>
+        <v>815</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A503" t="s">
-        <v>533</v>
+        <v>744</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>535</v>
+        <v>743</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A504" t="s">
-        <v>874</v>
+        <v>979</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>879</v>
+        <v>716</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A505" t="s">
-        <v>875</v>
+        <v>870</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>878</v>
+        <v>861</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A506" t="s">
-        <v>876</v>
+        <v>869</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>877</v>
+        <v>862</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A507" t="s">
-        <v>719</v>
+        <v>533</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>709</v>
+        <v>535</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A508" t="s">
-        <v>717</v>
+        <v>874</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>710</v>
+        <v>879</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A509" t="s">
-        <v>718</v>
+        <v>875</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>711</v>
+        <v>878</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A510" t="s">
-        <v>1050</v>
-      </c>
-      <c r="B510" t="s">
-        <v>1052</v>
+        <v>876</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>877</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A511" t="s">
-        <v>1051</v>
-      </c>
-      <c r="B511" t="s">
-        <v>1053</v>
+        <v>719</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>709</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A512" t="s">
-        <v>402</v>
+        <v>717</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>403</v>
+        <v>710</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A513" t="s">
-        <v>407</v>
+        <v>718</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>405</v>
+        <v>711</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A514" t="s">
-        <v>408</v>
-      </c>
-      <c r="B514" s="1" t="s">
-        <v>406</v>
+        <v>1050</v>
+      </c>
+      <c r="B514" t="s">
+        <v>1052</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A515" t="s">
-        <v>229</v>
-      </c>
-      <c r="B515" s="1" t="s">
-        <v>890</v>
+        <v>1051</v>
+      </c>
+      <c r="B515" t="s">
+        <v>1053</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A516" t="s">
-        <v>230</v>
+        <v>402</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>889</v>
+        <v>403</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A517" t="s">
-        <v>231</v>
+        <v>407</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>888</v>
+        <v>405</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A518" t="s">
-        <v>232</v>
+        <v>408</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>887</v>
+        <v>406</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A519" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>886</v>
+        <v>890</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A520" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>885</v>
+        <v>889</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A521" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A522" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>892</v>
+        <v>887</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A523" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>893</v>
+        <v>886</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A524" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>894</v>
+        <v>885</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A525" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>902</v>
+        <v>891</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A526" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A527" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A528" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A529" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A530" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A531" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
     </row>
     <row r="532" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A532" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
     </row>
     <row r="533" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A533" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C533" s="2" t="s">
-        <v>248</v>
+        <v>901</v>
       </c>
     </row>
     <row r="534" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A534" t="s">
-        <v>339</v>
+        <v>244</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C534" s="2" t="s">
-        <v>340</v>
+        <v>898</v>
       </c>
     </row>
     <row r="535" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A535" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C535" s="2" t="s">
-        <v>287</v>
+        <v>899</v>
       </c>
     </row>
     <row r="536" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A536" t="s">
-        <v>479</v>
+        <v>246</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>487</v>
+        <v>900</v>
       </c>
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A537" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>630</v>
+        <v>248</v>
       </c>
       <c r="C537" s="2" t="s">
-        <v>631</v>
+        <v>248</v>
       </c>
     </row>
     <row r="538" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A538" t="s">
-        <v>296</v>
+        <v>339</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>301</v>
+        <v>341</v>
       </c>
       <c r="C538" s="2" t="s">
-        <v>298</v>
+        <v>340</v>
       </c>
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A539" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="C539" s="2" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A540" t="s">
-        <v>252</v>
+        <v>479</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C540" s="2" t="s">
-        <v>253</v>
+        <v>487</v>
       </c>
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A541" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>283</v>
+        <v>630</v>
       </c>
       <c r="C541" s="2" t="s">
-        <v>286</v>
+        <v>631</v>
       </c>
     </row>
     <row r="542" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A542" t="s">
-        <v>272</v>
+        <v>296</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>282</v>
+        <v>301</v>
       </c>
       <c r="C542" s="2" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
     </row>
     <row r="543" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A543" t="s">
-        <v>254</v>
+        <v>297</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="C543" s="2" t="s">
-        <v>255</v>
+        <v>304</v>
       </c>
     </row>
     <row r="544" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A544" t="s">
-        <v>1060</v>
+        <v>252</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>1068</v>
+        <v>253</v>
+      </c>
+      <c r="C544" s="2" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="545" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A545" t="s">
-        <v>319</v>
+        <v>268</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>320</v>
+        <v>283</v>
       </c>
       <c r="C545" s="2" t="s">
-        <v>321</v>
+        <v>286</v>
       </c>
     </row>
     <row r="546" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A546" t="s">
-        <v>1059</v>
+        <v>272</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1067</v>
+        <v>282</v>
+      </c>
+      <c r="C546" s="2" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="547" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A547" t="s">
-        <v>850</v>
+        <v>254</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>853</v>
+        <v>255</v>
+      </c>
+      <c r="C547" s="2" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="548" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A548" t="s">
-        <v>294</v>
+        <v>1060</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C548" s="2" t="s">
-        <v>299</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A549" t="s">
-        <v>295</v>
+        <v>319</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>303</v>
+        <v>320</v>
       </c>
       <c r="C549" s="2" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
     </row>
     <row r="550" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A550" t="s">
-        <v>337</v>
+        <v>1059</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C550" s="2" t="s">
-        <v>347</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="551" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A551" t="s">
-        <v>256</v>
+        <v>850</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C551" s="2" t="s">
-        <v>257</v>
+        <v>853</v>
       </c>
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A552" t="s">
-        <v>1061</v>
+        <v>294</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>1069</v>
+        <v>302</v>
+      </c>
+      <c r="C552" s="2" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A553" t="s">
-        <v>338</v>
+        <v>295</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>344</v>
+        <v>303</v>
       </c>
       <c r="C553" s="2" t="s">
-        <v>348</v>
+        <v>305</v>
       </c>
     </row>
     <row r="554" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A554" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C554" s="2" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="555" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A555" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C555" s="2" t="s">
-        <v>293</v>
+        <v>257</v>
       </c>
     </row>
     <row r="556" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A556" t="s">
-        <v>1058</v>
+        <v>1061</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>1066</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="557" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A557" t="s">
-        <v>851</v>
+        <v>338</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>856</v>
+        <v>344</v>
+      </c>
+      <c r="C557" s="2" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="558" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A558" t="s">
-        <v>260</v>
+        <v>334</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>261</v>
+        <v>346</v>
       </c>
       <c r="C558" s="2" t="s">
-        <v>261</v>
+        <v>354</v>
       </c>
     </row>
     <row r="559" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A559" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="C559" s="2" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
     </row>
     <row r="560" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A560" t="s">
-        <v>275</v>
+        <v>1058</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="C560" s="2" t="s">
-        <v>288</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="561" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A561" t="s">
-        <v>612</v>
+        <v>851</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>613</v>
+        <v>856</v>
       </c>
     </row>
     <row r="562" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A562" t="s">
-        <v>1062</v>
+        <v>260</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>1065</v>
+        <v>261</v>
+      </c>
+      <c r="C562" s="2" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="563" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A563" t="s">
-        <v>614</v>
+        <v>271</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>615</v>
+        <v>276</v>
+      </c>
+      <c r="C563" s="2" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="564" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A564" t="s">
-        <v>848</v>
+        <v>275</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>854</v>
+        <v>281</v>
+      </c>
+      <c r="C564" s="2" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="565" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A565" t="s">
-        <v>849</v>
+        <v>612</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>855</v>
+        <v>613</v>
       </c>
     </row>
     <row r="566" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A566" t="s">
-        <v>370</v>
+        <v>1062</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="C566" s="2" t="s">
-        <v>376</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="567" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A567" t="s">
-        <v>1056</v>
+        <v>614</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>1063</v>
+        <v>615</v>
       </c>
     </row>
     <row r="568" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A568" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
     </row>
     <row r="569" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A569" t="s">
-        <v>336</v>
+        <v>849</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>342</v>
+        <v>855</v>
       </c>
     </row>
     <row r="570" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A570" t="s">
-        <v>262</v>
+        <v>370</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>263</v>
+        <v>375</v>
       </c>
       <c r="C570" s="2" t="s">
-        <v>332</v>
+        <v>376</v>
       </c>
     </row>
     <row r="571" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A571" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="572" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A572" t="s">
-        <v>264</v>
+        <v>852</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C572" s="2" t="s">
-        <v>265</v>
+        <v>857</v>
       </c>
     </row>
     <row r="573" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A573" t="s">
-        <v>270</v>
+        <v>336</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="C573" s="2" t="s">
-        <v>289</v>
+        <v>342</v>
       </c>
     </row>
     <row r="574" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A574" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="C574" s="2" t="s">
-        <v>290</v>
+        <v>332</v>
       </c>
     </row>
     <row r="575" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A575" t="s">
-        <v>266</v>
+        <v>1057</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C575" s="2" t="s">
-        <v>267</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A576" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="C576" s="2" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
     </row>
     <row r="577" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A577" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C577" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="578" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A578" t="s">
+        <v>274</v>
+      </c>
+      <c r="B578" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C578" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="579" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A579" t="s">
+        <v>266</v>
+      </c>
+      <c r="B579" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C579" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="580" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A580" t="s">
+        <v>269</v>
+      </c>
+      <c r="B580" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C580" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="581" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A581" t="s">
+        <v>273</v>
+      </c>
+      <c r="B581" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C581" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="582" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A582" t="s">
         <v>335</v>
       </c>
-      <c r="B578" s="1" t="s">
+      <c r="B582" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C578" s="2" t="s">
+      <c r="C582" s="2" t="s">
         <v>353</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K571">
-    <sortState ref="A2:K578">
+    <sortState ref="A2:K582">
       <sortCondition ref="A1:A571"/>
     </sortState>
   </autoFilter>
@@ -8936,10 +8992,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B15"/>
+      <selection activeCell="A9" sqref="A9:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8992,58 +9048,34 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1077</v>
+        <v>1091</v>
       </c>
       <c r="B9" t="s">
-        <v>1087</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1078</v>
+        <v>1090</v>
       </c>
       <c r="B10" t="s">
-        <v>1086</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1079</v>
+        <v>1093</v>
       </c>
       <c r="B11" t="s">
-        <v>1088</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1080</v>
+        <v>1092</v>
       </c>
       <c r="B12" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>1085</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>1081</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>1082</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1083</v>
+        <v>1097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed crash for morphed biomass press
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -1513,9 +1513,6 @@
     <t>Allows Riftbreakers to collect and utilized morphed biomass from plants and creatues in the metallic biome and utilize it to produce morphium.</t>
   </si>
   <si>
-    <t>gui/menu/research/name/biomass_morpherd_processing</t>
-  </si>
-  <si>
     <t>Morphed Biomass Handling</t>
   </si>
   <si>
@@ -3325,9 +3322,6 @@
     <t>Extracts fluorine from fluor rich mycelium</t>
   </si>
   <si>
-    <t>gui/menu/research/name/biomass_morpherd_processing_lvl_2</t>
-  </si>
-  <si>
     <t>Advanced Morphed Biomass Handling</t>
   </si>
   <si>
@@ -3377,6 +3371,12 @@
   </si>
   <si>
     <t>Captures atmospheric fluorine compounds from atmosphere</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/biomass_morphed_processing</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/biomass_morphed_processing_lvl_2</t>
   </si>
 </sst>
 </file>
@@ -4222,8 +4222,8 @@
   <dimension ref="A1:K592"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4326,15 +4326,15 @@
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4419,18 +4419,18 @@
     </row>
     <row r="21" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>1047</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>1048</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4475,18 +4475,18 @@
     </row>
     <row r="28" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>607</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>608</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4502,63 +4502,63 @@
         <v>49</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>903</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>904</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>905</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4579,10 +4579,10 @@
     </row>
     <row r="41" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -4590,7 +4590,7 @@
         <v>304</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>311</v>
@@ -4598,18 +4598,18 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>627</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>628</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -4721,42 +4721,42 @@
     </row>
     <row r="58" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>578</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>580</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4796,82 +4796,82 @@
     </row>
     <row r="67" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
+        <v>801</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>802</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4919,26 +4919,26 @@
     </row>
     <row r="82" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -5031,10 +5031,10 @@
     </row>
     <row r="96" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>510</v>
+      </c>
+      <c r="B96" s="1" t="s">
         <v>511</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5074,7 +5074,7 @@
         <v>444</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5151,26 +5151,26 @@
     </row>
     <row r="111" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5242,15 +5242,15 @@
         <v>90</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
+        <v>547</v>
+      </c>
+      <c r="B123" s="1" t="s">
         <v>548</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5335,10 +5335,10 @@
     </row>
     <row r="134" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>1044</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5383,18 +5383,18 @@
     </row>
     <row r="140" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
+        <v>602</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>603</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5415,58 +5415,58 @@
     </row>
     <row r="144" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>1075</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>1076</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B150" s="1" t="s">
         <v>1079</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>1080</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5487,10 +5487,10 @@
     </row>
     <row r="153" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5498,7 +5498,7 @@
         <v>305</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>310</v>
@@ -5509,7 +5509,7 @@
         <v>307</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>310</v>
@@ -5520,7 +5520,7 @@
         <v>308</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>310</v>
@@ -5528,10 +5528,10 @@
     </row>
     <row r="157" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5566,7 +5566,7 @@
         <v>290</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5574,7 +5574,7 @@
         <v>291</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -5611,10 +5611,10 @@
     </row>
     <row r="167" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
+        <v>582</v>
+      </c>
+      <c r="B167" s="1" t="s">
         <v>583</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5663,82 +5663,82 @@
     </row>
     <row r="172" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
+        <v>868</v>
+      </c>
+      <c r="B175" s="1" t="s">
         <v>869</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
+        <v>803</v>
+      </c>
+      <c r="B181" s="1" t="s">
         <v>804</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5775,26 +5775,26 @@
     </row>
     <row r="186" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5802,7 +5802,7 @@
         <v>421</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5810,7 +5810,7 @@
         <v>422</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5818,7 +5818,7 @@
         <v>429</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5826,7 +5826,7 @@
         <v>430</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5842,7 +5842,7 @@
         <v>415</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5850,7 +5850,7 @@
         <v>414</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5858,7 +5858,7 @@
         <v>416</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5866,31 +5866,31 @@
         <v>418</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
+        <v>507</v>
+      </c>
+      <c r="B200" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5898,7 +5898,7 @@
         <v>427</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5906,7 +5906,7 @@
         <v>428</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5914,7 +5914,7 @@
         <v>424</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5922,7 +5922,7 @@
         <v>425</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5930,7 +5930,7 @@
         <v>426</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5938,7 +5938,7 @@
         <v>423</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5954,7 +5954,7 @@
         <v>434</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5962,7 +5962,7 @@
         <v>435</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5970,7 +5970,7 @@
         <v>436</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5986,7 +5986,7 @@
         <v>437</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5994,7 +5994,7 @@
         <v>431</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6002,31 +6002,31 @@
         <v>432</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6039,18 +6039,18 @@
     </row>
     <row r="219" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
+        <v>503</v>
+      </c>
+      <c r="B220" s="1" t="s">
         <v>504</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6063,226 +6063,226 @@
     </row>
     <row r="222" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B222" s="1" t="s">
         <v>1060</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>1061</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
+        <v>984</v>
+      </c>
+      <c r="B228" s="1" t="s">
         <v>985</v>
-      </c>
-      <c r="B228" s="1" t="s">
-        <v>986</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
@@ -6327,26 +6327,26 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
@@ -6367,26 +6367,26 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
@@ -6399,282 +6399,282 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
+        <v>600</v>
+      </c>
+      <c r="B266" s="1" t="s">
         <v>601</v>
-      </c>
-      <c r="B266" s="1" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B291" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
+        <v>821</v>
+      </c>
+      <c r="B292" s="1" t="s">
         <v>822</v>
-      </c>
-      <c r="B292" s="1" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B293" s="1" t="s">
         <v>1007</v>
-      </c>
-      <c r="B293" s="1" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.35">
@@ -6823,162 +6823,162 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="331" spans="1:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.35">
@@ -6986,7 +6986,7 @@
         <v>360</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.35">
@@ -7007,58 +7007,58 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
+        <v>977</v>
+      </c>
+      <c r="B344" s="1" t="s">
         <v>978</v>
-      </c>
-      <c r="B344" s="1" t="s">
-        <v>979</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
+        <v>584</v>
+      </c>
+      <c r="B345" s="1" t="s">
         <v>585</v>
-      </c>
-      <c r="B345" s="1" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.35">
@@ -7087,10 +7087,10 @@
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -7119,58 +7119,58 @@
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
@@ -7191,138 +7191,138 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
+        <v>838</v>
+      </c>
+      <c r="B372" s="1" t="s">
         <v>839</v>
-      </c>
-      <c r="B372" s="1" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -7335,10 +7335,10 @@
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -7351,178 +7351,178 @@
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
+        <v>825</v>
+      </c>
+      <c r="B383" s="1" t="s">
         <v>826</v>
-      </c>
-      <c r="B383" s="1" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.35">
@@ -7567,26 +7567,26 @@
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.35">
@@ -7607,263 +7607,263 @@
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B418" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="B418" s="1" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
-        <v>1100</v>
+        <v>1117</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
+        <v>981</v>
+      </c>
+      <c r="B424" s="1" t="s">
         <v>982</v>
-      </c>
-      <c r="B424" s="1" t="s">
-        <v>983</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
+        <v>604</v>
+      </c>
+      <c r="B432" s="1" t="s">
         <v>605</v>
-      </c>
-      <c r="B432" s="1" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B447" s="1" t="s">
         <v>462</v>
@@ -7871,50 +7871,50 @@
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.35">
@@ -8063,162 +8063,162 @@
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A472" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A473" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A474" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A475" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A476" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A477" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A478" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A479" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A480" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A481" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A482" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A483" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A484" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A486" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A487" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A488" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A489" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A490" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A491" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.35">
@@ -8247,82 +8247,82 @@
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A495" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A496" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A497" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A498" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A499" t="s">
+        <v>974</v>
+      </c>
+      <c r="B499" s="1" t="s">
         <v>975</v>
-      </c>
-      <c r="B499" s="1" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A500" t="s">
+        <v>587</v>
+      </c>
+      <c r="B500" s="1" t="s">
         <v>588</v>
-      </c>
-      <c r="B500" s="1" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A501" t="s">
+        <v>589</v>
+      </c>
+      <c r="B501" s="1" t="s">
         <v>590</v>
-      </c>
-      <c r="B501" s="1" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A502" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A503" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A504" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.35">
@@ -8351,10 +8351,10 @@
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A508" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.35">
@@ -8383,58 +8383,58 @@
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A512" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A513" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A514" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A515" t="s">
+        <v>883</v>
+      </c>
+      <c r="B515" s="1" t="s">
         <v>884</v>
-      </c>
-      <c r="B515" s="1" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A516" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A517" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A518" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.35">
@@ -8455,162 +8455,162 @@
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A521" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A522" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A523" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A524" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A525" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A526" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A527" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A528" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A529" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A530" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A531" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="532" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A532" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="533" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A533" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="534" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A534" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="535" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A535" t="s">
+        <v>855</v>
+      </c>
+      <c r="B535" s="1" t="s">
         <v>856</v>
-      </c>
-      <c r="B535" s="1" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="536" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A536" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A537" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="538" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A538" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="539" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A539" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="540" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A540" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="541" spans="1:3" x14ac:dyDescent="0.35">
@@ -8639,13 +8639,13 @@
     </row>
     <row r="544" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A544" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B544" s="1" t="s">
         <v>1086</v>
       </c>
-      <c r="B544" s="1" t="s">
+      <c r="C544" s="2" t="s">
         <v>1087</v>
-      </c>
-      <c r="C544" s="2" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="545" spans="1:3" x14ac:dyDescent="0.35">
@@ -8691,13 +8691,13 @@
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A549" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B549" s="1" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C549" s="2" t="s">
         <v>1083</v>
-      </c>
-      <c r="C549" s="2" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="550" spans="1:3" x14ac:dyDescent="0.35">
@@ -8705,10 +8705,10 @@
         <v>233</v>
       </c>
       <c r="B550" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="C550" s="2" t="s">
         <v>610</v>
-      </c>
-      <c r="C550" s="2" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="551" spans="1:3" x14ac:dyDescent="0.35">
@@ -8779,10 +8779,10 @@
     </row>
     <row r="557" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A557" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="558" spans="1:3" x14ac:dyDescent="0.35">
@@ -8798,18 +8798,18 @@
     </row>
     <row r="559" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A559" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="560" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A560" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="561" spans="1:3" x14ac:dyDescent="0.35">
@@ -8858,10 +8858,10 @@
     </row>
     <row r="565" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A565" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="566" spans="1:3" x14ac:dyDescent="0.35">
@@ -8899,18 +8899,18 @@
     </row>
     <row r="569" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A569" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="570" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A570" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="571" spans="1:3" x14ac:dyDescent="0.35">
@@ -8948,42 +8948,42 @@
     </row>
     <row r="574" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A574" t="s">
+        <v>591</v>
+      </c>
+      <c r="B574" s="1" t="s">
         <v>592</v>
-      </c>
-      <c r="B574" s="1" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="575" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A575" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A576" t="s">
+        <v>593</v>
+      </c>
+      <c r="B576" s="1" t="s">
         <v>594</v>
-      </c>
-      <c r="B576" s="1" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="577" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A577" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="578" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A578" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="579" spans="1:3" x14ac:dyDescent="0.35">
@@ -8999,18 +8999,18 @@
     </row>
     <row r="580" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A580" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="581" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A581" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B581" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="582" spans="1:3" x14ac:dyDescent="0.35">
@@ -9034,10 +9034,10 @@
     </row>
     <row r="584" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A584" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B584" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="585" spans="1:3" x14ac:dyDescent="0.35">
@@ -9086,13 +9086,13 @@
     </row>
     <row r="589" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A589" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B589" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="C589" s="2" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="590" spans="1:3" x14ac:dyDescent="0.35">
@@ -9194,39 +9194,39 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
split plasma charger from fusion plant research
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="1234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="1246">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -3725,6 +3725,42 @@
   </si>
   <si>
     <t>Must be built on top of Carbonium ore deposit. Reagent renders the deposit renewable and does not consume it. Can use only unrefined Carbonium straight from the ground.</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/deep_ionization</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/deep_ionization_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/deep_ionization_lvl_3</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/deep_ionization</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/deep_ionization_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/deep_ionization_lvl_3</t>
+  </si>
+  <si>
+    <t>Deep ionization</t>
+  </si>
+  <si>
+    <t>Advanced deep ionization</t>
+  </si>
+  <si>
+    <t>Extreme ionization</t>
+  </si>
+  <si>
+    <t>High energy physics allows the production of deeply ionized plasmas with strong electrical charge</t>
+  </si>
+  <si>
+    <t>Advanced techiques allow production of even deeper ionized plasmas carriying extreme charge</t>
+  </si>
+  <si>
+    <t>Production of superhot plasmas with total atomic ionization. Any more energy and the plasma becomes instable with fusion reactions emerging.</t>
   </si>
 </sst>
 </file>
@@ -4567,11 +4603,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K648"/>
+  <dimension ref="A1:K654"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D627" sqref="D627"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7315,415 +7351,415 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
-        <v>813</v>
+        <v>1237</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>814</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
-        <v>994</v>
+        <v>1238</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>995</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
-        <v>1092</v>
+        <v>1239</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>1095</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
-        <v>1093</v>
+        <v>813</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>1096</v>
+        <v>814</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
-        <v>805</v>
+        <v>994</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>802</v>
+        <v>995</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
-        <v>804</v>
+        <v>1092</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>803</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
-        <v>706</v>
+        <v>1093</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>709</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
-        <v>144</v>
+        <v>805</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>145</v>
+        <v>802</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
-        <v>146</v>
+        <v>804</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>147</v>
+        <v>803</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
-        <v>148</v>
+        <v>706</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>149</v>
+        <v>709</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>745</v>
+        <v>174</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>739</v>
+        <v>175</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>746</v>
+        <v>176</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>740</v>
+        <v>177</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>747</v>
+        <v>178</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>741</v>
+        <v>179</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>727</v>
+        <v>739</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>728</v>
+        <v>740</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>729</v>
+        <v>741</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>760</v>
+        <v>751</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>761</v>
+        <v>752</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>762</v>
+        <v>753</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>754</v>
+        <v>760</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>742</v>
+        <v>730</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>755</v>
+        <v>761</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>743</v>
+        <v>731</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>756</v>
+        <v>762</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>744</v>
+        <v>732</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>736</v>
+        <v>742</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>737</v>
+        <v>743</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>738</v>
+        <v>744</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>1082</v>
+        <v>757</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>1088</v>
+        <v>736</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>1083</v>
+        <v>758</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>1088</v>
+        <v>737</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>357</v>
+        <v>759</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>568</v>
+        <v>738</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>362</v>
+        <v>1082</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>366</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>363</v>
+        <v>1083</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>365</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>955</v>
+        <v>357</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>966</v>
+        <v>568</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>956</v>
+        <v>362</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>966</v>
+        <v>366</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>957</v>
+        <v>363</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>966</v>
+        <v>365</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>964</v>
+        <v>955</v>
       </c>
       <c r="B386" s="1" t="s">
         <v>966</v>
@@ -7731,7 +7767,7 @@
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
-        <v>965</v>
+        <v>956</v>
       </c>
       <c r="B387" s="1" t="s">
         <v>966</v>
@@ -7739,2194 +7775,2242 @@
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
-        <v>576</v>
+        <v>957</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>577</v>
+        <v>966</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
-        <v>578</v>
+        <v>964</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>577</v>
+        <v>966</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
-        <v>389</v>
+        <v>965</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>397</v>
+        <v>966</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
-        <v>391</v>
+        <v>576</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>398</v>
+        <v>577</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>393</v>
+        <v>578</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>399</v>
+        <v>577</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>705</v>
+        <v>389</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>708</v>
+        <v>397</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>367</v>
+        <v>391</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>370</v>
+        <v>398</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>374</v>
+        <v>393</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>371</v>
+        <v>399</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>376</v>
+        <v>705</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>371</v>
+        <v>708</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>980</v>
+        <v>367</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>1023</v>
+        <v>370</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>981</v>
+        <v>374</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>1024</v>
+        <v>371</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>982</v>
+        <v>376</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>1025</v>
+        <v>371</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>872</v>
+        <v>980</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>879</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>871</v>
+        <v>981</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>868</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>870</v>
+        <v>982</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>879</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>797</v>
+        <v>872</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>799</v>
+        <v>879</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>180</v>
+        <v>871</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>181</v>
+        <v>868</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>182</v>
+        <v>870</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>183</v>
+        <v>879</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>719</v>
+        <v>797</v>
       </c>
       <c r="B406" s="1" t="s">
-        <v>684</v>
+        <v>799</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>720</v>
+        <v>180</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>716</v>
+        <v>181</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>789</v>
+        <v>182</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>791</v>
+        <v>183</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>790</v>
+        <v>719</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>792</v>
+        <v>684</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>722</v>
+        <v>789</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>717</v>
+        <v>791</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>713</v>
+        <v>790</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>712</v>
+        <v>792</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>929</v>
+        <v>721</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>685</v>
+        <v>718</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>829</v>
+        <v>722</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>831</v>
+        <v>717</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>830</v>
+        <v>713</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>831</v>
+        <v>712</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>510</v>
+        <v>929</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>512</v>
+        <v>685</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>842</v>
+        <v>829</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>851</v>
+        <v>831</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
-        <v>843</v>
+        <v>830</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>852</v>
+        <v>831</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
-        <v>844</v>
+        <v>510</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>853</v>
+        <v>512</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
-        <v>691</v>
+        <v>842</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>683</v>
+        <v>851</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
-        <v>997</v>
+        <v>843</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>1004</v>
+        <v>852</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
-        <v>998</v>
+        <v>844</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>1003</v>
+        <v>853</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
-        <v>378</v>
+        <v>691</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>381</v>
+        <v>683</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
-        <v>763</v>
+        <v>997</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>569</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
-        <v>386</v>
+        <v>998</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>387</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
-        <v>817</v>
+        <v>378</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>818</v>
+        <v>381</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
-        <v>806</v>
+        <v>763</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>809</v>
+        <v>569</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
-        <v>807</v>
+        <v>386</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>810</v>
+        <v>387</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
-        <v>513</v>
+        <v>817</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>533</v>
+        <v>818</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
-        <v>1196</v>
+        <v>806</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>1162</v>
+        <v>809</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
-        <v>514</v>
+        <v>807</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>670</v>
+        <v>810</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
-        <v>669</v>
+        <v>513</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>1165</v>
+        <v>533</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>515</v>
+        <v>1196</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>536</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
-        <v>1197</v>
+        <v>514</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>1168</v>
+        <v>670</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
-        <v>516</v>
+        <v>669</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>671</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
-        <v>668</v>
+        <v>515</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>1169</v>
+        <v>536</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
-        <v>517</v>
+        <v>1197</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>534</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
-        <v>1198</v>
+        <v>516</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>1163</v>
+        <v>671</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
-        <v>518</v>
+        <v>668</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>672</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
-        <v>667</v>
+        <v>517</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>1166</v>
+        <v>534</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
-        <v>519</v>
+        <v>1198</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>537</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
-        <v>1199</v>
+        <v>518</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>1170</v>
+        <v>672</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
-        <v>520</v>
+        <v>667</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>673</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
-        <v>666</v>
+        <v>519</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>1171</v>
+        <v>537</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
-        <v>521</v>
+        <v>1199</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>535</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
-        <v>1200</v>
+        <v>520</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>1164</v>
+        <v>673</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
-        <v>522</v>
+        <v>666</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>674</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
-        <v>665</v>
+        <v>521</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>1167</v>
+        <v>535</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
-        <v>1040</v>
+        <v>1200</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>1043</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
-        <v>1039</v>
+        <v>522</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>1044</v>
+        <v>674</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
-        <v>1028</v>
+        <v>665</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>1037</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
-        <v>1029</v>
+        <v>1040</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>1038</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
-        <v>184</v>
+        <v>1039</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>185</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
-        <v>1201</v>
+        <v>1028</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>1209</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
-        <v>1217</v>
+        <v>1029</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>1225</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A460" t="s">
-        <v>190</v>
+        <v>1203</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>191</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A461" t="s">
-        <v>192</v>
+        <v>1219</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>193</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A462" t="s">
-        <v>622</v>
+        <v>188</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>627</v>
+        <v>189</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A463" t="s">
-        <v>623</v>
+        <v>190</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>631</v>
+        <v>191</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A464" t="s">
-        <v>624</v>
+        <v>192</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>632</v>
+        <v>193</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A465" t="s">
-        <v>194</v>
+        <v>622</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>195</v>
+        <v>627</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A466" t="s">
-        <v>1202</v>
+        <v>623</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>1210</v>
+        <v>631</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A467" t="s">
-        <v>1218</v>
+        <v>624</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>1226</v>
+        <v>632</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A468" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A469" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A470" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A471" t="s">
-        <v>693</v>
+        <v>196</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>696</v>
+        <v>197</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A472" t="s">
-        <v>694</v>
+        <v>1204</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>697</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A473" t="s">
-        <v>695</v>
+        <v>1220</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>698</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A474" t="s">
-        <v>1104</v>
+        <v>693</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>493</v>
+        <v>696</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A475" t="s">
-        <v>1105</v>
+        <v>694</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>1087</v>
+        <v>697</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A476" t="s">
-        <v>587</v>
+        <v>695</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>589</v>
+        <v>698</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A477" t="s">
-        <v>588</v>
+        <v>1104</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>590</v>
+        <v>493</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A478" t="s">
-        <v>1050</v>
+        <v>1105</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>1058</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A479" t="s">
-        <v>1051</v>
+        <v>587</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>1059</v>
+        <v>589</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A480" t="s">
-        <v>969</v>
+        <v>588</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>970</v>
+        <v>590</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A481" t="s">
-        <v>945</v>
+        <v>1050</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>948</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A482" t="s">
-        <v>946</v>
+        <v>1051</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>949</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A483" t="s">
-        <v>947</v>
+        <v>969</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>950</v>
+        <v>970</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A484" t="s">
-        <v>930</v>
+        <v>945</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>934</v>
+        <v>948</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
-        <v>931</v>
+        <v>946</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>936</v>
+        <v>949</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A486" t="s">
-        <v>932</v>
+        <v>947</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>935</v>
+        <v>950</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A487" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A488" t="s">
-        <v>596</v>
+        <v>931</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>597</v>
+        <v>936</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A489" t="s">
-        <v>651</v>
+        <v>932</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>653</v>
+        <v>935</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A490" t="s">
-        <v>652</v>
+        <v>933</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>654</v>
+        <v>937</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A491" t="s">
-        <v>888</v>
+        <v>596</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>884</v>
+        <v>597</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A492" t="s">
-        <v>899</v>
+        <v>651</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>902</v>
+        <v>653</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A493" t="s">
-        <v>906</v>
+        <v>652</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>909</v>
+        <v>654</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A494" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A495" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A496" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A497" t="s">
-        <v>921</v>
+        <v>887</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A498" t="s">
-        <v>922</v>
+        <v>900</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A499" t="s">
-        <v>923</v>
+        <v>907</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A500" t="s">
-        <v>889</v>
+        <v>921</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A501" t="s">
-        <v>901</v>
+        <v>922</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A502" t="s">
-        <v>908</v>
+        <v>923</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="503" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A503" t="s">
-        <v>808</v>
+        <v>889</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>459</v>
+        <v>885</v>
       </c>
     </row>
     <row r="504" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A504" t="s">
-        <v>1019</v>
+        <v>901</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>996</v>
+        <v>905</v>
       </c>
     </row>
     <row r="505" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A505" t="s">
-        <v>1090</v>
+        <v>908</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>1089</v>
+        <v>912</v>
       </c>
     </row>
     <row r="506" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A506" t="s">
-        <v>1091</v>
+        <v>1234</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>1094</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="507" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A507" t="s">
-        <v>800</v>
+        <v>1235</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>802</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="508" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A508" t="s">
-        <v>801</v>
+        <v>1236</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>803</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="509" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A509" t="s">
-        <v>704</v>
+        <v>808</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>707</v>
+        <v>459</v>
       </c>
     </row>
     <row r="510" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A510" t="s">
-        <v>198</v>
+        <v>1019</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>199</v>
+        <v>996</v>
       </c>
     </row>
     <row r="511" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A511" t="s">
-        <v>200</v>
+        <v>1090</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>201</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="512" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A512" t="s">
-        <v>202</v>
+        <v>1091</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>203</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="513" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A513" t="s">
-        <v>204</v>
+        <v>800</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>205</v>
+        <v>802</v>
       </c>
     </row>
     <row r="514" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A514" t="s">
-        <v>206</v>
+        <v>801</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>207</v>
+        <v>803</v>
       </c>
     </row>
     <row r="515" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A515" t="s">
-        <v>208</v>
+        <v>704</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>209</v>
+        <v>707</v>
       </c>
     </row>
     <row r="516" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A516" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>157</v>
+        <v>199</v>
       </c>
     </row>
     <row r="517" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A517" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>159</v>
+        <v>201</v>
       </c>
     </row>
     <row r="518" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A518" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>161</v>
+        <v>203</v>
       </c>
     </row>
     <row r="519" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A519" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
     </row>
     <row r="520" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A520" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>165</v>
+        <v>207</v>
       </c>
     </row>
     <row r="521" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A521" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>167</v>
+        <v>209</v>
       </c>
     </row>
     <row r="522" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A522" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="523" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A523" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A524" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="525" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A525" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="526" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A526" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="527" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A527" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="528" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A528" t="s">
-        <v>764</v>
+        <v>216</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>834</v>
+        <v>169</v>
       </c>
     </row>
     <row r="529" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A529" t="s">
-        <v>765</v>
+        <v>217</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>740</v>
+        <v>171</v>
       </c>
     </row>
     <row r="530" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A530" t="s">
-        <v>766</v>
+        <v>218</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>741</v>
+        <v>173</v>
       </c>
     </row>
     <row r="531" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A531" t="s">
-        <v>767</v>
+        <v>219</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>835</v>
+        <v>175</v>
       </c>
     </row>
     <row r="532" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A532" t="s">
-        <v>768</v>
+        <v>220</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>728</v>
+        <v>177</v>
       </c>
     </row>
     <row r="533" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A533" t="s">
-        <v>769</v>
+        <v>221</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>729</v>
+        <v>179</v>
       </c>
     </row>
     <row r="534" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A534" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="535" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A535" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>734</v>
+        <v>740</v>
       </c>
     </row>
     <row r="536" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A536" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>735</v>
+        <v>741</v>
       </c>
     </row>
     <row r="537" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A537" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="538" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A538" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="539" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A539" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="540" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A540" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="541" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A541" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>743</v>
+        <v>734</v>
       </c>
     </row>
     <row r="542" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A542" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>744</v>
+        <v>735</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A543" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="544" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A544" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A545" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A546" t="s">
-        <v>1080</v>
+        <v>776</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>1084</v>
+        <v>838</v>
       </c>
     </row>
     <row r="547" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A547" t="s">
-        <v>1081</v>
+        <v>777</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>1085</v>
+        <v>743</v>
       </c>
     </row>
     <row r="548" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A548" t="s">
-        <v>356</v>
+        <v>778</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>358</v>
+        <v>744</v>
       </c>
     </row>
     <row r="549" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A549" t="s">
-        <v>361</v>
+        <v>779</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>359</v>
+        <v>839</v>
       </c>
     </row>
     <row r="550" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A550" t="s">
-        <v>364</v>
+        <v>780</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>360</v>
+        <v>737</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A551" t="s">
-        <v>943</v>
+        <v>781</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>941</v>
+        <v>738</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A552" t="s">
-        <v>938</v>
+        <v>1080</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>942</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A553" t="s">
-        <v>939</v>
+        <v>1081</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>944</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A554" t="s">
-        <v>940</v>
+        <v>356</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>961</v>
+        <v>358</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A555" t="s">
-        <v>962</v>
+        <v>361</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>963</v>
+        <v>359</v>
       </c>
     </row>
     <row r="556" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A556" t="s">
-        <v>579</v>
+        <v>364</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>580</v>
+        <v>360</v>
       </c>
     </row>
     <row r="557" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A557" t="s">
-        <v>581</v>
+        <v>943</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>582</v>
+        <v>941</v>
       </c>
     </row>
     <row r="558" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A558" t="s">
-        <v>606</v>
+        <v>938</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>609</v>
+        <v>942</v>
       </c>
     </row>
     <row r="559" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A559" t="s">
-        <v>610</v>
+        <v>939</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>612</v>
+        <v>944</v>
       </c>
     </row>
     <row r="560" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A560" t="s">
-        <v>611</v>
+        <v>940</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>617</v>
+        <v>961</v>
       </c>
     </row>
     <row r="561" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A561" t="s">
-        <v>388</v>
+        <v>962</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>394</v>
+        <v>963</v>
       </c>
     </row>
     <row r="562" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A562" t="s">
-        <v>390</v>
+        <v>579</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>395</v>
+        <v>580</v>
       </c>
     </row>
     <row r="563" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A563" t="s">
-        <v>392</v>
+        <v>581</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>396</v>
+        <v>582</v>
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A564" t="s">
-        <v>703</v>
+        <v>606</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>640</v>
+        <v>609</v>
       </c>
     </row>
     <row r="565" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A565" t="s">
-        <v>368</v>
+        <v>610</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>369</v>
+        <v>612</v>
       </c>
     </row>
     <row r="566" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A566" t="s">
-        <v>375</v>
+        <v>611</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>372</v>
+        <v>617</v>
       </c>
     </row>
     <row r="567" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A567" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>373</v>
+        <v>394</v>
       </c>
     </row>
     <row r="568" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A568" t="s">
-        <v>1020</v>
+        <v>390</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>983</v>
+        <v>395</v>
       </c>
     </row>
     <row r="569" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A569" t="s">
-        <v>1021</v>
+        <v>392</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>984</v>
+        <v>396</v>
       </c>
     </row>
     <row r="570" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A570" t="s">
-        <v>1022</v>
+        <v>703</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>985</v>
+        <v>640</v>
       </c>
     </row>
     <row r="571" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A571" t="s">
-        <v>875</v>
+        <v>368</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>876</v>
+        <v>369</v>
       </c>
     </row>
     <row r="572" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A572" t="s">
-        <v>873</v>
+        <v>375</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>877</v>
+        <v>372</v>
       </c>
     </row>
     <row r="573" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A573" t="s">
-        <v>874</v>
+        <v>377</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>878</v>
+        <v>373</v>
       </c>
     </row>
     <row r="574" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A574" t="s">
-        <v>798</v>
+        <v>1020</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>796</v>
+        <v>983</v>
       </c>
     </row>
     <row r="575" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A575" t="s">
-        <v>222</v>
+        <v>1021</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>223</v>
+        <v>984</v>
       </c>
     </row>
     <row r="576" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A576" t="s">
-        <v>224</v>
+        <v>1022</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>225</v>
+        <v>985</v>
       </c>
     </row>
     <row r="577" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A577" t="s">
-        <v>723</v>
+        <v>875</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>686</v>
+        <v>876</v>
       </c>
     </row>
     <row r="578" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A578" t="s">
-        <v>724</v>
+        <v>873</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>561</v>
+        <v>877</v>
       </c>
     </row>
     <row r="579" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A579" t="s">
-        <v>782</v>
+        <v>874</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>544</v>
+        <v>878</v>
       </c>
     </row>
     <row r="580" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A580" t="s">
-        <v>725</v>
+        <v>798</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>545</v>
+        <v>796</v>
       </c>
     </row>
     <row r="581" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A581" t="s">
-        <v>726</v>
+        <v>222</v>
       </c>
       <c r="B581" s="1" t="s">
-        <v>546</v>
+        <v>223</v>
       </c>
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A582" t="s">
-        <v>783</v>
+        <v>224</v>
       </c>
       <c r="B582" s="1" t="s">
-        <v>785</v>
+        <v>225</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A583" t="s">
-        <v>784</v>
+        <v>723</v>
       </c>
       <c r="B583" s="1" t="s">
-        <v>786</v>
+        <v>686</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A584" t="s">
-        <v>715</v>
+        <v>724</v>
       </c>
       <c r="B584" s="1" t="s">
-        <v>714</v>
+        <v>561</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A585" t="s">
-        <v>928</v>
+        <v>782</v>
       </c>
       <c r="B585" s="1" t="s">
-        <v>687</v>
+        <v>544</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A586" t="s">
-        <v>841</v>
+        <v>725</v>
       </c>
       <c r="B586" s="1" t="s">
-        <v>832</v>
+        <v>545</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A587" t="s">
-        <v>840</v>
+        <v>726</v>
       </c>
       <c r="B587" s="1" t="s">
-        <v>833</v>
+        <v>546</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A588" t="s">
-        <v>509</v>
+        <v>783</v>
       </c>
       <c r="B588" s="1" t="s">
-        <v>511</v>
+        <v>785</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A589" t="s">
-        <v>845</v>
+        <v>784</v>
       </c>
       <c r="B589" s="1" t="s">
-        <v>850</v>
+        <v>786</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A590" t="s">
-        <v>846</v>
+        <v>715</v>
       </c>
       <c r="B590" s="1" t="s">
-        <v>849</v>
+        <v>714</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A591" t="s">
-        <v>847</v>
+        <v>928</v>
       </c>
       <c r="B591" s="1" t="s">
-        <v>848</v>
+        <v>687</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A592" t="s">
-        <v>690</v>
+        <v>841</v>
       </c>
       <c r="B592" s="1" t="s">
-        <v>680</v>
+        <v>832</v>
       </c>
     </row>
     <row r="593" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A593" t="s">
-        <v>688</v>
+        <v>840</v>
       </c>
       <c r="B593" s="1" t="s">
-        <v>681</v>
+        <v>833</v>
       </c>
     </row>
     <row r="594" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A594" t="s">
-        <v>689</v>
+        <v>509</v>
       </c>
       <c r="B594" s="1" t="s">
-        <v>682</v>
+        <v>511</v>
       </c>
     </row>
     <row r="595" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A595" t="s">
-        <v>999</v>
+        <v>845</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>1001</v>
+        <v>850</v>
       </c>
     </row>
     <row r="596" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A596" t="s">
-        <v>1000</v>
+        <v>846</v>
       </c>
       <c r="B596" s="1" t="s">
-        <v>1002</v>
+        <v>849</v>
       </c>
     </row>
     <row r="597" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A597" t="s">
-        <v>379</v>
+        <v>847</v>
       </c>
       <c r="B597" s="1" t="s">
-        <v>380</v>
+        <v>848</v>
       </c>
     </row>
     <row r="598" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A598" t="s">
-        <v>384</v>
+        <v>690</v>
       </c>
       <c r="B598" s="1" t="s">
-        <v>382</v>
+        <v>680</v>
       </c>
     </row>
     <row r="599" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A599" t="s">
-        <v>385</v>
+        <v>688</v>
       </c>
       <c r="B599" s="1" t="s">
-        <v>383</v>
+        <v>681</v>
       </c>
     </row>
     <row r="600" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A600" t="s">
-        <v>1073</v>
+        <v>689</v>
       </c>
       <c r="B600" s="1" t="s">
-        <v>1074</v>
-      </c>
-      <c r="C600" s="2" t="s">
-        <v>1075</v>
+        <v>682</v>
       </c>
     </row>
     <row r="601" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A601" t="s">
-        <v>226</v>
+        <v>999</v>
       </c>
       <c r="B601" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C601" s="2" t="s">
-        <v>227</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="602" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A602" t="s">
-        <v>316</v>
+        <v>1000</v>
       </c>
       <c r="B602" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C602" s="2" t="s">
-        <v>317</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="603" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A603" t="s">
-        <v>228</v>
+        <v>379</v>
       </c>
       <c r="B603" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C603" s="2" t="s">
-        <v>266</v>
+        <v>380</v>
       </c>
     </row>
     <row r="604" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A604" t="s">
-        <v>456</v>
+        <v>384</v>
       </c>
       <c r="B604" s="1" t="s">
-        <v>464</v>
+        <v>382</v>
       </c>
     </row>
     <row r="605" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A605" t="s">
-        <v>1078</v>
+        <v>385</v>
       </c>
       <c r="B605" s="1" t="s">
-        <v>1070</v>
-      </c>
-      <c r="C605" s="2" t="s">
-        <v>1071</v>
+        <v>383</v>
       </c>
     </row>
     <row r="606" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A606" t="s">
-        <v>230</v>
+        <v>1073</v>
       </c>
       <c r="B606" s="1" t="s">
-        <v>601</v>
+        <v>1074</v>
       </c>
       <c r="C606" s="2" t="s">
-        <v>602</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="607" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A607" t="s">
-        <v>275</v>
+        <v>226</v>
       </c>
       <c r="B607" s="1" t="s">
-        <v>280</v>
+        <v>227</v>
       </c>
       <c r="C607" s="2" t="s">
-        <v>277</v>
+        <v>227</v>
       </c>
     </row>
     <row r="608" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A608" t="s">
-        <v>276</v>
+        <v>316</v>
       </c>
       <c r="B608" s="1" t="s">
-        <v>279</v>
+        <v>318</v>
       </c>
       <c r="C608" s="2" t="s">
-        <v>283</v>
+        <v>317</v>
       </c>
     </row>
     <row r="609" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A609" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B609" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C609" s="2" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
     </row>
     <row r="610" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A610" t="s">
-        <v>247</v>
+        <v>456</v>
       </c>
       <c r="B610" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C610" s="2" t="s">
-        <v>265</v>
+        <v>464</v>
       </c>
     </row>
     <row r="611" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A611" t="s">
-        <v>251</v>
+        <v>1078</v>
       </c>
       <c r="B611" s="1" t="s">
-        <v>261</v>
+        <v>1070</v>
       </c>
       <c r="C611" s="2" t="s">
-        <v>264</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="612" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A612" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B612" s="1" t="s">
-        <v>234</v>
+        <v>601</v>
       </c>
       <c r="C612" s="2" t="s">
-        <v>234</v>
+        <v>602</v>
       </c>
     </row>
     <row r="613" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A613" t="s">
-        <v>1009</v>
+        <v>275</v>
       </c>
       <c r="B613" s="1" t="s">
-        <v>1017</v>
+        <v>280</v>
+      </c>
+      <c r="C613" s="2" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="614" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A614" t="s">
-        <v>298</v>
+        <v>276</v>
       </c>
       <c r="B614" s="1" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="C614" s="2" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
     </row>
     <row r="615" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A615" t="s">
-        <v>1008</v>
+        <v>231</v>
       </c>
       <c r="B615" s="1" t="s">
-        <v>1016</v>
+        <v>232</v>
+      </c>
+      <c r="C615" s="2" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="616" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A616" t="s">
-        <v>821</v>
+        <v>247</v>
       </c>
       <c r="B616" s="1" t="s">
-        <v>824</v>
+        <v>262</v>
+      </c>
+      <c r="C616" s="2" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="617" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A617" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
       <c r="B617" s="1" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="C617" s="2" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
     </row>
     <row r="618" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A618" t="s">
-        <v>274</v>
+        <v>233</v>
       </c>
       <c r="B618" s="1" t="s">
-        <v>282</v>
+        <v>234</v>
       </c>
       <c r="C618" s="2" t="s">
-        <v>284</v>
+        <v>234</v>
       </c>
     </row>
     <row r="619" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A619" t="s">
-        <v>314</v>
+        <v>1009</v>
       </c>
       <c r="B619" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C619" s="2" t="s">
-        <v>324</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="620" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A620" t="s">
-        <v>235</v>
+        <v>298</v>
       </c>
       <c r="B620" s="1" t="s">
-        <v>236</v>
+        <v>299</v>
       </c>
       <c r="C620" s="2" t="s">
-        <v>236</v>
+        <v>300</v>
       </c>
     </row>
     <row r="621" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A621" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="B621" s="1" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="622" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A622" t="s">
-        <v>315</v>
+        <v>821</v>
       </c>
       <c r="B622" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C622" s="2" t="s">
-        <v>325</v>
+        <v>824</v>
       </c>
     </row>
     <row r="623" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A623" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="B623" s="1" t="s">
-        <v>323</v>
+        <v>281</v>
       </c>
       <c r="C623" s="2" t="s">
-        <v>331</v>
+        <v>278</v>
       </c>
     </row>
     <row r="624" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A624" t="s">
-        <v>237</v>
+        <v>274</v>
       </c>
       <c r="B624" s="1" t="s">
-        <v>238</v>
+        <v>282</v>
       </c>
       <c r="C624" s="2" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
     </row>
     <row r="625" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A625" t="s">
-        <v>1007</v>
+        <v>314</v>
       </c>
       <c r="B625" s="1" t="s">
-        <v>1015</v>
+        <v>320</v>
+      </c>
+      <c r="C625" s="2" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="626" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A626" t="s">
-        <v>822</v>
+        <v>235</v>
       </c>
       <c r="B626" s="1" t="s">
-        <v>827</v>
+        <v>236</v>
+      </c>
+      <c r="C626" s="2" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="627" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A627" t="s">
-        <v>239</v>
+        <v>1010</v>
       </c>
       <c r="B627" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C627" s="2" t="s">
-        <v>240</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="628" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A628" t="s">
-        <v>250</v>
+        <v>315</v>
       </c>
       <c r="B628" s="1" t="s">
-        <v>255</v>
+        <v>321</v>
       </c>
       <c r="C628" s="2" t="s">
-        <v>263</v>
+        <v>325</v>
       </c>
     </row>
     <row r="629" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A629" t="s">
-        <v>254</v>
+        <v>311</v>
       </c>
       <c r="B629" s="1" t="s">
-        <v>260</v>
+        <v>323</v>
       </c>
       <c r="C629" s="2" t="s">
-        <v>267</v>
+        <v>331</v>
       </c>
     </row>
     <row r="630" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A630" t="s">
-        <v>583</v>
+        <v>237</v>
       </c>
       <c r="B630" s="1" t="s">
-        <v>584</v>
+        <v>238</v>
+      </c>
+      <c r="C630" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A631" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="B631" s="1" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A632" t="s">
-        <v>585</v>
+        <v>822</v>
       </c>
       <c r="B632" s="1" t="s">
-        <v>586</v>
+        <v>827</v>
       </c>
     </row>
     <row r="633" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A633" t="s">
-        <v>819</v>
+        <v>239</v>
       </c>
       <c r="B633" s="1" t="s">
-        <v>825</v>
+        <v>240</v>
+      </c>
+      <c r="C633" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A634" t="s">
-        <v>820</v>
+        <v>250</v>
       </c>
       <c r="B634" s="1" t="s">
-        <v>826</v>
+        <v>255</v>
+      </c>
+      <c r="C634" s="2" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A635" t="s">
-        <v>347</v>
+        <v>254</v>
       </c>
       <c r="B635" s="1" t="s">
-        <v>352</v>
+        <v>260</v>
       </c>
       <c r="C635" s="2" t="s">
-        <v>353</v>
+        <v>267</v>
       </c>
     </row>
     <row r="636" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A636" t="s">
-        <v>1005</v>
+        <v>583</v>
       </c>
       <c r="B636" s="1" t="s">
-        <v>1012</v>
+        <v>584</v>
       </c>
     </row>
     <row r="637" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A637" t="s">
-        <v>823</v>
+        <v>1011</v>
       </c>
       <c r="B637" s="1" t="s">
-        <v>828</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="638" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A638" t="s">
-        <v>313</v>
+        <v>585</v>
       </c>
       <c r="B638" s="1" t="s">
-        <v>319</v>
+        <v>586</v>
       </c>
     </row>
     <row r="639" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A639" t="s">
-        <v>241</v>
+        <v>819</v>
       </c>
       <c r="B639" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C639" s="2" t="s">
-        <v>309</v>
+        <v>825</v>
       </c>
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A640" t="s">
-        <v>1006</v>
+        <v>820</v>
       </c>
       <c r="B640" s="1" t="s">
-        <v>1013</v>
+        <v>826</v>
       </c>
     </row>
     <row r="641" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A641" t="s">
-        <v>243</v>
+        <v>347</v>
       </c>
       <c r="B641" s="1" t="s">
-        <v>244</v>
+        <v>352</v>
       </c>
       <c r="C641" s="2" t="s">
-        <v>244</v>
+        <v>353</v>
       </c>
     </row>
     <row r="642" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A642" t="s">
-        <v>249</v>
+        <v>1005</v>
       </c>
       <c r="B642" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C642" s="2" t="s">
-        <v>268</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="643" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A643" t="s">
-        <v>253</v>
+        <v>823</v>
       </c>
       <c r="B643" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C643" s="2" t="s">
-        <v>269</v>
+        <v>828</v>
       </c>
     </row>
     <row r="644" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A644" t="s">
-        <v>245</v>
+        <v>313</v>
       </c>
       <c r="B644" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C644" s="2" t="s">
-        <v>246</v>
+        <v>319</v>
       </c>
     </row>
     <row r="645" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A645" t="s">
-        <v>1069</v>
+        <v>241</v>
       </c>
       <c r="B645" s="1" t="s">
-        <v>1072</v>
+        <v>242</v>
       </c>
       <c r="C645" s="2" t="s">
-        <v>1076</v>
+        <v>309</v>
       </c>
     </row>
     <row r="646" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A646" t="s">
-        <v>248</v>
+        <v>1006</v>
       </c>
       <c r="B646" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C646" s="2" t="s">
-        <v>270</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="647" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A647" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B647" s="1" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C647" s="2" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
     </row>
     <row r="648" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A648" t="s">
+        <v>249</v>
+      </c>
+      <c r="B648" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C648" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="649" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A649" t="s">
+        <v>253</v>
+      </c>
+      <c r="B649" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C649" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="650" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A650" t="s">
+        <v>245</v>
+      </c>
+      <c r="B650" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C650" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="651" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A651" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B651" s="1" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C651" s="2" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="652" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A652" t="s">
+        <v>248</v>
+      </c>
+      <c r="B652" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C652" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="653" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A653" t="s">
+        <v>252</v>
+      </c>
+      <c r="B653" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C653" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="654" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A654" t="s">
         <v>312</v>
       </c>
-      <c r="B648" s="1" t="s">
+      <c r="B654" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="C648" s="2" t="s">
+      <c r="C654" s="2" t="s">
         <v>330</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K647">
-    <sortState ref="A2:K648">
+    <sortState ref="A2:K654">
       <sortCondition ref="A1:A647"/>
     </sortState>
   </autoFilter>
@@ -9940,7 +10024,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B30"/>
+      <selection activeCell="A14" sqref="A14:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
integrated cryo station level 2
</commit_message>
<xml_diff>
--- a/gui/rebalance_localizations.xlsx
+++ b/gui/rebalance_localizations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="1338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="1342">
   <si>
     <t>ENGLISH</t>
   </si>
@@ -4037,6 +4037,18 @@
   </si>
   <si>
     <t>gui/menu/research/description/regenerating_extractor</t>
+  </si>
+  <si>
+    <t>gui/menu/research/name/cryo_technology_lvl_2</t>
+  </si>
+  <si>
+    <t>gui/menu/research/description/cryo_technology_lvl_2</t>
+  </si>
+  <si>
+    <t>Advanced Cryo Technology</t>
+  </si>
+  <si>
+    <t>Improved harnessing of ferdonite allows even more effective application of specialized ground cooling. This creates larger areas usable for buildings in magma biome</t>
   </si>
 </sst>
 </file>
@@ -4879,11 +4891,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K700"/>
+  <dimension ref="A1:K702"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7731,23 +7743,23 @@
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
-        <v>888</v>
+        <v>1339</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>1142</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
-        <v>910</v>
+        <v>888</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>1146</v>
@@ -7755,23 +7767,23 @@
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
-        <v>887</v>
+        <v>914</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
-        <v>911</v>
+        <v>887</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>1147</v>
@@ -7779,23 +7791,23 @@
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
-        <v>893</v>
+        <v>915</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>1145</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
-        <v>912</v>
+        <v>893</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>1148</v>
@@ -7803,23 +7815,23 @@
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
-        <v>889</v>
+        <v>916</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>1143</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
-        <v>913</v>
+        <v>889</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>1149</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>1149</v>
@@ -7827,407 +7839,407 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
-        <v>1233</v>
+        <v>917</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>1239</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
-        <v>810</v>
+        <v>1235</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>811</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
-        <v>991</v>
+        <v>810</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>992</v>
+        <v>811</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
-        <v>1088</v>
+        <v>991</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>1091</v>
+        <v>992</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
-        <v>802</v>
+        <v>1089</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>799</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
-        <v>703</v>
+        <v>801</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>706</v>
+        <v>800</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
-        <v>143</v>
+        <v>703</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>144</v>
+        <v>706</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="387" spans="1:2